<commit_message>
Updated P&H plant, metal and area analysis and corresponding dashboard and csv files.
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15720" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="147">
   <si>
     <t>Unit</t>
   </si>
@@ -472,6 +472,15 @@
   </si>
   <si>
     <t>capacity_credit_wind_constant_q1</t>
+  </si>
+  <si>
+    <t>investment_hv_net_high</t>
+  </si>
+  <si>
+    <t>investment_hv_net_low</t>
+  </si>
+  <si>
+    <t>investment_hv_net_per_turbine</t>
   </si>
 </sst>
 </file>
@@ -652,7 +661,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -942,8 +951,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="446">
+  <cellStyleXfs count="452">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1390,8 +1425,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1651,6 +1692,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1660,8 +1708,11 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="446">
+  <cellStyles count="452">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1898,6 +1949,9 @@
     <cellStyle name="Followed Hyperlink" xfId="441" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="443" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="445" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="447" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="449" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2107,6 +2161,9 @@
     <cellStyle name="Hyperlink" xfId="440" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="442" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="444" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="446" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="448" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="450" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -3514,11 +3571,9 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:P96"/>
+  <dimension ref="A2:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3566,16 +3621,16 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="57" customHeight="1">
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="148" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="144"/>
-      <c r="D5" s="144"/>
-      <c r="E5" s="144"/>
-      <c r="F5" s="144"/>
-      <c r="G5" s="144"/>
-      <c r="H5" s="144"/>
-      <c r="I5" s="145"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="149"/>
+      <c r="I5" s="150"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
@@ -5596,7 +5651,7 @@
         <v>0</v>
       </c>
       <c r="M85" s="35" t="str">
-        <f t="shared" ref="M85:M95" si="9">IF(L85=TRUE," ","Please set value")</f>
+        <f t="shared" ref="M85:M98" si="9">IF(L85=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N85" s="88"/>
@@ -5618,7 +5673,7 @@
       <c r="J86"/>
       <c r="K86"/>
       <c r="L86" s="40" t="b">
-        <f t="shared" ref="L86:L95" si="10">IF(COUNTBLANK(E86)=1,FALSE,TRUE)</f>
+        <f t="shared" ref="L86:L98" si="10">IF(COUNTBLANK(E86)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M86" s="35" t="str">
@@ -5734,45 +5789,69 @@
         <v>106</v>
       </c>
     </row>
-    <row r="91" spans="2:15">
+    <row r="91" spans="2:15" ht="16" thickBot="1">
       <c r="B91" s="31"/>
-      <c r="E91" s="137"/>
-      <c r="G91" s="136"/>
-      <c r="I91" s="7"/>
-      <c r="L91" s="142"/>
-      <c r="M91" s="110"/>
+      <c r="C91" t="s">
+        <v>145</v>
+      </c>
+      <c r="D91"/>
+      <c r="E91" s="151"/>
+      <c r="F91"/>
+      <c r="G91" s="61"/>
+      <c r="H91"/>
+      <c r="I91" s="144"/>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="L91" s="40" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M91" s="35" t="str">
+        <f t="shared" si="9"/>
+        <v>Please set value</v>
+      </c>
       <c r="N91" s="88"/>
-      <c r="O91" s="15"/>
+      <c r="O91" s="146" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="92" spans="2:15" ht="16" thickBot="1">
-      <c r="B92" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="138"/>
-      <c r="F92" s="4"/>
-      <c r="G92" s="139"/>
-      <c r="H92" s="4"/>
-      <c r="I92" s="140"/>
-      <c r="J92" s="4"/>
-      <c r="K92" s="4"/>
-      <c r="L92" s="141"/>
-      <c r="M92" s="104"/>
+      <c r="B92" s="31"/>
+      <c r="C92" t="s">
+        <v>144</v>
+      </c>
+      <c r="D92"/>
+      <c r="E92" s="69"/>
+      <c r="F92"/>
+      <c r="G92" s="61"/>
+      <c r="H92"/>
+      <c r="I92" s="60"/>
+      <c r="J92"/>
+      <c r="K92"/>
+      <c r="L92" s="40" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M92" s="35" t="str">
+        <f t="shared" si="9"/>
+        <v>Please set value</v>
+      </c>
       <c r="N92" s="88"/>
-      <c r="O92" s="15"/>
+      <c r="O92" s="135" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="93" spans="2:15" ht="16" thickBot="1">
       <c r="B93" s="31"/>
-      <c r="C93" t="s">
-        <v>141</v>
+      <c r="C93" s="132" t="s">
+        <v>146</v>
       </c>
       <c r="D93"/>
-      <c r="E93" s="67"/>
+      <c r="E93" s="143"/>
       <c r="F93"/>
       <c r="G93" s="61"/>
       <c r="H93"/>
-      <c r="I93" s="60"/>
+      <c r="I93" s="145"/>
       <c r="J93"/>
       <c r="K93"/>
       <c r="L93" s="40" t="b">
@@ -5784,84 +5863,138 @@
         <v>Please set value</v>
       </c>
       <c r="N93" s="88"/>
-      <c r="O93" s="135" t="s">
+      <c r="O93" s="147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="94" spans="2:15">
+      <c r="B94" s="31"/>
+      <c r="E94" s="137"/>
+      <c r="G94" s="136"/>
+      <c r="I94" s="7"/>
+      <c r="L94" s="142"/>
+      <c r="M94" s="110"/>
+      <c r="N94" s="88"/>
+      <c r="O94" s="15"/>
+    </row>
+    <row r="95" spans="2:15" ht="16" thickBot="1">
+      <c r="B95" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="138"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="139"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="140"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="141"/>
+      <c r="M95" s="104"/>
+      <c r="N95" s="88"/>
+      <c r="O95" s="15"/>
+    </row>
+    <row r="96" spans="2:15" ht="16" thickBot="1">
+      <c r="B96" s="31"/>
+      <c r="C96" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="94" spans="2:15" ht="16" thickBot="1">
-      <c r="B94" s="31"/>
-      <c r="C94" t="s">
-        <v>142</v>
-      </c>
-      <c r="D94"/>
-      <c r="E94" s="67"/>
-      <c r="F94"/>
-      <c r="G94" s="61"/>
-      <c r="H94"/>
-      <c r="I94" s="60"/>
-      <c r="J94"/>
-      <c r="K94"/>
-      <c r="L94" s="40" t="b">
+      <c r="D96"/>
+      <c r="E96" s="67"/>
+      <c r="F96"/>
+      <c r="G96" s="61"/>
+      <c r="H96"/>
+      <c r="I96" s="60"/>
+      <c r="J96"/>
+      <c r="K96"/>
+      <c r="L96" s="40" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M94" s="35" t="str">
+      <c r="M96" s="35" t="str">
         <f t="shared" si="9"/>
         <v>Please set value</v>
       </c>
-      <c r="N94" s="88"/>
-      <c r="O94" s="135" t="s">
+      <c r="N96" s="88"/>
+      <c r="O96" s="135" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="97" spans="2:15" ht="16" thickBot="1">
+      <c r="B97" s="31"/>
+      <c r="C97" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="95" spans="2:15" ht="16" thickBot="1">
-      <c r="B95" s="31"/>
-      <c r="C95" t="s">
-        <v>143</v>
-      </c>
-      <c r="D95"/>
-      <c r="E95" s="67"/>
-      <c r="F95"/>
-      <c r="G95" s="61"/>
-      <c r="H95"/>
-      <c r="I95" s="60"/>
-      <c r="J95"/>
-      <c r="K95"/>
-      <c r="L95" s="40" t="b">
+      <c r="D97"/>
+      <c r="E97" s="67"/>
+      <c r="F97"/>
+      <c r="G97" s="61"/>
+      <c r="H97"/>
+      <c r="I97" s="60"/>
+      <c r="J97"/>
+      <c r="K97"/>
+      <c r="L97" s="40" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M95" s="35" t="str">
+      <c r="M97" s="35" t="str">
         <f t="shared" si="9"/>
         <v>Please set value</v>
       </c>
-      <c r="N95" s="88"/>
-      <c r="O95" s="135" t="s">
+      <c r="N97" s="88"/>
+      <c r="O97" s="135" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="98" spans="2:15" ht="16" thickBot="1">
+      <c r="B98" s="31"/>
+      <c r="C98" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="96" spans="2:15" ht="16" thickBot="1">
-      <c r="B96" s="44"/>
-      <c r="C96" s="36"/>
-      <c r="D96" s="36"/>
-      <c r="E96" s="54"/>
-      <c r="F96" s="36"/>
-      <c r="G96" s="36"/>
-      <c r="H96" s="36"/>
-      <c r="I96" s="36"/>
-      <c r="J96" s="36"/>
-      <c r="K96" s="36"/>
-      <c r="L96" s="36"/>
-      <c r="M96" s="36"/>
-      <c r="N96" s="31"/>
-      <c r="O96" s="7"/>
+      <c r="D98"/>
+      <c r="E98" s="67"/>
+      <c r="F98"/>
+      <c r="G98" s="61"/>
+      <c r="H98"/>
+      <c r="I98" s="60"/>
+      <c r="J98"/>
+      <c r="K98"/>
+      <c r="L98" s="40" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M98" s="35" t="str">
+        <f t="shared" si="9"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N98" s="88"/>
+      <c r="O98" s="135" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="2:15" ht="16" thickBot="1">
+      <c r="B99" s="44"/>
+      <c r="C99" s="36"/>
+      <c r="D99" s="36"/>
+      <c r="E99" s="54"/>
+      <c r="F99" s="36"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="36"/>
+      <c r="I99" s="36"/>
+      <c r="J99" s="36"/>
+      <c r="K99" s="36"/>
+      <c r="L99" s="36"/>
+      <c r="M99" s="36"/>
+      <c r="N99" s="31"/>
+      <c r="O99" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="B2"/>
   <mergeCells count="1">
     <mergeCell ref="B5:I5"/>
   </mergeCells>
-  <conditionalFormatting sqref="L76:L82 L39:L44 L71:L73 L18:L36 L47:L52 L54 L56:L67 L89:L95">
+  <conditionalFormatting sqref="L76:L82 L39:L44 L71:L73 L18:L36 L47:L52 L54 L56:L67 L89:L98">
     <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -5881,7 +6014,7 @@
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E68:E96 E39:E43 E46:E58 D59:D62 E63:E65">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E68:E99 E39:E43 E46:E58 D59:D62 E63:E65">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6196,10 +6329,10 @@
     </row>
     <row r="5" spans="1:48">
       <c r="A5" s="117"/>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="148" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="145"/>
+      <c r="C5" s="150"/>
       <c r="D5" s="117"/>
       <c r="E5" s="115"/>
       <c r="F5" s="115"/>
@@ -12018,10 +12151,10 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:E119"/>
+  <dimension ref="B1:E122"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93:E95"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13068,7 +13201,7 @@
         <v>5</v>
       </c>
       <c r="E71" s="107" t="e">
-        <f t="shared" ref="E71:E95" si="3">IF(COUNTBLANK(B71)=0,"- "&amp;B71&amp;" = "&amp;FIXED(C71,D71,1),"")</f>
+        <f t="shared" ref="E71:E98" si="3">IF(COUNTBLANK(B71)=0,"- "&amp;B71&amp;" = "&amp;FIXED(C71,D71,1),"")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -13388,28 +13521,50 @@
       </c>
     </row>
     <row r="91" spans="2:5">
-      <c r="B91" s="31"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
-      <c r="E91" s="32"/>
+      <c r="B91" s="106" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C91)=0,Dashboard!C91,"")</f>
+        <v>investment_hv_net_low</v>
+      </c>
+      <c r="C91" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E91)=0,Dashboard!E91,"")</f>
+        <v/>
+      </c>
+      <c r="D91" s="41">
+        <v>2</v>
+      </c>
+      <c r="E91" s="107" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="92" spans="2:5">
-      <c r="B92" s="31"/>
-      <c r="C92" s="7"/>
-      <c r="D92" s="7"/>
-      <c r="E92" s="32"/>
+      <c r="B92" s="106" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C92)=0,Dashboard!C92,"")</f>
+        <v>investment_hv_net_high</v>
+      </c>
+      <c r="C92" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E92)=0,Dashboard!E92,"")</f>
+        <v/>
+      </c>
+      <c r="D92" s="41">
+        <v>2</v>
+      </c>
+      <c r="E92" s="107" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="93" spans="2:5">
       <c r="B93" s="106" t="str">
         <f>IF(COUNTBLANK(Dashboard!C93)=0,Dashboard!C93,"")</f>
-        <v>capacity_credit_wind_constant_p1</v>
+        <v>investment_hv_net_per_turbine</v>
       </c>
       <c r="C93" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E93)=0,Dashboard!E93,"")</f>
         <v/>
       </c>
-      <c r="D93" s="35">
-        <v>0</v>
+      <c r="D93" s="41">
+        <v>1</v>
       </c>
       <c r="E93" s="107" t="e">
         <f t="shared" si="3"/>
@@ -13417,56 +13572,73 @@
       </c>
     </row>
     <row r="94" spans="2:5">
-      <c r="B94" s="106" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C94)=0,Dashboard!C94,"")</f>
-        <v>capacity_credit_wind_constant_p2</v>
-      </c>
-      <c r="C94" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E94)=0,Dashboard!E94,"")</f>
+      <c r="B94" s="31"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="32"/>
+    </row>
+    <row r="95" spans="2:5">
+      <c r="B95" s="31"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="32"/>
+    </row>
+    <row r="96" spans="2:5">
+      <c r="B96" s="106" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C96)=0,Dashboard!C96,"")</f>
+        <v>capacity_credit_wind_constant_p1</v>
+      </c>
+      <c r="C96" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E96)=0,Dashboard!E96,"")</f>
         <v/>
       </c>
-      <c r="D94" s="35">
+      <c r="D96" s="35">
         <v>0</v>
       </c>
-      <c r="E94" s="107" t="e">
+      <c r="E96" s="107" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="95" spans="2:5">
-      <c r="B95" s="106" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C95)=0,Dashboard!C95,"")</f>
-        <v>capacity_credit_wind_constant_q1</v>
-      </c>
-      <c r="C95" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E95)=0,Dashboard!E95,"")</f>
+    <row r="97" spans="2:5">
+      <c r="B97" s="106" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C97)=0,Dashboard!C97,"")</f>
+        <v>capacity_credit_wind_constant_p2</v>
+      </c>
+      <c r="C97" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E97)=0,Dashboard!E97,"")</f>
         <v/>
       </c>
-      <c r="D95" s="35">
+      <c r="D97" s="35">
         <v>0</v>
       </c>
-      <c r="E95" s="107" t="e">
+      <c r="E97" s="107" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="96" spans="2:5" ht="16" thickBot="1">
-      <c r="B96" s="44"/>
-      <c r="C96" s="99"/>
-      <c r="D96" s="36"/>
-      <c r="E96" s="100"/>
-    </row>
-    <row r="97" spans="2:5">
-      <c r="B97" s="91"/>
-      <c r="E97" s="92"/>
-    </row>
     <row r="98" spans="2:5">
-      <c r="B98" s="91"/>
-      <c r="E98" s="92"/>
-    </row>
-    <row r="99" spans="2:5">
-      <c r="B99" s="91"/>
-      <c r="E99" s="92"/>
+      <c r="B98" s="106" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C98)=0,Dashboard!C98,"")</f>
+        <v>capacity_credit_wind_constant_q1</v>
+      </c>
+      <c r="C98" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E98)=0,Dashboard!E98,"")</f>
+        <v/>
+      </c>
+      <c r="D98" s="35">
+        <v>0</v>
+      </c>
+      <c r="E98" s="107" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="16" thickBot="1">
+      <c r="B99" s="44"/>
+      <c r="C99" s="99"/>
+      <c r="D99" s="36"/>
+      <c r="E99" s="100"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="91"/>
@@ -13547,6 +13719,18 @@
     <row r="119" spans="2:5">
       <c r="B119" s="91"/>
       <c r="E119" s="92"/>
+    </row>
+    <row r="120" spans="2:5">
+      <c r="B120" s="91"/>
+      <c r="E120" s="92"/>
+    </row>
+    <row r="121" spans="2:5">
+      <c r="B121" s="91"/>
+      <c r="E121" s="92"/>
+    </row>
+    <row r="122" spans="2:5">
+      <c r="B122" s="91"/>
+      <c r="E122" s="92"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13564,11 +13748,9 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:A72"/>
+  <dimension ref="A1:A75"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
-    </sheetView>
+    <sheetView topLeftCell="A64" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -13991,19 +14173,37 @@
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="35" t="e">
-        <f>'compile results'!E93</f>
+        <f>'compile results'!E96</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="35" t="e">
-        <f>'compile results'!E94</f>
+        <f>'compile results'!E97</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="35" t="e">
-        <f>'compile results'!E95</f>
+        <f>'compile results'!E98</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="35" t="e">
+        <f>'compile results'!E91</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="35" t="e">
+        <f>'compile results'!E92</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="35" t="e">
+        <f>'compile results'!E93</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Published state of ETDataset on 21 July 2014.
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500" activeTab="2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="151">
   <si>
     <t>Unit</t>
   </si>
@@ -487,6 +487,12 @@
   </si>
   <si>
     <t>ETM key - Set to true if you want your dataset to run in etmodel</t>
+  </si>
+  <si>
+    <t>capacity_credit_wind_minimum</t>
+  </si>
+  <si>
+    <t>capacity_credit_wind_maximum</t>
   </si>
 </sst>
 </file>
@@ -984,7 +990,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="456">
+  <cellStyleXfs count="462">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1441,8 +1447,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1715,6 +1727,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1725,7 +1740,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="456">
+  <cellStyles count="462">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1967,6 +1982,9 @@
     <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="453" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="461" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2181,6 +2199,9 @@
     <cellStyle name="Hyperlink" xfId="450" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="452" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="454" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="456" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="458" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="460" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -3588,7 +3609,7 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:P99"/>
+  <dimension ref="A2:P101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3638,16 +3659,16 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="57" customHeight="1">
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="151" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="151"/>
-      <c r="D5" s="151"/>
-      <c r="E5" s="151"/>
-      <c r="F5" s="151"/>
-      <c r="G5" s="151"/>
-      <c r="H5" s="151"/>
-      <c r="I5" s="152"/>
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
+      <c r="E5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="152"/>
+      <c r="H5" s="152"/>
+      <c r="I5" s="153"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
@@ -5668,7 +5689,7 @@
         <v>0</v>
       </c>
       <c r="M85" s="35" t="str">
-        <f t="shared" ref="M85:M98" si="9">IF(L85=TRUE," ","Please set value")</f>
+        <f t="shared" ref="M85:M100" si="9">IF(L85=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N85" s="85"/>
@@ -5690,7 +5711,7 @@
       <c r="J86"/>
       <c r="K86"/>
       <c r="L86" s="40" t="b">
-        <f t="shared" ref="L86:L98" si="10">IF(COUNTBLANK(E86)=1,FALSE,TRUE)</f>
+        <f t="shared" ref="L86:L100" si="10">IF(COUNTBLANK(E86)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M86" s="35" t="str">
@@ -5991,26 +6012,78 @@
       </c>
     </row>
     <row r="99" spans="2:15" ht="16" thickBot="1">
-      <c r="B99" s="44"/>
-      <c r="C99" s="36"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="52"/>
-      <c r="F99" s="36"/>
-      <c r="G99" s="36"/>
-      <c r="H99" s="36"/>
-      <c r="I99" s="36"/>
-      <c r="J99" s="36"/>
-      <c r="K99" s="36"/>
-      <c r="L99" s="36"/>
-      <c r="M99" s="36"/>
-      <c r="N99" s="31"/>
-      <c r="O99" s="7"/>
+      <c r="B99" s="31"/>
+      <c r="C99" t="s">
+        <v>149</v>
+      </c>
+      <c r="D99"/>
+      <c r="E99" s="66"/>
+      <c r="F99"/>
+      <c r="G99" s="58"/>
+      <c r="H99"/>
+      <c r="I99" s="57"/>
+      <c r="J99"/>
+      <c r="K99"/>
+      <c r="L99" s="40" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M99" s="35" t="str">
+        <f t="shared" si="9"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N99" s="85"/>
+      <c r="O99" s="132" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="100" spans="2:15" ht="16" thickBot="1">
+      <c r="B100" s="31"/>
+      <c r="C100" t="s">
+        <v>150</v>
+      </c>
+      <c r="D100"/>
+      <c r="E100" s="150"/>
+      <c r="F100"/>
+      <c r="G100" s="58"/>
+      <c r="H100"/>
+      <c r="I100" s="142"/>
+      <c r="J100"/>
+      <c r="K100"/>
+      <c r="L100" s="40" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M100" s="35" t="str">
+        <f t="shared" si="9"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N100" s="85"/>
+      <c r="O100" s="132" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="101" spans="2:15" ht="16" thickBot="1">
+      <c r="B101" s="44"/>
+      <c r="C101" s="36"/>
+      <c r="D101" s="36"/>
+      <c r="E101" s="52"/>
+      <c r="F101" s="36"/>
+      <c r="G101" s="36"/>
+      <c r="H101" s="36"/>
+      <c r="I101" s="36"/>
+      <c r="J101" s="36"/>
+      <c r="K101" s="36"/>
+      <c r="L101" s="36"/>
+      <c r="M101" s="36"/>
+      <c r="N101" s="31"/>
+      <c r="O101" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:I5"/>
   </mergeCells>
-  <conditionalFormatting sqref="L76:L82 L39:L44 L71:L73 L18:L36 L47:L52 L54 L56:L67 L89:L98">
+  <conditionalFormatting sqref="L76:L82 L39:L44 L71:L73 L18:L36 L47:L52 L54 L56:L67 L89:L100">
     <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -6030,7 +6103,7 @@
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E68:E99 E39:E43 E46:E58 D59:D62 E63:E65">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E68:E101 E39:E43 E46:E58 D59:D62 E63:E65">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6345,10 +6418,10 @@
     </row>
     <row r="5" spans="1:48">
       <c r="A5" s="114"/>
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="151" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="152"/>
+      <c r="C5" s="153"/>
       <c r="D5" s="114"/>
       <c r="E5" s="112"/>
       <c r="F5" s="112"/>
@@ -12167,10 +12240,10 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:E122"/>
+  <dimension ref="B1:E124"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13217,7 +13290,7 @@
         <v>5</v>
       </c>
       <c r="E71" s="104" t="e">
-        <f t="shared" ref="E71:E98" si="3">IF(COUNTBLANK(B71)=0,"- "&amp;B71&amp;" = "&amp;FIXED(C71,D71,1),"")</f>
+        <f t="shared" ref="E71:E100" si="3">IF(COUNTBLANK(B71)=0,"- "&amp;B71&amp;" = "&amp;FIXED(C71,D71,1),"")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -13650,19 +13723,43 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="99" spans="2:5" ht="16" thickBot="1">
-      <c r="B99" s="44"/>
-      <c r="C99" s="96"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="97"/>
+    <row r="99" spans="2:5">
+      <c r="B99" s="103" t="s">
+        <v>149</v>
+      </c>
+      <c r="C99" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E99)=0,Dashboard!E99,"")</f>
+        <v/>
+      </c>
+      <c r="D99" s="41">
+        <v>2</v>
+      </c>
+      <c r="E99" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="100" spans="2:5">
-      <c r="B100" s="88"/>
-      <c r="E100" s="89"/>
-    </row>
-    <row r="101" spans="2:5">
-      <c r="B101" s="88"/>
-      <c r="E101" s="89"/>
+      <c r="B100" s="103" t="s">
+        <v>150</v>
+      </c>
+      <c r="C100" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E100)=0,Dashboard!E100,"")</f>
+        <v/>
+      </c>
+      <c r="D100" s="41">
+        <v>2</v>
+      </c>
+      <c r="E100" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" ht="16" thickBot="1">
+      <c r="B101" s="44"/>
+      <c r="C101" s="96"/>
+      <c r="D101" s="36"/>
+      <c r="E101" s="97"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="88"/>
@@ -13747,6 +13844,14 @@
     <row r="122" spans="2:5">
       <c r="B122" s="88"/>
       <c r="E122" s="89"/>
+    </row>
+    <row r="123" spans="2:5">
+      <c r="B123" s="88"/>
+      <c r="E123" s="89"/>
+    </row>
+    <row r="124" spans="2:5">
+      <c r="B124" s="88"/>
+      <c r="E124" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13764,9 +13869,9 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:A75"/>
+  <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -14207,18 +14312,30 @@
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="35" t="e">
+        <f>'compile results'!E99</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="35" t="e">
+        <f>'compile results'!E100</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="35" t="e">
         <f>'compile results'!E91</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="35" t="e">
+    <row r="76" spans="1:1">
+      <c r="A76" s="35" t="e">
         <f>'compile results'!E92</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="35" t="e">
+    <row r="77" spans="1:1">
+      <c r="A77" s="35" t="e">
         <f>'compile results'!E93</f>
         <v>#VALUE!</v>
       </c>

</xml_diff>

<commit_message>
Published state of ETDataset on 9 January 2015.
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="145">
   <si>
     <t>Unit</t>
   </si>
@@ -459,18 +459,6 @@
     <t>the split between old and new residences is taken from the residences analysis</t>
   </si>
   <si>
-    <t>Capacity credit wind</t>
-  </si>
-  <si>
-    <t>capacity_credit_wind_constant_p1</t>
-  </si>
-  <si>
-    <t>capacity_credit_wind_constant_p2</t>
-  </si>
-  <si>
-    <t>capacity_credit_wind_constant_q1</t>
-  </si>
-  <si>
     <t>investment_hv_net_high</t>
   </si>
   <si>
@@ -487,12 +475,6 @@
   </si>
   <si>
     <t>ETM key - Set to true if you want your dataset to run in etmodel</t>
-  </si>
-  <si>
-    <t>capacity_credit_wind_minimum</t>
-  </si>
-  <si>
-    <t>capacity_credit_wind_maximum</t>
   </si>
 </sst>
 </file>
@@ -673,7 +655,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -953,17 +935,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -1454,7 +1425,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1690,44 +1661,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3176,9 +3129,7 @@
   </sheetPr>
   <dimension ref="B2:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3609,9 +3560,11 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:P101"/>
+  <dimension ref="A2:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3659,16 +3612,16 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="57" customHeight="1">
-      <c r="B5" s="151" t="s">
+      <c r="B5" s="143" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
-      <c r="I5" s="153"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="144"/>
+      <c r="F5" s="144"/>
+      <c r="G5" s="144"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="145"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
@@ -3773,7 +3726,7 @@
       <c r="D11" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="146"/>
+      <c r="E11" s="139"/>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
@@ -3797,14 +3750,14 @@
       <c r="D12" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="147"/>
+      <c r="E12" s="140"/>
       <c r="F12" s="35"/>
       <c r="G12" s="35"/>
       <c r="H12" s="35"/>
       <c r="I12" s="35"/>
       <c r="J12" s="35"/>
       <c r="K12" s="35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="L12" s="35"/>
       <c r="M12" s="35"/>
@@ -3821,14 +3774,14 @@
       <c r="D13" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="147"/>
+      <c r="E13" s="140"/>
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
       <c r="H13" s="35"/>
       <c r="I13" s="35"/>
       <c r="J13" s="35"/>
       <c r="K13" s="35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
@@ -3845,14 +3798,14 @@
       <c r="D14" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="149"/>
+      <c r="E14" s="142"/>
       <c r="F14" s="35"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
       <c r="J14" s="35"/>
       <c r="K14" s="35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
@@ -3869,14 +3822,14 @@
       <c r="D15" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="148"/>
+      <c r="E15" s="141"/>
       <c r="F15" s="35"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
       <c r="I15" s="35"/>
       <c r="J15" s="35"/>
       <c r="K15" s="35" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L15" s="35"/>
       <c r="M15" s="35"/>
@@ -5689,7 +5642,7 @@
         <v>0</v>
       </c>
       <c r="M85" s="35" t="str">
-        <f t="shared" ref="M85:M100" si="9">IF(L85=TRUE," ","Please set value")</f>
+        <f t="shared" ref="M85:M93" si="9">IF(L85=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N85" s="85"/>
@@ -5711,7 +5664,7 @@
       <c r="J86"/>
       <c r="K86"/>
       <c r="L86" s="40" t="b">
-        <f t="shared" ref="L86:L100" si="10">IF(COUNTBLANK(E86)=1,FALSE,TRUE)</f>
+        <f t="shared" ref="L86:L93" si="10">IF(COUNTBLANK(E86)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M86" s="35" t="str">
@@ -5830,14 +5783,14 @@
     <row r="91" spans="2:15" ht="16" thickBot="1">
       <c r="B91" s="31"/>
       <c r="C91" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D91"/>
-      <c r="E91" s="145"/>
+      <c r="E91" s="138"/>
       <c r="F91"/>
       <c r="G91" s="58"/>
       <c r="H91"/>
-      <c r="I91" s="141"/>
+      <c r="I91" s="134"/>
       <c r="J91"/>
       <c r="K91"/>
       <c r="L91" s="40" t="b">
@@ -5849,14 +5802,14 @@
         <v>Please set value</v>
       </c>
       <c r="N91" s="85"/>
-      <c r="O91" s="143" t="s">
-        <v>144</v>
+      <c r="O91" s="136" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="92" spans="2:15" ht="16" thickBot="1">
       <c r="B92" s="31"/>
       <c r="C92" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D92"/>
       <c r="E92" s="66"/>
@@ -5876,20 +5829,20 @@
       </c>
       <c r="N92" s="85"/>
       <c r="O92" s="132" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" spans="2:15" ht="16" thickBot="1">
       <c r="B93" s="31"/>
       <c r="C93" s="129" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D93"/>
-      <c r="E93" s="140"/>
+      <c r="E93" s="133"/>
       <c r="F93"/>
       <c r="G93" s="58"/>
       <c r="H93"/>
-      <c r="I93" s="142"/>
+      <c r="I93" s="135"/>
       <c r="J93"/>
       <c r="K93"/>
       <c r="L93" s="40" t="b">
@@ -5901,189 +5854,31 @@
         <v>Please set value</v>
       </c>
       <c r="N93" s="85"/>
-      <c r="O93" s="144" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="94" spans="2:15">
-      <c r="B94" s="31"/>
-      <c r="E94" s="134"/>
-      <c r="G94" s="133"/>
-      <c r="I94" s="7"/>
-      <c r="L94" s="139"/>
-      <c r="M94" s="107"/>
-      <c r="N94" s="85"/>
-      <c r="O94" s="15"/>
-    </row>
-    <row r="95" spans="2:15" ht="16" thickBot="1">
-      <c r="B95" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
-      <c r="E95" s="135"/>
-      <c r="F95" s="4"/>
-      <c r="G95" s="136"/>
-      <c r="H95" s="4"/>
-      <c r="I95" s="137"/>
-      <c r="J95" s="4"/>
-      <c r="K95" s="4"/>
-      <c r="L95" s="138"/>
-      <c r="M95" s="101"/>
-      <c r="N95" s="85"/>
-      <c r="O95" s="15"/>
-    </row>
-    <row r="96" spans="2:15" ht="16" thickBot="1">
-      <c r="B96" s="31"/>
-      <c r="C96" t="s">
-        <v>140</v>
-      </c>
-      <c r="D96"/>
-      <c r="E96" s="64"/>
-      <c r="F96"/>
-      <c r="G96" s="58"/>
-      <c r="H96"/>
-      <c r="I96" s="57"/>
-      <c r="J96"/>
-      <c r="K96"/>
-      <c r="L96" s="40" t="b">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M96" s="35" t="str">
-        <f t="shared" si="9"/>
-        <v>Please set value</v>
-      </c>
-      <c r="N96" s="85"/>
-      <c r="O96" s="132" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="97" spans="2:15" ht="16" thickBot="1">
-      <c r="B97" s="31"/>
-      <c r="C97" t="s">
+      <c r="O93" s="137" t="s">
         <v>141</v>
       </c>
-      <c r="D97"/>
-      <c r="E97" s="64"/>
-      <c r="F97"/>
-      <c r="G97" s="58"/>
-      <c r="H97"/>
-      <c r="I97" s="57"/>
-      <c r="J97"/>
-      <c r="K97"/>
-      <c r="L97" s="40" t="b">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M97" s="35" t="str">
-        <f t="shared" si="9"/>
-        <v>Please set value</v>
-      </c>
-      <c r="N97" s="85"/>
-      <c r="O97" s="132" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="98" spans="2:15" ht="16" thickBot="1">
-      <c r="B98" s="31"/>
-      <c r="C98" t="s">
-        <v>142</v>
-      </c>
-      <c r="D98"/>
-      <c r="E98" s="64"/>
-      <c r="F98"/>
-      <c r="G98" s="58"/>
-      <c r="H98"/>
-      <c r="I98" s="57"/>
-      <c r="J98"/>
-      <c r="K98"/>
-      <c r="L98" s="40" t="b">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M98" s="35" t="str">
-        <f t="shared" si="9"/>
-        <v>Please set value</v>
-      </c>
-      <c r="N98" s="85"/>
-      <c r="O98" s="132" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="99" spans="2:15" ht="16" thickBot="1">
-      <c r="B99" s="31"/>
-      <c r="C99" t="s">
-        <v>149</v>
-      </c>
-      <c r="D99"/>
-      <c r="E99" s="66"/>
-      <c r="F99"/>
-      <c r="G99" s="58"/>
-      <c r="H99"/>
-      <c r="I99" s="57"/>
-      <c r="J99"/>
-      <c r="K99"/>
-      <c r="L99" s="40" t="b">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M99" s="35" t="str">
-        <f t="shared" si="9"/>
-        <v>Please set value</v>
-      </c>
-      <c r="N99" s="85"/>
-      <c r="O99" s="132" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="100" spans="2:15" ht="16" thickBot="1">
-      <c r="B100" s="31"/>
-      <c r="C100" t="s">
-        <v>150</v>
-      </c>
-      <c r="D100"/>
-      <c r="E100" s="150"/>
-      <c r="F100"/>
-      <c r="G100" s="58"/>
-      <c r="H100"/>
-      <c r="I100" s="142"/>
-      <c r="J100"/>
-      <c r="K100"/>
-      <c r="L100" s="40" t="b">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M100" s="35" t="str">
-        <f t="shared" si="9"/>
-        <v>Please set value</v>
-      </c>
-      <c r="N100" s="85"/>
-      <c r="O100" s="132" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="101" spans="2:15" ht="16" thickBot="1">
-      <c r="B101" s="44"/>
-      <c r="C101" s="36"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="52"/>
-      <c r="F101" s="36"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="36"/>
-      <c r="I101" s="36"/>
-      <c r="J101" s="36"/>
-      <c r="K101" s="36"/>
-      <c r="L101" s="36"/>
-      <c r="M101" s="36"/>
-      <c r="N101" s="31"/>
-      <c r="O101" s="7"/>
+    </row>
+    <row r="94" spans="2:15" ht="16" thickBot="1">
+      <c r="B94" s="44"/>
+      <c r="C94" s="36"/>
+      <c r="D94" s="36"/>
+      <c r="E94" s="52"/>
+      <c r="F94" s="36"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="36"/>
+      <c r="I94" s="36"/>
+      <c r="J94" s="36"/>
+      <c r="K94" s="36"/>
+      <c r="L94" s="36"/>
+      <c r="M94" s="36"/>
+      <c r="N94" s="31"/>
+      <c r="O94" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:I5"/>
   </mergeCells>
-  <conditionalFormatting sqref="L76:L82 L39:L44 L71:L73 L18:L36 L47:L52 L54 L56:L67 L89:L100">
+  <conditionalFormatting sqref="L76:L82 L39:L44 L71:L73 L18:L36 L47:L52 L54 L56:L67 L89:L93">
     <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -6103,7 +5898,7 @@
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E68:E101 E39:E43 E46:E58 D59:D62 E63:E65">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39:E43 E46:E58 D59:D62 E63:E65 E68:E94">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6418,10 +6213,10 @@
     </row>
     <row r="5" spans="1:48">
       <c r="A5" s="114"/>
-      <c r="B5" s="151" t="s">
+      <c r="B5" s="143" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="153"/>
+      <c r="C5" s="145"/>
       <c r="D5" s="114"/>
       <c r="E5" s="112"/>
       <c r="F5" s="112"/>
@@ -12240,10 +12035,10 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:E124"/>
+  <dimension ref="B1:E117"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:XFD100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13290,7 +13085,7 @@
         <v>5</v>
       </c>
       <c r="E71" s="104" t="e">
-        <f t="shared" ref="E71:E100" si="3">IF(COUNTBLANK(B71)=0,"- "&amp;B71&amp;" = "&amp;FIXED(C71,D71,1),"")</f>
+        <f t="shared" ref="E71:E93" si="3">IF(COUNTBLANK(B71)=0,"- "&amp;B71&amp;" = "&amp;FIXED(C71,D71,1),"")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -13660,106 +13455,39 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="94" spans="2:5">
-      <c r="B94" s="31"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="32"/>
+    <row r="94" spans="2:5" ht="16" thickBot="1">
+      <c r="B94" s="44"/>
+      <c r="C94" s="96"/>
+      <c r="D94" s="36"/>
+      <c r="E94" s="97"/>
     </row>
     <row r="95" spans="2:5">
-      <c r="B95" s="31"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="32"/>
+      <c r="B95" s="88"/>
+      <c r="E95" s="89"/>
     </row>
     <row r="96" spans="2:5">
-      <c r="B96" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C96)=0,Dashboard!C96,"")</f>
-        <v>capacity_credit_wind_constant_p1</v>
-      </c>
-      <c r="C96" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E96)=0,Dashboard!E96,"")</f>
-        <v/>
-      </c>
-      <c r="D96" s="35">
-        <v>0</v>
-      </c>
-      <c r="E96" s="104" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="B96" s="88"/>
+      <c r="E96" s="89"/>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C97)=0,Dashboard!C97,"")</f>
-        <v>capacity_credit_wind_constant_p2</v>
-      </c>
-      <c r="C97" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E97)=0,Dashboard!E97,"")</f>
-        <v/>
-      </c>
-      <c r="D97" s="35">
-        <v>0</v>
-      </c>
-      <c r="E97" s="104" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="B97" s="88"/>
+      <c r="E97" s="89"/>
     </row>
     <row r="98" spans="2:5">
-      <c r="B98" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C98)=0,Dashboard!C98,"")</f>
-        <v>capacity_credit_wind_constant_q1</v>
-      </c>
-      <c r="C98" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E98)=0,Dashboard!E98,"")</f>
-        <v/>
-      </c>
-      <c r="D98" s="35">
-        <v>0</v>
-      </c>
-      <c r="E98" s="104" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="B98" s="88"/>
+      <c r="E98" s="89"/>
     </row>
     <row r="99" spans="2:5">
-      <c r="B99" s="103" t="s">
-        <v>149</v>
-      </c>
-      <c r="C99" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E99)=0,Dashboard!E99,"")</f>
-        <v/>
-      </c>
-      <c r="D99" s="41">
-        <v>2</v>
-      </c>
-      <c r="E99" s="104" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="B99" s="88"/>
+      <c r="E99" s="89"/>
     </row>
     <row r="100" spans="2:5">
-      <c r="B100" s="103" t="s">
-        <v>150</v>
-      </c>
-      <c r="C100" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E100)=0,Dashboard!E100,"")</f>
-        <v/>
-      </c>
-      <c r="D100" s="41">
-        <v>2</v>
-      </c>
-      <c r="E100" s="104" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" ht="16" thickBot="1">
-      <c r="B101" s="44"/>
-      <c r="C101" s="96"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="97"/>
+      <c r="B100" s="88"/>
+      <c r="E100" s="89"/>
+    </row>
+    <row r="101" spans="2:5">
+      <c r="B101" s="88"/>
+      <c r="E101" s="89"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="88"/>
@@ -13824,34 +13552,6 @@
     <row r="117" spans="2:5">
       <c r="B117" s="88"/>
       <c r="E117" s="89"/>
-    </row>
-    <row r="118" spans="2:5">
-      <c r="B118" s="88"/>
-      <c r="E118" s="89"/>
-    </row>
-    <row r="119" spans="2:5">
-      <c r="B119" s="88"/>
-      <c r="E119" s="89"/>
-    </row>
-    <row r="120" spans="2:5">
-      <c r="B120" s="88"/>
-      <c r="E120" s="89"/>
-    </row>
-    <row r="121" spans="2:5">
-      <c r="B121" s="88"/>
-      <c r="E121" s="89"/>
-    </row>
-    <row r="122" spans="2:5">
-      <c r="B122" s="88"/>
-      <c r="E122" s="89"/>
-    </row>
-    <row r="123" spans="2:5">
-      <c r="B123" s="88"/>
-      <c r="E123" s="89"/>
-    </row>
-    <row r="124" spans="2:5">
-      <c r="B124" s="88"/>
-      <c r="E124" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13869,7 +13569,7 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:A77"/>
+  <dimension ref="A1:A72"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -14294,48 +13994,18 @@
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="35" t="e">
-        <f>'compile results'!E96</f>
+        <f>'compile results'!E91</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="35" t="e">
-        <f>'compile results'!E97</f>
+        <f>'compile results'!E92</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="35" t="e">
-        <f>'compile results'!E98</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="35" t="e">
-        <f>'compile results'!E99</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="35" t="e">
-        <f>'compile results'!E100</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="35" t="e">
-        <f>'compile results'!E91</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="35" t="e">
-        <f>'compile results'!E92</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="35" t="e">
         <f>'compile results'!E93</f>
         <v>#VALUE!</v>
       </c>

</xml_diff>

<commit_message>
Published state of ETDataset on 12 February 2016
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="switch_iea">'[1]Fuel allocation'!$C$89</definedName>
     <definedName name="switch_protermo">'[1]Fuel allocation'!$C$48</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="147">
   <si>
     <t>Unit</t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>ETM key - Set to true if you want your dataset to run in etmodel</t>
+  </si>
+  <si>
+    <t>number_of_cars</t>
+  </si>
+  <si>
+    <t>Transport</t>
   </si>
 </sst>
 </file>
@@ -961,7 +967,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="462">
+  <cellStyleXfs count="476">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1237,6 +1243,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1693,7 +1713,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="462">
+  <cellStyles count="476">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1938,6 +1958,13 @@
     <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="459" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="461" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="463" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="465" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="467" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="471" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="473" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="475" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2155,9 +2182,27 @@
     <cellStyle name="Hyperlink" xfId="456" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="458" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="460" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="462" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="464" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="466" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="470" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="472" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="474" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FFCCFFCC"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFCCFFCC"/>
@@ -3129,7 +3174,7 @@
   </sheetPr>
   <dimension ref="B2:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A8" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3560,10 +3605,10 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:P94"/>
+  <dimension ref="A2:P97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5858,37 +5903,102 @@
         <v>141</v>
       </c>
     </row>
-    <row r="94" spans="2:15" ht="16" thickBot="1">
-      <c r="B94" s="44"/>
-      <c r="C94" s="36"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="52"/>
-      <c r="F94" s="36"/>
-      <c r="G94" s="36"/>
-      <c r="H94" s="36"/>
-      <c r="I94" s="36"/>
-      <c r="J94" s="36"/>
-      <c r="K94" s="36"/>
-      <c r="L94" s="36"/>
-      <c r="M94" s="36"/>
-      <c r="N94" s="31"/>
-      <c r="O94" s="7"/>
+    <row r="94" spans="2:15">
+      <c r="B94" s="31"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="54"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7"/>
+      <c r="L94" s="7"/>
+      <c r="M94" s="7"/>
+      <c r="N94" s="85"/>
+      <c r="O94" s="15"/>
+    </row>
+    <row r="95" spans="2:15" ht="16" thickBot="1">
+      <c r="B95" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="55"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
+      <c r="N95" s="85"/>
+      <c r="O95" s="15"/>
+    </row>
+    <row r="96" spans="2:15" ht="16" thickBot="1">
+      <c r="B96" s="31"/>
+      <c r="C96" t="s">
+        <v>145</v>
+      </c>
+      <c r="D96"/>
+      <c r="E96" s="53"/>
+      <c r="F96"/>
+      <c r="G96" s="58"/>
+      <c r="H96"/>
+      <c r="I96" s="57"/>
+      <c r="J96"/>
+      <c r="K96"/>
+      <c r="L96" s="40" t="b">
+        <f>IF(COUNTBLANK(E96)=1,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="M96" s="35" t="str">
+        <f t="shared" ref="M96" si="11">IF(L96=TRUE," ","Please set value")</f>
+        <v>Please set value</v>
+      </c>
+      <c r="N96" s="85"/>
+      <c r="O96" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="2:15" ht="16" thickBot="1">
+      <c r="B97" s="44"/>
+      <c r="C97" s="36"/>
+      <c r="D97" s="36"/>
+      <c r="E97" s="52"/>
+      <c r="F97" s="36"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="36"/>
+      <c r="I97" s="36"/>
+      <c r="J97" s="36"/>
+      <c r="K97" s="36"/>
+      <c r="L97" s="36"/>
+      <c r="M97" s="36"/>
+      <c r="N97" s="31"/>
+      <c r="O97" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="L76:L82 L39:L44 L71:L73 L18:L36 L47:L52 L54 L56:L67 L89:L93">
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L85:L88">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L68">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L96">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -5898,7 +6008,7 @@
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39:E43 E46:E58 D59:D62 E63:E65 E68:E94">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39:E43 E46:E58 D59:D62 E63:E65 E68:E97">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -5997,7 +6107,9 @@
   </sheetPr>
   <dimension ref="A1:AV120"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -12022,6 +12134,7 @@
     <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -12035,10 +12148,10 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:E117"/>
+  <dimension ref="B1:E120"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:XFD100"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13085,7 +13198,7 @@
         <v>5</v>
       </c>
       <c r="E71" s="104" t="e">
-        <f t="shared" ref="E71:E93" si="3">IF(COUNTBLANK(B71)=0,"- "&amp;B71&amp;" = "&amp;FIXED(C71,D71,1),"")</f>
+        <f t="shared" ref="E71:E96" si="3">IF(COUNTBLANK(B71)=0,"- "&amp;B71&amp;" = "&amp;FIXED(C71,D71,1),"")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -13455,23 +13568,58 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="94" spans="2:5" ht="16" thickBot="1">
-      <c r="B94" s="44"/>
-      <c r="C94" s="96"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="97"/>
+    <row r="94" spans="2:5">
+      <c r="B94" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C94)=0,Dashboard!C94,"")</f>
+        <v/>
+      </c>
+      <c r="C94" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E94)=0,Dashboard!E94,"")</f>
+        <v/>
+      </c>
+      <c r="D94" s="7"/>
+      <c r="E94" s="105" t="str">
+        <f t="shared" ref="E94:E95" si="4">IF(COUNTBLANK(B94)=0,"- "&amp;B94&amp;" = "&amp;FIXED(C94,D94,1),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="95" spans="2:5">
-      <c r="B95" s="88"/>
-      <c r="E95" s="89"/>
+      <c r="B95" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C95)=0,Dashboard!C95,"")</f>
+        <v/>
+      </c>
+      <c r="C95" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E95)=0,Dashboard!E95,"")</f>
+        <v/>
+      </c>
+      <c r="D95" s="7"/>
+      <c r="E95" s="105" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
     <row r="96" spans="2:5">
-      <c r="B96" s="88"/>
-      <c r="E96" s="89"/>
-    </row>
-    <row r="97" spans="2:5">
-      <c r="B97" s="88"/>
-      <c r="E97" s="89"/>
+      <c r="B96" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C96)=0,Dashboard!C96,"")</f>
+        <v>number_of_cars</v>
+      </c>
+      <c r="C96" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E96)=0,Dashboard!E96,"")</f>
+        <v/>
+      </c>
+      <c r="D96" s="41">
+        <v>1</v>
+      </c>
+      <c r="E96" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="16" thickBot="1">
+      <c r="B97" s="44"/>
+      <c r="C97" s="96"/>
+      <c r="D97" s="36"/>
+      <c r="E97" s="97"/>
     </row>
     <row r="98" spans="2:5">
       <c r="B98" s="88"/>
@@ -13552,6 +13700,18 @@
     <row r="117" spans="2:5">
       <c r="B117" s="88"/>
       <c r="E117" s="89"/>
+    </row>
+    <row r="118" spans="2:5">
+      <c r="B118" s="88"/>
+      <c r="E118" s="89"/>
+    </row>
+    <row r="119" spans="2:5">
+      <c r="B119" s="88"/>
+      <c r="E119" s="89"/>
+    </row>
+    <row r="120" spans="2:5">
+      <c r="B120" s="88"/>
+      <c r="E120" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13569,9 +13729,11 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:A72"/>
+  <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -14007,6 +14169,12 @@
     <row r="72" spans="1:1">
       <c r="A72" s="35" t="e">
         <f>'compile results'!E93</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="35" t="e">
+        <f>'compile results'!E96</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Published state of ETDataset on 10 August 2016
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="switch_iea">'[1]Fuel allocation'!$C$89</definedName>
     <definedName name="switch_protermo">'[1]Fuel allocation'!$C$48</definedName>
   </definedNames>
-  <calcPr calcId="140000" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="154">
   <si>
     <t>Unit</t>
   </si>
@@ -481,6 +481,27 @@
   </si>
   <si>
     <t>Transport</t>
+  </si>
+  <si>
+    <t>has_aggregated_other_industry</t>
+  </si>
+  <si>
+    <t>ETM key - TRUE unless you'd like to further split the other industry (contact Quintel for that)</t>
+  </si>
+  <si>
+    <t>ETM key - TRUE unless you performed the additional analysis in 4b chemical_industry</t>
+  </si>
+  <si>
+    <t>has_aggregated_chemical_industry</t>
+  </si>
+  <si>
+    <t>Added industry attributes</t>
+  </si>
+  <si>
+    <t>has_detailed_chemical_industry</t>
+  </si>
+  <si>
+    <t>has_detailed_other_industry</t>
   </si>
 </sst>
 </file>
@@ -967,7 +988,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="476">
+  <cellStyleXfs count="492">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1444,8 +1465,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1703,6 +1740,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1713,7 +1753,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="476">
+  <cellStyles count="492">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1965,6 +2005,14 @@
     <cellStyle name="Followed Hyperlink" xfId="471" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="473" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="475" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="477" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="491" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2189,9 +2237,39 @@
     <cellStyle name="Hyperlink" xfId="470" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="472" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="474" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="476" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="478" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="490" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FFCCFFCC"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCFFCC"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFCCFFCC"/>
@@ -3426,7 +3504,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D7" sqref="D7:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3495,9 +3573,15 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" s="75"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="74"/>
+      <c r="B9" s="75">
+        <v>42580</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="74">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="75"/>
@@ -3605,10 +3689,10 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:P97"/>
+  <dimension ref="A2:P99"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3623,7 +3707,7 @@
     <col min="8" max="8" width="3.83203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="65.33203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="3.83203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="74.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="78" style="2" customWidth="1"/>
     <col min="12" max="12" width="40" style="2" customWidth="1"/>
     <col min="13" max="13" width="34.33203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="3.83203125" style="2" customWidth="1"/>
@@ -3657,16 +3741,16 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="57" customHeight="1">
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="144" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="144"/>
-      <c r="D5" s="144"/>
-      <c r="E5" s="144"/>
-      <c r="F5" s="144"/>
-      <c r="G5" s="144"/>
-      <c r="H5" s="144"/>
-      <c r="I5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="146"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
@@ -4489,102 +4573,104 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
-      <c r="B37" s="38"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
+    <row r="37" spans="1:15" ht="16" thickBot="1">
+      <c r="B37" s="34"/>
+      <c r="C37" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="110"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="L37" s="40" t="b">
+        <f>IF(OR((AND(COUNTBLANK(E37)=0,E37="true")),AND(COUNTBLANK(E37)=0,E37="false")),TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="35" t="str">
+        <f t="shared" ref="M37" si="2">IF(L37=TRUE," ","Please set value to 'TRUE' or 'FALSE'")</f>
+        <v>Please set value to 'TRUE' or 'FALSE'</v>
+      </c>
       <c r="N37" s="85"/>
-      <c r="O37" s="15"/>
+      <c r="O37" s="86" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="38" spans="1:15" ht="16" thickBot="1">
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="34"/>
+      <c r="C38" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="110"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="L38" s="40" t="b">
+        <f>IF(OR((AND(COUNTBLANK(E38)=0,E38="true")),AND(COUNTBLANK(E38)=0,E38="false")),TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="35" t="str">
+        <f t="shared" ref="M38" si="3">IF(L38=TRUE," ","Please set value to 'TRUE' or 'FALSE'")</f>
+        <v>Please set value to 'TRUE' or 'FALSE'</v>
+      </c>
+      <c r="N38" s="85"/>
+      <c r="O38" s="86" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="B39" s="38"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="85"/>
+      <c r="O39" s="15"/>
+    </row>
+    <row r="40" spans="1:15" ht="16" thickBot="1">
+      <c r="B40" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="85"/>
-      <c r="O38" s="15"/>
-    </row>
-    <row r="39" spans="1:15" ht="16" thickBot="1">
-      <c r="B39" s="34"/>
-      <c r="C39" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="E39" s="64"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39" s="57"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="L39" s="40" t="b">
-        <f t="shared" ref="L39:L44" si="2">IF(COUNTBLANK(E39)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M39" s="35" t="str">
-        <f t="shared" ref="M39:M44" si="3">IF(L39=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
-      <c r="N39" s="85"/>
-      <c r="O39" s="86" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="16" thickBot="1">
-      <c r="B40" s="34"/>
-      <c r="C40" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="E40" s="64"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40" s="57"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="40" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M40" s="35" t="str">
-        <f t="shared" si="3"/>
-        <v>Please set value</v>
-      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
       <c r="N40" s="85"/>
-      <c r="O40" s="86" t="s">
-        <v>71</v>
-      </c>
+      <c r="O40" s="15"/>
     </row>
     <row r="41" spans="1:15" ht="16" thickBot="1">
       <c r="B41" s="34"/>
       <c r="C41" s="35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D41" s="35" t="s">
         <v>2</v>
@@ -4595,29 +4681,29 @@
       <c r="H41"/>
       <c r="I41" s="57"/>
       <c r="J41" s="35"/>
-      <c r="K41" s="35" t="s">
-        <v>115</v>
+      <c r="K41" s="41" t="s">
+        <v>110</v>
       </c>
       <c r="L41" s="40" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L41:L46" si="4">IF(COUNTBLANK(E41)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M41" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="M41:M46" si="5">IF(L41=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N41" s="85"/>
       <c r="O41" s="86" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="16" thickBot="1">
       <c r="B42" s="34"/>
       <c r="C42" s="35" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="D42" s="35" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="E42" s="64"/>
       <c r="F42"/>
@@ -4627,55 +4713,57 @@
       <c r="J42" s="35"/>
       <c r="K42" s="35"/>
       <c r="L42" s="40" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M42" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Please set value</v>
       </c>
       <c r="N42" s="85"/>
       <c r="O42" s="86" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="16" thickBot="1">
       <c r="B43" s="34"/>
       <c r="C43" s="35" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D43" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="65"/>
+      <c r="E43" s="64"/>
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
       <c r="I43" s="57"/>
       <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
+      <c r="K43" s="35" t="s">
+        <v>115</v>
+      </c>
       <c r="L43" s="40" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M43" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Please set value</v>
       </c>
       <c r="N43" s="85"/>
       <c r="O43" s="86" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="16" thickBot="1">
       <c r="B44" s="34"/>
       <c r="C44" s="35" t="s">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="D44" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="E44" s="65"/>
+        <v>37</v>
+      </c>
+      <c r="E44" s="64"/>
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44"/>
@@ -4683,117 +4771,117 @@
       <c r="J44" s="35"/>
       <c r="K44" s="35"/>
       <c r="L44" s="40" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="35" t="str">
-        <f t="shared" si="3"/>
-        <v>Please set value</v>
-      </c>
-      <c r="N44" s="85"/>
-      <c r="O44" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="B45" s="38"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="85"/>
-      <c r="O45" s="15"/>
-    </row>
-    <row r="46" spans="1:15" ht="16" thickBot="1">
-      <c r="B46" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="85"/>
-      <c r="O46" s="15"/>
-    </row>
-    <row r="47" spans="1:15" ht="16" thickBot="1">
-      <c r="B47" s="34"/>
-      <c r="C47" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" s="66"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="57"/>
-      <c r="J47" s="35"/>
-      <c r="K47" s="35"/>
-      <c r="L47" s="40" t="b">
-        <f t="shared" ref="L47:L68" si="4">IF(COUNTBLANK(E47)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M47" s="35" t="str">
-        <f>IF(L47=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
-      <c r="N47" s="85"/>
-      <c r="O47" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="16" thickBot="1">
-      <c r="B48" s="34"/>
-      <c r="C48" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="D48" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="E48" s="66"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="57"/>
-      <c r="J48" s="35"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="40" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M48" s="35" t="str">
-        <f t="shared" ref="M48:M68" si="5">IF(L48=TRUE," ","Please set value")</f>
+      <c r="M44" s="35" t="str">
+        <f t="shared" si="5"/>
         <v>Please set value</v>
       </c>
+      <c r="N44" s="85"/>
+      <c r="O44" s="86" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="16" thickBot="1">
+      <c r="B45" s="34"/>
+      <c r="C45" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="65"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="40" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N45" s="85"/>
+      <c r="O45" s="86" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="16" thickBot="1">
+      <c r="B46" s="34"/>
+      <c r="C46" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="65"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="40" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N46" s="85"/>
+      <c r="O46" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="B47" s="38"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="85"/>
+      <c r="O47" s="15"/>
+    </row>
+    <row r="48" spans="1:15" ht="16" thickBot="1">
+      <c r="B48" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
       <c r="N48" s="85"/>
-      <c r="O48" s="15" t="s">
-        <v>74</v>
-      </c>
+      <c r="O48" s="15"/>
     </row>
     <row r="49" spans="2:15" ht="16" thickBot="1">
       <c r="B49" s="34"/>
       <c r="C49" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D49" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="53"/>
+      <c r="E49" s="66"/>
       <c r="F49" s="35"/>
       <c r="G49" s="59"/>
       <c r="H49" s="35"/>
@@ -4801,25 +4889,27 @@
       <c r="J49" s="35"/>
       <c r="K49" s="35"/>
       <c r="L49" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="L49:L70" si="6">IF(COUNTBLANK(E49)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M49" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(L49=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N49" s="85"/>
       <c r="O49" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="2:15" ht="16" thickBot="1">
       <c r="B50" s="34"/>
       <c r="C50" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50" s="35"/>
-      <c r="E50" s="53"/>
+        <v>74</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" s="66"/>
       <c r="F50" s="35"/>
       <c r="G50" s="59"/>
       <c r="H50" s="35"/>
@@ -4827,24 +4917,26 @@
       <c r="J50" s="35"/>
       <c r="K50" s="35"/>
       <c r="L50" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M50" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="M50:M70" si="7">IF(L50=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N50" s="85"/>
       <c r="O50" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="2:15" ht="16" thickBot="1">
       <c r="B51" s="34"/>
       <c r="C51" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="D51" s="35"/>
+        <v>75</v>
+      </c>
+      <c r="D51" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="E51" s="53"/>
       <c r="F51" s="35"/>
       <c r="G51" s="59"/>
@@ -4853,22 +4945,22 @@
       <c r="J51" s="35"/>
       <c r="K51" s="35"/>
       <c r="L51" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M51" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Please set value</v>
       </c>
       <c r="N51" s="85"/>
       <c r="O51" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="2:15" ht="16" thickBot="1">
       <c r="B52" s="34"/>
       <c r="C52" s="35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D52" s="35"/>
       <c r="E52" s="53"/>
@@ -4879,75 +4971,78 @@
       <c r="J52" s="35"/>
       <c r="K52" s="35"/>
       <c r="L52" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M52" s="41" t="str">
-        <f t="shared" si="5"/>
+      <c r="M52" s="35" t="str">
+        <f t="shared" si="7"/>
         <v>Please set value</v>
       </c>
       <c r="N52" s="85"/>
       <c r="O52" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="2:15" ht="16" thickBot="1">
       <c r="B53" s="34"/>
       <c r="C53" s="35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D53" s="35"/>
-      <c r="E53" s="130">
-        <f>'6_residences'!C11</f>
-        <v>0</v>
-      </c>
-      <c r="F53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="35"/>
       <c r="G53" s="59"/>
       <c r="H53" s="35"/>
-      <c r="I53" s="131"/>
+      <c r="I53" s="57"/>
       <c r="J53" s="35"/>
-      <c r="K53" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="L53" s="129"/>
-      <c r="M53" s="129"/>
+      <c r="K53" s="35"/>
+      <c r="L53" s="40" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M53" s="35" t="str">
+        <f t="shared" si="7"/>
+        <v>Please set value</v>
+      </c>
       <c r="N53" s="85"/>
-      <c r="O53" s="15"/>
+      <c r="O53" s="15" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="54" spans="2:15" ht="16" thickBot="1">
       <c r="B54" s="34"/>
       <c r="C54" s="35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D54" s="35"/>
       <c r="E54" s="53"/>
-      <c r="F54"/>
+      <c r="F54" s="35"/>
       <c r="G54" s="59"/>
       <c r="H54" s="35"/>
       <c r="I54" s="57"/>
       <c r="J54" s="35"/>
       <c r="K54" s="35"/>
       <c r="L54" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M54" s="41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Please set value</v>
       </c>
       <c r="N54" s="85"/>
       <c r="O54" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="2:15" ht="16" thickBot="1">
       <c r="B55" s="34"/>
       <c r="C55" s="35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D55" s="35"/>
       <c r="E55" s="130">
-        <f>'6_residences'!C10</f>
+        <f>'6_residences'!C11</f>
         <v>0</v>
       </c>
       <c r="F55"/>
@@ -4955,7 +5050,7 @@
       <c r="H55" s="35"/>
       <c r="I55" s="131"/>
       <c r="J55" s="35"/>
-      <c r="K55" s="35" t="s">
+      <c r="K55" s="58" t="s">
         <v>137</v>
       </c>
       <c r="L55" s="129"/>
@@ -4966,442 +5061,439 @@
     <row r="56" spans="2:15" ht="16" thickBot="1">
       <c r="B56" s="34"/>
       <c r="C56" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="D56" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="E56" s="66"/>
+        <v>81</v>
+      </c>
+      <c r="D56" s="35"/>
+      <c r="E56" s="53"/>
       <c r="F56"/>
       <c r="G56" s="59"/>
       <c r="H56" s="35"/>
-      <c r="I56" s="16"/>
+      <c r="I56" s="57"/>
       <c r="J56" s="35"/>
-      <c r="K56" s="129"/>
+      <c r="K56" s="35"/>
       <c r="L56" s="40" t="b">
-        <f>IF(COUNTBLANK(E56)=1,FALSE,TRUE)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M56" s="35" t="str">
-        <f>IF(L56=TRUE," ","Please set value")</f>
+      <c r="M56" s="41" t="str">
+        <f t="shared" si="7"/>
         <v>Please set value</v>
       </c>
       <c r="N56" s="85"/>
       <c r="O56" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="2:15" ht="16" thickBot="1">
       <c r="B57" s="34"/>
       <c r="C57" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="D57" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="E57" s="66"/>
+        <v>82</v>
+      </c>
+      <c r="D57" s="35"/>
+      <c r="E57" s="130">
+        <f>'6_residences'!C10</f>
+        <v>0</v>
+      </c>
       <c r="F57"/>
       <c r="G57" s="59"/>
       <c r="H57" s="35"/>
-      <c r="I57" s="57"/>
+      <c r="I57" s="131"/>
       <c r="J57" s="35"/>
-      <c r="K57" s="35"/>
-      <c r="L57" s="40" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M57" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>Please set value</v>
-      </c>
+      <c r="K57" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="L57" s="129"/>
+      <c r="M57" s="129"/>
       <c r="N57" s="85"/>
-      <c r="O57" s="15" t="s">
-        <v>84</v>
-      </c>
+      <c r="O57" s="15"/>
     </row>
     <row r="58" spans="2:15" ht="16" thickBot="1">
       <c r="B58" s="34"/>
       <c r="C58" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="D58" s="41"/>
-      <c r="E58" s="53"/>
-      <c r="F58" s="35"/>
+        <v>83</v>
+      </c>
+      <c r="D58" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" s="66"/>
+      <c r="F58"/>
       <c r="G58" s="59"/>
       <c r="H58" s="35"/>
-      <c r="I58" s="57"/>
+      <c r="I58" s="16"/>
       <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
+      <c r="K58" s="129"/>
       <c r="L58" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTBLANK(E58)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M58" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(L58=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N58" s="85"/>
       <c r="O58" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="2:15" ht="16" thickBot="1">
       <c r="B59" s="34"/>
       <c r="C59" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="D59" s="62"/>
-      <c r="E59" s="63"/>
-      <c r="F59" s="35"/>
-      <c r="G59"/>
+        <v>84</v>
+      </c>
+      <c r="D59" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E59" s="66"/>
+      <c r="F59"/>
+      <c r="G59" s="59"/>
       <c r="H59" s="35"/>
       <c r="I59" s="57"/>
       <c r="J59" s="35"/>
       <c r="K59" s="35"/>
       <c r="L59" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M59" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Please set value</v>
       </c>
       <c r="N59" s="85"/>
       <c r="O59" s="15" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="2:15" ht="16" thickBot="1">
       <c r="B60" s="34"/>
       <c r="C60" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="D60" s="87"/>
-      <c r="E60" s="63"/>
+        <v>85</v>
+      </c>
+      <c r="D60" s="41"/>
+      <c r="E60" s="53"/>
       <c r="F60" s="35"/>
-      <c r="G60"/>
+      <c r="G60" s="59"/>
       <c r="H60" s="35"/>
       <c r="I60" s="57"/>
       <c r="J60" s="35"/>
       <c r="K60" s="35"/>
       <c r="L60" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M60" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Please set value</v>
       </c>
       <c r="N60" s="85"/>
       <c r="O60" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="2:15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" ht="16" thickBot="1">
       <c r="B61" s="34"/>
       <c r="C61" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="D61" s="87"/>
-      <c r="E61" s="127">
-        <f>'6_residences'!C9*Dashboard!E60</f>
-        <v>0</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="D61" s="62"/>
+      <c r="E61" s="63"/>
       <c r="F61" s="35"/>
       <c r="G61"/>
       <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
+      <c r="I61" s="57"/>
       <c r="J61" s="35"/>
-      <c r="K61" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="L61" s="126"/>
-      <c r="M61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="40" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M61" s="35" t="str">
+        <f t="shared" si="7"/>
+        <v>Please set value</v>
+      </c>
       <c r="N61" s="85"/>
-      <c r="O61" s="15"/>
+      <c r="O61" s="15" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="62" spans="2:15" ht="16" thickBot="1">
       <c r="B62" s="34"/>
       <c r="C62" s="35" t="s">
-        <v>88</v>
+        <v>130</v>
       </c>
       <c r="D62" s="87"/>
-      <c r="E62" s="127">
-        <f>'6_residences'!C8*Dashboard!E60</f>
-        <v>0</v>
-      </c>
+      <c r="E62" s="63"/>
       <c r="F62" s="35"/>
       <c r="G62"/>
       <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
+      <c r="I62" s="57"/>
       <c r="J62" s="35"/>
-      <c r="K62" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="L62" s="126"/>
-      <c r="M62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="40" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M62" s="35" t="str">
+        <f t="shared" si="7"/>
+        <v>Please set value</v>
+      </c>
       <c r="N62" s="85"/>
-      <c r="O62" s="15"/>
-    </row>
-    <row r="63" spans="2:15" ht="16" thickBot="1">
+      <c r="O62" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="2:15">
       <c r="B63" s="34"/>
       <c r="C63" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="D63" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="E63" s="66"/>
+        <v>87</v>
+      </c>
+      <c r="D63" s="87"/>
+      <c r="E63" s="127">
+        <f>'6_residences'!C9*Dashboard!E62</f>
+        <v>0</v>
+      </c>
       <c r="F63" s="35"/>
-      <c r="G63" s="59"/>
+      <c r="G63"/>
       <c r="H63" s="35"/>
-      <c r="I63" s="57"/>
+      <c r="I63" s="35"/>
       <c r="J63" s="35"/>
-      <c r="K63" s="128"/>
-      <c r="L63" s="40" t="b">
-        <f>IF(COUNTBLANK(E63)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M63" s="35" t="str">
-        <f>IF(L63=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
+      <c r="K63" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="L63" s="126"/>
+      <c r="M63" s="35"/>
       <c r="N63" s="85"/>
-      <c r="O63" s="132" t="s">
-        <v>89</v>
-      </c>
+      <c r="O63" s="15"/>
     </row>
     <row r="64" spans="2:15" ht="16" thickBot="1">
       <c r="B64" s="34"/>
       <c r="C64" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="D64" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="E64" s="66"/>
+        <v>88</v>
+      </c>
+      <c r="D64" s="87"/>
+      <c r="E64" s="127">
+        <f>'6_residences'!C8*Dashboard!E62</f>
+        <v>0</v>
+      </c>
       <c r="F64" s="35"/>
-      <c r="G64" s="59"/>
+      <c r="G64"/>
       <c r="H64" s="35"/>
-      <c r="I64" s="16"/>
+      <c r="I64" s="35"/>
       <c r="J64" s="35"/>
-      <c r="K64" s="129"/>
-      <c r="L64" s="40" t="b">
-        <f>IF(COUNTBLANK(E64)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M64" s="35" t="str">
-        <f>IF(L64=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
+      <c r="K64" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="L64" s="126"/>
+      <c r="M64" s="35"/>
       <c r="N64" s="85"/>
-      <c r="O64" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="O64" s="15"/>
     </row>
     <row r="65" spans="2:15" ht="16" thickBot="1">
       <c r="B65" s="34"/>
       <c r="C65" s="35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D65" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="E65" s="53"/>
+      <c r="E65" s="66"/>
       <c r="F65" s="35"/>
       <c r="G65" s="59"/>
       <c r="H65" s="35"/>
       <c r="I65" s="57"/>
       <c r="J65" s="35"/>
-      <c r="K65" s="41"/>
+      <c r="K65" s="128"/>
       <c r="L65" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTBLANK(E65)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M65" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(L65=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N65" s="85"/>
-      <c r="O65" s="15" t="s">
-        <v>91</v>
+      <c r="O65" s="132" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="2:15" ht="16" thickBot="1">
       <c r="B66" s="34"/>
       <c r="C66" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="D66" s="35"/>
-      <c r="E66" s="60"/>
+        <v>90</v>
+      </c>
+      <c r="D66" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E66" s="66"/>
       <c r="F66" s="35"/>
-      <c r="G66"/>
+      <c r="G66" s="59"/>
       <c r="H66" s="35"/>
-      <c r="I66" s="57"/>
+      <c r="I66" s="16"/>
       <c r="J66" s="35"/>
-      <c r="K66" s="35"/>
+      <c r="K66" s="129"/>
       <c r="L66" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTBLANK(E66)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M66" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(L66=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N66" s="85"/>
       <c r="O66" s="15" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="2:15" ht="16" thickBot="1">
-      <c r="B67" s="31"/>
+      <c r="B67" s="34"/>
       <c r="C67" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="D67" s="35"/>
-      <c r="E67" s="60"/>
+        <v>91</v>
+      </c>
+      <c r="D67" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E67" s="53"/>
       <c r="F67" s="35"/>
-      <c r="G67"/>
+      <c r="G67" s="59"/>
       <c r="H67" s="35"/>
       <c r="I67" s="57"/>
       <c r="J67" s="35"/>
-      <c r="K67" s="35"/>
+      <c r="K67" s="41"/>
       <c r="L67" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M67" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Please set value</v>
       </c>
       <c r="N67" s="85"/>
       <c r="O67" s="15" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="2:15" ht="16" thickBot="1">
-      <c r="B68" s="31"/>
-      <c r="C68" t="s">
-        <v>106</v>
-      </c>
-      <c r="D68"/>
-      <c r="E68" s="53"/>
-      <c r="F68"/>
-      <c r="G68" s="58"/>
-      <c r="H68"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" s="35"/>
+      <c r="E68" s="60"/>
+      <c r="F68" s="35"/>
+      <c r="G68"/>
+      <c r="H68" s="35"/>
       <c r="I68" s="57"/>
-      <c r="J68"/>
-      <c r="K68"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="35"/>
       <c r="L68" s="40" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M68" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Please set value</v>
       </c>
       <c r="N68" s="85"/>
       <c r="O68" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15" ht="16" thickBot="1">
+      <c r="B69" s="31"/>
+      <c r="C69" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D69" s="35"/>
+      <c r="E69" s="60"/>
+      <c r="F69" s="35"/>
+      <c r="G69"/>
+      <c r="H69" s="35"/>
+      <c r="I69" s="57"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="35"/>
+      <c r="L69" s="40" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M69" s="35" t="str">
+        <f t="shared" si="7"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N69" s="85"/>
+      <c r="O69" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15" ht="16" thickBot="1">
+      <c r="B70" s="31"/>
+      <c r="C70" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="69" spans="2:15">
-      <c r="B69" s="31"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="7"/>
-      <c r="I69" s="7"/>
-      <c r="J69" s="7"/>
-      <c r="K69" s="7"/>
-      <c r="L69" s="7"/>
-      <c r="M69" s="7"/>
-      <c r="N69" s="85"/>
-      <c r="O69" s="15"/>
-    </row>
-    <row r="70" spans="2:15" ht="16" thickBot="1">
-      <c r="B70" s="42" t="s">
+      <c r="D70"/>
+      <c r="E70" s="53"/>
+      <c r="F70"/>
+      <c r="G70" s="58"/>
+      <c r="H70"/>
+      <c r="I70" s="57"/>
+      <c r="J70"/>
+      <c r="K70"/>
+      <c r="L70" s="40" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M70" s="35" t="str">
+        <f t="shared" si="7"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N70" s="85"/>
+      <c r="O70" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15">
+      <c r="B71" s="31"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="54"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="85"/>
+      <c r="O71" s="15"/>
+    </row>
+    <row r="72" spans="2:15" ht="16" thickBot="1">
+      <c r="B72" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="55"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="85"/>
-      <c r="O70" s="15"/>
-    </row>
-    <row r="71" spans="2:15" ht="16" thickBot="1">
-      <c r="B71" s="31"/>
-      <c r="C71" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="D71" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E71" s="53"/>
-      <c r="F71" s="35"/>
-      <c r="G71"/>
-      <c r="H71" s="35"/>
-      <c r="I71" s="57"/>
-      <c r="J71" s="35"/>
-      <c r="K71" s="35"/>
-      <c r="L71" s="40" t="b">
-        <f>IF(COUNTBLANK(E71)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M71" s="35" t="str">
-        <f>IF(L71=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
-      <c r="N71" s="85"/>
-      <c r="O71" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="72" spans="2:15" ht="16" thickBot="1">
-      <c r="B72" s="31"/>
-      <c r="C72" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D72" s="35"/>
-      <c r="E72" s="66"/>
-      <c r="F72" s="35"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="35"/>
-      <c r="I72" s="57"/>
-      <c r="J72" s="35"/>
-      <c r="K72" s="35"/>
-      <c r="L72" s="40" t="b">
-        <f>IF(COUNTBLANK(E72)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M72" s="35" t="str">
-        <f t="shared" ref="M72:M73" si="6">IF(L72=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="55"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
       <c r="N72" s="85"/>
-      <c r="O72" s="15" t="s">
-        <v>94</v>
-      </c>
+      <c r="O72" s="15"/>
     </row>
     <row r="73" spans="2:15" ht="16" thickBot="1">
       <c r="B73" s="31"/>
       <c r="C73" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="D73" s="35"/>
-      <c r="E73" s="61"/>
+        <v>93</v>
+      </c>
+      <c r="D73" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" s="53"/>
       <c r="F73" s="35"/>
-      <c r="G73" s="59"/>
+      <c r="G73"/>
       <c r="H73" s="35"/>
       <c r="I73" s="57"/>
       <c r="J73" s="35"/>
@@ -5411,104 +5503,104 @@
         <v>0</v>
       </c>
       <c r="M73" s="35" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(L73=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N73" s="85"/>
       <c r="O73" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="2:15" ht="16" thickBot="1">
+      <c r="B74" s="31"/>
+      <c r="C74" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D74" s="35"/>
+      <c r="E74" s="66"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="59"/>
+      <c r="H74" s="35"/>
+      <c r="I74" s="57"/>
+      <c r="J74" s="35"/>
+      <c r="K74" s="35"/>
+      <c r="L74" s="40" t="b">
+        <f>IF(COUNTBLANK(E74)=1,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="M74" s="35" t="str">
+        <f t="shared" ref="M74:M75" si="8">IF(L74=TRUE," ","Please set value")</f>
+        <v>Please set value</v>
+      </c>
+      <c r="N74" s="85"/>
+      <c r="O74" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="2:15" ht="16" thickBot="1">
+      <c r="B75" s="31"/>
+      <c r="C75" s="35" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="74" spans="2:15">
-      <c r="B74" s="43"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="12"/>
-      <c r="K74" s="12"/>
-      <c r="L74" s="12"/>
-      <c r="M74" s="12"/>
-      <c r="N74" s="85"/>
-      <c r="O74" s="15"/>
-    </row>
-    <row r="75" spans="2:15" ht="16" thickBot="1">
-      <c r="B75" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="54"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="I75" s="7"/>
-      <c r="J75" s="7"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="7"/>
-      <c r="M75" s="7"/>
-      <c r="N75" s="85"/>
-      <c r="O75" s="15"/>
-    </row>
-    <row r="76" spans="2:15" ht="16" thickBot="1">
-      <c r="B76" s="31"/>
-      <c r="C76" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="D76" s="35"/>
-      <c r="E76" s="53"/>
-      <c r="F76"/>
-      <c r="G76" s="59"/>
-      <c r="H76" s="35"/>
-      <c r="I76" s="57"/>
-      <c r="J76" s="35"/>
-      <c r="K76" s="35"/>
-      <c r="L76" s="40" t="b">
-        <f t="shared" ref="L76:L82" si="7">IF(COUNTBLANK(E76)=1,FALSE,TRUE)</f>
+      <c r="D75" s="35"/>
+      <c r="E75" s="61"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="59"/>
+      <c r="H75" s="35"/>
+      <c r="I75" s="57"/>
+      <c r="J75" s="35"/>
+      <c r="K75" s="35"/>
+      <c r="L75" s="40" t="b">
+        <f>IF(COUNTBLANK(E75)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="M76" s="35" t="str">
-        <f t="shared" ref="M76:M79" si="8">IF(L76=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
-      <c r="N76" s="85"/>
-      <c r="O76" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="77" spans="2:15" ht="16" thickBot="1">
-      <c r="B77" s="31"/>
-      <c r="C77" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="D77" s="35"/>
-      <c r="E77" s="53"/>
-      <c r="F77"/>
-      <c r="G77" s="59"/>
-      <c r="H77" s="35"/>
-      <c r="I77" s="57"/>
-      <c r="J77" s="35"/>
-      <c r="K77" s="35"/>
-      <c r="L77" s="40" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M77" s="35" t="str">
+      <c r="M75" s="35" t="str">
         <f t="shared" si="8"/>
         <v>Please set value</v>
       </c>
+      <c r="N75" s="85"/>
+      <c r="O75" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="2:15">
+      <c r="B76" s="43"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="56"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12"/>
+      <c r="M76" s="12"/>
+      <c r="N76" s="85"/>
+      <c r="O76" s="15"/>
+    </row>
+    <row r="77" spans="2:15" ht="16" thickBot="1">
+      <c r="B77" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="54"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="7"/>
       <c r="N77" s="85"/>
-      <c r="O77" s="15" t="s">
-        <v>97</v>
-      </c>
+      <c r="O77" s="15"/>
     </row>
     <row r="78" spans="2:15" ht="16" thickBot="1">
       <c r="B78" s="31"/>
       <c r="C78" s="35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D78" s="35"/>
       <c r="E78" s="53"/>
@@ -5519,100 +5611,100 @@
       <c r="J78" s="35"/>
       <c r="K78" s="35"/>
       <c r="L78" s="40" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="L78:L84" si="9">IF(COUNTBLANK(E78)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M78" s="35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="M78:M81" si="10">IF(L78=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N78" s="85"/>
       <c r="O78" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="2:15" ht="16" thickBot="1">
       <c r="B79" s="31"/>
       <c r="C79" s="35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D79" s="35"/>
       <c r="E79" s="53"/>
       <c r="F79"/>
-      <c r="G79" s="58"/>
+      <c r="G79" s="59"/>
       <c r="H79" s="35"/>
       <c r="I79" s="57"/>
       <c r="J79" s="35"/>
       <c r="K79" s="35"/>
       <c r="L79" s="40" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M79" s="35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>Please set value</v>
       </c>
       <c r="N79" s="85"/>
       <c r="O79" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="2:15" ht="16" thickBot="1">
-      <c r="B80" s="34"/>
+      <c r="B80" s="31"/>
       <c r="C80" s="35" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="D80" s="35"/>
-      <c r="E80" s="67"/>
-      <c r="F80" s="35"/>
+      <c r="E80" s="53"/>
+      <c r="F80"/>
       <c r="G80" s="59"/>
       <c r="H80" s="35"/>
       <c r="I80" s="57"/>
       <c r="J80" s="35"/>
       <c r="K80" s="35"/>
       <c r="L80" s="40" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M80" s="35" t="str">
-        <f>IF(L80=TRUE," ","Please set value")</f>
+        <f t="shared" si="10"/>
         <v>Please set value</v>
       </c>
       <c r="N80" s="85"/>
       <c r="O80" s="15" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="2:15" ht="16" thickBot="1">
-      <c r="B81" s="34"/>
+      <c r="B81" s="31"/>
       <c r="C81" s="35" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="D81" s="35"/>
-      <c r="E81" s="67"/>
-      <c r="F81" s="35"/>
-      <c r="G81" s="59"/>
+      <c r="E81" s="53"/>
+      <c r="F81"/>
+      <c r="G81" s="58"/>
       <c r="H81" s="35"/>
       <c r="I81" s="57"/>
       <c r="J81" s="35"/>
       <c r="K81" s="35"/>
       <c r="L81" s="40" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M81" s="35" t="str">
-        <f>IF(L81=TRUE," ","Please set value")</f>
+        <f t="shared" si="10"/>
         <v>Please set value</v>
       </c>
       <c r="N81" s="85"/>
       <c r="O81" s="15" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="2:15" ht="16" thickBot="1">
       <c r="B82" s="34"/>
       <c r="C82" s="35" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D82" s="35"/>
       <c r="E82" s="67"/>
@@ -5623,7 +5715,7 @@
       <c r="J82" s="35"/>
       <c r="K82" s="35"/>
       <c r="L82" s="40" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M82" s="35" t="str">
@@ -5632,99 +5724,99 @@
       </c>
       <c r="N82" s="85"/>
       <c r="O82" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15" ht="16" thickBot="1">
+      <c r="B83" s="34"/>
+      <c r="C83" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D83" s="35"/>
+      <c r="E83" s="67"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="59"/>
+      <c r="H83" s="35"/>
+      <c r="I83" s="57"/>
+      <c r="J83" s="35"/>
+      <c r="K83" s="35"/>
+      <c r="L83" s="40" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M83" s="35" t="str">
+        <f>IF(L83=TRUE," ","Please set value")</f>
+        <v>Please set value</v>
+      </c>
+      <c r="N83" s="85"/>
+      <c r="O83" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="2:15" ht="16" thickBot="1">
+      <c r="B84" s="34"/>
+      <c r="C84" s="35" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="83" spans="2:15">
-      <c r="B83" s="31"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7"/>
-      <c r="E83" s="54"/>
-      <c r="F83" s="7"/>
-      <c r="G83" s="7"/>
-      <c r="H83" s="7"/>
-      <c r="I83" s="7"/>
-      <c r="J83" s="7"/>
-      <c r="K83" s="7"/>
-      <c r="L83" s="7"/>
-      <c r="M83" s="7"/>
-      <c r="N83" s="85"/>
-      <c r="O83" s="15"/>
-    </row>
-    <row r="84" spans="2:15" ht="16" thickBot="1">
-      <c r="B84" s="42" t="s">
+      <c r="D84" s="35"/>
+      <c r="E84" s="67"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="59"/>
+      <c r="H84" s="35"/>
+      <c r="I84" s="57"/>
+      <c r="J84" s="35"/>
+      <c r="K84" s="35"/>
+      <c r="L84" s="40" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M84" s="35" t="str">
+        <f>IF(L84=TRUE," ","Please set value")</f>
+        <v>Please set value</v>
+      </c>
+      <c r="N84" s="85"/>
+      <c r="O84" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="2:15">
+      <c r="B85" s="31"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="54"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="7"/>
+      <c r="N85" s="85"/>
+      <c r="O85" s="15"/>
+    </row>
+    <row r="86" spans="2:15" ht="16" thickBot="1">
+      <c r="B86" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="55"/>
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="4"/>
-      <c r="K84" s="4"/>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
-      <c r="N84" s="85"/>
-      <c r="O84" s="15"/>
-    </row>
-    <row r="85" spans="2:15" ht="16" thickBot="1">
-      <c r="B85" s="31"/>
-      <c r="C85" t="s">
-        <v>100</v>
-      </c>
-      <c r="D85"/>
-      <c r="E85" s="53"/>
-      <c r="F85"/>
-      <c r="G85" s="58"/>
-      <c r="H85"/>
-      <c r="I85" s="57"/>
-      <c r="J85"/>
-      <c r="K85"/>
-      <c r="L85" s="40" t="b">
-        <f>IF(COUNTBLANK(E85)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M85" s="35" t="str">
-        <f t="shared" ref="M85:M93" si="9">IF(L85=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
-      <c r="N85" s="85"/>
-      <c r="O85" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="86" spans="2:15" ht="16" thickBot="1">
-      <c r="B86" s="31"/>
-      <c r="C86" t="s">
-        <v>101</v>
-      </c>
-      <c r="D86"/>
-      <c r="E86" s="53"/>
-      <c r="F86"/>
-      <c r="G86" s="58"/>
-      <c r="H86"/>
-      <c r="I86" s="57"/>
-      <c r="J86"/>
-      <c r="K86"/>
-      <c r="L86" s="40" t="b">
-        <f t="shared" ref="L86:L93" si="10">IF(COUNTBLANK(E86)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M86" s="35" t="str">
-        <f t="shared" si="9"/>
-        <v>Please set value</v>
-      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
       <c r="N86" s="85"/>
-      <c r="O86" s="15" t="s">
-        <v>101</v>
-      </c>
+      <c r="O86" s="15"/>
     </row>
     <row r="87" spans="2:15" ht="16" thickBot="1">
       <c r="B87" s="31"/>
       <c r="C87" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D87"/>
       <c r="E87" s="53"/>
@@ -5735,22 +5827,22 @@
       <c r="J87"/>
       <c r="K87"/>
       <c r="L87" s="40" t="b">
-        <f t="shared" si="10"/>
+        <f>IF(COUNTBLANK(E87)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M87" s="35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="M87:M95" si="11">IF(L87=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N87" s="85"/>
       <c r="O87" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="2:15" ht="16" thickBot="1">
       <c r="B88" s="31"/>
       <c r="C88" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D88"/>
       <c r="E88" s="53"/>
@@ -5761,22 +5853,22 @@
       <c r="J88"/>
       <c r="K88"/>
       <c r="L88" s="40" t="b">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="L88:L95" si="12">IF(COUNTBLANK(E88)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M88" s="35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Please set value</v>
       </c>
       <c r="N88" s="85"/>
       <c r="O88" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="2:15" ht="16" thickBot="1">
       <c r="B89" s="31"/>
       <c r="C89" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D89"/>
       <c r="E89" s="53"/>
@@ -5787,22 +5879,22 @@
       <c r="J89"/>
       <c r="K89"/>
       <c r="L89" s="40" t="b">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M89" s="35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Please set value</v>
       </c>
       <c r="N89" s="85"/>
       <c r="O89" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="2:15" ht="16" thickBot="1">
       <c r="B90" s="31"/>
       <c r="C90" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D90"/>
       <c r="E90" s="53"/>
@@ -5813,51 +5905,51 @@
       <c r="J90"/>
       <c r="K90"/>
       <c r="L90" s="40" t="b">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M90" s="35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Please set value</v>
       </c>
       <c r="N90" s="85"/>
       <c r="O90" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="2:15" ht="16" thickBot="1">
       <c r="B91" s="31"/>
       <c r="C91" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="D91"/>
-      <c r="E91" s="138"/>
+      <c r="E91" s="53"/>
       <c r="F91"/>
       <c r="G91" s="58"/>
       <c r="H91"/>
-      <c r="I91" s="134"/>
+      <c r="I91" s="57"/>
       <c r="J91"/>
       <c r="K91"/>
       <c r="L91" s="40" t="b">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M91" s="35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Please set value</v>
       </c>
       <c r="N91" s="85"/>
-      <c r="O91" s="136" t="s">
-        <v>140</v>
+      <c r="O91" s="15" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="2:15" ht="16" thickBot="1">
       <c r="B92" s="31"/>
       <c r="C92" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="D92"/>
-      <c r="E92" s="66"/>
+      <c r="E92" s="53"/>
       <c r="F92"/>
       <c r="G92" s="58"/>
       <c r="H92"/>
@@ -5865,140 +5957,202 @@
       <c r="J92"/>
       <c r="K92"/>
       <c r="L92" s="40" t="b">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M92" s="35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Please set value</v>
       </c>
       <c r="N92" s="85"/>
-      <c r="O92" s="132" t="s">
-        <v>139</v>
+      <c r="O92" s="15" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="2:15" ht="16" thickBot="1">
       <c r="B93" s="31"/>
-      <c r="C93" s="129" t="s">
-        <v>141</v>
+      <c r="C93" t="s">
+        <v>140</v>
       </c>
       <c r="D93"/>
-      <c r="E93" s="133"/>
+      <c r="E93" s="138"/>
       <c r="F93"/>
       <c r="G93" s="58"/>
       <c r="H93"/>
-      <c r="I93" s="135"/>
+      <c r="I93" s="134"/>
       <c r="J93"/>
       <c r="K93"/>
       <c r="L93" s="40" t="b">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M93" s="35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Please set value</v>
       </c>
       <c r="N93" s="85"/>
-      <c r="O93" s="137" t="s">
+      <c r="O93" s="136" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="2:15" ht="16" thickBot="1">
+      <c r="B94" s="31"/>
+      <c r="C94" t="s">
+        <v>139</v>
+      </c>
+      <c r="D94"/>
+      <c r="E94" s="66"/>
+      <c r="F94"/>
+      <c r="G94" s="58"/>
+      <c r="H94"/>
+      <c r="I94" s="57"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94" s="40" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M94" s="35" t="str">
+        <f t="shared" si="11"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N94" s="85"/>
+      <c r="O94" s="132" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="95" spans="2:15" ht="16" thickBot="1">
+      <c r="B95" s="31"/>
+      <c r="C95" s="129" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="94" spans="2:15">
-      <c r="B94" s="31"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="54"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-      <c r="I94" s="7"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="7"/>
-      <c r="L94" s="7"/>
-      <c r="M94" s="7"/>
-      <c r="N94" s="85"/>
-      <c r="O94" s="15"/>
-    </row>
-    <row r="95" spans="2:15" ht="16" thickBot="1">
-      <c r="B95" s="42" t="s">
+      <c r="D95"/>
+      <c r="E95" s="133"/>
+      <c r="F95"/>
+      <c r="G95" s="58"/>
+      <c r="H95"/>
+      <c r="I95" s="135"/>
+      <c r="J95"/>
+      <c r="K95"/>
+      <c r="L95" s="40" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M95" s="35" t="str">
+        <f t="shared" si="11"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N95" s="85"/>
+      <c r="O95" s="137" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="96" spans="2:15">
+      <c r="B96" s="31"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="54"/>
+      <c r="F96" s="7"/>
+      <c r="G96" s="7"/>
+      <c r="H96" s="7"/>
+      <c r="I96" s="7"/>
+      <c r="J96" s="7"/>
+      <c r="K96" s="7"/>
+      <c r="L96" s="7"/>
+      <c r="M96" s="7"/>
+      <c r="N96" s="85"/>
+      <c r="O96" s="15"/>
+    </row>
+    <row r="97" spans="2:15" ht="16" thickBot="1">
+      <c r="B97" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
-      <c r="E95" s="55"/>
-      <c r="F95" s="4"/>
-      <c r="G95" s="4"/>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
-      <c r="J95" s="4"/>
-      <c r="K95" s="4"/>
-      <c r="L95" s="4"/>
-      <c r="M95" s="4"/>
-      <c r="N95" s="85"/>
-      <c r="O95" s="15"/>
-    </row>
-    <row r="96" spans="2:15" ht="16" thickBot="1">
-      <c r="B96" s="31"/>
-      <c r="C96" t="s">
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="55"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="85"/>
+      <c r="O97" s="15"/>
+    </row>
+    <row r="98" spans="2:15" ht="16" thickBot="1">
+      <c r="B98" s="31"/>
+      <c r="C98" t="s">
         <v>145</v>
       </c>
-      <c r="D96"/>
-      <c r="E96" s="53"/>
-      <c r="F96"/>
-      <c r="G96" s="58"/>
-      <c r="H96"/>
-      <c r="I96" s="57"/>
-      <c r="J96"/>
-      <c r="K96"/>
-      <c r="L96" s="40" t="b">
-        <f>IF(COUNTBLANK(E96)=1,FALSE,TRUE)</f>
+      <c r="D98"/>
+      <c r="E98" s="53"/>
+      <c r="F98"/>
+      <c r="G98" s="58"/>
+      <c r="H98"/>
+      <c r="I98" s="57"/>
+      <c r="J98"/>
+      <c r="K98"/>
+      <c r="L98" s="40" t="b">
+        <f>IF(COUNTBLANK(E98)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="M96" s="35" t="str">
-        <f t="shared" ref="M96" si="11">IF(L96=TRUE," ","Please set value")</f>
+      <c r="M98" s="35" t="str">
+        <f t="shared" ref="M98" si="13">IF(L98=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
-      <c r="N96" s="85"/>
-      <c r="O96" s="15" t="s">
+      <c r="N98" s="85"/>
+      <c r="O98" s="15" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="97" spans="2:15" ht="16" thickBot="1">
-      <c r="B97" s="44"/>
-      <c r="C97" s="36"/>
-      <c r="D97" s="36"/>
-      <c r="E97" s="52"/>
-      <c r="F97" s="36"/>
-      <c r="G97" s="36"/>
-      <c r="H97" s="36"/>
-      <c r="I97" s="36"/>
-      <c r="J97" s="36"/>
-      <c r="K97" s="36"/>
-      <c r="L97" s="36"/>
-      <c r="M97" s="36"/>
-      <c r="N97" s="31"/>
-      <c r="O97" s="7"/>
+    <row r="99" spans="2:15" ht="16" thickBot="1">
+      <c r="B99" s="44"/>
+      <c r="C99" s="36"/>
+      <c r="D99" s="36"/>
+      <c r="E99" s="52"/>
+      <c r="F99" s="36"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="36"/>
+      <c r="I99" s="36"/>
+      <c r="J99" s="36"/>
+      <c r="K99" s="36"/>
+      <c r="L99" s="36"/>
+      <c r="M99" s="36"/>
+      <c r="N99" s="31"/>
+      <c r="O99" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:I5"/>
   </mergeCells>
-  <conditionalFormatting sqref="L76:L82 L39:L44 L71:L73 L18:L36 L47:L52 L54 L56:L67 L89:L93">
-    <cfRule type="cellIs" dxfId="3" priority="14" operator="equal">
+  <conditionalFormatting sqref="L78:L84 L41:L46 L73:L75 L18:L36 L49:L54 L56 L58:L69 L91:L95">
+    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L85:L88">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+  <conditionalFormatting sqref="L87:L90">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L68">
+  <conditionalFormatting sqref="L70">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L98">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L37">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L96">
+  <conditionalFormatting sqref="L38">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -6008,7 +6162,7 @@
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39:E43 E46:E58 D59:D62 E63:E65 E68:E97">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E41:E45 E48:E60 D61:D64 E65:E67 E70:E99">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6325,10 +6479,10 @@
     </row>
     <row r="5" spans="1:48">
       <c r="A5" s="114"/>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="144" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="145"/>
+      <c r="C5" s="146"/>
       <c r="D5" s="114"/>
       <c r="E5" s="112"/>
       <c r="F5" s="112"/>
@@ -12148,10 +12302,10 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:E120"/>
+  <dimension ref="B1:E123"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12240,7 +12394,7 @@
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="104" t="str">
-        <f t="shared" ref="E11:E38" si="0">IF(COUNTBLANK(B11)=0,"- "&amp;B11&amp;" = "&amp;LOWER(C11),"")</f>
+        <f t="shared" ref="E11:E41" si="0">IF(COUNTBLANK(B11)=0,"- "&amp;B11&amp;" = "&amp;LOWER(C11),"")</f>
         <v xml:space="preserve">- area = </v>
       </c>
     </row>
@@ -12620,110 +12774,102 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="102" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C37)=0,Dashboard!C37,"")</f>
-        <v/>
-      </c>
-      <c r="C37" s="90" t="str">
+      <c r="B37" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!O37)=0,Dashboard!O37,"")</f>
+        <v>has_aggregated_chemical_industry</v>
+      </c>
+      <c r="C37" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E37)=0,Dashboard!E37,"")</f>
         <v/>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="105" t="str">
+      <c r="D37" s="35"/>
+      <c r="E37" s="104" t="str">
+        <f>IF(COUNTBLANK(B37)=0,"- "&amp;B37&amp;" = "&amp;LOWER(C37),"")</f>
+        <v xml:space="preserve">- has_aggregated_chemical_industry = </v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="103" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" s="143" t="str">
+        <f>IF(Dashboard!E37="true","false", IF(Dashboard!E37="false","true","ERROR"))</f>
+        <v>ERROR</v>
+      </c>
+      <c r="D38" s="35"/>
+      <c r="E38" s="105" t="str">
+        <f t="shared" si="0"/>
+        <v>- has_detailed_chemical_industry = error</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!O38)=0,Dashboard!O38,"")</f>
+        <v>has_aggregated_other_industry</v>
+      </c>
+      <c r="C39" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E38)=0,Dashboard!E38,"")</f>
+        <v/>
+      </c>
+      <c r="D39" s="35"/>
+      <c r="E39" s="105" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">- has_aggregated_other_industry = </v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="103" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" s="143" t="str">
+        <f>IF(Dashboard!E38="true","false", IF(Dashboard!E38="false","true","ERROR"))</f>
+        <v>ERROR</v>
+      </c>
+      <c r="D40" s="35"/>
+      <c r="E40" s="105" t="str">
+        <f t="shared" si="0"/>
+        <v>- has_detailed_other_industry = error</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C40)=0,Dashboard!C40,"")</f>
+        <v/>
+      </c>
+      <c r="C41" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E40)=0,Dashboard!E40,"")</f>
+        <v/>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="105" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="102" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C38)=0,Dashboard!C38,"")</f>
-        <v/>
-      </c>
-      <c r="C38" s="90" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E38)=0,Dashboard!E38,"")</f>
-        <v/>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="105" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C39)=0,Dashboard!C39,"")</f>
+    <row r="42" spans="2:5">
+      <c r="B42" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C41)=0,Dashboard!C41,"")</f>
         <v>areable_land</v>
       </c>
-      <c r="C39" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E39)=0,Dashboard!E39,"")</f>
-        <v/>
-      </c>
-      <c r="D39" s="35">
-        <v>1</v>
-      </c>
-      <c r="E39" s="104" t="e">
-        <f t="shared" ref="E39:E70" si="2">IF(COUNTBLANK(B39)=0,"- "&amp;B39&amp;" = "&amp;FIXED(C39,D39,1),"")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C40)=0,Dashboard!C40,"")</f>
-        <v>coast_line</v>
-      </c>
-      <c r="C40" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E40)=0,Dashboard!E40,"")</f>
-        <v/>
-      </c>
-      <c r="D40" s="35">
-        <v>1</v>
-      </c>
-      <c r="E40" s="104" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5">
-      <c r="B41" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C41)=0,Dashboard!C41,"")</f>
-        <v>land_available_for_solar</v>
-      </c>
-      <c r="C41" s="35" t="str">
+      <c r="C42" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E41)=0,Dashboard!E41,"")</f>
         <v/>
       </c>
-      <c r="D41" s="35">
-        <v>3</v>
-      </c>
-      <c r="E41" s="104" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C42)=0,Dashboard!C42,"")</f>
-        <v>number_of_inhabitants</v>
-      </c>
-      <c r="C42" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E42)=0,Dashboard!E42,"")</f>
-        <v/>
-      </c>
       <c r="D42" s="35">
         <v>1</v>
       </c>
       <c r="E42" s="104" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E42:E73" si="2">IF(COUNTBLANK(B42)=0,"- "&amp;B42&amp;" = "&amp;FIXED(C42,D42,1),"")</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C43)=0,Dashboard!C43,"")</f>
-        <v>offshore_suitable_for_wind</v>
+        <f>IF(COUNTBLANK(Dashboard!C42)=0,Dashboard!C42,"")</f>
+        <v>coast_line</v>
       </c>
       <c r="C43" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E43)=0,Dashboard!E43,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E42)=0,Dashboard!E42,"")</f>
         <v/>
       </c>
       <c r="D43" s="35">
@@ -12736,15 +12882,15 @@
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C44)=0,Dashboard!C44,"")</f>
-        <v>onshore_suitable_for_wind</v>
+        <f>IF(COUNTBLANK(Dashboard!C43)=0,Dashboard!C43,"")</f>
+        <v>land_available_for_solar</v>
       </c>
       <c r="C44" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E44)=0,Dashboard!E44,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E43)=0,Dashboard!E43,"")</f>
         <v/>
       </c>
       <c r="D44" s="35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E44" s="104" t="e">
         <f t="shared" si="2"/>
@@ -12752,46 +12898,50 @@
       </c>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="102" t="str">
+      <c r="B45" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C44)=0,Dashboard!C44,"")</f>
+        <v>number_of_inhabitants</v>
+      </c>
+      <c r="C45" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E44)=0,Dashboard!E44,"")</f>
+        <v/>
+      </c>
+      <c r="D45" s="35">
+        <v>1</v>
+      </c>
+      <c r="E45" s="104" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="B46" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C45)=0,Dashboard!C45,"")</f>
-        <v/>
-      </c>
-      <c r="C45" s="90" t="str">
+        <v>offshore_suitable_for_wind</v>
+      </c>
+      <c r="C46" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E45)=0,Dashboard!E45,"")</f>
         <v/>
       </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="105" t="str">
+      <c r="D46" s="35">
+        <v>1</v>
+      </c>
+      <c r="E46" s="104" t="e">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="2:5">
-      <c r="B46" s="102" t="str">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C46)=0,Dashboard!C46,"")</f>
-        <v/>
-      </c>
-      <c r="C46" s="90" t="str">
+        <v>onshore_suitable_for_wind</v>
+      </c>
+      <c r="C47" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E46)=0,Dashboard!E46,"")</f>
         <v/>
       </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="105" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="2:5">
-      <c r="B47" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C47)=0,Dashboard!C47,"")</f>
-        <v>buildings_insulation_constant_1</v>
-      </c>
-      <c r="C47" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E47)=0,Dashboard!E47,"")</f>
-        <v/>
-      </c>
       <c r="D47" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" s="104" t="e">
         <f t="shared" si="2"/>
@@ -12799,50 +12949,46 @@
       </c>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="103" t="str">
+      <c r="B48" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C47)=0,Dashboard!C47,"")</f>
+        <v/>
+      </c>
+      <c r="C48" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E47)=0,Dashboard!E47,"")</f>
+        <v/>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="105" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" s="102" t="str">
         <f>IF(COUNTBLANK(Dashboard!C48)=0,Dashboard!C48,"")</f>
-        <v>buildings_insulation_constant_2</v>
-      </c>
-      <c r="C48" s="35" t="str">
+        <v/>
+      </c>
+      <c r="C49" s="90" t="str">
         <f>IF(COUNTBLANK(Dashboard!E48)=0,Dashboard!E48,"")</f>
         <v/>
       </c>
-      <c r="D48" s="35">
-        <v>2</v>
-      </c>
-      <c r="E48" s="104" t="e">
+      <c r="D49" s="7"/>
+      <c r="E49" s="105" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="103" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C49)=0,Dashboard!C49,"")</f>
-        <v>buildings_insulation_cost_constant</v>
-      </c>
-      <c r="C49" s="35" t="str">
+        <v>buildings_insulation_constant_1</v>
+      </c>
+      <c r="C50" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E49)=0,Dashboard!E49,"")</f>
         <v/>
       </c>
-      <c r="D49" s="35">
-        <v>1</v>
-      </c>
-      <c r="E49" s="104" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5">
-      <c r="B50" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C50)=0,Dashboard!C50,"")</f>
-        <v>insulation_level_buildings_max</v>
-      </c>
-      <c r="C50" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E50)=0,Dashboard!E50,"")</f>
-        <v/>
-      </c>
       <c r="D50" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E50" s="104" t="e">
         <f t="shared" si="2"/>
@@ -12851,15 +12997,15 @@
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C51)=0,Dashboard!C51,"")</f>
-        <v>insulation_level_buildings_min</v>
+        <f>IF(COUNTBLANK(Dashboard!C50)=0,Dashboard!C50,"")</f>
+        <v>buildings_insulation_constant_2</v>
       </c>
       <c r="C51" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E51)=0,Dashboard!E51,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E50)=0,Dashboard!E50,"")</f>
         <v/>
       </c>
       <c r="D51" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" s="104" t="e">
         <f t="shared" si="2"/>
@@ -12868,11 +13014,11 @@
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C52)=0,Dashboard!C52,"")</f>
-        <v>insulation_level_new_houses_max</v>
+        <f>IF(COUNTBLANK(Dashboard!C51)=0,Dashboard!C51,"")</f>
+        <v>buildings_insulation_cost_constant</v>
       </c>
       <c r="C52" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E52)=0,Dashboard!E52,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E51)=0,Dashboard!E51,"")</f>
         <v/>
       </c>
       <c r="D52" s="35">
@@ -12885,28 +13031,28 @@
     </row>
     <row r="53" spans="2:5">
       <c r="B53" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C53)=0,Dashboard!C53,"")</f>
-        <v>insulation_level_new_houses_min</v>
-      </c>
-      <c r="C53" s="35">
-        <f>IF(COUNTBLANK(Dashboard!E53)=0,Dashboard!E53,"")</f>
-        <v>0</v>
+        <f>IF(COUNTBLANK(Dashboard!C52)=0,Dashboard!C52,"")</f>
+        <v>insulation_level_buildings_max</v>
+      </c>
+      <c r="C53" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E52)=0,Dashboard!E52,"")</f>
+        <v/>
       </c>
       <c r="D53" s="35">
         <v>1</v>
       </c>
-      <c r="E53" s="104" t="str">
+      <c r="E53" s="104" t="e">
         <f t="shared" si="2"/>
-        <v>- insulation_level_new_houses_min = 0.0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C54)=0,Dashboard!C54,"")</f>
-        <v>insulation_level_old_houses_max</v>
+        <f>IF(COUNTBLANK(Dashboard!C53)=0,Dashboard!C53,"")</f>
+        <v>insulation_level_buildings_min</v>
       </c>
       <c r="C54" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E54)=0,Dashboard!E54,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E53)=0,Dashboard!E53,"")</f>
         <v/>
       </c>
       <c r="D54" s="35">
@@ -12919,49 +13065,49 @@
     </row>
     <row r="55" spans="2:5">
       <c r="B55" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C54)=0,Dashboard!C54,"")</f>
+        <v>insulation_level_new_houses_max</v>
+      </c>
+      <c r="C55" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E54)=0,Dashboard!E54,"")</f>
+        <v/>
+      </c>
+      <c r="D55" s="35">
+        <v>1</v>
+      </c>
+      <c r="E55" s="104" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5">
+      <c r="B56" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C55)=0,Dashboard!C55,"")</f>
-        <v>insulation_level_old_houses_min</v>
-      </c>
-      <c r="C55" s="35">
+        <v>insulation_level_new_houses_min</v>
+      </c>
+      <c r="C56" s="35">
         <f>IF(COUNTBLANK(Dashboard!E55)=0,Dashboard!E55,"")</f>
         <v>0</v>
       </c>
-      <c r="D55" s="35">
+      <c r="D56" s="35">
         <v>1</v>
       </c>
-      <c r="E55" s="104" t="str">
+      <c r="E56" s="104" t="str">
         <f t="shared" si="2"/>
-        <v>- insulation_level_old_houses_min = 0.0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5">
-      <c r="B56" s="103" t="str">
+        <v>- insulation_level_new_houses_min = 0.0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C56)=0,Dashboard!C56,"")</f>
-        <v>new_houses_insulation_constant_1</v>
-      </c>
-      <c r="C56" s="35" t="str">
+        <v>insulation_level_old_houses_max</v>
+      </c>
+      <c r="C57" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E56)=0,Dashboard!E56,"")</f>
         <v/>
       </c>
-      <c r="D56" s="35">
-        <v>2</v>
-      </c>
-      <c r="E56" s="104" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5">
-      <c r="B57" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C57)=0,Dashboard!C57,"")</f>
-        <v>new_houses_insulation_constant_2</v>
-      </c>
-      <c r="C57" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E57)=0,Dashboard!E57,"")</f>
-        <v/>
-      </c>
       <c r="D57" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57" s="104" t="e">
         <f t="shared" si="2"/>
@@ -12970,32 +13116,32 @@
     </row>
     <row r="58" spans="2:5">
       <c r="B58" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C57)=0,Dashboard!C57,"")</f>
+        <v>insulation_level_old_houses_min</v>
+      </c>
+      <c r="C58" s="35">
+        <f>IF(COUNTBLANK(Dashboard!E57)=0,Dashboard!E57,"")</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="35">
+        <v>1</v>
+      </c>
+      <c r="E58" s="104" t="str">
+        <f t="shared" si="2"/>
+        <v>- insulation_level_old_houses_min = 0.0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="B59" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C58)=0,Dashboard!C58,"")</f>
-        <v>new_houses_insulation_cost_constant</v>
-      </c>
-      <c r="C58" s="35" t="str">
+        <v>new_houses_insulation_constant_1</v>
+      </c>
+      <c r="C59" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E58)=0,Dashboard!E58,"")</f>
         <v/>
       </c>
-      <c r="D58" s="35">
-        <v>1</v>
-      </c>
-      <c r="E58" s="104" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5">
-      <c r="B59" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C59)=0,Dashboard!C59,"")</f>
-        <v>number_of_buildings</v>
-      </c>
-      <c r="C59" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E59)=0,Dashboard!E59,"")</f>
-        <v/>
-      </c>
       <c r="D59" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E59" s="104" t="e">
         <f t="shared" si="2"/>
@@ -13004,15 +13150,15 @@
     </row>
     <row r="60" spans="2:5">
       <c r="B60" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C60)=0,Dashboard!C60,"")</f>
-        <v>number_of_residences</v>
+        <f>IF(COUNTBLANK(Dashboard!C59)=0,Dashboard!C59,"")</f>
+        <v>new_houses_insulation_constant_2</v>
       </c>
       <c r="C60" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E60)=0,Dashboard!E60,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E59)=0,Dashboard!E59,"")</f>
         <v/>
       </c>
       <c r="D60" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E60" s="104" t="e">
         <f t="shared" si="2"/>
@@ -13021,49 +13167,49 @@
     </row>
     <row r="61" spans="2:5">
       <c r="B61" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C61)=0,Dashboard!C61,"")</f>
-        <v>number_of_new_residences</v>
-      </c>
-      <c r="C61" s="35">
-        <f>IF(COUNTBLANK(Dashboard!E61)=0,Dashboard!E61,"")</f>
-        <v>0</v>
+        <f>IF(COUNTBLANK(Dashboard!C60)=0,Dashboard!C60,"")</f>
+        <v>new_houses_insulation_cost_constant</v>
+      </c>
+      <c r="C61" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E60)=0,Dashboard!E60,"")</f>
+        <v/>
       </c>
       <c r="D61" s="35">
         <v>1</v>
       </c>
-      <c r="E61" s="104" t="str">
+      <c r="E61" s="104" t="e">
         <f t="shared" si="2"/>
-        <v>- number_of_new_residences = 0.0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="62" spans="2:5">
       <c r="B62" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C62)=0,Dashboard!C62,"")</f>
-        <v>number_of_old_residences</v>
-      </c>
-      <c r="C62" s="35">
-        <f>IF(COUNTBLANK(Dashboard!E62)=0,Dashboard!E62,"")</f>
-        <v>0</v>
+        <f>IF(COUNTBLANK(Dashboard!C61)=0,Dashboard!C61,"")</f>
+        <v>number_of_buildings</v>
+      </c>
+      <c r="C62" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E61)=0,Dashboard!E61,"")</f>
+        <v/>
       </c>
       <c r="D62" s="35">
         <v>1</v>
       </c>
-      <c r="E62" s="104" t="str">
+      <c r="E62" s="104" t="e">
         <f t="shared" si="2"/>
-        <v>- number_of_old_residences = 0.0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="63" spans="2:5">
       <c r="B63" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C63)=0,Dashboard!C63,"")</f>
-        <v>old_houses_insulation_constant_1</v>
+        <f>IF(COUNTBLANK(Dashboard!C62)=0,Dashboard!C62,"")</f>
+        <v>number_of_residences</v>
       </c>
       <c r="C63" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E63)=0,Dashboard!E63,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E62)=0,Dashboard!E62,"")</f>
         <v/>
       </c>
       <c r="D63" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63" s="104" t="e">
         <f t="shared" si="2"/>
@@ -13072,49 +13218,49 @@
     </row>
     <row r="64" spans="2:5">
       <c r="B64" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C64)=0,Dashboard!C64,"")</f>
-        <v>old_houses_insulation_constant_2</v>
-      </c>
-      <c r="C64" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E64)=0,Dashboard!E64,"")</f>
-        <v/>
+        <f>IF(COUNTBLANK(Dashboard!C63)=0,Dashboard!C63,"")</f>
+        <v>number_of_new_residences</v>
+      </c>
+      <c r="C64" s="35">
+        <f>IF(COUNTBLANK(Dashboard!E63)=0,Dashboard!E63,"")</f>
+        <v>0</v>
       </c>
       <c r="D64" s="35">
-        <v>2</v>
-      </c>
-      <c r="E64" s="104" t="e">
+        <v>1</v>
+      </c>
+      <c r="E64" s="104" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>- number_of_new_residences = 0.0</v>
       </c>
     </row>
     <row r="65" spans="2:5">
       <c r="B65" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C64)=0,Dashboard!C64,"")</f>
+        <v>number_of_old_residences</v>
+      </c>
+      <c r="C65" s="35">
+        <f>IF(COUNTBLANK(Dashboard!E64)=0,Dashboard!E64,"")</f>
+        <v>0</v>
+      </c>
+      <c r="D65" s="35">
+        <v>1</v>
+      </c>
+      <c r="E65" s="104" t="str">
+        <f t="shared" si="2"/>
+        <v>- number_of_old_residences = 0.0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="B66" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C65)=0,Dashboard!C65,"")</f>
-        <v>old_houses_insulation_cost_constant</v>
-      </c>
-      <c r="C65" s="35" t="str">
+        <v>old_houses_insulation_constant_1</v>
+      </c>
+      <c r="C66" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E65)=0,Dashboard!E65,"")</f>
         <v/>
       </c>
-      <c r="D65" s="35">
-        <v>1</v>
-      </c>
-      <c r="E65" s="104" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5">
-      <c r="B66" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C66)=0,Dashboard!C66,"")</f>
-        <v>residences_roof_surface_available_for_pv</v>
-      </c>
-      <c r="C66" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E66)=0,Dashboard!E66,"")</f>
-        <v/>
-      </c>
       <c r="D66" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E66" s="104" t="e">
         <f t="shared" si="2"/>
@@ -13123,15 +13269,15 @@
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C67)=0,Dashboard!C67,"")</f>
-        <v>buildings_roof_surface_available_for_pv</v>
+        <f>IF(COUNTBLANK(Dashboard!C66)=0,Dashboard!C66,"")</f>
+        <v>old_houses_insulation_constant_2</v>
       </c>
       <c r="C67" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E67)=0,Dashboard!E67,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E66)=0,Dashboard!E66,"")</f>
         <v/>
       </c>
       <c r="D67" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E67" s="104" t="e">
         <f t="shared" si="2"/>
@@ -13140,11 +13286,11 @@
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C68)=0,Dashboard!C68,"")</f>
-        <v>technical_lifetime_insulation</v>
+        <f>IF(COUNTBLANK(Dashboard!C67)=0,Dashboard!C67,"")</f>
+        <v>old_houses_insulation_cost_constant</v>
       </c>
       <c r="C68" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E68)=0,Dashboard!E68,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E67)=0,Dashboard!E67,"")</f>
         <v/>
       </c>
       <c r="D68" s="35">
@@ -13156,127 +13302,131 @@
       </c>
     </row>
     <row r="69" spans="2:5">
-      <c r="B69" s="102" t="str">
+      <c r="B69" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C68)=0,Dashboard!C68,"")</f>
+        <v>residences_roof_surface_available_for_pv</v>
+      </c>
+      <c r="C69" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E68)=0,Dashboard!E68,"")</f>
+        <v/>
+      </c>
+      <c r="D69" s="35">
+        <v>1</v>
+      </c>
+      <c r="E69" s="104" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="B70" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C69)=0,Dashboard!C69,"")</f>
-        <v/>
-      </c>
-      <c r="C69" s="90" t="str">
+        <v>buildings_roof_surface_available_for_pv</v>
+      </c>
+      <c r="C70" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E69)=0,Dashboard!E69,"")</f>
         <v/>
       </c>
-      <c r="D69" s="7"/>
-      <c r="E69" s="105" t="str">
+      <c r="D70" s="35">
+        <v>1</v>
+      </c>
+      <c r="E70" s="104" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C70)=0,Dashboard!C70,"")</f>
+        <v>technical_lifetime_insulation</v>
+      </c>
+      <c r="C71" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E70)=0,Dashboard!E70,"")</f>
+        <v/>
+      </c>
+      <c r="D71" s="35">
+        <v>1</v>
+      </c>
+      <c r="E71" s="104" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C71)=0,Dashboard!C71,"")</f>
+        <v/>
+      </c>
+      <c r="C72" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E71)=0,Dashboard!E71,"")</f>
+        <v/>
+      </c>
+      <c r="D72" s="7"/>
+      <c r="E72" s="105" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:5">
-      <c r="B70" s="102" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C70)=0,Dashboard!C70,"")</f>
+    <row r="73" spans="2:5">
+      <c r="B73" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C72)=0,Dashboard!C72,"")</f>
         <v/>
       </c>
-      <c r="C70" s="90" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E70)=0,Dashboard!E70,"")</f>
+      <c r="C73" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E72)=0,Dashboard!E72,"")</f>
         <v/>
       </c>
-      <c r="D70" s="7"/>
-      <c r="E70" s="105" t="str">
+      <c r="D73" s="7"/>
+      <c r="E73" s="105" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="2:5">
-      <c r="B71" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C71)=0,Dashboard!C71,"")</f>
+    <row r="74" spans="2:5">
+      <c r="B74" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C73)=0,Dashboard!C73,"")</f>
         <v>co2_emission_1990</v>
       </c>
-      <c r="C71" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E71)=0,Dashboard!E71,"")</f>
+      <c r="C74" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E73)=0,Dashboard!E73,"")</f>
         <v/>
       </c>
-      <c r="D71" s="35">
+      <c r="D74" s="35">
         <v>5</v>
       </c>
-      <c r="E71" s="104" t="e">
-        <f t="shared" ref="E71:E96" si="3">IF(COUNTBLANK(B71)=0,"- "&amp;B71&amp;" = "&amp;FIXED(C71,D71,1),"")</f>
+      <c r="E74" s="104" t="e">
+        <f t="shared" ref="E74:E99" si="3">IF(COUNTBLANK(B74)=0,"- "&amp;B74&amp;" = "&amp;FIXED(C74,D74,1),"")</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="72" spans="2:5">
-      <c r="B72" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C72)=0,Dashboard!C72,"")</f>
+    <row r="75" spans="2:5">
+      <c r="B75" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C74)=0,Dashboard!C74,"")</f>
         <v>co2_percentage_free</v>
       </c>
-      <c r="C72" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E72)=0,Dashboard!E72,"")</f>
+      <c r="C75" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E74)=0,Dashboard!E74,"")</f>
         <v/>
       </c>
-      <c r="D72" s="35">
+      <c r="D75" s="35">
         <v>2</v>
       </c>
-      <c r="E72" s="104" t="e">
+      <c r="E75" s="104" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="73" spans="2:5">
-      <c r="B73" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C73)=0,Dashboard!C73,"")</f>
+    <row r="76" spans="2:5">
+      <c r="B76" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C75)=0,Dashboard!C75,"")</f>
         <v>co2_price</v>
       </c>
-      <c r="C73" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E73)=0,Dashboard!E73,"")</f>
-        <v/>
-      </c>
-      <c r="D73" s="35">
-        <v>5</v>
-      </c>
-      <c r="E73" s="104" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5">
-      <c r="B74" s="102" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C74)=0,Dashboard!C74,"")</f>
-        <v/>
-      </c>
-      <c r="C74" s="90" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E74)=0,Dashboard!E74,"")</f>
-        <v/>
-      </c>
-      <c r="D74" s="7"/>
-      <c r="E74" s="105" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="2:5">
-      <c r="B75" s="102" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C75)=0,Dashboard!C75,"")</f>
-        <v/>
-      </c>
-      <c r="C75" s="90" t="str">
+      <c r="C76" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E75)=0,Dashboard!E75,"")</f>
         <v/>
       </c>
-      <c r="D75" s="7"/>
-      <c r="E75" s="105" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="2:5">
-      <c r="B76" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C76)=0,Dashboard!C76,"")</f>
-        <v>economic_multiplier</v>
-      </c>
-      <c r="C76" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E76)=0,Dashboard!E76,"")</f>
-        <v/>
-      </c>
       <c r="D76" s="35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E76" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13284,46 +13434,42 @@
       </c>
     </row>
     <row r="77" spans="2:5">
-      <c r="B77" s="103" t="str">
+      <c r="B77" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C76)=0,Dashboard!C76,"")</f>
+        <v/>
+      </c>
+      <c r="C77" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E76)=0,Dashboard!E76,"")</f>
+        <v/>
+      </c>
+      <c r="D77" s="7"/>
+      <c r="E77" s="105" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="2:5">
+      <c r="B78" s="102" t="str">
         <f>IF(COUNTBLANK(Dashboard!C77)=0,Dashboard!C77,"")</f>
-        <v>employment_fraction_production</v>
-      </c>
-      <c r="C77" s="35" t="str">
+        <v/>
+      </c>
+      <c r="C78" s="90" t="str">
         <f>IF(COUNTBLANK(Dashboard!E77)=0,Dashboard!E77,"")</f>
         <v/>
       </c>
-      <c r="D77" s="35">
-        <v>1</v>
-      </c>
-      <c r="E77" s="104" t="e">
+      <c r="D78" s="7"/>
+      <c r="E78" s="105" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5">
-      <c r="B78" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C78)=0,Dashboard!C78,"")</f>
-        <v>employment_local_fraction</v>
-      </c>
-      <c r="C78" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E78)=0,Dashboard!E78,"")</f>
         <v/>
-      </c>
-      <c r="D78" s="35">
-        <v>1</v>
-      </c>
-      <c r="E78" s="104" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="79" spans="2:5">
       <c r="B79" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C79)=0,Dashboard!C79,"")</f>
-        <v>man_hours_per_man_year</v>
+        <f>IF(COUNTBLANK(Dashboard!C78)=0,Dashboard!C78,"")</f>
+        <v>economic_multiplier</v>
       </c>
       <c r="C79" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E79)=0,Dashboard!E79,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E78)=0,Dashboard!E78,"")</f>
         <v/>
       </c>
       <c r="D79" s="35">
@@ -13336,15 +13482,15 @@
     </row>
     <row r="80" spans="2:5">
       <c r="B80" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C80)=0,Dashboard!C80,"")</f>
-        <v>buildings_insulation_employment_constant</v>
+        <f>IF(COUNTBLANK(Dashboard!C79)=0,Dashboard!C79,"")</f>
+        <v>employment_fraction_production</v>
       </c>
       <c r="C80" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E80)=0,Dashboard!E80,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E79)=0,Dashboard!E79,"")</f>
         <v/>
       </c>
       <c r="D80" s="35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E80" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13353,15 +13499,15 @@
     </row>
     <row r="81" spans="2:5">
       <c r="B81" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C81)=0,Dashboard!C81,"")</f>
-        <v>new_houses_insulation_employment_constant</v>
+        <f>IF(COUNTBLANK(Dashboard!C80)=0,Dashboard!C80,"")</f>
+        <v>employment_local_fraction</v>
       </c>
       <c r="C81" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E81)=0,Dashboard!E81,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E80)=0,Dashboard!E80,"")</f>
         <v/>
       </c>
       <c r="D81" s="35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E81" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13370,15 +13516,15 @@
     </row>
     <row r="82" spans="2:5">
       <c r="B82" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C82)=0,Dashboard!C82,"")</f>
-        <v>old_houses_insulation_employment_constant</v>
+        <f>IF(COUNTBLANK(Dashboard!C81)=0,Dashboard!C81,"")</f>
+        <v>man_hours_per_man_year</v>
       </c>
       <c r="C82" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E82)=0,Dashboard!E82,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E81)=0,Dashboard!E81,"")</f>
         <v/>
       </c>
       <c r="D82" s="35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E82" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13386,46 +13532,50 @@
       </c>
     </row>
     <row r="83" spans="2:5">
-      <c r="B83" s="102" t="str">
+      <c r="B83" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C82)=0,Dashboard!C82,"")</f>
+        <v>buildings_insulation_employment_constant</v>
+      </c>
+      <c r="C83" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E82)=0,Dashboard!E82,"")</f>
+        <v/>
+      </c>
+      <c r="D83" s="35">
+        <v>4</v>
+      </c>
+      <c r="E83" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5">
+      <c r="B84" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C83)=0,Dashboard!C83,"")</f>
-        <v/>
-      </c>
-      <c r="C83" s="90" t="str">
+        <v>new_houses_insulation_employment_constant</v>
+      </c>
+      <c r="C84" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E83)=0,Dashboard!E83,"")</f>
         <v/>
       </c>
-      <c r="D83" s="7"/>
-      <c r="E83" s="105" t="str">
+      <c r="D84" s="35">
+        <v>3</v>
+      </c>
+      <c r="E84" s="104" t="e">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="2:5">
-      <c r="B84" s="102" t="str">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5">
+      <c r="B85" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C84)=0,Dashboard!C84,"")</f>
-        <v/>
-      </c>
-      <c r="C84" s="90" t="str">
+        <v>old_houses_insulation_employment_constant</v>
+      </c>
+      <c r="C85" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E84)=0,Dashboard!E84,"")</f>
         <v/>
       </c>
-      <c r="D84" s="7"/>
-      <c r="E84" s="105" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="2:5">
-      <c r="B85" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C85)=0,Dashboard!C85,"")</f>
-        <v>annual_infrastructure_cost_electricity</v>
-      </c>
-      <c r="C85" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E85)=0,Dashboard!E85,"")</f>
-        <v/>
-      </c>
       <c r="D85" s="35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E85" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13433,46 +13583,42 @@
       </c>
     </row>
     <row r="86" spans="2:5">
-      <c r="B86" s="103" t="str">
+      <c r="B86" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C85)=0,Dashboard!C85,"")</f>
+        <v/>
+      </c>
+      <c r="C86" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E85)=0,Dashboard!E85,"")</f>
+        <v/>
+      </c>
+      <c r="D86" s="7"/>
+      <c r="E86" s="105" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="2:5">
+      <c r="B87" s="102" t="str">
         <f>IF(COUNTBLANK(Dashboard!C86)=0,Dashboard!C86,"")</f>
-        <v>annual_infrastructure_cost_gas</v>
-      </c>
-      <c r="C86" s="35" t="str">
+        <v/>
+      </c>
+      <c r="C87" s="90" t="str">
         <f>IF(COUNTBLANK(Dashboard!E86)=0,Dashboard!E86,"")</f>
         <v/>
       </c>
-      <c r="D86" s="35">
-        <v>1</v>
-      </c>
-      <c r="E86" s="104" t="e">
+      <c r="D87" s="7"/>
+      <c r="E87" s="105" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5">
-      <c r="B87" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C87)=0,Dashboard!C87,"")</f>
-        <v>capacity_buffer_decentral_in_mj_s</v>
-      </c>
-      <c r="C87" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E87)=0,Dashboard!E87,"")</f>
         <v/>
-      </c>
-      <c r="D87" s="35">
-        <v>1</v>
-      </c>
-      <c r="E87" s="104" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="88" spans="2:5">
       <c r="B88" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C88)=0,Dashboard!C88,"")</f>
-        <v>capacity_buffer_in_mj_s</v>
+        <f>IF(COUNTBLANK(Dashboard!C87)=0,Dashboard!C87,"")</f>
+        <v>annual_infrastructure_cost_electricity</v>
       </c>
       <c r="C88" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E88)=0,Dashboard!E88,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E87)=0,Dashboard!E87,"")</f>
         <v/>
       </c>
       <c r="D88" s="35">
@@ -13485,11 +13631,11 @@
     </row>
     <row r="89" spans="2:5">
       <c r="B89" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C89)=0,Dashboard!C89,"")</f>
-        <v>export_electricity_primary_demand_factor</v>
+        <f>IF(COUNTBLANK(Dashboard!C88)=0,Dashboard!C88,"")</f>
+        <v>annual_infrastructure_cost_gas</v>
       </c>
       <c r="C89" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E89)=0,Dashboard!E89,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E88)=0,Dashboard!E88,"")</f>
         <v/>
       </c>
       <c r="D89" s="35">
@@ -13502,15 +13648,15 @@
     </row>
     <row r="90" spans="2:5">
       <c r="B90" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C90)=0,Dashboard!C90,"")</f>
-        <v>import_electricity_primary_demand_factor</v>
+        <f>IF(COUNTBLANK(Dashboard!C89)=0,Dashboard!C89,"")</f>
+        <v>capacity_buffer_decentral_in_mj_s</v>
       </c>
       <c r="C90" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E90)=0,Dashboard!E90,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E89)=0,Dashboard!E89,"")</f>
         <v/>
       </c>
       <c r="D90" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E90" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13519,15 +13665,15 @@
     </row>
     <row r="91" spans="2:5">
       <c r="B91" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C91)=0,Dashboard!C91,"")</f>
-        <v>investment_hv_net_low</v>
+        <f>IF(COUNTBLANK(Dashboard!C90)=0,Dashboard!C90,"")</f>
+        <v>capacity_buffer_in_mj_s</v>
       </c>
       <c r="C91" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E91)=0,Dashboard!E91,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E90)=0,Dashboard!E90,"")</f>
         <v/>
       </c>
-      <c r="D91" s="41">
-        <v>2</v>
+      <c r="D91" s="35">
+        <v>1</v>
       </c>
       <c r="E91" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13536,15 +13682,15 @@
     </row>
     <row r="92" spans="2:5">
       <c r="B92" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C92)=0,Dashboard!C92,"")</f>
-        <v>investment_hv_net_high</v>
+        <f>IF(COUNTBLANK(Dashboard!C91)=0,Dashboard!C91,"")</f>
+        <v>export_electricity_primary_demand_factor</v>
       </c>
       <c r="C92" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E92)=0,Dashboard!E92,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E91)=0,Dashboard!E91,"")</f>
         <v/>
       </c>
-      <c r="D92" s="41">
-        <v>2</v>
+      <c r="D92" s="35">
+        <v>1</v>
       </c>
       <c r="E92" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13553,15 +13699,15 @@
     </row>
     <row r="93" spans="2:5">
       <c r="B93" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C93)=0,Dashboard!C93,"")</f>
-        <v>investment_hv_net_per_turbine</v>
+        <f>IF(COUNTBLANK(Dashboard!C92)=0,Dashboard!C92,"")</f>
+        <v>import_electricity_primary_demand_factor</v>
       </c>
       <c r="C93" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E93)=0,Dashboard!E93,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E92)=0,Dashboard!E92,"")</f>
         <v/>
       </c>
-      <c r="D93" s="41">
-        <v>1</v>
+      <c r="D93" s="35">
+        <v>2</v>
       </c>
       <c r="E93" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13569,42 +13715,46 @@
       </c>
     </row>
     <row r="94" spans="2:5">
-      <c r="B94" s="102" t="str">
+      <c r="B94" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C93)=0,Dashboard!C93,"")</f>
+        <v>investment_hv_net_low</v>
+      </c>
+      <c r="C94" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E93)=0,Dashboard!E93,"")</f>
+        <v/>
+      </c>
+      <c r="D94" s="41">
+        <v>2</v>
+      </c>
+      <c r="E94" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5">
+      <c r="B95" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C94)=0,Dashboard!C94,"")</f>
-        <v/>
-      </c>
-      <c r="C94" s="90" t="str">
+        <v>investment_hv_net_high</v>
+      </c>
+      <c r="C95" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E94)=0,Dashboard!E94,"")</f>
         <v/>
       </c>
-      <c r="D94" s="7"/>
-      <c r="E94" s="105" t="str">
-        <f t="shared" ref="E94:E95" si="4">IF(COUNTBLANK(B94)=0,"- "&amp;B94&amp;" = "&amp;FIXED(C94,D94,1),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="2:5">
-      <c r="B95" s="102" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C95)=0,Dashboard!C95,"")</f>
-        <v/>
-      </c>
-      <c r="C95" s="90" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E95)=0,Dashboard!E95,"")</f>
-        <v/>
-      </c>
-      <c r="D95" s="7"/>
-      <c r="E95" s="105" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+      <c r="D95" s="41">
+        <v>2</v>
+      </c>
+      <c r="E95" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C96)=0,Dashboard!C96,"")</f>
-        <v>number_of_cars</v>
+        <f>IF(COUNTBLANK(Dashboard!C95)=0,Dashboard!C95,"")</f>
+        <v>investment_hv_net_per_turbine</v>
       </c>
       <c r="C96" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E96)=0,Dashboard!E96,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E95)=0,Dashboard!E95,"")</f>
         <v/>
       </c>
       <c r="D96" s="41">
@@ -13615,23 +13765,58 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="97" spans="2:5" ht="16" thickBot="1">
-      <c r="B97" s="44"/>
-      <c r="C97" s="96"/>
-      <c r="D97" s="36"/>
-      <c r="E97" s="97"/>
+    <row r="97" spans="2:5">
+      <c r="B97" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C96)=0,Dashboard!C96,"")</f>
+        <v/>
+      </c>
+      <c r="C97" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E96)=0,Dashboard!E96,"")</f>
+        <v/>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="E97" s="105" t="str">
+        <f t="shared" ref="E97:E98" si="4">IF(COUNTBLANK(B97)=0,"- "&amp;B97&amp;" = "&amp;FIXED(C97,D97,1),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="98" spans="2:5">
-      <c r="B98" s="88"/>
-      <c r="E98" s="89"/>
+      <c r="B98" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C97)=0,Dashboard!C97,"")</f>
+        <v/>
+      </c>
+      <c r="C98" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E97)=0,Dashboard!E97,"")</f>
+        <v/>
+      </c>
+      <c r="D98" s="7"/>
+      <c r="E98" s="105" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
     <row r="99" spans="2:5">
-      <c r="B99" s="88"/>
-      <c r="E99" s="89"/>
-    </row>
-    <row r="100" spans="2:5">
-      <c r="B100" s="88"/>
-      <c r="E100" s="89"/>
+      <c r="B99" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C98)=0,Dashboard!C98,"")</f>
+        <v>number_of_cars</v>
+      </c>
+      <c r="C99" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E98)=0,Dashboard!E98,"")</f>
+        <v/>
+      </c>
+      <c r="D99" s="41">
+        <v>1</v>
+      </c>
+      <c r="E99" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" ht="16" thickBot="1">
+      <c r="B100" s="44"/>
+      <c r="C100" s="96"/>
+      <c r="D100" s="36"/>
+      <c r="E100" s="97"/>
     </row>
     <row r="101" spans="2:5">
       <c r="B101" s="88"/>
@@ -13712,6 +13897,18 @@
     <row r="120" spans="2:5">
       <c r="B120" s="88"/>
       <c r="E120" s="89"/>
+    </row>
+    <row r="121" spans="2:5">
+      <c r="B121" s="88"/>
+      <c r="E121" s="89"/>
+    </row>
+    <row r="122" spans="2:5">
+      <c r="B122" s="88"/>
+      <c r="E122" s="89"/>
+    </row>
+    <row r="123" spans="2:5">
+      <c r="B123" s="88"/>
+      <c r="E123" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13729,10 +13926,10 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:A73"/>
+  <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13891,182 +14088,182 @@
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="35" t="e">
-        <f>'compile results'!E85</f>
-        <v>#VALUE!</v>
+      <c r="A26" s="35" t="str">
+        <f>'compile results'!E37</f>
+        <v xml:space="preserve">- has_aggregated_chemical_industry = </v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="35" t="e">
-        <f>'compile results'!E86</f>
-        <v>#VALUE!</v>
+      <c r="A27" s="35" t="str">
+        <f>'compile results'!E38</f>
+        <v>- has_detailed_chemical_industry = error</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="35" t="e">
+      <c r="A28" s="35" t="str">
         <f>'compile results'!E39</f>
-        <v>#VALUE!</v>
+        <v xml:space="preserve">- has_aggregated_other_industry = </v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="35" t="e">
-        <f>'compile results'!E47</f>
-        <v>#VALUE!</v>
+      <c r="A29" s="35" t="str">
+        <f>'compile results'!E40</f>
+        <v>- has_detailed_other_industry = error</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="35" t="e">
-        <f>'compile results'!E48</f>
+        <f>'compile results'!E88</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="35" t="e">
-        <f>'compile results'!E49</f>
+        <f>'compile results'!E89</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="35" t="e">
+        <f>'compile results'!E42</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="35" t="e">
+        <f>'compile results'!E50</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="35" t="e">
+        <f>'compile results'!E51</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="35" t="e">
+        <f>'compile results'!E52</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="35" t="e">
+        <f>'compile results'!E83</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="35" t="e">
+        <f>'compile results'!E90</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="35" t="e">
+        <f>'compile results'!E91</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="35" t="e">
+        <f>'compile results'!E74</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="35" t="e">
+        <f>'compile results'!E75</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="35" t="e">
+        <f>'compile results'!E76</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="35" t="e">
+        <f>'compile results'!E43</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="35" t="e">
+        <f>'compile results'!E79</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="35" t="e">
         <f>'compile results'!E80</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="35" t="e">
-        <f>'compile results'!E87</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="35" t="e">
-        <f>'compile results'!E88</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="35" t="e">
-        <f>'compile results'!E71</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="35" t="e">
-        <f>'compile results'!E72</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="35" t="e">
-        <f>'compile results'!E73</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="35" t="e">
-        <f>'compile results'!E40</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="35" t="e">
-        <f>'compile results'!E76</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="35" t="e">
-        <f>'compile results'!E77</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="35" t="e">
-        <f>'compile results'!E78</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="35" t="e">
-        <f>'compile results'!E89</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="35" t="e">
-        <f>'compile results'!E90</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="35" t="e">
-        <f>'compile results'!E50</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
     <row r="45" spans="1:1">
       <c r="A45" s="35" t="e">
-        <f>'compile results'!E51</f>
+        <f>'compile results'!E81</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="35" t="e">
-        <f>'compile results'!E52</f>
+        <f>'compile results'!E92</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="35" t="str">
-        <f>'compile results'!E53</f>
-        <v>- insulation_level_new_houses_min = 0.0</v>
+      <c r="A47" s="35" t="e">
+        <f>'compile results'!E93</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="35" t="e">
+        <f>'compile results'!E53</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="35" t="e">
         <f>'compile results'!E54</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="35" t="str">
-        <f>'compile results'!E55</f>
-        <v>- insulation_level_old_houses_min = 0.0</v>
-      </c>
-    </row>
     <row r="50" spans="1:1">
       <c r="A50" s="35" t="e">
-        <f>'compile results'!E41</f>
+        <f>'compile results'!E55</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="35" t="e">
-        <f>'compile results'!E79</f>
-        <v>#VALUE!</v>
+      <c r="A51" s="35" t="str">
+        <f>'compile results'!E56</f>
+        <v>- insulation_level_new_houses_min = 0.0</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="35" t="e">
-        <f>'compile results'!E56</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="35" t="e">
         <f>'compile results'!E57</f>
         <v>#VALUE!</v>
       </c>
     </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="35" t="str">
+        <f>'compile results'!E58</f>
+        <v>- insulation_level_old_houses_min = 0.0</v>
+      </c>
+    </row>
     <row r="54" spans="1:1">
       <c r="A54" s="35" t="e">
-        <f>'compile results'!E58</f>
+        <f>'compile results'!E44</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="35" t="e">
-        <f>'compile results'!E81</f>
+        <f>'compile results'!E82</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -14084,97 +14281,121 @@
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="35" t="e">
-        <f>'compile results'!E42</f>
+        <f>'compile results'!E61</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="35" t="str">
-        <f>'compile results'!E61</f>
-        <v>- number_of_new_residences = 0.0</v>
+      <c r="A59" s="35" t="e">
+        <f>'compile results'!E84</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="35" t="str">
+      <c r="A60" s="35" t="e">
         <f>'compile results'!E62</f>
-        <v>- number_of_old_residences = 0.0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="35" t="e">
-        <f>'compile results'!E43</f>
+        <f>'compile results'!E63</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="35" t="e">
-        <f>'compile results'!E63</f>
+        <f>'compile results'!E45</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="35" t="e">
+      <c r="A63" s="35" t="str">
         <f>'compile results'!E64</f>
-        <v>#VALUE!</v>
+        <v>- number_of_new_residences = 0.0</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="35" t="e">
+      <c r="A64" s="35" t="str">
         <f>'compile results'!E65</f>
-        <v>#VALUE!</v>
+        <v>- number_of_old_residences = 0.0</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="35" t="e">
-        <f>'compile results'!E82</f>
+        <f>'compile results'!E46</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="35" t="e">
-        <f>'compile results'!E44</f>
+        <f>'compile results'!E66</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="35" t="e">
-        <f>'compile results'!E66</f>
+        <f>'compile results'!E67</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="35" t="e">
-        <f>'compile results'!E67</f>
+        <f>'compile results'!E68</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="35" t="e">
-        <f>'compile results'!E68</f>
+        <f>'compile results'!E85</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="35" t="e">
-        <f>'compile results'!E91</f>
+        <f>'compile results'!E47</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="35" t="e">
-        <f>'compile results'!E92</f>
+        <f>'compile results'!E69</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="35" t="e">
-        <f>'compile results'!E93</f>
+        <f>'compile results'!E70</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="35" t="e">
+        <f>'compile results'!E71</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="35" t="e">
+        <f>'compile results'!E94</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="35" t="e">
+        <f>'compile results'!E95</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="35" t="e">
         <f>'compile results'!E96</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="35" t="e">
+        <f>'compile results'!E99</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Published state of ETDataset on 16 September 2016
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16140" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="155">
   <si>
     <t>Unit</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>has_detailed_other_industry</t>
+  </si>
+  <si>
+    <t>interconnector_capacity</t>
   </si>
 </sst>
 </file>
@@ -988,7 +991,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="492">
+  <cellStyleXfs count="494">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1481,8 +1484,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1743,6 +1748,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1753,7 +1761,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="492">
+  <cellStyles count="494">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2013,6 +2021,7 @@
     <cellStyle name="Followed Hyperlink" xfId="487" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="489" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="491" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="493" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2245,9 +2254,21 @@
     <cellStyle name="Hyperlink" xfId="486" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="488" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="490" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="492" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FFCCFFCC"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFCCFFCC"/>
@@ -3689,10 +3710,10 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:P99"/>
+  <dimension ref="A2:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3741,16 +3762,16 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="57" customHeight="1">
-      <c r="B5" s="144" t="s">
+      <c r="B5" s="145" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="145"/>
-      <c r="D5" s="145"/>
-      <c r="E5" s="145"/>
-      <c r="F5" s="145"/>
-      <c r="G5" s="145"/>
-      <c r="H5" s="145"/>
-      <c r="I5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="147"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
@@ -5831,7 +5852,7 @@
         <v>0</v>
       </c>
       <c r="M87" s="35" t="str">
-        <f t="shared" ref="M87:M95" si="11">IF(L87=TRUE," ","Please set value")</f>
+        <f t="shared" ref="M87:M96" si="11">IF(L87=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N87" s="85"/>
@@ -5853,7 +5874,7 @@
       <c r="J88"/>
       <c r="K88"/>
       <c r="L88" s="40" t="b">
-        <f t="shared" ref="L88:L95" si="12">IF(COUNTBLANK(E88)=1,FALSE,TRUE)</f>
+        <f t="shared" ref="L88:L96" si="12">IF(COUNTBLANK(E88)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M88" s="35" t="str">
@@ -5972,10 +5993,10 @@
     <row r="93" spans="2:15" ht="16" thickBot="1">
       <c r="B93" s="31"/>
       <c r="C93" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="D93"/>
-      <c r="E93" s="138"/>
+      <c r="E93" s="144"/>
       <c r="F93"/>
       <c r="G93" s="58"/>
       <c r="H93"/>
@@ -5983,29 +6004,29 @@
       <c r="J93"/>
       <c r="K93"/>
       <c r="L93" s="40" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="L93" si="13">IF(COUNTBLANK(E93)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M93" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="M93" si="14">IF(L93=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N93" s="85"/>
-      <c r="O93" s="136" t="s">
-        <v>140</v>
+      <c r="O93" s="15" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="94" spans="2:15" ht="16" thickBot="1">
       <c r="B94" s="31"/>
       <c r="C94" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D94"/>
-      <c r="E94" s="66"/>
+      <c r="E94" s="138"/>
       <c r="F94"/>
       <c r="G94" s="58"/>
       <c r="H94"/>
-      <c r="I94" s="57"/>
+      <c r="I94" s="134"/>
       <c r="J94"/>
       <c r="K94"/>
       <c r="L94" s="40" t="b">
@@ -6017,21 +6038,21 @@
         <v>Please set value</v>
       </c>
       <c r="N94" s="85"/>
-      <c r="O94" s="132" t="s">
-        <v>139</v>
+      <c r="O94" s="136" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="95" spans="2:15" ht="16" thickBot="1">
       <c r="B95" s="31"/>
-      <c r="C95" s="129" t="s">
-        <v>141</v>
+      <c r="C95" t="s">
+        <v>139</v>
       </c>
       <c r="D95"/>
-      <c r="E95" s="133"/>
+      <c r="E95" s="66"/>
       <c r="F95"/>
       <c r="G95" s="58"/>
       <c r="H95"/>
-      <c r="I95" s="135"/>
+      <c r="I95" s="57"/>
       <c r="J95"/>
       <c r="K95"/>
       <c r="L95" s="40" t="b">
@@ -6043,116 +6064,147 @@
         <v>Please set value</v>
       </c>
       <c r="N95" s="85"/>
-      <c r="O95" s="137" t="s">
+      <c r="O95" s="132" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="96" spans="2:15" ht="16" thickBot="1">
+      <c r="B96" s="31"/>
+      <c r="C96" s="129" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="96" spans="2:15">
-      <c r="B96" s="31"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="54"/>
-      <c r="F96" s="7"/>
-      <c r="G96" s="7"/>
-      <c r="H96" s="7"/>
-      <c r="I96" s="7"/>
-      <c r="J96" s="7"/>
-      <c r="K96" s="7"/>
-      <c r="L96" s="7"/>
-      <c r="M96" s="7"/>
+      <c r="D96"/>
+      <c r="E96" s="133"/>
+      <c r="F96"/>
+      <c r="G96" s="58"/>
+      <c r="H96"/>
+      <c r="I96" s="135"/>
+      <c r="J96"/>
+      <c r="K96"/>
+      <c r="L96" s="40" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M96" s="35" t="str">
+        <f t="shared" si="11"/>
+        <v>Please set value</v>
+      </c>
       <c r="N96" s="85"/>
-      <c r="O96" s="15"/>
-    </row>
-    <row r="97" spans="2:15" ht="16" thickBot="1">
-      <c r="B97" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
-      <c r="E97" s="55"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
-      <c r="J97" s="4"/>
-      <c r="K97" s="4"/>
-      <c r="L97" s="4"/>
-      <c r="M97" s="4"/>
+      <c r="O96" s="137" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="97" spans="2:15">
+      <c r="B97" s="31"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="54"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="7"/>
       <c r="N97" s="85"/>
       <c r="O97" s="15"/>
     </row>
     <row r="98" spans="2:15" ht="16" thickBot="1">
-      <c r="B98" s="31"/>
-      <c r="C98" t="s">
+      <c r="B98" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="55"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="85"/>
+      <c r="O98" s="15"/>
+    </row>
+    <row r="99" spans="2:15" ht="16" thickBot="1">
+      <c r="B99" s="31"/>
+      <c r="C99" t="s">
         <v>145</v>
       </c>
-      <c r="D98"/>
-      <c r="E98" s="53"/>
-      <c r="F98"/>
-      <c r="G98" s="58"/>
-      <c r="H98"/>
-      <c r="I98" s="57"/>
-      <c r="J98"/>
-      <c r="K98"/>
-      <c r="L98" s="40" t="b">
-        <f>IF(COUNTBLANK(E98)=1,FALSE,TRUE)</f>
+      <c r="D99"/>
+      <c r="E99" s="53"/>
+      <c r="F99"/>
+      <c r="G99" s="58"/>
+      <c r="H99"/>
+      <c r="I99" s="57"/>
+      <c r="J99"/>
+      <c r="K99"/>
+      <c r="L99" s="40" t="b">
+        <f>IF(COUNTBLANK(E99)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="M98" s="35" t="str">
-        <f t="shared" ref="M98" si="13">IF(L98=TRUE," ","Please set value")</f>
+      <c r="M99" s="35" t="str">
+        <f t="shared" ref="M99" si="15">IF(L99=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
-      <c r="N98" s="85"/>
-      <c r="O98" s="15" t="s">
+      <c r="N99" s="85"/>
+      <c r="O99" s="15" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="2:15" ht="16" thickBot="1">
-      <c r="B99" s="44"/>
-      <c r="C99" s="36"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="52"/>
-      <c r="F99" s="36"/>
-      <c r="G99" s="36"/>
-      <c r="H99" s="36"/>
-      <c r="I99" s="36"/>
-      <c r="J99" s="36"/>
-      <c r="K99" s="36"/>
-      <c r="L99" s="36"/>
-      <c r="M99" s="36"/>
-      <c r="N99" s="31"/>
-      <c r="O99" s="7"/>
+    <row r="100" spans="2:15" ht="16" thickBot="1">
+      <c r="B100" s="44"/>
+      <c r="C100" s="36"/>
+      <c r="D100" s="36"/>
+      <c r="E100" s="52"/>
+      <c r="F100" s="36"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="36"/>
+      <c r="I100" s="36"/>
+      <c r="J100" s="36"/>
+      <c r="K100" s="36"/>
+      <c r="L100" s="36"/>
+      <c r="M100" s="36"/>
+      <c r="N100" s="31"/>
+      <c r="O100" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:I5"/>
   </mergeCells>
-  <conditionalFormatting sqref="L78:L84 L41:L46 L73:L75 L18:L36 L49:L54 L56 L58:L69 L91:L95">
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+  <conditionalFormatting sqref="L78:L84 L41:L46 L73:L75 L18:L36 L49:L54 L56 L58:L69 L91:L92 L94:L96">
+    <cfRule type="cellIs" dxfId="6" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L87:L90">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L70">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L99">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L98">
+  <conditionalFormatting sqref="L37">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L37">
+  <conditionalFormatting sqref="L38">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L38">
+  <conditionalFormatting sqref="L93">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -6162,7 +6214,7 @@
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E41:E45 E48:E60 D61:D64 E65:E67 E70:E99">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E41:E45 E48:E60 D61:D64 E65:E67 E70:E100">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6479,10 +6531,10 @@
     </row>
     <row r="5" spans="1:48">
       <c r="A5" s="114"/>
-      <c r="B5" s="144" t="s">
+      <c r="B5" s="145" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="146"/>
+      <c r="C5" s="147"/>
       <c r="D5" s="114"/>
       <c r="E5" s="112"/>
       <c r="F5" s="112"/>
@@ -12302,10 +12354,10 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:E123"/>
+  <dimension ref="B1:E124"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13395,7 +13447,7 @@
         <v>5</v>
       </c>
       <c r="E74" s="104" t="e">
-        <f t="shared" ref="E74:E99" si="3">IF(COUNTBLANK(B74)=0,"- "&amp;B74&amp;" = "&amp;FIXED(C74,D74,1),"")</f>
+        <f t="shared" ref="E74:E100" si="3">IF(COUNTBLANK(B74)=0,"- "&amp;B74&amp;" = "&amp;FIXED(C74,D74,1),"")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -13715,16 +13767,15 @@
       </c>
     </row>
     <row r="94" spans="2:5">
-      <c r="B94" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C93)=0,Dashboard!C93,"")</f>
-        <v>investment_hv_net_low</v>
+      <c r="B94" s="103" t="s">
+        <v>154</v>
       </c>
       <c r="C94" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E93)=0,Dashboard!E93,"")</f>
         <v/>
       </c>
       <c r="D94" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E94" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13734,7 +13785,7 @@
     <row r="95" spans="2:5">
       <c r="B95" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C94)=0,Dashboard!C94,"")</f>
-        <v>investment_hv_net_high</v>
+        <v>investment_hv_net_low</v>
       </c>
       <c r="C95" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E94)=0,Dashboard!E94,"")</f>
@@ -13751,14 +13802,14 @@
     <row r="96" spans="2:5">
       <c r="B96" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C95)=0,Dashboard!C95,"")</f>
-        <v>investment_hv_net_per_turbine</v>
+        <v>investment_hv_net_high</v>
       </c>
       <c r="C96" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E95)=0,Dashboard!E95,"")</f>
         <v/>
       </c>
       <c r="D96" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E96" s="104" t="e">
         <f t="shared" si="3"/>
@@ -13766,18 +13817,20 @@
       </c>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="102" t="str">
+      <c r="B97" s="103" t="str">
         <f>IF(COUNTBLANK(Dashboard!C96)=0,Dashboard!C96,"")</f>
-        <v/>
-      </c>
-      <c r="C97" s="90" t="str">
+        <v>investment_hv_net_per_turbine</v>
+      </c>
+      <c r="C97" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E96)=0,Dashboard!E96,"")</f>
         <v/>
       </c>
-      <c r="D97" s="7"/>
-      <c r="E97" s="105" t="str">
-        <f t="shared" ref="E97:E98" si="4">IF(COUNTBLANK(B97)=0,"- "&amp;B97&amp;" = "&amp;FIXED(C97,D97,1),"")</f>
-        <v/>
+      <c r="D97" s="41">
+        <v>1</v>
+      </c>
+      <c r="E97" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="98" spans="2:5">
@@ -13791,36 +13844,47 @@
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="105" t="str">
+        <f t="shared" ref="E98:E99" si="4">IF(COUNTBLANK(B98)=0,"- "&amp;B98&amp;" = "&amp;FIXED(C98,D98,1),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="2:5">
+      <c r="B99" s="102" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C98)=0,Dashboard!C98,"")</f>
+        <v/>
+      </c>
+      <c r="C99" s="90" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E98)=0,Dashboard!E98,"")</f>
+        <v/>
+      </c>
+      <c r="D99" s="7"/>
+      <c r="E99" s="105" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="99" spans="2:5">
-      <c r="B99" s="103" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C98)=0,Dashboard!C98,"")</f>
+    <row r="100" spans="2:5">
+      <c r="B100" s="103" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C99)=0,Dashboard!C99,"")</f>
         <v>number_of_cars</v>
       </c>
-      <c r="C99" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E98)=0,Dashboard!E98,"")</f>
+      <c r="C100" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E99)=0,Dashboard!E99,"")</f>
         <v/>
       </c>
-      <c r="D99" s="41">
+      <c r="D100" s="41">
         <v>1</v>
       </c>
-      <c r="E99" s="104" t="e">
+      <c r="E100" s="104" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="100" spans="2:5" ht="16" thickBot="1">
-      <c r="B100" s="44"/>
-      <c r="C100" s="96"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="97"/>
-    </row>
-    <row r="101" spans="2:5">
-      <c r="B101" s="88"/>
-      <c r="E101" s="89"/>
+    <row r="101" spans="2:5" ht="16" thickBot="1">
+      <c r="B101" s="44"/>
+      <c r="C101" s="96"/>
+      <c r="D101" s="36"/>
+      <c r="E101" s="97"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="88"/>
@@ -13909,6 +13973,10 @@
     <row r="123" spans="2:5">
       <c r="B123" s="88"/>
       <c r="E123" s="89"/>
+    </row>
+    <row r="124" spans="2:5">
+      <c r="B124" s="88"/>
+      <c r="E124" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13926,10 +13994,10 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:A77"/>
+  <dimension ref="A1:A78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14395,7 +14463,13 @@
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="35" t="e">
-        <f>'compile results'!E99</f>
+        <f>'compile results'!E97</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="35" t="e">
+        <f>'compile results'!E100</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Published state of ETDataset on 16 May 2017
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16140" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="159">
   <si>
     <t>Unit</t>
   </si>
@@ -505,6 +505,18 @@
   </si>
   <si>
     <t>interconnector_capacity</t>
+  </si>
+  <si>
+    <t>electric_vehicle_profile_1_share</t>
+  </si>
+  <si>
+    <t>electric_vehicle_profile_2_share</t>
+  </si>
+  <si>
+    <t>electric_vehicle_profile_3_share</t>
+  </si>
+  <si>
+    <t>Added electric vehicle profile shares</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1003,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="494">
+  <cellStyleXfs count="500">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1486,8 +1498,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1751,6 +1769,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1761,7 +1782,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="494">
+  <cellStyles count="500">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2022,6 +2043,9 @@
     <cellStyle name="Followed Hyperlink" xfId="489" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="491" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="493" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="495" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="497" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="499" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2255,6 +2279,9 @@
     <cellStyle name="Hyperlink" xfId="488" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="490" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="492" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="494" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="496" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="498" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -3273,22 +3300,22 @@
   </sheetPr>
   <dimension ref="B2:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.625" style="2"/>
     <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="51.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="34.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="51.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="2"/>
+    <col min="6" max="6" width="34.625" style="2" customWidth="1"/>
     <col min="7" max="7" width="4.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="20.875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="20">
+    <row r="2" spans="2:8" ht="21">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3362,14 +3389,14 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="2:8" ht="16" thickBot="1">
+    <row r="12" spans="2:8" ht="17" thickBot="1">
       <c r="B12" s="14"/>
       <c r="C12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="2:8" ht="16" thickBot="1">
+    <row r="13" spans="2:8" ht="17" thickBot="1">
       <c r="B13" s="14"/>
       <c r="C13" s="16" t="s">
         <v>14</v>
@@ -3525,21 +3552,21 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" style="2"/>
+    <col min="2" max="2" width="17.625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="16384" width="10.625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7"/>
     </row>
-    <row r="2" spans="1:4" ht="20">
+    <row r="2" spans="1:4" ht="21">
       <c r="B2" s="1" t="s">
         <v>118</v>
       </c>
@@ -3605,9 +3632,15 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10" s="75"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="74"/>
+      <c r="B10" s="75">
+        <v>42863</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="74">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="75"/>
@@ -3710,38 +3743,36 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:P100"/>
+  <dimension ref="A2:P103"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.625" style="2"/>
+    <col min="2" max="2" width="17.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.625" style="2" customWidth="1"/>
     <col min="5" max="5" width="18" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.83203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="65.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="3.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="65.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="3.875" style="2" customWidth="1"/>
     <col min="11" max="11" width="78" style="2" customWidth="1"/>
     <col min="12" max="12" width="40" style="2" customWidth="1"/>
-    <col min="13" max="13" width="34.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="3.83203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="46.33203125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="2"/>
+    <col min="13" max="13" width="34.375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="3.875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="46.375" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="10.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="20">
+    <row r="2" spans="2:16" ht="21">
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="20">
+    <row r="3" spans="2:16" ht="21">
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="2:16">
@@ -3762,16 +3793,16 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="57" customHeight="1">
-      <c r="B5" s="145" t="s">
+      <c r="B5" s="146" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="146"/>
-      <c r="D5" s="146"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="146"/>
-      <c r="H5" s="146"/>
-      <c r="I5" s="147"/>
+      <c r="C5" s="147"/>
+      <c r="D5" s="147"/>
+      <c r="E5" s="147"/>
+      <c r="F5" s="147"/>
+      <c r="G5" s="147"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="148"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
@@ -3779,7 +3810,7 @@
       <c r="N5" s="39"/>
       <c r="P5" s="28"/>
     </row>
-    <row r="6" spans="2:16" ht="16" thickBot="1"/>
+    <row r="6" spans="2:16" ht="17" thickBot="1"/>
     <row r="7" spans="2:16">
       <c r="B7" s="29" t="s">
         <v>31</v>
@@ -3850,7 +3881,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="16" thickBot="1">
+    <row r="10" spans="2:16" ht="17" thickBot="1">
       <c r="B10" s="37" t="s">
         <v>35</v>
       </c>
@@ -3868,7 +3899,7 @@
       <c r="N10" s="31"/>
       <c r="O10" s="7"/>
     </row>
-    <row r="11" spans="2:16" ht="16" thickBot="1">
+    <row r="11" spans="2:16" ht="17" thickBot="1">
       <c r="B11" s="34"/>
       <c r="C11" s="35" t="s">
         <v>44</v>
@@ -3892,7 +3923,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="16" thickBot="1">
+    <row r="12" spans="2:16" ht="17" thickBot="1">
       <c r="B12" s="34"/>
       <c r="C12" s="35" t="s">
         <v>45</v>
@@ -3916,7 +3947,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="16" thickBot="1">
+    <row r="13" spans="2:16" ht="17" thickBot="1">
       <c r="B13" s="34"/>
       <c r="C13" s="35" t="s">
         <v>46</v>
@@ -3940,7 +3971,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="16" thickBot="1">
+    <row r="14" spans="2:16" ht="17" thickBot="1">
       <c r="B14" s="34"/>
       <c r="C14" s="35" t="s">
         <v>60</v>
@@ -3964,7 +3995,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="16" thickBot="1">
+    <row r="15" spans="2:16" ht="17" thickBot="1">
       <c r="B15" s="34"/>
       <c r="C15" s="35" t="s">
         <v>47</v>
@@ -4004,7 +4035,7 @@
       <c r="N16" s="85"/>
       <c r="O16" s="15"/>
     </row>
-    <row r="17" spans="2:15" ht="16" thickBot="1">
+    <row r="17" spans="2:15" ht="17" thickBot="1">
       <c r="B17" s="34" t="s">
         <v>36</v>
       </c>
@@ -4022,7 +4053,7 @@
       <c r="N17" s="85"/>
       <c r="O17" s="15"/>
     </row>
-    <row r="18" spans="2:15" ht="16" thickBot="1">
+    <row r="18" spans="2:15" ht="17" thickBot="1">
       <c r="B18" s="34"/>
       <c r="C18" s="35" t="s">
         <v>48</v>
@@ -4052,7 +4083,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="16" thickBot="1">
+    <row r="19" spans="2:15" ht="17" thickBot="1">
       <c r="B19" s="34"/>
       <c r="C19" s="35" t="s">
         <v>61</v>
@@ -4082,7 +4113,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="16" thickBot="1">
+    <row r="20" spans="2:15" ht="17" thickBot="1">
       <c r="B20" s="34"/>
       <c r="C20" s="35" t="s">
         <v>54</v>
@@ -4112,7 +4143,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="16" thickBot="1">
+    <row r="21" spans="2:15" ht="17" thickBot="1">
       <c r="B21" s="34"/>
       <c r="C21" s="35" t="s">
         <v>62</v>
@@ -4142,7 +4173,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="16" thickBot="1">
+    <row r="22" spans="2:15" ht="17" thickBot="1">
       <c r="B22" s="34"/>
       <c r="C22" s="35" t="s">
         <v>63</v>
@@ -4172,7 +4203,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="16" thickBot="1">
+    <row r="23" spans="2:15" ht="17" thickBot="1">
       <c r="B23" s="34"/>
       <c r="C23" s="35" t="s">
         <v>49</v>
@@ -4202,7 +4233,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="2:15" ht="16" thickBot="1">
+    <row r="24" spans="2:15" ht="17" thickBot="1">
       <c r="B24" s="34"/>
       <c r="C24" s="35" t="s">
         <v>64</v>
@@ -4232,7 +4263,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="2:15" ht="16" thickBot="1">
+    <row r="25" spans="2:15" ht="17" thickBot="1">
       <c r="B25" s="34"/>
       <c r="C25" s="35" t="s">
         <v>50</v>
@@ -4262,7 +4293,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:15" ht="16" thickBot="1">
+    <row r="26" spans="2:15" ht="17" thickBot="1">
       <c r="B26" s="34"/>
       <c r="C26" s="35" t="s">
         <v>65</v>
@@ -4292,7 +4323,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="16" thickBot="1">
+    <row r="27" spans="2:15" ht="17" thickBot="1">
       <c r="B27" s="34"/>
       <c r="C27" s="35" t="s">
         <v>55</v>
@@ -4322,7 +4353,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="2:15" ht="16" thickBot="1">
+    <row r="28" spans="2:15" ht="17" thickBot="1">
       <c r="B28" s="34"/>
       <c r="C28" s="35" t="s">
         <v>66</v>
@@ -4352,7 +4383,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="2:15" ht="16" thickBot="1">
+    <row r="29" spans="2:15" ht="17" thickBot="1">
       <c r="B29" s="34"/>
       <c r="C29" s="35" t="s">
         <v>51</v>
@@ -4382,7 +4413,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="2:15" ht="16" thickBot="1">
+    <row r="30" spans="2:15" ht="17" thickBot="1">
       <c r="B30" s="34"/>
       <c r="C30" s="35" t="s">
         <v>56</v>
@@ -4412,7 +4443,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="2:15" ht="16" thickBot="1">
+    <row r="31" spans="2:15" ht="17" thickBot="1">
       <c r="B31" s="34"/>
       <c r="C31" s="35" t="s">
         <v>57</v>
@@ -4442,7 +4473,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="2:15" ht="16" thickBot="1">
+    <row r="32" spans="2:15" ht="17" thickBot="1">
       <c r="B32" s="34"/>
       <c r="C32" s="35" t="s">
         <v>52</v>
@@ -4472,7 +4503,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="16" thickBot="1">
+    <row r="33" spans="1:15" ht="17" thickBot="1">
       <c r="A33" s="32"/>
       <c r="B33" s="34"/>
       <c r="C33" s="35" t="s">
@@ -4503,7 +4534,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="16" thickBot="1">
+    <row r="34" spans="1:15" ht="17" thickBot="1">
       <c r="A34" s="7"/>
       <c r="B34" s="34"/>
       <c r="C34" s="35" t="s">
@@ -4534,7 +4565,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="16" thickBot="1">
+    <row r="35" spans="1:15" ht="17" thickBot="1">
       <c r="B35" s="34"/>
       <c r="C35" s="35" t="s">
         <v>117</v>
@@ -4564,7 +4595,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="16" thickBot="1">
+    <row r="36" spans="1:15" ht="17" thickBot="1">
       <c r="B36" s="34"/>
       <c r="C36" s="35" t="s">
         <v>53</v>
@@ -4594,7 +4625,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="16" thickBot="1">
+    <row r="37" spans="1:15" ht="17" thickBot="1">
       <c r="B37" s="34"/>
       <c r="C37" s="35" t="s">
         <v>150</v>
@@ -4624,7 +4655,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="16" thickBot="1">
+    <row r="38" spans="1:15" ht="17" thickBot="1">
       <c r="B38" s="34"/>
       <c r="C38" s="35" t="s">
         <v>147</v>
@@ -4670,7 +4701,7 @@
       <c r="N39" s="85"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:15" ht="16" thickBot="1">
+    <row r="40" spans="1:15" ht="17" thickBot="1">
       <c r="B40" s="34" t="s">
         <v>114</v>
       </c>
@@ -4688,7 +4719,7 @@
       <c r="N40" s="85"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15" ht="16" thickBot="1">
+    <row r="41" spans="1:15" ht="17" thickBot="1">
       <c r="B41" s="34"/>
       <c r="C41" s="35" t="s">
         <v>70</v>
@@ -4718,7 +4749,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="16" thickBot="1">
+    <row r="42" spans="1:15" ht="17" thickBot="1">
       <c r="B42" s="34"/>
       <c r="C42" s="35" t="s">
         <v>71</v>
@@ -4746,7 +4777,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="16" thickBot="1">
+    <row r="43" spans="1:15" ht="17" thickBot="1">
       <c r="B43" s="34"/>
       <c r="C43" s="35" t="s">
         <v>72</v>
@@ -4776,7 +4807,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="16" thickBot="1">
+    <row r="44" spans="1:15" ht="17" thickBot="1">
       <c r="B44" s="34"/>
       <c r="C44" s="35" t="s">
         <v>131</v>
@@ -4804,7 +4835,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="16" thickBot="1">
+    <row r="45" spans="1:15" ht="17" thickBot="1">
       <c r="B45" s="34"/>
       <c r="C45" s="35" t="s">
         <v>68</v>
@@ -4832,7 +4863,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="16" thickBot="1">
+    <row r="46" spans="1:15" ht="17" thickBot="1">
       <c r="B46" s="34"/>
       <c r="C46" s="35" t="s">
         <v>69</v>
@@ -4876,7 +4907,7 @@
       <c r="N47" s="85"/>
       <c r="O47" s="15"/>
     </row>
-    <row r="48" spans="1:15" ht="16" thickBot="1">
+    <row r="48" spans="1:15" ht="17" thickBot="1">
       <c r="B48" s="34" t="s">
         <v>113</v>
       </c>
@@ -4894,7 +4925,7 @@
       <c r="N48" s="85"/>
       <c r="O48" s="15"/>
     </row>
-    <row r="49" spans="2:15" ht="16" thickBot="1">
+    <row r="49" spans="2:15" ht="17" thickBot="1">
       <c r="B49" s="34"/>
       <c r="C49" s="35" t="s">
         <v>73</v>
@@ -4922,7 +4953,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="2:15" ht="16" thickBot="1">
+    <row r="50" spans="2:15" ht="17" thickBot="1">
       <c r="B50" s="34"/>
       <c r="C50" s="35" t="s">
         <v>74</v>
@@ -4950,7 +4981,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="2:15" ht="16" thickBot="1">
+    <row r="51" spans="2:15" ht="17" thickBot="1">
       <c r="B51" s="34"/>
       <c r="C51" s="35" t="s">
         <v>75</v>
@@ -4978,7 +5009,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="2:15" ht="16" thickBot="1">
+    <row r="52" spans="2:15" ht="17" thickBot="1">
       <c r="B52" s="34"/>
       <c r="C52" s="35" t="s">
         <v>77</v>
@@ -5004,7 +5035,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="2:15" ht="16" thickBot="1">
+    <row r="53" spans="2:15" ht="17" thickBot="1">
       <c r="B53" s="34"/>
       <c r="C53" s="35" t="s">
         <v>78</v>
@@ -5030,7 +5061,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="2:15" ht="16" thickBot="1">
+    <row r="54" spans="2:15" ht="17" thickBot="1">
       <c r="B54" s="34"/>
       <c r="C54" s="35" t="s">
         <v>79</v>
@@ -5056,7 +5087,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="2:15" ht="16" thickBot="1">
+    <row r="55" spans="2:15" ht="17" thickBot="1">
       <c r="B55" s="34"/>
       <c r="C55" s="35" t="s">
         <v>80</v>
@@ -5079,7 +5110,7 @@
       <c r="N55" s="85"/>
       <c r="O55" s="15"/>
     </row>
-    <row r="56" spans="2:15" ht="16" thickBot="1">
+    <row r="56" spans="2:15" ht="17" thickBot="1">
       <c r="B56" s="34"/>
       <c r="C56" s="35" t="s">
         <v>81</v>
@@ -5105,7 +5136,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="2:15" ht="16" thickBot="1">
+    <row r="57" spans="2:15" ht="17" thickBot="1">
       <c r="B57" s="34"/>
       <c r="C57" s="35" t="s">
         <v>82</v>
@@ -5128,7 +5159,7 @@
       <c r="N57" s="85"/>
       <c r="O57" s="15"/>
     </row>
-    <row r="58" spans="2:15" ht="16" thickBot="1">
+    <row r="58" spans="2:15" ht="17" thickBot="1">
       <c r="B58" s="34"/>
       <c r="C58" s="35" t="s">
         <v>83</v>
@@ -5156,7 +5187,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="2:15" ht="16" thickBot="1">
+    <row r="59" spans="2:15" ht="17" thickBot="1">
       <c r="B59" s="34"/>
       <c r="C59" s="35" t="s">
         <v>84</v>
@@ -5184,7 +5215,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="2:15" ht="16" thickBot="1">
+    <row r="60" spans="2:15" ht="17" thickBot="1">
       <c r="B60" s="34"/>
       <c r="C60" s="35" t="s">
         <v>85</v>
@@ -5210,7 +5241,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="2:15" ht="16" thickBot="1">
+    <row r="61" spans="2:15" ht="17" thickBot="1">
       <c r="B61" s="34"/>
       <c r="C61" s="35" t="s">
         <v>134</v>
@@ -5236,7 +5267,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="2:15" ht="16" thickBot="1">
+    <row r="62" spans="2:15" ht="17" thickBot="1">
       <c r="B62" s="34"/>
       <c r="C62" s="35" t="s">
         <v>130</v>
@@ -5285,7 +5316,7 @@
       <c r="N63" s="85"/>
       <c r="O63" s="15"/>
     </row>
-    <row r="64" spans="2:15" ht="16" thickBot="1">
+    <row r="64" spans="2:15" ht="17" thickBot="1">
       <c r="B64" s="34"/>
       <c r="C64" s="35" t="s">
         <v>88</v>
@@ -5308,7 +5339,7 @@
       <c r="N64" s="85"/>
       <c r="O64" s="15"/>
     </row>
-    <row r="65" spans="2:15" ht="16" thickBot="1">
+    <row r="65" spans="2:15" ht="17" thickBot="1">
       <c r="B65" s="34"/>
       <c r="C65" s="35" t="s">
         <v>89</v>
@@ -5336,7 +5367,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="2:15" ht="16" thickBot="1">
+    <row r="66" spans="2:15" ht="17" thickBot="1">
       <c r="B66" s="34"/>
       <c r="C66" s="35" t="s">
         <v>90</v>
@@ -5364,7 +5395,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="2:15" ht="16" thickBot="1">
+    <row r="67" spans="2:15" ht="17" thickBot="1">
       <c r="B67" s="34"/>
       <c r="C67" s="35" t="s">
         <v>91</v>
@@ -5392,7 +5423,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="2:15" ht="16" thickBot="1">
+    <row r="68" spans="2:15" ht="17" thickBot="1">
       <c r="B68" s="34"/>
       <c r="C68" s="35" t="s">
         <v>132</v>
@@ -5418,7 +5449,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="2:15" ht="16" thickBot="1">
+    <row r="69" spans="2:15" ht="17" thickBot="1">
       <c r="B69" s="31"/>
       <c r="C69" s="35" t="s">
         <v>133</v>
@@ -5444,7 +5475,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="2:15" ht="16" thickBot="1">
+    <row r="70" spans="2:15" ht="17" thickBot="1">
       <c r="B70" s="31"/>
       <c r="C70" t="s">
         <v>106</v>
@@ -5486,7 +5517,7 @@
       <c r="N71" s="85"/>
       <c r="O71" s="15"/>
     </row>
-    <row r="72" spans="2:15" ht="16" thickBot="1">
+    <row r="72" spans="2:15" ht="17" thickBot="1">
       <c r="B72" s="42" t="s">
         <v>29</v>
       </c>
@@ -5504,7 +5535,7 @@
       <c r="N72" s="85"/>
       <c r="O72" s="15"/>
     </row>
-    <row r="73" spans="2:15" ht="16" thickBot="1">
+    <row r="73" spans="2:15" ht="17" thickBot="1">
       <c r="B73" s="31"/>
       <c r="C73" s="35" t="s">
         <v>93</v>
@@ -5532,7 +5563,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="2:15" ht="16" thickBot="1">
+    <row r="74" spans="2:15" ht="17" thickBot="1">
       <c r="B74" s="31"/>
       <c r="C74" s="35" t="s">
         <v>94</v>
@@ -5558,7 +5589,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="75" spans="2:15" ht="16" thickBot="1">
+    <row r="75" spans="2:15" ht="17" thickBot="1">
       <c r="B75" s="31"/>
       <c r="C75" s="35" t="s">
         <v>95</v>
@@ -5600,7 +5631,7 @@
       <c r="N76" s="85"/>
       <c r="O76" s="15"/>
     </row>
-    <row r="77" spans="2:15" ht="16" thickBot="1">
+    <row r="77" spans="2:15" ht="17" thickBot="1">
       <c r="B77" s="31" t="s">
         <v>67</v>
       </c>
@@ -5618,7 +5649,7 @@
       <c r="N77" s="85"/>
       <c r="O77" s="15"/>
     </row>
-    <row r="78" spans="2:15" ht="16" thickBot="1">
+    <row r="78" spans="2:15" ht="17" thickBot="1">
       <c r="B78" s="31"/>
       <c r="C78" s="35" t="s">
         <v>96</v>
@@ -5644,7 +5675,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="2:15" ht="16" thickBot="1">
+    <row r="79" spans="2:15" ht="17" thickBot="1">
       <c r="B79" s="31"/>
       <c r="C79" s="35" t="s">
         <v>97</v>
@@ -5670,7 +5701,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="80" spans="2:15" ht="16" thickBot="1">
+    <row r="80" spans="2:15" ht="17" thickBot="1">
       <c r="B80" s="31"/>
       <c r="C80" s="35" t="s">
         <v>98</v>
@@ -5696,7 +5727,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="81" spans="2:15" ht="16" thickBot="1">
+    <row r="81" spans="2:15" ht="17" thickBot="1">
       <c r="B81" s="31"/>
       <c r="C81" s="35" t="s">
         <v>99</v>
@@ -5722,7 +5753,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="82" spans="2:15" ht="16" thickBot="1">
+    <row r="82" spans="2:15" ht="17" thickBot="1">
       <c r="B82" s="34"/>
       <c r="C82" s="35" t="s">
         <v>76</v>
@@ -5748,7 +5779,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="2:15" ht="16" thickBot="1">
+    <row r="83" spans="2:15" ht="17" thickBot="1">
       <c r="B83" s="34"/>
       <c r="C83" s="35" t="s">
         <v>86</v>
@@ -5774,7 +5805,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="2:15" ht="16" thickBot="1">
+    <row r="84" spans="2:15" ht="17" thickBot="1">
       <c r="B84" s="34"/>
       <c r="C84" s="35" t="s">
         <v>92</v>
@@ -5816,7 +5847,7 @@
       <c r="N85" s="85"/>
       <c r="O85" s="15"/>
     </row>
-    <row r="86" spans="2:15" ht="16" thickBot="1">
+    <row r="86" spans="2:15" ht="17" thickBot="1">
       <c r="B86" s="42" t="s">
         <v>116</v>
       </c>
@@ -5834,7 +5865,7 @@
       <c r="N86" s="85"/>
       <c r="O86" s="15"/>
     </row>
-    <row r="87" spans="2:15" ht="16" thickBot="1">
+    <row r="87" spans="2:15" ht="17" thickBot="1">
       <c r="B87" s="31"/>
       <c r="C87" t="s">
         <v>100</v>
@@ -5860,7 +5891,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="2:15" ht="16" thickBot="1">
+    <row r="88" spans="2:15" ht="17" thickBot="1">
       <c r="B88" s="31"/>
       <c r="C88" t="s">
         <v>101</v>
@@ -5886,7 +5917,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="89" spans="2:15" ht="16" thickBot="1">
+    <row r="89" spans="2:15" ht="17" thickBot="1">
       <c r="B89" s="31"/>
       <c r="C89" t="s">
         <v>102</v>
@@ -5912,7 +5943,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="2:15" ht="16" thickBot="1">
+    <row r="90" spans="2:15" ht="17" thickBot="1">
       <c r="B90" s="31"/>
       <c r="C90" t="s">
         <v>103</v>
@@ -5938,7 +5969,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="2:15" ht="16" thickBot="1">
+    <row r="91" spans="2:15" ht="17" thickBot="1">
       <c r="B91" s="31"/>
       <c r="C91" t="s">
         <v>104</v>
@@ -5964,7 +5995,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="2:15" ht="16" thickBot="1">
+    <row r="92" spans="2:15" ht="17" thickBot="1">
       <c r="B92" s="31"/>
       <c r="C92" t="s">
         <v>105</v>
@@ -5990,7 +6021,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="93" spans="2:15" ht="16" thickBot="1">
+    <row r="93" spans="2:15" ht="17" thickBot="1">
       <c r="B93" s="31"/>
       <c r="C93" t="s">
         <v>154</v>
@@ -6016,7 +6047,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="94" spans="2:15" ht="16" thickBot="1">
+    <row r="94" spans="2:15" ht="17" thickBot="1">
       <c r="B94" s="31"/>
       <c r="C94" t="s">
         <v>140</v>
@@ -6042,7 +6073,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="95" spans="2:15" ht="16" thickBot="1">
+    <row r="95" spans="2:15" ht="17" thickBot="1">
       <c r="B95" s="31"/>
       <c r="C95" t="s">
         <v>139</v>
@@ -6068,7 +6099,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="96" spans="2:15" ht="16" thickBot="1">
+    <row r="96" spans="2:15" ht="17" thickBot="1">
       <c r="B96" s="31"/>
       <c r="C96" s="129" t="s">
         <v>141</v>
@@ -6110,7 +6141,7 @@
       <c r="N97" s="85"/>
       <c r="O97" s="15"/>
     </row>
-    <row r="98" spans="2:15" ht="16" thickBot="1">
+    <row r="98" spans="2:15" ht="17" thickBot="1">
       <c r="B98" s="42" t="s">
         <v>146</v>
       </c>
@@ -6128,7 +6159,7 @@
       <c r="N98" s="85"/>
       <c r="O98" s="15"/>
     </row>
-    <row r="99" spans="2:15" ht="16" thickBot="1">
+    <row r="99" spans="2:15" ht="17" thickBot="1">
       <c r="B99" s="31"/>
       <c r="C99" t="s">
         <v>145</v>
@@ -6146,7 +6177,7 @@
         <v>0</v>
       </c>
       <c r="M99" s="35" t="str">
-        <f t="shared" ref="M99" si="15">IF(L99=TRUE," ","Please set value")</f>
+        <f t="shared" ref="M99:M102" si="15">IF(L99=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N99" s="85"/>
@@ -6154,21 +6185,99 @@
         <v>145</v>
       </c>
     </row>
-    <row r="100" spans="2:15" ht="16" thickBot="1">
-      <c r="B100" s="44"/>
-      <c r="C100" s="36"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="52"/>
-      <c r="F100" s="36"/>
-      <c r="G100" s="36"/>
-      <c r="H100" s="36"/>
-      <c r="I100" s="36"/>
-      <c r="J100" s="36"/>
-      <c r="K100" s="36"/>
-      <c r="L100" s="36"/>
-      <c r="M100" s="36"/>
-      <c r="N100" s="31"/>
-      <c r="O100" s="7"/>
+    <row r="100" spans="2:15" ht="17" thickBot="1">
+      <c r="B100" s="31"/>
+      <c r="C100" t="s">
+        <v>155</v>
+      </c>
+      <c r="D100"/>
+      <c r="E100" s="66"/>
+      <c r="F100"/>
+      <c r="G100" s="58"/>
+      <c r="H100"/>
+      <c r="I100" s="57"/>
+      <c r="J100"/>
+      <c r="K100"/>
+      <c r="L100" s="40" t="b">
+        <f t="shared" ref="L100:L102" si="16">IF(COUNTBLANK(E100)=1,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="M100" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N100" s="85"/>
+      <c r="O100" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="101" spans="2:15" ht="17" thickBot="1">
+      <c r="B101" s="31"/>
+      <c r="C101" t="s">
+        <v>156</v>
+      </c>
+      <c r="D101"/>
+      <c r="E101" s="145"/>
+      <c r="F101"/>
+      <c r="G101" s="58"/>
+      <c r="H101"/>
+      <c r="I101" s="135"/>
+      <c r="J101"/>
+      <c r="K101"/>
+      <c r="L101" s="40" t="b">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M101" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N101" s="85"/>
+      <c r="O101" s="15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" spans="2:15" ht="17" thickBot="1">
+      <c r="B102" s="31"/>
+      <c r="C102" t="s">
+        <v>157</v>
+      </c>
+      <c r="D102"/>
+      <c r="E102" s="145"/>
+      <c r="F102"/>
+      <c r="G102" s="58"/>
+      <c r="H102"/>
+      <c r="I102" s="135"/>
+      <c r="J102"/>
+      <c r="K102"/>
+      <c r="L102" s="40" t="b">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M102" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N102" s="85"/>
+      <c r="O102" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="103" spans="2:15" ht="17" thickBot="1">
+      <c r="B103" s="44"/>
+      <c r="C103" s="36"/>
+      <c r="D103" s="36"/>
+      <c r="E103" s="52"/>
+      <c r="F103" s="36"/>
+      <c r="G103" s="36"/>
+      <c r="H103" s="36"/>
+      <c r="I103" s="36"/>
+      <c r="J103" s="36"/>
+      <c r="K103" s="36"/>
+      <c r="L103" s="36"/>
+      <c r="M103" s="36"/>
+      <c r="N103" s="31"/>
+      <c r="O103" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6189,7 +6298,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L99">
+  <conditionalFormatting sqref="L99:L102">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -6214,7 +6323,7 @@
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E41:E45 E48:E60 D61:D64 E65:E67 E70:E100">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E41:E45 E48:E60 D61:D64 E65:E67 E70:E103">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6313,16 +6422,14 @@
   </sheetPr>
   <dimension ref="A1:AV120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="113" customWidth="1"/>
-    <col min="2" max="2" width="55.6640625" style="113" customWidth="1"/>
+    <col min="1" max="1" width="4.375" style="113" customWidth="1"/>
+    <col min="2" max="2" width="55.625" style="113" customWidth="1"/>
     <col min="3" max="3" width="30.5" style="113" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="113"/>
+    <col min="4" max="16384" width="10.625" style="113"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -6375,7 +6482,7 @@
       <c r="AU1" s="112"/>
       <c r="AV1" s="112"/>
     </row>
-    <row r="2" spans="1:48" ht="20">
+    <row r="2" spans="1:48" ht="21">
       <c r="A2" s="114"/>
       <c r="B2" s="111" t="s">
         <v>135</v>
@@ -6531,10 +6638,10 @@
     </row>
     <row r="5" spans="1:48">
       <c r="A5" s="114"/>
-      <c r="B5" s="145" t="s">
+      <c r="B5" s="146" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="147"/>
+      <c r="C5" s="148"/>
       <c r="D5" s="114"/>
       <c r="E5" s="112"/>
       <c r="F5" s="112"/>
@@ -6581,7 +6688,7 @@
       <c r="AU5" s="112"/>
       <c r="AV5" s="112"/>
     </row>
-    <row r="6" spans="1:48" ht="16" thickBot="1">
+    <row r="6" spans="1:48" ht="17" thickBot="1">
       <c r="A6" s="114"/>
       <c r="B6" s="114"/>
       <c r="C6" s="114"/>
@@ -6835,7 +6942,7 @@
       <c r="AU10" s="112"/>
       <c r="AV10" s="112"/>
     </row>
-    <row r="11" spans="1:48" ht="16" thickBot="1">
+    <row r="11" spans="1:48" ht="17" thickBot="1">
       <c r="A11" s="112"/>
       <c r="B11" s="123"/>
       <c r="C11" s="120"/>
@@ -12354,21 +12461,19 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:E124"/>
+  <dimension ref="B1:E127"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="39.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" style="2"/>
+    <col min="2" max="2" width="39.875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="88" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="88" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="32.625" style="88" customWidth="1"/>
+    <col min="5" max="5" width="47.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
@@ -12376,14 +12481,14 @@
       <c r="D1" s="2"/>
       <c r="E1" s="46"/>
     </row>
-    <row r="2" spans="2:5" ht="20">
+    <row r="2" spans="2:5" ht="21">
       <c r="B2" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="2:5" ht="20">
+    <row r="3" spans="2:5" ht="21">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -12402,7 +12507,7 @@
       <c r="D5" s="12"/>
       <c r="E5" s="109"/>
     </row>
-    <row r="6" spans="2:5" ht="16" thickBot="1"/>
+    <row r="6" spans="2:5" ht="17" thickBot="1"/>
     <row r="7" spans="2:5">
       <c r="B7" s="94" t="s">
         <v>33</v>
@@ -13447,7 +13552,7 @@
         <v>5</v>
       </c>
       <c r="E74" s="104" t="e">
-        <f t="shared" ref="E74:E100" si="3">IF(COUNTBLANK(B74)=0,"- "&amp;B74&amp;" = "&amp;FIXED(C74,D74,1),"")</f>
+        <f t="shared" ref="E74:E103" si="3">IF(COUNTBLANK(B74)=0,"- "&amp;B74&amp;" = "&amp;FIXED(C74,D74,1),"")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -13880,23 +13985,59 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="101" spans="2:5" ht="16" thickBot="1">
-      <c r="B101" s="44"/>
-      <c r="C101" s="96"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="97"/>
+    <row r="101" spans="2:5">
+      <c r="B101" s="103" t="s">
+        <v>155</v>
+      </c>
+      <c r="C101" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E100)=0,Dashboard!E100,"")</f>
+        <v/>
+      </c>
+      <c r="D101" s="41">
+        <v>2</v>
+      </c>
+      <c r="E101" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="102" spans="2:5">
-      <c r="B102" s="88"/>
-      <c r="E102" s="89"/>
+      <c r="B102" s="103" t="s">
+        <v>156</v>
+      </c>
+      <c r="C102" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E101)=0,Dashboard!E101,"")</f>
+        <v/>
+      </c>
+      <c r="D102" s="41">
+        <v>2</v>
+      </c>
+      <c r="E102" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="103" spans="2:5">
-      <c r="B103" s="88"/>
-      <c r="E103" s="89"/>
-    </row>
-    <row r="104" spans="2:5">
-      <c r="B104" s="88"/>
-      <c r="E104" s="89"/>
+      <c r="B103" s="103" t="s">
+        <v>157</v>
+      </c>
+      <c r="C103" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E102)=0,Dashboard!E102,"")</f>
+        <v/>
+      </c>
+      <c r="D103" s="41">
+        <v>2</v>
+      </c>
+      <c r="E103" s="104" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" ht="17" thickBot="1">
+      <c r="B104" s="44"/>
+      <c r="C104" s="96"/>
+      <c r="D104" s="36"/>
+      <c r="E104" s="97"/>
     </row>
     <row r="105" spans="2:5">
       <c r="B105" s="88"/>
@@ -13977,6 +14118,18 @@
     <row r="124" spans="2:5">
       <c r="B124" s="88"/>
       <c r="E124" s="89"/>
+    </row>
+    <row r="125" spans="2:5">
+      <c r="B125" s="88"/>
+      <c r="E125" s="89"/>
+    </row>
+    <row r="126" spans="2:5">
+      <c r="B126" s="88"/>
+      <c r="E126" s="89"/>
+    </row>
+    <row r="127" spans="2:5">
+      <c r="B127" s="88"/>
+      <c r="E127" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13994,15 +14147,15 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:A78"/>
+  <dimension ref="A1:A81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -14470,6 +14623,24 @@
     <row r="78" spans="1:1">
       <c r="A78" s="35" t="e">
         <f>'compile results'!E100</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="35" t="e">
+        <f>'compile results'!E101</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="35" t="e">
+        <f>'compile results'!E102</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="35" t="e">
+        <f>'compile results'!E103</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Published state of ETDataset on November 18 2019
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roosdekok/Projects/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907656D2-1AD6-7E4D-8947-2DD7005BAC7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A022EE-67FC-F343-B00C-900E3F459A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="25300" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="3" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="220">
   <si>
     <t>Unit</t>
   </si>
@@ -243,9 +243,6 @@
     <t>has_agriculture</t>
   </si>
   <si>
-    <t>has_climate</t>
-  </si>
-  <si>
     <t>has_coastline</t>
   </si>
   <si>
@@ -709,6 +706,15 @@
   </si>
   <si>
     <t>total_land_area</t>
+  </si>
+  <si>
+    <t>November 14, 2019</t>
+  </si>
+  <si>
+    <t>Replace has_climate by has_weather_curves attribute</t>
+  </si>
+  <si>
+    <t>has_weather_curves</t>
   </si>
 </sst>
 </file>
@@ -2606,7 +2612,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2675,7 +2681,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2744,7 +2750,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3744,7 +3750,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3760,7 +3766,7 @@
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3768,10 +3774,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="70" t="s">
         <v>90</v>
-      </c>
-      <c r="D4" s="70" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3781,10 +3787,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="73" t="s">
         <v>92</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>93</v>
       </c>
       <c r="D6" s="74">
         <v>0.01</v>
@@ -3792,10 +3798,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="73" t="s">
         <v>94</v>
-      </c>
-      <c r="C7" s="73" t="s">
-        <v>95</v>
       </c>
       <c r="D7" s="74">
         <v>0.02</v>
@@ -3803,10 +3809,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="58" t="s">
         <v>96</v>
-      </c>
-      <c r="C8" s="58" t="s">
-        <v>97</v>
       </c>
       <c r="D8" s="80">
         <v>0.03</v>
@@ -3817,7 +3823,7 @@
         <v>42580</v>
       </c>
       <c r="C9" s="73" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="74">
         <v>0.04</v>
@@ -3828,7 +3834,7 @@
         <v>42863</v>
       </c>
       <c r="C10" s="73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D10" s="74">
         <v>0.05</v>
@@ -3836,10 +3842,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="73" t="s">
         <v>158</v>
-      </c>
-      <c r="C11" s="73" t="s">
-        <v>159</v>
       </c>
       <c r="D11" s="74">
         <v>0.06</v>
@@ -3847,10 +3853,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="75" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="73" t="s">
         <v>162</v>
-      </c>
-      <c r="C12" s="73" t="s">
-        <v>163</v>
       </c>
       <c r="D12" s="74">
         <v>7.0000000000000007E-2</v>
@@ -3861,7 +3867,7 @@
         <v>43445</v>
       </c>
       <c r="C13" s="73" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D13" s="74">
         <v>0.08</v>
@@ -3872,16 +3878,22 @@
         <v>43565</v>
       </c>
       <c r="C14" s="73" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D14" s="74">
         <v>0.09</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="75"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="74"/>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B15" s="75" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" s="76" t="s">
+        <v>218</v>
+      </c>
+      <c r="D15" s="74">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="75"/>
@@ -3956,8 +3968,8 @@
   </sheetPr>
   <dimension ref="A2:P157"/>
   <sheetViews>
-    <sheetView topLeftCell="L34" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4007,7 +4019,7 @@
     </row>
     <row r="5" spans="2:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="133" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="134"/>
       <c r="D5" s="134"/>
@@ -4073,11 +4085,11 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6" t="s">
@@ -4121,7 +4133,7 @@
         <v>37</v>
       </c>
       <c r="E11" s="121" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
@@ -4129,7 +4141,7 @@
       <c r="I11" s="57"/>
       <c r="J11" s="35"/>
       <c r="K11" s="35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L11" s="35"/>
       <c r="M11" s="35"/>
@@ -4141,7 +4153,7 @@
     <row r="12" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="34"/>
       <c r="C12" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D12" s="35" t="s">
         <v>37</v>
@@ -4153,13 +4165,13 @@
       <c r="I12" s="57"/>
       <c r="J12" s="35"/>
       <c r="K12" s="35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L12" s="35"/>
       <c r="M12" s="35"/>
       <c r="N12" s="85"/>
       <c r="O12" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4177,7 +4189,7 @@
       <c r="I13" s="57"/>
       <c r="J13" s="35"/>
       <c r="K13" s="35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
@@ -4201,7 +4213,7 @@
       <c r="I14" s="57"/>
       <c r="J14" s="35"/>
       <c r="K14" s="35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
@@ -4225,7 +4237,7 @@
       <c r="I15" s="57"/>
       <c r="J15" s="35"/>
       <c r="K15" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L15" s="35"/>
       <c r="M15" s="35"/>
@@ -4249,7 +4261,7 @@
       <c r="I16" s="57"/>
       <c r="J16" s="35"/>
       <c r="K16" s="35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L16" s="35"/>
       <c r="M16" s="35"/>
@@ -4387,7 +4399,7 @@
     <row r="22" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="34"/>
       <c r="C22" s="35" t="s">
-        <v>62</v>
+        <v>219</v>
       </c>
       <c r="D22" s="35" t="s">
         <v>37</v>
@@ -4411,13 +4423,13 @@
       </c>
       <c r="N22" s="85"/>
       <c r="O22" s="86" t="s">
-        <v>62</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="34"/>
       <c r="C23" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" s="35" t="s">
         <v>37</v>
@@ -4441,7 +4453,7 @@
       </c>
       <c r="N23" s="85"/>
       <c r="O23" s="86" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4477,7 +4489,7 @@
     <row r="25" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="34"/>
       <c r="C25" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="35" t="s">
         <v>37</v>
@@ -4501,7 +4513,7 @@
       </c>
       <c r="N25" s="85"/>
       <c r="O25" s="86" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4537,7 +4549,7 @@
     <row r="27" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="34"/>
       <c r="C27" s="41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D27" s="35"/>
       <c r="E27" s="105"/>
@@ -4559,13 +4571,13 @@
       </c>
       <c r="N27" s="85"/>
       <c r="O27" s="41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="34"/>
       <c r="C28" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" s="35" t="s">
         <v>37</v>
@@ -4589,7 +4601,7 @@
       </c>
       <c r="N28" s="85"/>
       <c r="O28" s="86" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4625,7 +4637,7 @@
     <row r="30" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="34"/>
       <c r="C30" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D30" s="35" t="s">
         <v>37</v>
@@ -4649,7 +4661,7 @@
       </c>
       <c r="N30" s="85"/>
       <c r="O30" s="86" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4837,7 +4849,7 @@
     <row r="37" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="34"/>
       <c r="C37" s="35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D37" s="35" t="s">
         <v>37</v>
@@ -4861,7 +4873,7 @@
       </c>
       <c r="N37" s="85"/>
       <c r="O37" s="86" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4897,7 +4909,7 @@
     <row r="39" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="34"/>
       <c r="C39" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D39" s="41" t="s">
         <v>37</v>
@@ -4918,13 +4930,13 @@
       </c>
       <c r="N39" s="85"/>
       <c r="O39" s="86" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="34"/>
       <c r="C40" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D40" s="35" t="s">
         <v>37</v>
@@ -4936,7 +4948,7 @@
       <c r="I40" s="57"/>
       <c r="J40" s="35"/>
       <c r="K40" s="35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L40" s="40" t="b">
         <f t="shared" si="0"/>
@@ -4948,7 +4960,7 @@
       </c>
       <c r="N40" s="85"/>
       <c r="O40" s="86" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -4969,7 +4981,7 @@
     </row>
     <row r="42" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -4988,7 +5000,7 @@
     <row r="43" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="34"/>
       <c r="C43" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D43" s="35" t="s">
         <v>2</v>
@@ -5010,13 +5022,13 @@
       </c>
       <c r="N43" s="85"/>
       <c r="O43" s="86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="34"/>
       <c r="C44" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D44" s="35" t="s">
         <v>1</v>
@@ -5038,16 +5050,16 @@
       </c>
       <c r="N44" s="85"/>
       <c r="O44" s="86" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="34"/>
       <c r="C45" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" s="35" t="s">
         <v>124</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>125</v>
       </c>
       <c r="E45" s="64"/>
       <c r="F45"/>
@@ -5064,13 +5076,13 @@
       </c>
       <c r="N45" s="85"/>
       <c r="O45" s="86" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="34"/>
       <c r="C46" s="41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="35"/>
       <c r="E46" s="64"/>
@@ -5088,13 +5100,13 @@
       </c>
       <c r="N46" s="85"/>
       <c r="O46" s="127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="34"/>
       <c r="C47" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D47" s="41" t="s">
         <v>2</v>
@@ -5114,13 +5126,13 @@
       </c>
       <c r="N47" s="85"/>
       <c r="O47" s="127" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="34"/>
       <c r="C48" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D48" s="35" t="s">
         <v>37</v>
@@ -5142,13 +5154,13 @@
       </c>
       <c r="N48" s="85"/>
       <c r="O48" s="86" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="34"/>
       <c r="C49" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D49" s="35" t="s">
         <v>2</v>
@@ -5170,13 +5182,13 @@
       </c>
       <c r="N49" s="85"/>
       <c r="O49" s="86" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="34"/>
       <c r="C50" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D50" s="41" t="s">
         <v>3</v>
@@ -5198,13 +5210,13 @@
       </c>
       <c r="N50" s="85"/>
       <c r="O50" s="86" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="34"/>
       <c r="C51" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D51" s="35" t="s">
         <v>3</v>
@@ -5226,13 +5238,13 @@
       </c>
       <c r="N51" s="85"/>
       <c r="O51" s="86" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="34"/>
       <c r="C52" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D52" s="35" t="s">
         <v>3</v>
@@ -5254,13 +5266,13 @@
       </c>
       <c r="N52" s="85"/>
       <c r="O52" s="86" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="34"/>
       <c r="C53" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D53" s="35" t="s">
         <v>3</v>
@@ -5282,13 +5294,13 @@
       </c>
       <c r="N53" s="85"/>
       <c r="O53" s="86" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="34"/>
       <c r="C54" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D54" s="41" t="s">
         <v>37</v>
@@ -5310,13 +5322,13 @@
       </c>
       <c r="N54" s="85"/>
       <c r="O54" s="86" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="34"/>
       <c r="C55" s="35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D55" s="35" t="s">
         <v>37</v>
@@ -5338,13 +5350,13 @@
       </c>
       <c r="N55" s="85"/>
       <c r="O55" s="86" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B56" s="34"/>
       <c r="C56" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D56" s="35" t="s">
         <v>37</v>
@@ -5366,7 +5378,7 @@
       </c>
       <c r="N56" s="85"/>
       <c r="O56" s="86" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.2">
@@ -5387,7 +5399,7 @@
     </row>
     <row r="58" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -5406,7 +5418,7 @@
     <row r="59" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="34"/>
       <c r="C59" s="35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D59" s="62"/>
       <c r="E59" s="63"/>
@@ -5426,13 +5438,13 @@
       </c>
       <c r="N59" s="85"/>
       <c r="O59" s="86" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B60" s="34"/>
       <c r="C60" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D60" s="87"/>
       <c r="E60" s="63"/>
@@ -5452,13 +5464,13 @@
       </c>
       <c r="N60" s="85"/>
       <c r="O60" s="86" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B61" s="34"/>
       <c r="C61" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D61" s="87"/>
       <c r="E61" s="63">
@@ -5471,19 +5483,19 @@
       <c r="I61" s="57"/>
       <c r="J61" s="35"/>
       <c r="K61" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L61" s="118"/>
       <c r="M61" s="35"/>
       <c r="N61" s="85"/>
       <c r="O61" s="86" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B62" s="34"/>
       <c r="C62" s="41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D62" s="87"/>
       <c r="E62" s="63">
@@ -5500,13 +5512,13 @@
       <c r="M62" s="35"/>
       <c r="N62" s="85"/>
       <c r="O62" s="86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="34"/>
       <c r="C63" s="41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D63" s="87"/>
       <c r="E63" s="63">
@@ -5523,13 +5535,13 @@
       <c r="M63" s="35"/>
       <c r="N63" s="85"/>
       <c r="O63" s="86" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="34"/>
       <c r="C64" s="41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D64" s="87"/>
       <c r="E64" s="63">
@@ -5546,13 +5558,13 @@
       <c r="M64" s="35"/>
       <c r="N64" s="85"/>
       <c r="O64" s="86" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B65" s="34"/>
       <c r="C65" s="35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D65" s="87"/>
       <c r="E65" s="63">
@@ -5569,13 +5581,13 @@
       <c r="M65" s="35"/>
       <c r="N65" s="85"/>
       <c r="O65" s="86" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B66" s="34"/>
       <c r="C66" s="41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D66" s="87"/>
       <c r="E66" s="63"/>
@@ -5589,13 +5601,13 @@
       <c r="M66" s="35"/>
       <c r="N66" s="85"/>
       <c r="O66" s="86" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="34"/>
       <c r="C67" s="58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D67" s="87"/>
       <c r="E67" s="63"/>
@@ -5609,13 +5621,13 @@
       <c r="M67" s="35"/>
       <c r="N67" s="85"/>
       <c r="O67" s="86" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B68" s="34"/>
       <c r="C68" s="41" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D68" s="87"/>
       <c r="E68" s="63"/>
@@ -5629,13 +5641,13 @@
       <c r="M68" s="35"/>
       <c r="N68" s="85"/>
       <c r="O68" s="86" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B69" s="34"/>
       <c r="C69" s="41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D69" s="87"/>
       <c r="E69" s="63"/>
@@ -5649,13 +5661,13 @@
       <c r="M69" s="35"/>
       <c r="N69" s="85"/>
       <c r="O69" s="86" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B70" s="34"/>
       <c r="C70" s="41" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D70" s="87"/>
       <c r="E70" s="63"/>
@@ -5669,13 +5681,13 @@
       <c r="M70" s="35"/>
       <c r="N70" s="85"/>
       <c r="O70" s="86" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="34"/>
       <c r="C71" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D71" s="87"/>
       <c r="E71" s="63"/>
@@ -5689,13 +5701,13 @@
       <c r="M71" s="35"/>
       <c r="N71" s="85"/>
       <c r="O71" s="86" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="34"/>
       <c r="C72" s="58" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D72" s="87"/>
       <c r="E72" s="63"/>
@@ -5709,13 +5721,13 @@
       <c r="M72" s="35"/>
       <c r="N72" s="85"/>
       <c r="O72" s="86" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="73" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B73" s="34"/>
       <c r="C73" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D73" s="87"/>
       <c r="E73" s="63"/>
@@ -5729,13 +5741,13 @@
       <c r="M73" s="35"/>
       <c r="N73" s="85"/>
       <c r="O73" s="86" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B74" s="34"/>
       <c r="C74" s="41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D74" s="87"/>
       <c r="E74" s="63"/>
@@ -5749,13 +5761,13 @@
       <c r="M74" s="35"/>
       <c r="N74" s="85"/>
       <c r="O74" s="86" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B75" s="34"/>
       <c r="C75" s="41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D75" s="87"/>
       <c r="E75" s="63"/>
@@ -5769,13 +5781,13 @@
       <c r="M75" s="35"/>
       <c r="N75" s="85"/>
       <c r="O75" s="86" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="34"/>
       <c r="C76" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D76" s="87"/>
       <c r="E76" s="63"/>
@@ -5789,13 +5801,13 @@
       <c r="M76" s="35"/>
       <c r="N76" s="85"/>
       <c r="O76" s="86" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B77" s="34"/>
       <c r="C77" s="41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D77" s="87"/>
       <c r="E77" s="63"/>
@@ -5809,13 +5821,13 @@
       <c r="M77" s="35"/>
       <c r="N77" s="85"/>
       <c r="O77" s="86" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="78" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="34"/>
       <c r="C78" s="41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D78" s="87"/>
       <c r="E78" s="63"/>
@@ -5829,13 +5841,13 @@
       <c r="M78" s="35"/>
       <c r="N78" s="85"/>
       <c r="O78" s="86" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B79" s="34"/>
       <c r="C79" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D79" s="87"/>
       <c r="E79" s="63"/>
@@ -5849,13 +5861,13 @@
       <c r="M79" s="35"/>
       <c r="N79" s="85"/>
       <c r="O79" s="86" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B80" s="34"/>
       <c r="C80" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D80" s="87"/>
       <c r="E80" s="63"/>
@@ -5869,13 +5881,13 @@
       <c r="M80" s="35"/>
       <c r="N80" s="85"/>
       <c r="O80" s="86" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="81" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B81" s="34"/>
       <c r="C81" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D81" s="87"/>
       <c r="E81" s="63"/>
@@ -5889,13 +5901,13 @@
       <c r="M81" s="35"/>
       <c r="N81" s="85"/>
       <c r="O81" s="86" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="82" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B82" s="34"/>
       <c r="C82" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D82" s="87"/>
       <c r="E82" s="63"/>
@@ -5909,13 +5921,13 @@
       <c r="M82" s="35"/>
       <c r="N82" s="85"/>
       <c r="O82" s="86" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="83" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B83" s="34"/>
       <c r="C83" s="41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D83" s="87"/>
       <c r="E83" s="63"/>
@@ -5929,13 +5941,13 @@
       <c r="M83" s="35"/>
       <c r="N83" s="85"/>
       <c r="O83" s="86" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="84" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B84" s="34"/>
       <c r="C84" s="41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D84" s="87"/>
       <c r="E84" s="63"/>
@@ -5949,13 +5961,13 @@
       <c r="M84" s="35"/>
       <c r="N84" s="85"/>
       <c r="O84" s="86" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="85" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B85" s="34"/>
       <c r="C85" s="41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D85" s="87"/>
       <c r="E85" s="63"/>
@@ -5969,13 +5981,13 @@
       <c r="M85" s="35"/>
       <c r="N85" s="85"/>
       <c r="O85" s="86" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="86" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B86" s="34"/>
       <c r="C86" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D86" s="87"/>
       <c r="E86" s="63"/>
@@ -5989,13 +6001,13 @@
       <c r="M86" s="35"/>
       <c r="N86" s="85"/>
       <c r="O86" s="86" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B87" s="34"/>
       <c r="C87" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D87" s="87"/>
       <c r="E87" s="63"/>
@@ -6009,13 +6021,13 @@
       <c r="M87" s="35"/>
       <c r="N87" s="85"/>
       <c r="O87" s="86" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="88" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B88" s="34"/>
       <c r="C88" s="41" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D88" s="87"/>
       <c r="E88" s="63"/>
@@ -6029,13 +6041,13 @@
       <c r="M88" s="35"/>
       <c r="N88" s="85"/>
       <c r="O88" s="86" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="34"/>
       <c r="C89" s="41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D89" s="87"/>
       <c r="E89" s="63"/>
@@ -6049,13 +6061,13 @@
       <c r="M89" s="35"/>
       <c r="N89" s="85"/>
       <c r="O89" s="86" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B90" s="34"/>
       <c r="C90" s="41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D90" s="87"/>
       <c r="E90" s="63"/>
@@ -6069,13 +6081,13 @@
       <c r="M90" s="35"/>
       <c r="N90" s="85"/>
       <c r="O90" s="86" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B91" s="34"/>
       <c r="C91" s="41" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D91" s="87"/>
       <c r="E91" s="63" t="e">
@@ -6098,13 +6110,13 @@
       <c r="M91" s="35"/>
       <c r="N91" s="85"/>
       <c r="O91" s="86" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B92" s="34"/>
       <c r="C92" s="41" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D92" s="87"/>
       <c r="E92" s="63" t="e">
@@ -6124,13 +6136,13 @@
       <c r="M92" s="35"/>
       <c r="N92" s="85"/>
       <c r="O92" s="86" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="93" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B93" s="34"/>
       <c r="C93" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D93" s="87"/>
       <c r="E93" s="63">
@@ -6150,13 +6162,13 @@
       <c r="M93" s="35"/>
       <c r="N93" s="85"/>
       <c r="O93" s="86" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B94" s="34"/>
       <c r="C94" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D94" s="87"/>
       <c r="E94" s="63" t="e">
@@ -6179,13 +6191,13 @@
       <c r="M94" s="35"/>
       <c r="N94" s="85"/>
       <c r="O94" s="86" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B95" s="34"/>
       <c r="C95" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D95" s="87"/>
       <c r="E95" s="63" t="e">
@@ -6205,13 +6217,13 @@
       <c r="M95" s="35"/>
       <c r="N95" s="85"/>
       <c r="O95" s="86" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="96" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B96" s="34"/>
       <c r="C96" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D96" s="87"/>
       <c r="E96" s="63">
@@ -6231,13 +6243,13 @@
       <c r="M96" s="35"/>
       <c r="N96" s="85"/>
       <c r="O96" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="97" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B97" s="34"/>
       <c r="C97" s="41" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D97" s="87"/>
       <c r="E97" s="63" t="e">
@@ -6260,13 +6272,13 @@
       <c r="M97" s="35"/>
       <c r="N97" s="85"/>
       <c r="O97" s="86" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="98" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B98" s="34"/>
       <c r="C98" s="41" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D98" s="87"/>
       <c r="E98" s="63" t="e">
@@ -6286,13 +6298,13 @@
       <c r="M98" s="35"/>
       <c r="N98" s="85"/>
       <c r="O98" s="86" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B99" s="34"/>
       <c r="C99" s="41" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D99" s="87"/>
       <c r="E99" s="63">
@@ -6312,13 +6324,13 @@
       <c r="M99" s="35"/>
       <c r="N99" s="85"/>
       <c r="O99" s="86" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="100" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="34"/>
       <c r="C100" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D100" s="87"/>
       <c r="E100" s="63" t="e">
@@ -6341,13 +6353,13 @@
       <c r="M100" s="35"/>
       <c r="N100" s="85"/>
       <c r="O100" s="86" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="101" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B101" s="34"/>
       <c r="C101" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D101" s="87"/>
       <c r="E101" s="63" t="e">
@@ -6367,13 +6379,13 @@
       <c r="M101" s="35"/>
       <c r="N101" s="85"/>
       <c r="O101" s="86" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B102" s="34"/>
       <c r="C102" s="41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D102" s="87"/>
       <c r="E102" s="63">
@@ -6393,13 +6405,13 @@
       <c r="M102" s="35"/>
       <c r="N102" s="85"/>
       <c r="O102" s="86" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B103" s="34"/>
       <c r="C103" s="41" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D103" s="87"/>
       <c r="E103" s="63" t="e">
@@ -6422,13 +6434,13 @@
       <c r="M103" s="35"/>
       <c r="N103" s="85"/>
       <c r="O103" s="86" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="104" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B104" s="34"/>
       <c r="C104" s="41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D104" s="87"/>
       <c r="E104" s="63" t="e">
@@ -6448,13 +6460,13 @@
       <c r="M104" s="35"/>
       <c r="N104" s="85"/>
       <c r="O104" s="86" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B105" s="34"/>
       <c r="C105" s="41" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D105" s="87"/>
       <c r="E105" s="63">
@@ -6474,13 +6486,13 @@
       <c r="M105" s="35"/>
       <c r="N105" s="85"/>
       <c r="O105" s="86" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B106" s="34"/>
       <c r="C106" s="35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D106" s="35"/>
       <c r="E106" s="63"/>
@@ -6500,13 +6512,13 @@
       </c>
       <c r="N106" s="85"/>
       <c r="O106" s="86" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B107" s="31"/>
       <c r="C107" s="35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D107" s="35"/>
       <c r="E107" s="60"/>
@@ -6526,13 +6538,13 @@
       </c>
       <c r="N107" s="85"/>
       <c r="O107" s="86" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B108" s="31"/>
       <c r="C108" s="41" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D108" s="35"/>
       <c r="E108" s="60"/>
@@ -6552,13 +6564,13 @@
       </c>
       <c r="N108" s="85"/>
       <c r="O108" s="86" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="109" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B109" s="31"/>
       <c r="C109" s="41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D109" s="35"/>
       <c r="E109" s="60"/>
@@ -6578,7 +6590,7 @@
       </c>
       <c r="N109" s="85"/>
       <c r="O109" s="86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.2">
@@ -6618,7 +6630,7 @@
     <row r="112" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B112" s="31"/>
       <c r="C112" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D112" s="35" t="s">
         <v>3</v>
@@ -6640,13 +6652,13 @@
       </c>
       <c r="N112" s="85"/>
       <c r="O112" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="113" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B113" s="31"/>
       <c r="C113" s="41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D113" s="35" t="s">
         <v>3</v>
@@ -6668,13 +6680,13 @@
       </c>
       <c r="N113" s="85"/>
       <c r="O113" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="114" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B114" s="31"/>
       <c r="C114" s="41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D114" s="35" t="s">
         <v>3</v>
@@ -6696,13 +6708,13 @@
       </c>
       <c r="N114" s="85"/>
       <c r="O114" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B115" s="31"/>
       <c r="C115" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D115" s="35"/>
       <c r="E115" s="66"/>
@@ -6722,13 +6734,13 @@
       </c>
       <c r="N115" s="85"/>
       <c r="O115" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="116" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="31"/>
       <c r="C116" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D116" s="35"/>
       <c r="E116" s="61"/>
@@ -6748,7 +6760,7 @@
       </c>
       <c r="N116" s="85"/>
       <c r="O116" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="117" spans="2:15" x14ac:dyDescent="0.2">
@@ -6769,7 +6781,7 @@
     </row>
     <row r="118" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B118" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
@@ -6788,7 +6800,7 @@
     <row r="119" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B119" s="31"/>
       <c r="C119" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D119" s="35"/>
       <c r="E119" s="53"/>
@@ -6808,13 +6820,13 @@
       </c>
       <c r="N119" s="85"/>
       <c r="O119" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="120" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B120" s="31"/>
       <c r="C120" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D120" s="35"/>
       <c r="E120" s="53"/>
@@ -6834,13 +6846,13 @@
       </c>
       <c r="N120" s="85"/>
       <c r="O120" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="121" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B121" s="31"/>
       <c r="C121" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D121" s="35"/>
       <c r="E121" s="53"/>
@@ -6860,13 +6872,13 @@
       </c>
       <c r="N121" s="85"/>
       <c r="O121" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="122" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B122" s="31"/>
       <c r="C122" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D122" s="35"/>
       <c r="E122" s="53"/>
@@ -6886,13 +6898,13 @@
       </c>
       <c r="N122" s="85"/>
       <c r="O122" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="123" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B123" s="34"/>
       <c r="C123" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D123" s="35"/>
       <c r="E123" s="67"/>
@@ -6912,13 +6924,13 @@
       </c>
       <c r="N123" s="85"/>
       <c r="O123" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="124" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B124" s="34"/>
       <c r="C124" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D124" s="35"/>
       <c r="E124" s="67"/>
@@ -6938,7 +6950,7 @@
       </c>
       <c r="N124" s="85"/>
       <c r="O124" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="125" spans="2:15" x14ac:dyDescent="0.2">
@@ -6959,7 +6971,7 @@
     </row>
     <row r="126" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B126" s="42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
@@ -6978,10 +6990,10 @@
     <row r="127" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B127" s="31"/>
       <c r="C127" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D127" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E127" s="53"/>
       <c r="F127"/>
@@ -7000,16 +7012,16 @@
       </c>
       <c r="N127" s="85"/>
       <c r="O127" s="128" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="128" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B128" s="31"/>
       <c r="C128" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D128" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E128" s="53"/>
       <c r="F128"/>
@@ -7028,13 +7040,13 @@
       </c>
       <c r="N128" s="85"/>
       <c r="O128" s="128" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="129" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B129" s="31"/>
       <c r="C129" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D129" t="s">
         <v>37</v>
@@ -7056,16 +7068,16 @@
       </c>
       <c r="N129" s="85"/>
       <c r="O129" s="128" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="130" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B130" s="31"/>
       <c r="C130" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D130" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E130" s="53"/>
       <c r="F130"/>
@@ -7084,16 +7096,16 @@
       </c>
       <c r="N130" s="85"/>
       <c r="O130" s="128" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="131" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B131" s="31"/>
       <c r="C131" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D131" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E131" s="53"/>
       <c r="F131"/>
@@ -7112,16 +7124,16 @@
       </c>
       <c r="N131" s="85"/>
       <c r="O131" s="128" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="132" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B132" s="31"/>
       <c r="C132" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D132" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E132" s="53"/>
       <c r="F132"/>
@@ -7140,13 +7152,13 @@
       </c>
       <c r="N132" s="85"/>
       <c r="O132" s="128" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="133" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B133" s="31"/>
       <c r="C133" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D133" t="s">
         <v>37</v>
@@ -7168,16 +7180,16 @@
       </c>
       <c r="N133" s="85"/>
       <c r="O133" s="128" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="134" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B134" s="31"/>
       <c r="C134" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D134" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E134" s="125"/>
       <c r="F134"/>
@@ -7196,16 +7208,16 @@
       </c>
       <c r="N134" s="85"/>
       <c r="O134" s="128" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="135" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B135" s="31"/>
       <c r="C135" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D135" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E135" s="125"/>
       <c r="F135"/>
@@ -7224,16 +7236,16 @@
       </c>
       <c r="N135" s="85"/>
       <c r="O135" s="128" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="136" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B136" s="31"/>
       <c r="C136" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D136" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E136" s="125"/>
       <c r="F136"/>
@@ -7252,13 +7264,13 @@
       </c>
       <c r="N136" s="85"/>
       <c r="O136" s="128" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="137" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B137" s="31"/>
       <c r="C137" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D137" t="s">
         <v>37</v>
@@ -7280,16 +7292,16 @@
       </c>
       <c r="N137" s="85"/>
       <c r="O137" s="128" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="138" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B138" s="31"/>
       <c r="C138" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D138" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E138" s="125"/>
       <c r="F138"/>
@@ -7308,16 +7320,16 @@
       </c>
       <c r="N138" s="85"/>
       <c r="O138" s="128" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="139" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B139" s="31"/>
       <c r="C139" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D139" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E139" s="125"/>
       <c r="F139"/>
@@ -7336,16 +7348,16 @@
       </c>
       <c r="N139" s="85"/>
       <c r="O139" s="128" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="140" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B140" s="31"/>
       <c r="C140" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D140" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E140" s="125"/>
       <c r="F140"/>
@@ -7364,13 +7376,13 @@
       </c>
       <c r="N140" s="85"/>
       <c r="O140" s="128" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="141" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B141" s="31"/>
       <c r="C141" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D141" t="s">
         <v>37</v>
@@ -7392,16 +7404,16 @@
       </c>
       <c r="N141" s="85"/>
       <c r="O141" s="128" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="142" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B142" s="31"/>
       <c r="C142" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D142" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E142" s="125"/>
       <c r="F142"/>
@@ -7420,16 +7432,16 @@
       </c>
       <c r="N142" s="85"/>
       <c r="O142" s="128" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="143" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B143" s="31"/>
       <c r="C143" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D143" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E143" s="125"/>
       <c r="F143"/>
@@ -7448,16 +7460,16 @@
       </c>
       <c r="N143" s="85"/>
       <c r="O143" s="128" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="144" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B144" s="31"/>
       <c r="C144" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D144" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E144" s="125"/>
       <c r="F144"/>
@@ -7476,13 +7488,13 @@
       </c>
       <c r="N144" s="85"/>
       <c r="O144" s="128" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="145" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B145" s="31"/>
       <c r="C145" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D145" t="s">
         <v>37</v>
@@ -7504,16 +7516,16 @@
       </c>
       <c r="N145" s="85"/>
       <c r="O145" s="128" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="146" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B146" s="31"/>
       <c r="C146" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D146" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E146" s="125"/>
       <c r="F146"/>
@@ -7532,16 +7544,16 @@
       </c>
       <c r="N146" s="85"/>
       <c r="O146" s="128" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="147" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B147" s="31"/>
       <c r="C147" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D147" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E147" s="125"/>
       <c r="F147"/>
@@ -7560,16 +7572,16 @@
       </c>
       <c r="N147" s="85"/>
       <c r="O147" s="128" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="148" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B148" s="31"/>
       <c r="C148" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D148" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E148" s="125"/>
       <c r="F148"/>
@@ -7588,16 +7600,16 @@
       </c>
       <c r="N148" s="85"/>
       <c r="O148" s="128" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="149" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B149" s="31"/>
       <c r="C149" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D149" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E149" s="125"/>
       <c r="F149"/>
@@ -7616,16 +7628,16 @@
       </c>
       <c r="N149" s="85"/>
       <c r="O149" s="128" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="150" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B150" s="31"/>
       <c r="C150" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D150" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E150" s="57"/>
       <c r="F150"/>
@@ -7644,7 +7656,7 @@
       </c>
       <c r="N150" s="85"/>
       <c r="O150" s="128" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="151" spans="2:15" x14ac:dyDescent="0.2">
@@ -7665,7 +7677,7 @@
     </row>
     <row r="152" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B152" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
@@ -7684,7 +7696,7 @@
     <row r="153" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B153" s="31"/>
       <c r="C153" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D153"/>
       <c r="E153" s="53"/>
@@ -7704,13 +7716,13 @@
       </c>
       <c r="N153" s="85"/>
       <c r="O153" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="154" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B154" s="31"/>
       <c r="C154" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D154"/>
       <c r="E154" s="66"/>
@@ -7730,13 +7742,13 @@
       </c>
       <c r="N154" s="85"/>
       <c r="O154" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="155" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B155" s="31"/>
       <c r="C155" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D155"/>
       <c r="E155" s="126"/>
@@ -7756,13 +7768,13 @@
       </c>
       <c r="N155" s="85"/>
       <c r="O155" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="156" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B156" s="31"/>
       <c r="C156" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D156"/>
       <c r="E156" s="126"/>
@@ -7782,7 +7794,7 @@
       </c>
       <c r="N156" s="85"/>
       <c r="O156" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="157" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -7998,7 +8010,7 @@
     <row r="2" spans="1:48" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="109"/>
       <c r="B2" s="106" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="107"/>
       <c r="D2" s="109"/>
@@ -8152,7 +8164,7 @@
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="109"/>
       <c r="B5" s="133" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="135"/>
       <c r="D5" s="109"/>
@@ -13745,8 +13757,8 @@
   </sheetPr>
   <dimension ref="B1:E159"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B50" sqref="A50:XFD50"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13767,7 +13779,7 @@
     </row>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -13779,7 +13791,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="90" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -13800,10 +13812,10 @@
         <v>34</v>
       </c>
       <c r="D7" s="96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -13992,7 +14004,7 @@
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="99" t="str">
         <f>IF(COUNTBLANK(Dashboard!C22)=0,Dashboard!C22,"")</f>
-        <v>has_climate</v>
+        <v>has_weather_curves</v>
       </c>
       <c r="C23" s="35" t="str">
         <f>IF(COUNTBLANK(Dashboard!E22)=0,Dashboard!E22,"")</f>
@@ -14001,7 +14013,7 @@
       <c r="D23" s="35"/>
       <c r="E23" s="100" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">- has_climate = </v>
+        <v xml:space="preserve">- has_weather_curves = </v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
@@ -16261,8 +16273,8 @@
   </sheetPr>
   <dimension ref="A1:A146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="116" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16333,7 +16345,7 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="str">
         <f>'compile results'!E23</f>
-        <v xml:space="preserve">- has_climate = </v>
+        <v xml:space="preserve">- has_weather_curves = </v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Published state of ETDataset on March 03 2020
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roosdekok/Projects/etdataset/analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A022EE-67FC-F343-B00C-900E3F459A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA8348B-BFF7-CC40-AE98-72A2F2F5A924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="25300" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15020" yWindow="460" windowWidth="35020" windowHeight="28340" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="250">
   <si>
     <t>Unit</t>
   </si>
@@ -715,6 +717,96 @@
   </si>
   <si>
     <t>has_weather_curves</t>
+  </si>
+  <si>
+    <t>February 25, 2020</t>
+  </si>
+  <si>
+    <t>Add heat infrastructure attributes</t>
+  </si>
+  <si>
+    <t>heat_share_of_apartments_with_block_heating</t>
+  </si>
+  <si>
+    <t>heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket</t>
+  </si>
+  <si>
+    <t>heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket</t>
+  </si>
+  <si>
+    <t>heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket</t>
+  </si>
+  <si>
+    <t>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket</t>
+  </si>
+  <si>
+    <t>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket</t>
+  </si>
+  <si>
+    <t>heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket</t>
+  </si>
+  <si>
+    <t>heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket</t>
+  </si>
+  <si>
+    <t>heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket</t>
+  </si>
+  <si>
+    <t>heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket</t>
+  </si>
+  <si>
+    <t>heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket</t>
+  </si>
+  <si>
+    <t>heat_households_indoor_pipelines_investment_costs_with_block_heating_eur</t>
+  </si>
+  <si>
+    <t>heat_households_indoor_pipelines_investment_costs_without_block_heating_eur</t>
+  </si>
+  <si>
+    <t>heat_buildings_indoor_investment_costs_eur_per_kw</t>
+  </si>
+  <si>
+    <t>heat_buildings_heat_meter_investment_costs_eur_per_kw</t>
+  </si>
+  <si>
+    <t>heat_buildings_heat_meter_investment_costs_eur_per_connection</t>
+  </si>
+  <si>
+    <t>heat_exchanger_station_investment_costs_eur_per_kw</t>
+  </si>
+  <si>
+    <t>heat_sub_station_investment_costs_eur_per_kw</t>
+  </si>
+  <si>
+    <t>heat_distribution_pipelines_investment_costs_eur_per_meter</t>
+  </si>
+  <si>
+    <t>heat_primary_pipelines_investment_costs_per_kw</t>
+  </si>
+  <si>
+    <t>heat_yearly_indoor_infrastructure_maintenance_costs_factor</t>
+  </si>
+  <si>
+    <t>heat_yearly_outdoor_infrastructure_maintenance_costs_factor</t>
+  </si>
+  <si>
+    <t>share</t>
+  </si>
+  <si>
+    <t>meter/(house or building)</t>
+  </si>
+  <si>
+    <t>euro/kw</t>
+  </si>
+  <si>
+    <t>euro/building</t>
+  </si>
+  <si>
+    <t>euro/meter</t>
+  </si>
+  <si>
+    <t>factor</t>
   </si>
 </sst>
 </file>
@@ -3750,7 +3842,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3896,9 +3988,15 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="75"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="77"/>
+      <c r="B16" s="75" t="s">
+        <v>220</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="D16" s="77">
+        <v>0.12</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="75"/>
@@ -3966,10 +4064,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:P157"/>
+  <dimension ref="A2:P181"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView topLeftCell="A114" zoomScale="90" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M174" sqref="M174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7175,7 +7273,7 @@
         <v>0</v>
       </c>
       <c r="M133" s="35" t="str">
-        <f t="shared" ref="M133:M150" si="18">IF(L133=TRUE," ","Please set value")</f>
+        <f t="shared" ref="M133:M174" si="18">IF(L133=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N133" s="85"/>
@@ -7659,47 +7757,59 @@
         <v>78</v>
       </c>
     </row>
-    <row r="151" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B151" s="31"/>
-      <c r="C151" s="7"/>
-      <c r="D151" s="7"/>
-      <c r="E151" s="54"/>
-      <c r="F151" s="7"/>
-      <c r="G151" s="7"/>
-      <c r="H151" s="7"/>
-      <c r="I151" s="7"/>
-      <c r="J151" s="7"/>
-      <c r="K151" s="7"/>
-      <c r="L151" s="7"/>
-      <c r="M151" s="7"/>
+      <c r="C151"/>
+      <c r="D151"/>
+      <c r="E151" s="35"/>
+      <c r="F151"/>
+      <c r="G151" s="58"/>
+      <c r="H151"/>
+      <c r="I151" s="35"/>
+      <c r="J151"/>
+      <c r="K151"/>
+      <c r="L151" s="40"/>
+      <c r="M151" s="35"/>
       <c r="N151" s="85"/>
-      <c r="O151" s="15"/>
+      <c r="O151" s="128"/>
     </row>
     <row r="152" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="C152" s="4"/>
-      <c r="D152" s="4"/>
-      <c r="E152" s="55"/>
-      <c r="F152" s="4"/>
-      <c r="G152" s="4"/>
-      <c r="H152" s="4"/>
-      <c r="I152" s="4"/>
-      <c r="J152" s="4"/>
-      <c r="K152" s="4"/>
-      <c r="L152" s="4"/>
-      <c r="M152" s="4"/>
+      <c r="B152" s="31"/>
+      <c r="C152" t="s">
+        <v>222</v>
+      </c>
+      <c r="D152" t="s">
+        <v>244</v>
+      </c>
+      <c r="E152" s="57"/>
+      <c r="F152"/>
+      <c r="G152" s="58"/>
+      <c r="H152"/>
+      <c r="I152" s="57"/>
+      <c r="J152"/>
+      <c r="K152"/>
+      <c r="L152" s="40" t="b">
+        <f>IF(COUNTBLANK(E152)=1,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="M152" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
       <c r="N152" s="85"/>
-      <c r="O152" s="15"/>
+      <c r="O152" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="153" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B153" s="31"/>
       <c r="C153" t="s">
-        <v>110</v>
-      </c>
-      <c r="D153"/>
-      <c r="E153" s="53"/>
+        <v>223</v>
+      </c>
+      <c r="D153" t="s">
+        <v>245</v>
+      </c>
+      <c r="E153" s="57"/>
       <c r="F153"/>
       <c r="G153" s="58"/>
       <c r="H153"/>
@@ -7707,25 +7817,27 @@
       <c r="J153"/>
       <c r="K153"/>
       <c r="L153" s="40" t="b">
-        <f>IF(COUNTBLANK(E153)=1,FALSE,TRUE)</f>
+        <f t="shared" ref="L153:L173" si="19">IF(COUNTBLANK(E153)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M153" s="35" t="str">
-        <f t="shared" ref="M153:M156" si="19">IF(L153=TRUE," ","Please set value")</f>
+        <f t="shared" si="18"/>
         <v>Please set value</v>
       </c>
       <c r="N153" s="85"/>
-      <c r="O153" s="15" t="s">
-        <v>110</v>
+      <c r="O153" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="154" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B154" s="31"/>
       <c r="C154" t="s">
-        <v>117</v>
-      </c>
-      <c r="D154"/>
-      <c r="E154" s="66"/>
+        <v>224</v>
+      </c>
+      <c r="D154" t="s">
+        <v>245</v>
+      </c>
+      <c r="E154" s="57"/>
       <c r="F154"/>
       <c r="G154" s="58"/>
       <c r="H154"/>
@@ -7733,85 +7845,719 @@
       <c r="J154"/>
       <c r="K154"/>
       <c r="L154" s="40" t="b">
-        <f t="shared" ref="L154:L156" si="20">IF(COUNTBLANK(E154)=1,FALSE,TRUE)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M154" s="35" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>Please set value</v>
       </c>
       <c r="N154" s="85"/>
-      <c r="O154" s="15" t="s">
-        <v>117</v>
+      <c r="O154" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="155" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B155" s="31"/>
       <c r="C155" t="s">
-        <v>118</v>
-      </c>
-      <c r="D155"/>
-      <c r="E155" s="126"/>
+        <v>225</v>
+      </c>
+      <c r="D155" t="s">
+        <v>245</v>
+      </c>
+      <c r="E155" s="57"/>
       <c r="F155"/>
       <c r="G155" s="58"/>
       <c r="H155"/>
-      <c r="I155" s="120"/>
+      <c r="I155" s="57"/>
       <c r="J155"/>
       <c r="K155"/>
       <c r="L155" s="40" t="b">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M155" s="35" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>Please set value</v>
       </c>
       <c r="N155" s="85"/>
-      <c r="O155" s="15" t="s">
-        <v>118</v>
+      <c r="O155" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="156" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B156" s="31"/>
       <c r="C156" t="s">
-        <v>119</v>
-      </c>
-      <c r="D156"/>
-      <c r="E156" s="126"/>
+        <v>226</v>
+      </c>
+      <c r="D156" t="s">
+        <v>245</v>
+      </c>
+      <c r="E156" s="57"/>
       <c r="F156"/>
       <c r="G156" s="58"/>
       <c r="H156"/>
-      <c r="I156" s="120"/>
+      <c r="I156" s="57"/>
       <c r="J156"/>
       <c r="K156"/>
       <c r="L156" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M156" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N156" s="85"/>
+      <c r="O156" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="157" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="31"/>
+      <c r="C157" t="s">
+        <v>227</v>
+      </c>
+      <c r="D157" t="s">
+        <v>245</v>
+      </c>
+      <c r="E157" s="57"/>
+      <c r="F157"/>
+      <c r="G157" s="58"/>
+      <c r="H157"/>
+      <c r="I157" s="57"/>
+      <c r="J157"/>
+      <c r="K157"/>
+      <c r="L157" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M157" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N157" s="85"/>
+      <c r="O157" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="158" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="31"/>
+      <c r="C158" t="s">
+        <v>228</v>
+      </c>
+      <c r="D158" t="s">
+        <v>245</v>
+      </c>
+      <c r="E158" s="57"/>
+      <c r="F158"/>
+      <c r="G158" s="58"/>
+      <c r="H158"/>
+      <c r="I158" s="57"/>
+      <c r="J158"/>
+      <c r="K158"/>
+      <c r="L158" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M158" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N158" s="85"/>
+      <c r="O158" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="159" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="31"/>
+      <c r="C159" t="s">
+        <v>229</v>
+      </c>
+      <c r="D159" t="s">
+        <v>245</v>
+      </c>
+      <c r="E159" s="57"/>
+      <c r="F159"/>
+      <c r="G159" s="58"/>
+      <c r="H159"/>
+      <c r="I159" s="57"/>
+      <c r="J159"/>
+      <c r="K159"/>
+      <c r="L159" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M159" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N159" s="85"/>
+      <c r="O159" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="160" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="31"/>
+      <c r="C160" t="s">
+        <v>230</v>
+      </c>
+      <c r="D160" t="s">
+        <v>245</v>
+      </c>
+      <c r="E160" s="57"/>
+      <c r="F160"/>
+      <c r="G160" s="58"/>
+      <c r="H160"/>
+      <c r="I160" s="57"/>
+      <c r="J160"/>
+      <c r="K160"/>
+      <c r="L160" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M160" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N160" s="85"/>
+      <c r="O160" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="161" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="31"/>
+      <c r="C161" t="s">
+        <v>231</v>
+      </c>
+      <c r="D161" t="s">
+        <v>245</v>
+      </c>
+      <c r="E161" s="57"/>
+      <c r="F161"/>
+      <c r="G161" s="58"/>
+      <c r="H161"/>
+      <c r="I161" s="57"/>
+      <c r="J161"/>
+      <c r="K161"/>
+      <c r="L161" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M161" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N161" s="85"/>
+      <c r="O161" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="162" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="31"/>
+      <c r="C162" t="s">
+        <v>232</v>
+      </c>
+      <c r="D162" t="s">
+        <v>245</v>
+      </c>
+      <c r="E162" s="57"/>
+      <c r="F162"/>
+      <c r="G162" s="58"/>
+      <c r="H162"/>
+      <c r="I162" s="57"/>
+      <c r="J162"/>
+      <c r="K162"/>
+      <c r="L162" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M162" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N162" s="85"/>
+      <c r="O162" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="163" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="31"/>
+      <c r="C163" t="s">
+        <v>233</v>
+      </c>
+      <c r="D163" t="s">
+        <v>156</v>
+      </c>
+      <c r="E163" s="57"/>
+      <c r="F163"/>
+      <c r="G163" s="58"/>
+      <c r="H163"/>
+      <c r="I163" s="57"/>
+      <c r="J163"/>
+      <c r="K163"/>
+      <c r="L163" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M163" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N163" s="85"/>
+      <c r="O163" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="164" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="31"/>
+      <c r="C164" t="s">
+        <v>234</v>
+      </c>
+      <c r="D164" t="s">
+        <v>156</v>
+      </c>
+      <c r="E164" s="57"/>
+      <c r="F164"/>
+      <c r="G164" s="58"/>
+      <c r="H164"/>
+      <c r="I164" s="57"/>
+      <c r="J164"/>
+      <c r="K164"/>
+      <c r="L164" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M164" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N164" s="85"/>
+      <c r="O164" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="165" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="31"/>
+      <c r="C165" t="s">
+        <v>235</v>
+      </c>
+      <c r="D165" t="s">
+        <v>246</v>
+      </c>
+      <c r="E165" s="57"/>
+      <c r="F165"/>
+      <c r="G165" s="58"/>
+      <c r="H165"/>
+      <c r="I165" s="57"/>
+      <c r="J165"/>
+      <c r="K165"/>
+      <c r="L165" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M165" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N165" s="85"/>
+      <c r="O165" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="166" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="31"/>
+      <c r="C166" t="s">
+        <v>236</v>
+      </c>
+      <c r="D166" t="s">
+        <v>246</v>
+      </c>
+      <c r="E166" s="57"/>
+      <c r="F166"/>
+      <c r="G166" s="58"/>
+      <c r="H166"/>
+      <c r="I166" s="57"/>
+      <c r="J166"/>
+      <c r="K166"/>
+      <c r="L166" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M166" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N166" s="85"/>
+      <c r="O166" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="167" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="31"/>
+      <c r="C167" t="s">
+        <v>237</v>
+      </c>
+      <c r="D167" t="s">
+        <v>247</v>
+      </c>
+      <c r="E167" s="57"/>
+      <c r="F167"/>
+      <c r="G167" s="58"/>
+      <c r="H167"/>
+      <c r="I167" s="57"/>
+      <c r="J167"/>
+      <c r="K167"/>
+      <c r="L167" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M167" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N167" s="85"/>
+      <c r="O167" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="168" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="31"/>
+      <c r="C168" t="s">
+        <v>238</v>
+      </c>
+      <c r="D168" t="s">
+        <v>246</v>
+      </c>
+      <c r="E168" s="57"/>
+      <c r="F168"/>
+      <c r="G168" s="58"/>
+      <c r="H168"/>
+      <c r="I168" s="57"/>
+      <c r="J168"/>
+      <c r="K168"/>
+      <c r="L168" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M168" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N168" s="85"/>
+      <c r="O168" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="169" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B169" s="31"/>
+      <c r="C169" t="s">
+        <v>239</v>
+      </c>
+      <c r="D169" t="s">
+        <v>246</v>
+      </c>
+      <c r="E169" s="57"/>
+      <c r="F169"/>
+      <c r="G169" s="58"/>
+      <c r="H169"/>
+      <c r="I169" s="57"/>
+      <c r="J169"/>
+      <c r="K169"/>
+      <c r="L169" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M169" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N169" s="85"/>
+      <c r="O169" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="170" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B170" s="31"/>
+      <c r="C170" t="s">
+        <v>240</v>
+      </c>
+      <c r="D170" t="s">
+        <v>248</v>
+      </c>
+      <c r="E170" s="57"/>
+      <c r="F170"/>
+      <c r="G170" s="58"/>
+      <c r="H170"/>
+      <c r="I170" s="57"/>
+      <c r="J170"/>
+      <c r="K170"/>
+      <c r="L170" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M170" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N170" s="85"/>
+      <c r="O170" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="171" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B171" s="31"/>
+      <c r="C171" t="s">
+        <v>241</v>
+      </c>
+      <c r="D171" t="s">
+        <v>246</v>
+      </c>
+      <c r="E171" s="57"/>
+      <c r="F171"/>
+      <c r="G171" s="58"/>
+      <c r="H171"/>
+      <c r="I171" s="57"/>
+      <c r="J171"/>
+      <c r="K171"/>
+      <c r="L171" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M171" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N171" s="85"/>
+      <c r="O171" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="172" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B172" s="31"/>
+      <c r="C172" t="s">
+        <v>242</v>
+      </c>
+      <c r="D172" t="s">
+        <v>249</v>
+      </c>
+      <c r="E172" s="57"/>
+      <c r="F172"/>
+      <c r="G172" s="58"/>
+      <c r="H172"/>
+      <c r="I172" s="57"/>
+      <c r="J172"/>
+      <c r="K172"/>
+      <c r="L172" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M172" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N172" s="85"/>
+      <c r="O172" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="173" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B173" s="31"/>
+      <c r="C173" t="s">
+        <v>243</v>
+      </c>
+      <c r="D173" t="s">
+        <v>249</v>
+      </c>
+      <c r="E173" s="57"/>
+      <c r="F173"/>
+      <c r="G173" s="58"/>
+      <c r="H173"/>
+      <c r="I173" s="57"/>
+      <c r="J173"/>
+      <c r="K173"/>
+      <c r="L173" s="40" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M173" s="35" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N173" s="85"/>
+      <c r="O173" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="174" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B174" s="31"/>
+      <c r="C174"/>
+      <c r="D174"/>
+      <c r="E174" s="35"/>
+      <c r="F174"/>
+      <c r="G174" s="58"/>
+      <c r="H174"/>
+      <c r="I174" s="35"/>
+      <c r="J174"/>
+      <c r="K174"/>
+      <c r="L174" s="40"/>
+      <c r="M174" s="35"/>
+      <c r="N174" s="85"/>
+      <c r="O174" s="128"/>
+    </row>
+    <row r="175" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B175" s="31"/>
+      <c r="C175" s="7"/>
+      <c r="D175" s="7"/>
+      <c r="E175" s="54"/>
+      <c r="F175" s="7"/>
+      <c r="G175" s="7"/>
+      <c r="H175" s="7"/>
+      <c r="I175" s="7"/>
+      <c r="J175" s="7"/>
+      <c r="K175" s="7"/>
+      <c r="L175" s="7"/>
+      <c r="M175" s="7"/>
+      <c r="N175" s="85"/>
+      <c r="O175" s="15"/>
+    </row>
+    <row r="176" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B176" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C176" s="4"/>
+      <c r="D176" s="4"/>
+      <c r="E176" s="55"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="4"/>
+      <c r="H176" s="4"/>
+      <c r="I176" s="4"/>
+      <c r="J176" s="4"/>
+      <c r="K176" s="4"/>
+      <c r="L176" s="4"/>
+      <c r="M176" s="4"/>
+      <c r="N176" s="85"/>
+      <c r="O176" s="15"/>
+    </row>
+    <row r="177" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B177" s="31"/>
+      <c r="C177" t="s">
+        <v>110</v>
+      </c>
+      <c r="D177"/>
+      <c r="E177" s="53"/>
+      <c r="F177"/>
+      <c r="G177" s="58"/>
+      <c r="H177"/>
+      <c r="I177" s="57"/>
+      <c r="J177"/>
+      <c r="K177"/>
+      <c r="L177" s="40" t="b">
+        <f>IF(COUNTBLANK(E177)=1,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="M177" s="35" t="str">
+        <f t="shared" ref="M177:M180" si="20">IF(L177=TRUE," ","Please set value")</f>
+        <v>Please set value</v>
+      </c>
+      <c r="N177" s="85"/>
+      <c r="O177" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="178" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B178" s="31"/>
+      <c r="C178" t="s">
+        <v>117</v>
+      </c>
+      <c r="D178"/>
+      <c r="E178" s="66"/>
+      <c r="F178"/>
+      <c r="G178" s="58"/>
+      <c r="H178"/>
+      <c r="I178" s="57"/>
+      <c r="J178"/>
+      <c r="K178"/>
+      <c r="L178" s="40" t="b">
+        <f t="shared" ref="L178:L180" si="21">IF(COUNTBLANK(E178)=1,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="M178" s="35" t="str">
         <f t="shared" si="20"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N178" s="85"/>
+      <c r="O178" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="179" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="31"/>
+      <c r="C179" t="s">
+        <v>118</v>
+      </c>
+      <c r="D179"/>
+      <c r="E179" s="126"/>
+      <c r="F179"/>
+      <c r="G179" s="58"/>
+      <c r="H179"/>
+      <c r="I179" s="120"/>
+      <c r="J179"/>
+      <c r="K179"/>
+      <c r="L179" s="40" t="b">
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="M156" s="35" t="str">
-        <f t="shared" si="19"/>
+      <c r="M179" s="35" t="str">
+        <f t="shared" si="20"/>
         <v>Please set value</v>
       </c>
-      <c r="N156" s="85"/>
-      <c r="O156" s="15" t="s">
+      <c r="N179" s="85"/>
+      <c r="O179" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="180" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B180" s="31"/>
+      <c r="C180" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="157" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="44"/>
-      <c r="C157" s="36"/>
-      <c r="D157" s="36"/>
-      <c r="E157" s="52"/>
-      <c r="F157" s="36"/>
-      <c r="G157" s="36"/>
-      <c r="H157" s="36"/>
-      <c r="I157" s="36"/>
-      <c r="J157" s="36"/>
-      <c r="K157" s="36"/>
-      <c r="L157" s="36"/>
-      <c r="M157" s="36"/>
-      <c r="N157" s="31"/>
-      <c r="O157" s="7"/>
+      <c r="D180"/>
+      <c r="E180" s="126"/>
+      <c r="F180"/>
+      <c r="G180" s="58"/>
+      <c r="H180"/>
+      <c r="I180" s="120"/>
+      <c r="J180"/>
+      <c r="K180"/>
+      <c r="L180" s="40" t="b">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="M180" s="35" t="str">
+        <f t="shared" si="20"/>
+        <v>Please set value</v>
+      </c>
+      <c r="N180" s="85"/>
+      <c r="O180" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="181" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B181" s="44"/>
+      <c r="C181" s="36"/>
+      <c r="D181" s="36"/>
+      <c r="E181" s="52"/>
+      <c r="F181" s="36"/>
+      <c r="G181" s="36"/>
+      <c r="H181" s="36"/>
+      <c r="I181" s="36"/>
+      <c r="J181" s="36"/>
+      <c r="K181" s="36"/>
+      <c r="L181" s="36"/>
+      <c r="M181" s="36"/>
+      <c r="N181" s="31"/>
+      <c r="O181" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7827,12 +8573,12 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L153:L156">
+  <conditionalFormatting sqref="L177:L180">
     <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L133:L150">
+  <conditionalFormatting sqref="L133:L174">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -7850,12 +8596,12 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",K91)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E19" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E58 D59:D105 E43:E44 E110:E157 E48:E52" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E58 D59:D105 E43:E44 E110:E181 E48:E52" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -13755,10 +14501,10 @@
   <sheetPr codeName="Sheet4">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:E159"/>
+  <dimension ref="B1:E181"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A129" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E173" sqref="E173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15616,7 +16362,7 @@
         <v>64</v>
       </c>
       <c r="E121" s="100" t="str">
-        <f t="shared" ref="E121:E159" si="8">IF(COUNTBLANK(B121)=0,"- "&amp;B121&amp;" = "&amp;LOWER(C121),"")</f>
+        <f t="shared" ref="E121:E181" si="8">IF(COUNTBLANK(B121)=0,"- "&amp;B121&amp;" = "&amp;LOWER(C121),"")</f>
         <v xml:space="preserve">- man_hours_per_man_year = </v>
       </c>
     </row>
@@ -16021,6 +16767,7 @@
         <v/>
       </c>
       <c r="D145" s="35">
+        <f>D144+1</f>
         <v>88</v>
       </c>
       <c r="E145" s="100" t="str">
@@ -16038,6 +16785,7 @@
         <v/>
       </c>
       <c r="D146" s="35">
+        <f t="shared" ref="D146:D178" si="9">D145+1</f>
         <v>89</v>
       </c>
       <c r="E146" s="100" t="str">
@@ -16055,6 +16803,7 @@
         <v/>
       </c>
       <c r="D147" s="35">
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="E147" s="100" t="str">
@@ -16072,6 +16821,7 @@
         <v/>
       </c>
       <c r="D148" s="35">
+        <f t="shared" si="9"/>
         <v>91</v>
       </c>
       <c r="E148" s="100" t="str">
@@ -16089,6 +16839,7 @@
         <v/>
       </c>
       <c r="D149" s="35">
+        <f t="shared" si="9"/>
         <v>92</v>
       </c>
       <c r="E149" s="100" t="str">
@@ -16098,14 +16849,15 @@
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B150" s="99" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C151)=0,Dashboard!C151,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!C175)=0,Dashboard!C175,"")</f>
         <v/>
       </c>
       <c r="C150" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E151)=0,Dashboard!E151,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E175)=0,Dashboard!E175,"")</f>
         <v/>
       </c>
       <c r="D150" s="35">
+        <f t="shared" si="9"/>
         <v>93</v>
       </c>
       <c r="E150" s="100" t="str">
@@ -16116,146 +16868,482 @@
     <row r="151" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B151" s="99" t="str">
         <f>IF(COUNTBLANK(Dashboard!C152)=0,Dashboard!C152,"")</f>
-        <v/>
-      </c>
-      <c r="C151" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E152)=0,Dashboard!E152,"")</f>
-        <v/>
-      </c>
+        <v>heat_share_of_apartments_with_block_heating</v>
+      </c>
+      <c r="C151" s="35"/>
       <c r="D151" s="35">
+        <f t="shared" si="9"/>
         <v>94</v>
       </c>
       <c r="E151" s="100" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v xml:space="preserve">- heat_share_of_apartments_with_block_heating = </v>
       </c>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B152" s="99" t="str">
         <f>IF(COUNTBLANK(Dashboard!C153)=0,Dashboard!C153,"")</f>
-        <v>number_of_cars</v>
-      </c>
-      <c r="C152" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E153)=0,Dashboard!E153,"")</f>
-        <v/>
-      </c>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket</v>
+      </c>
+      <c r="C152" s="35"/>
       <c r="D152" s="35">
+        <f t="shared" si="9"/>
         <v>95</v>
       </c>
       <c r="E152" s="100" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">- number_of_cars = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket = </v>
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B153" s="99" t="str">
         <f>IF(COUNTBLANK(Dashboard!C154)=0,Dashboard!C154,"")</f>
-        <v>electric_vehicle_profile_1_share</v>
-      </c>
-      <c r="C153" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E154)=0,Dashboard!E154,"")</f>
-        <v/>
-      </c>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket</v>
+      </c>
+      <c r="C153" s="35"/>
       <c r="D153" s="35">
+        <f t="shared" si="9"/>
         <v>96</v>
       </c>
       <c r="E153" s="100" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket = </v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B154" s="99" t="str">
         <f>IF(COUNTBLANK(Dashboard!C155)=0,Dashboard!C155,"")</f>
-        <v>electric_vehicle_profile_2_share</v>
-      </c>
-      <c r="C154" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E155)=0,Dashboard!E155,"")</f>
-        <v/>
-      </c>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket</v>
+      </c>
+      <c r="C154" s="35"/>
       <c r="D154" s="35">
+        <f t="shared" si="9"/>
         <v>97</v>
       </c>
       <c r="E154" s="100" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket = </v>
       </c>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B155" s="99" t="str">
         <f>IF(COUNTBLANK(Dashboard!C156)=0,Dashboard!C156,"")</f>
-        <v>electric_vehicle_profile_3_share</v>
-      </c>
-      <c r="C155" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E156)=0,Dashboard!E156,"")</f>
-        <v/>
-      </c>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket</v>
+      </c>
+      <c r="C155" s="35"/>
       <c r="D155" s="35">
+        <f t="shared" si="9"/>
         <v>98</v>
       </c>
       <c r="E155" s="100" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket = </v>
       </c>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B156" s="99" t="str">
         <f>IF(COUNTBLANK(Dashboard!C157)=0,Dashboard!C157,"")</f>
-        <v/>
-      </c>
-      <c r="C156" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E157)=0,Dashboard!E157,"")</f>
-        <v/>
-      </c>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket</v>
+      </c>
+      <c r="C156" s="35"/>
       <c r="D156" s="35">
+        <f t="shared" si="9"/>
         <v>99</v>
       </c>
       <c r="E156" s="100" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket = </v>
       </c>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B157" s="99" t="str">
         <f>IF(COUNTBLANK(Dashboard!C158)=0,Dashboard!C158,"")</f>
-        <v/>
-      </c>
-      <c r="C157" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E158)=0,Dashboard!E158,"")</f>
-        <v/>
-      </c>
-      <c r="D157" s="35"/>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket</v>
+      </c>
+      <c r="C157" s="35"/>
+      <c r="D157" s="35">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
       <c r="E157" s="100" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket = </v>
       </c>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B158" s="99" t="str">
         <f>IF(COUNTBLANK(Dashboard!C159)=0,Dashboard!C159,"")</f>
-        <v/>
-      </c>
-      <c r="C158" s="35" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E159)=0,Dashboard!E159,"")</f>
-        <v/>
-      </c>
-      <c r="D158" s="35"/>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket</v>
+      </c>
+      <c r="C158" s="35"/>
+      <c r="D158" s="35">
+        <f t="shared" si="9"/>
+        <v>101</v>
+      </c>
       <c r="E158" s="100" t="str">
         <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket = </v>
+      </c>
+    </row>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B159" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C160)=0,Dashboard!C160,"")</f>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket</v>
+      </c>
+      <c r="C159" s="35"/>
+      <c r="D159" s="35">
+        <f t="shared" si="9"/>
+        <v>102</v>
+      </c>
+      <c r="E159" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket = </v>
+      </c>
+    </row>
+    <row r="160" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B160" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C161)=0,Dashboard!C161,"")</f>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket</v>
+      </c>
+      <c r="C160" s="35"/>
+      <c r="D160" s="35">
+        <f t="shared" si="9"/>
+        <v>103</v>
+      </c>
+      <c r="E160" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket = </v>
+      </c>
+    </row>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B161" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C162)=0,Dashboard!C162,"")</f>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket</v>
+      </c>
+      <c r="C161" s="35"/>
+      <c r="D161" s="35">
+        <f t="shared" si="9"/>
+        <v>104</v>
+      </c>
+      <c r="E161" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket = </v>
+      </c>
+    </row>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B162" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C163)=0,Dashboard!C163,"")</f>
+        <v>heat_households_indoor_pipelines_investment_costs_with_block_heating_eur</v>
+      </c>
+      <c r="C162" s="35"/>
+      <c r="D162" s="35">
+        <f t="shared" si="9"/>
+        <v>105</v>
+      </c>
+      <c r="E162" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_households_indoor_pipelines_investment_costs_with_block_heating_eur = </v>
+      </c>
+    </row>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B163" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C164)=0,Dashboard!C164,"")</f>
+        <v>heat_households_indoor_pipelines_investment_costs_without_block_heating_eur</v>
+      </c>
+      <c r="C163" s="35"/>
+      <c r="D163" s="35">
+        <f t="shared" si="9"/>
+        <v>106</v>
+      </c>
+      <c r="E163" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_households_indoor_pipelines_investment_costs_without_block_heating_eur = </v>
+      </c>
+    </row>
+    <row r="164" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B164" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C165)=0,Dashboard!C165,"")</f>
+        <v>heat_buildings_indoor_investment_costs_eur_per_kw</v>
+      </c>
+      <c r="C164" s="35"/>
+      <c r="D164" s="35">
+        <f t="shared" si="9"/>
+        <v>107</v>
+      </c>
+      <c r="E164" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_kw = </v>
+      </c>
+    </row>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B165" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C166)=0,Dashboard!C166,"")</f>
+        <v>heat_buildings_heat_meter_investment_costs_eur_per_kw</v>
+      </c>
+      <c r="C165" s="35"/>
+      <c r="D165" s="35">
+        <f t="shared" si="9"/>
+        <v>108</v>
+      </c>
+      <c r="E165" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_buildings_heat_meter_investment_costs_eur_per_kw = </v>
+      </c>
+    </row>
+    <row r="166" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B166" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C167)=0,Dashboard!C167,"")</f>
+        <v>heat_buildings_heat_meter_investment_costs_eur_per_connection</v>
+      </c>
+      <c r="C166" s="35"/>
+      <c r="D166" s="35">
+        <f t="shared" si="9"/>
+        <v>109</v>
+      </c>
+      <c r="E166" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_buildings_heat_meter_investment_costs_eur_per_connection = </v>
+      </c>
+    </row>
+    <row r="167" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B167" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C168)=0,Dashboard!C168,"")</f>
+        <v>heat_exchanger_station_investment_costs_eur_per_kw</v>
+      </c>
+      <c r="C167" s="35"/>
+      <c r="D167" s="35">
+        <f t="shared" si="9"/>
+        <v>110</v>
+      </c>
+      <c r="E167" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_exchanger_station_investment_costs_eur_per_kw = </v>
+      </c>
+    </row>
+    <row r="168" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B168" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C169)=0,Dashboard!C169,"")</f>
+        <v>heat_sub_station_investment_costs_eur_per_kw</v>
+      </c>
+      <c r="C168" s="35"/>
+      <c r="D168" s="35">
+        <f t="shared" si="9"/>
+        <v>111</v>
+      </c>
+      <c r="E168" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_sub_station_investment_costs_eur_per_kw = </v>
+      </c>
+    </row>
+    <row r="169" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B169" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C170)=0,Dashboard!C170,"")</f>
+        <v>heat_distribution_pipelines_investment_costs_eur_per_meter</v>
+      </c>
+      <c r="C169" s="35"/>
+      <c r="D169" s="35">
+        <f t="shared" si="9"/>
+        <v>112</v>
+      </c>
+      <c r="E169" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_distribution_pipelines_investment_costs_eur_per_meter = </v>
+      </c>
+    </row>
+    <row r="170" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B170" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C171)=0,Dashboard!C171,"")</f>
+        <v>heat_primary_pipelines_investment_costs_per_kw</v>
+      </c>
+      <c r="C170" s="35"/>
+      <c r="D170" s="35">
+        <f t="shared" si="9"/>
+        <v>113</v>
+      </c>
+      <c r="E170" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_primary_pipelines_investment_costs_per_kw = </v>
+      </c>
+    </row>
+    <row r="171" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B171" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C172)=0,Dashboard!C172,"")</f>
+        <v>heat_yearly_indoor_infrastructure_maintenance_costs_factor</v>
+      </c>
+      <c r="C171" s="35"/>
+      <c r="D171" s="35">
+        <f t="shared" si="9"/>
+        <v>114</v>
+      </c>
+      <c r="E171" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_yearly_indoor_infrastructure_maintenance_costs_factor = </v>
+      </c>
+    </row>
+    <row r="172" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B172" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C173)=0,Dashboard!C173,"")</f>
+        <v>heat_yearly_outdoor_infrastructure_maintenance_costs_factor</v>
+      </c>
+      <c r="C172" s="35"/>
+      <c r="D172" s="35">
+        <f t="shared" si="9"/>
+        <v>115</v>
+      </c>
+      <c r="E172" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- heat_yearly_outdoor_infrastructure_maintenance_costs_factor = </v>
+      </c>
+    </row>
+    <row r="173" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B173" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C176)=0,Dashboard!C176,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="159" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="130" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C160)=0,Dashboard!C160,"")</f>
+      <c r="C173" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E176)=0,Dashboard!E176,"")</f>
         <v/>
       </c>
-      <c r="C159" s="131" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E160)=0,Dashboard!E160,"")</f>
+      <c r="D173" s="35">
+        <f t="shared" si="9"/>
+        <v>116</v>
+      </c>
+      <c r="E173" s="100" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="D159" s="131"/>
-      <c r="E159" s="132" t="str">
+    </row>
+    <row r="174" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B174" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C177)=0,Dashboard!C177,"")</f>
+        <v>number_of_cars</v>
+      </c>
+      <c r="C174" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E177)=0,Dashboard!E177,"")</f>
+        <v/>
+      </c>
+      <c r="D174" s="35">
+        <f t="shared" si="9"/>
+        <v>117</v>
+      </c>
+      <c r="E174" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- number_of_cars = </v>
+      </c>
+    </row>
+    <row r="175" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B175" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C178)=0,Dashboard!C178,"")</f>
+        <v>electric_vehicle_profile_1_share</v>
+      </c>
+      <c r="C175" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E178)=0,Dashboard!E178,"")</f>
+        <v/>
+      </c>
+      <c r="D175" s="35">
+        <f t="shared" si="9"/>
+        <v>118</v>
+      </c>
+      <c r="E175" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
+      </c>
+    </row>
+    <row r="176" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B176" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C179)=0,Dashboard!C179,"")</f>
+        <v>electric_vehicle_profile_2_share</v>
+      </c>
+      <c r="C176" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E179)=0,Dashboard!E179,"")</f>
+        <v/>
+      </c>
+      <c r="D176" s="35">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+      <c r="E176" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
+      </c>
+    </row>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B177" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C180)=0,Dashboard!C180,"")</f>
+        <v>electric_vehicle_profile_3_share</v>
+      </c>
+      <c r="C177" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E180)=0,Dashboard!E180,"")</f>
+        <v/>
+      </c>
+      <c r="D177" s="35">
+        <f t="shared" si="9"/>
+        <v>120</v>
+      </c>
+      <c r="E177" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
+      </c>
+    </row>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B178" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C181)=0,Dashboard!C181,"")</f>
+        <v/>
+      </c>
+      <c r="C178" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E181)=0,Dashboard!E181,"")</f>
+        <v/>
+      </c>
+      <c r="D178" s="35">
+        <f t="shared" si="9"/>
+        <v>121</v>
+      </c>
+      <c r="E178" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B179" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C182)=0,Dashboard!C182,"")</f>
+        <v/>
+      </c>
+      <c r="C179" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E182)=0,Dashboard!E182,"")</f>
+        <v/>
+      </c>
+      <c r="D179" s="35"/>
+      <c r="E179" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B180" s="99" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C183)=0,Dashboard!C183,"")</f>
+        <v/>
+      </c>
+      <c r="C180" s="35" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E183)=0,Dashboard!E183,"")</f>
+        <v/>
+      </c>
+      <c r="D180" s="35"/>
+      <c r="E180" s="100" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="181" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B181" s="130" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C184)=0,Dashboard!C184,"")</f>
+        <v/>
+      </c>
+      <c r="C181" s="131" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E184)=0,Dashboard!E184,"")</f>
+        <v/>
+      </c>
+      <c r="D181" s="131"/>
+      <c r="E181" s="132" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -16271,10 +17359,10 @@
   <sheetPr codeName="Sheet5">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:A146"/>
+  <dimension ref="A1:A168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="116" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17058,66 +18146,198 @@
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="35" t="str">
-        <f>'compile results'!E152</f>
-        <v xml:space="preserve">- number_of_cars = </v>
+        <f>'compile results'!E151</f>
+        <v xml:space="preserve">- heat_share_of_apartments_with_block_heating = </v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="35" t="str">
-        <f>'compile results'!E153</f>
-        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
+        <f>'compile results'!E152</f>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket = </v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="35" t="str">
-        <f>'compile results'!E154</f>
-        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
+        <f>'compile results'!E153</f>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket = </v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="35" t="str">
+        <f>'compile results'!E154</f>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket = </v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="35" t="str">
         <f>'compile results'!E155</f>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket = </v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="35" t="str">
+        <f>'compile results'!E156</f>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket = </v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="35" t="str">
+        <f>'compile results'!E157</f>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket = </v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="35" t="str">
+        <f>'compile results'!E158</f>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket = </v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="35" t="str">
+        <f>'compile results'!E159</f>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket = </v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="35" t="str">
+        <f>'compile results'!E160</f>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket = </v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="35" t="str">
+        <f>'compile results'!E161</f>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket = </v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="35" t="str">
+        <f>'compile results'!E162</f>
+        <v xml:space="preserve">- heat_households_indoor_pipelines_investment_costs_with_block_heating_eur = </v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="35" t="str">
+        <f>'compile results'!E163</f>
+        <v xml:space="preserve">- heat_households_indoor_pipelines_investment_costs_without_block_heating_eur = </v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="35" t="str">
+        <f>'compile results'!E164</f>
+        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_kw = </v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="35" t="str">
+        <f>'compile results'!E165</f>
+        <v xml:space="preserve">- heat_buildings_heat_meter_investment_costs_eur_per_kw = </v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" s="35" t="str">
+        <f>'compile results'!E166</f>
+        <v xml:space="preserve">- heat_buildings_heat_meter_investment_costs_eur_per_connection = </v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" s="35" t="str">
+        <f>'compile results'!E167</f>
+        <v xml:space="preserve">- heat_exchanger_station_investment_costs_eur_per_kw = </v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" s="35" t="str">
+        <f>'compile results'!E168</f>
+        <v xml:space="preserve">- heat_sub_station_investment_costs_eur_per_kw = </v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" s="35" t="str">
+        <f>'compile results'!E169</f>
+        <v xml:space="preserve">- heat_distribution_pipelines_investment_costs_eur_per_meter = </v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="35" t="str">
+        <f>'compile results'!E170</f>
+        <v xml:space="preserve">- heat_primary_pipelines_investment_costs_per_kw = </v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="35" t="str">
+        <f>'compile results'!E171</f>
+        <v xml:space="preserve">- heat_yearly_indoor_infrastructure_maintenance_costs_factor = </v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" s="35" t="str">
+        <f>'compile results'!E172</f>
+        <v xml:space="preserve">- heat_yearly_outdoor_infrastructure_maintenance_costs_factor = </v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" s="35" t="str">
+        <f>'compile results'!E174</f>
+        <v xml:space="preserve">- number_of_cars = </v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="35" t="str">
+        <f>'compile results'!E175</f>
+        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" s="35" t="str">
+        <f>'compile results'!E176</f>
+        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="35" t="str">
+        <f>'compile results'!E177</f>
         <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134" s="35"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135" s="35"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="35"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137" s="35"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138" s="35"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A139" s="35"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A140" s="35"/>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A141" s="35"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142" s="35"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A143" s="35"/>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A144" s="35"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A145" s="35"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A146" s="35"/>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="35"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="35"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" s="35"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="35"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" s="35"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="35"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="35"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="35"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="35"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" s="35"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="35"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" s="35"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" s="35"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:A70">

</xml_diff>

<commit_message>
Published state of ETDataset for deploy May 2024
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C255DB-E376-9648-B472-C80AD2CFC5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A079A0-4504-144E-9646-C818E7E8D064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15220" yWindow="-28300" windowWidth="25600" windowHeight="27160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10380" yWindow="-28300" windowWidth="51200" windowHeight="27160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="3" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="337">
   <si>
     <t>Unit</t>
   </si>
@@ -1060,6 +1060,15 @@
   </si>
   <si>
     <t>Add has_aquathermal_potential attributes and add aquathermal_potential attributes</t>
+  </si>
+  <si>
+    <t>captured_biogenic_co2_price</t>
+  </si>
+  <si>
+    <t>February 28, 2024</t>
+  </si>
+  <si>
+    <t>Add captured_biogenic_co2_price</t>
   </si>
 </sst>
 </file>
@@ -3836,7 +3845,7 @@
   <dimension ref="B2:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3873,7 +3882,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>287</v>
+        <v>335</v>
       </c>
       <c r="D5" s="8"/>
     </row>
@@ -4064,7 +4073,7 @@
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4294,10 +4303,16 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="68"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="71"/>
+    <row r="24" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="68" t="s">
+        <v>335</v>
+      </c>
+      <c r="C24" s="69" t="s">
+        <v>336</v>
+      </c>
+      <c r="D24" s="71">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="65"/>
@@ -4330,10 +4345,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:P242"/>
+  <dimension ref="A2:P243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C226" sqref="C226"/>
+    <sheetView tabSelected="1" topLeftCell="C137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O162" sqref="O162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8268,7 +8283,7 @@
       <c r="J156"/>
       <c r="K156"/>
       <c r="L156" s="38" t="b">
-        <f t="shared" ref="L156:L160" si="16">IF(COUNTBLANK(E156)=0,TRUE,FALSE)</f>
+        <f t="shared" ref="L156:L161" si="16">IF(COUNTBLANK(E156)=0,TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="M156" t="str">
@@ -8356,7 +8371,7 @@
         <v>0</v>
       </c>
       <c r="M159" t="str">
-        <f t="shared" ref="M159:M160" si="18">IF(L159=TRUE," ","Please set value")</f>
+        <f t="shared" ref="M159:M161" si="18">IF(L159=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N159" s="30"/>
@@ -8392,75 +8407,75 @@
         <v>68</v>
       </c>
     </row>
-    <row r="161" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B161" s="40"/>
-      <c r="C161" s="11"/>
-      <c r="D161" s="11"/>
-      <c r="E161" s="52"/>
-      <c r="F161" s="11"/>
-      <c r="G161" s="11"/>
-      <c r="H161" s="11"/>
-      <c r="I161" s="11"/>
-      <c r="J161" s="11"/>
-      <c r="K161" s="11"/>
-      <c r="L161" s="11"/>
-      <c r="M161" s="11"/>
+    <row r="161" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="30"/>
+      <c r="C161" t="s">
+        <v>334</v>
+      </c>
+      <c r="D161" t="s">
+        <v>317</v>
+      </c>
+      <c r="E161" s="56"/>
+      <c r="F161"/>
+      <c r="G161"/>
+      <c r="H161"/>
+      <c r="I161" s="53"/>
+      <c r="J161"/>
+      <c r="K161"/>
+      <c r="L161" s="38" t="b">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M161" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
       <c r="N161" s="30"/>
-      <c r="O161" s="14"/>
-    </row>
-    <row r="162" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C162" s="4"/>
-      <c r="D162" s="4"/>
-      <c r="E162" s="51"/>
-      <c r="F162" s="4"/>
-      <c r="G162" s="4"/>
-      <c r="H162" s="4"/>
-      <c r="I162" s="4"/>
-      <c r="J162" s="4"/>
-      <c r="K162" s="4"/>
-      <c r="L162" s="4"/>
-      <c r="M162" s="4"/>
+      <c r="O161" s="14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="162" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B162" s="40"/>
+      <c r="C162" s="11"/>
+      <c r="D162" s="11"/>
+      <c r="E162" s="52"/>
+      <c r="F162" s="11"/>
+      <c r="G162" s="11"/>
+      <c r="H162" s="11"/>
+      <c r="I162" s="11"/>
+      <c r="J162" s="11"/>
+      <c r="K162" s="11"/>
+      <c r="L162" s="11"/>
+      <c r="M162" s="11"/>
       <c r="N162" s="30"/>
       <c r="O162" s="14"/>
     </row>
     <row r="163" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="30"/>
-      <c r="C163" t="s">
-        <v>122</v>
-      </c>
-      <c r="D163" t="s">
-        <v>137</v>
-      </c>
-      <c r="E163" s="49"/>
-      <c r="F163"/>
-      <c r="G163" s="54"/>
-      <c r="H163"/>
-      <c r="I163" s="53"/>
-      <c r="J163"/>
-      <c r="K163"/>
-      <c r="L163" s="38" t="b">
-        <f>IF(COUNTBLANK(E163)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M163" t="str">
-        <f t="shared" ref="M163:M168" si="19">IF(L163=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
+      <c r="B163" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C163" s="4"/>
+      <c r="D163" s="4"/>
+      <c r="E163" s="51"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
+      <c r="H163" s="4"/>
+      <c r="I163" s="4"/>
+      <c r="J163" s="4"/>
+      <c r="K163" s="4"/>
+      <c r="L163" s="4"/>
+      <c r="M163" s="4"/>
       <c r="N163" s="30"/>
-      <c r="O163" s="78" t="s">
-        <v>122</v>
-      </c>
+      <c r="O163" s="14"/>
     </row>
     <row r="164" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B164" s="30"/>
       <c r="C164" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D164" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E164" s="49"/>
       <c r="F164"/>
@@ -8470,25 +8485,25 @@
       <c r="J164"/>
       <c r="K164"/>
       <c r="L164" s="38" t="b">
-        <f t="shared" ref="L164:L168" si="20">IF(COUNTBLANK(E164)=1,FALSE,TRUE)</f>
+        <f>IF(COUNTBLANK(E164)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M164" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="M164:M169" si="19">IF(L164=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N164" s="30"/>
       <c r="O164" s="78" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="165" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B165" s="30"/>
       <c r="C165" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D165" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E165" s="49"/>
       <c r="F165"/>
@@ -8498,7 +8513,7 @@
       <c r="J165"/>
       <c r="K165"/>
       <c r="L165" s="38" t="b">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="L165:L169" si="20">IF(COUNTBLANK(E165)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M165" t="str">
@@ -8507,16 +8522,16 @@
       </c>
       <c r="N165" s="30"/>
       <c r="O165" s="78" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="166" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B166" s="30"/>
       <c r="C166" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D166" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="E166" s="49"/>
       <c r="F166"/>
@@ -8535,16 +8550,16 @@
       </c>
       <c r="N166" s="30"/>
       <c r="O166" s="78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="167" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B167" s="30"/>
       <c r="C167" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D167" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E167" s="49"/>
       <c r="F167"/>
@@ -8563,16 +8578,16 @@
       </c>
       <c r="N167" s="30"/>
       <c r="O167" s="78" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="168" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B168" s="30"/>
       <c r="C168" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D168" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E168" s="49"/>
       <c r="F168"/>
@@ -8591,44 +8606,44 @@
       </c>
       <c r="N168" s="30"/>
       <c r="O168" s="78" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="169" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B169" s="30"/>
       <c r="C169" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D169" t="s">
-        <v>34</v>
-      </c>
-      <c r="E169" s="98"/>
+        <v>138</v>
+      </c>
+      <c r="E169" s="49"/>
       <c r="F169"/>
       <c r="G169" s="54"/>
       <c r="H169"/>
-      <c r="I169" s="94"/>
+      <c r="I169" s="53"/>
       <c r="J169"/>
       <c r="K169"/>
       <c r="L169" s="38" t="b">
-        <f t="shared" ref="L169:L185" si="21">IF(COUNTBLANK(E169)=1,FALSE,TRUE)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M169" t="str">
-        <f t="shared" ref="M169:M230" si="22">IF(L169=TRUE," ","Please set value")</f>
+        <f t="shared" si="19"/>
         <v>Please set value</v>
       </c>
       <c r="N169" s="30"/>
       <c r="O169" s="78" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="170" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B170" s="30"/>
       <c r="C170" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D170" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="E170" s="98"/>
       <c r="F170"/>
@@ -8638,25 +8653,25 @@
       <c r="J170"/>
       <c r="K170"/>
       <c r="L170" s="38" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="L170:L186" si="21">IF(COUNTBLANK(E170)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M170" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="M170:M231" si="22">IF(L170=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N170" s="30"/>
       <c r="O170" s="78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="171" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B171" s="30"/>
       <c r="C171" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D171" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E171" s="98"/>
       <c r="F171"/>
@@ -8675,16 +8690,16 @@
       </c>
       <c r="N171" s="30"/>
       <c r="O171" s="78" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="172" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B172" s="30"/>
       <c r="C172" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D172" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E172" s="98"/>
       <c r="F172"/>
@@ -8703,16 +8718,16 @@
       </c>
       <c r="N172" s="30"/>
       <c r="O172" s="78" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="173" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B173" s="30"/>
       <c r="C173" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D173" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E173" s="98"/>
       <c r="F173"/>
@@ -8722,7 +8737,7 @@
       <c r="J173"/>
       <c r="K173"/>
       <c r="L173" s="38" t="b">
-        <f>IF(COUNTBLANK(E173)=1,FALSE,TRUE)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M173" t="str">
@@ -8731,16 +8746,16 @@
       </c>
       <c r="N173" s="30"/>
       <c r="O173" s="78" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="174" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B174" s="30"/>
       <c r="C174" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D174" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="E174" s="98"/>
       <c r="F174"/>
@@ -8750,7 +8765,7 @@
       <c r="J174"/>
       <c r="K174"/>
       <c r="L174" s="38" t="b">
-        <f t="shared" si="21"/>
+        <f>IF(COUNTBLANK(E174)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M174" t="str">
@@ -8759,16 +8774,16 @@
       </c>
       <c r="N174" s="30"/>
       <c r="O174" s="78" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="175" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B175" s="30"/>
       <c r="C175" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D175" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E175" s="98"/>
       <c r="F175"/>
@@ -8787,16 +8802,16 @@
       </c>
       <c r="N175" s="30"/>
       <c r="O175" s="78" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="176" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B176" s="30"/>
       <c r="C176" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D176" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E176" s="98"/>
       <c r="F176"/>
@@ -8815,16 +8830,16 @@
       </c>
       <c r="N176" s="30"/>
       <c r="O176" s="78" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="177" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B177" s="30"/>
       <c r="C177" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D177" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E177" s="98"/>
       <c r="F177"/>
@@ -8843,16 +8858,16 @@
       </c>
       <c r="N177" s="30"/>
       <c r="O177" s="78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="178" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B178" s="30"/>
       <c r="C178" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D178" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="E178" s="98"/>
       <c r="F178"/>
@@ -8871,16 +8886,16 @@
       </c>
       <c r="N178" s="30"/>
       <c r="O178" s="78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="179" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B179" s="30"/>
       <c r="C179" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D179" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E179" s="98"/>
       <c r="F179"/>
@@ -8899,16 +8914,16 @@
       </c>
       <c r="N179" s="30"/>
       <c r="O179" s="78" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="180" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B180" s="30"/>
       <c r="C180" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D180" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E180" s="98"/>
       <c r="F180"/>
@@ -8927,16 +8942,16 @@
       </c>
       <c r="N180" s="30"/>
       <c r="O180" s="78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="181" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B181" s="30"/>
       <c r="C181" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D181" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E181" s="98"/>
       <c r="F181"/>
@@ -8955,16 +8970,16 @@
       </c>
       <c r="N181" s="30"/>
       <c r="O181" s="78" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="182" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B182" s="30"/>
       <c r="C182" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D182" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="E182" s="98"/>
       <c r="F182"/>
@@ -8983,13 +8998,13 @@
       </c>
       <c r="N182" s="30"/>
       <c r="O182" s="78" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="183" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B183" s="30"/>
       <c r="C183" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D183" t="s">
         <v>138</v>
@@ -9011,16 +9026,16 @@
       </c>
       <c r="N183" s="30"/>
       <c r="O183" s="78" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="184" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B184" s="30"/>
       <c r="C184" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D184" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E184" s="98"/>
       <c r="F184"/>
@@ -9039,16 +9054,16 @@
       </c>
       <c r="N184" s="30"/>
       <c r="O184" s="78" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="185" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B185" s="30"/>
       <c r="C185" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="D185" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E185" s="98"/>
       <c r="F185"/>
@@ -9067,26 +9082,26 @@
       </c>
       <c r="N185" s="30"/>
       <c r="O185" s="78" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
     </row>
     <row r="186" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B186" s="30"/>
       <c r="C186" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="D186" t="s">
         <v>138</v>
       </c>
-      <c r="E186" s="53"/>
+      <c r="E186" s="98"/>
       <c r="F186"/>
       <c r="G186" s="54"/>
       <c r="H186"/>
-      <c r="I186" s="53"/>
+      <c r="I186" s="94"/>
       <c r="J186"/>
       <c r="K186"/>
       <c r="L186" s="38" t="b">
-        <f>IF(COUNTBLANK(E186)=1,FALSE,TRUE)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M186" t="str">
@@ -9095,60 +9110,60 @@
       </c>
       <c r="N186" s="30"/>
       <c r="O186" s="78" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
     </row>
     <row r="187" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B187" s="30"/>
-      <c r="C187"/>
-      <c r="D187"/>
-      <c r="E187"/>
+      <c r="C187" t="s">
+        <v>69</v>
+      </c>
+      <c r="D187" t="s">
+        <v>138</v>
+      </c>
+      <c r="E187" s="53"/>
       <c r="F187"/>
       <c r="G187" s="54"/>
       <c r="H187"/>
-      <c r="I187"/>
+      <c r="I187" s="53"/>
       <c r="J187"/>
       <c r="K187"/>
-      <c r="L187"/>
-      <c r="M187"/>
+      <c r="L187" s="38" t="b">
+        <f>IF(COUNTBLANK(E187)=1,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="M187" t="str">
+        <f t="shared" si="22"/>
+        <v>Please set value</v>
+      </c>
       <c r="N187" s="30"/>
-      <c r="O187" s="78"/>
+      <c r="O187" s="78" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="188" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B188" s="30"/>
-      <c r="C188" t="s">
-        <v>154</v>
-      </c>
-      <c r="D188" t="s">
-        <v>169</v>
-      </c>
-      <c r="E188" s="53"/>
+      <c r="C188"/>
+      <c r="D188"/>
+      <c r="E188"/>
       <c r="F188"/>
       <c r="G188" s="54"/>
       <c r="H188"/>
-      <c r="I188" s="53"/>
+      <c r="I188"/>
       <c r="J188"/>
       <c r="K188"/>
-      <c r="L188" s="38" t="b">
-        <f>IF(COUNTBLANK(E188)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M188" t="str">
-        <f t="shared" si="22"/>
-        <v>Please set value</v>
-      </c>
+      <c r="L188"/>
+      <c r="M188"/>
       <c r="N188" s="30"/>
-      <c r="O188" t="s">
-        <v>154</v>
-      </c>
+      <c r="O188" s="78"/>
     </row>
     <row r="189" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B189" s="30"/>
       <c r="C189" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D189" t="s">
-        <v>236</v>
+        <v>169</v>
       </c>
       <c r="E189" s="53"/>
       <c r="F189"/>
@@ -9158,7 +9173,7 @@
       <c r="J189"/>
       <c r="K189"/>
       <c r="L189" s="38" t="b">
-        <f t="shared" ref="L189:L230" si="23">IF(COUNTBLANK(E189)=1,FALSE,TRUE)</f>
+        <f>IF(COUNTBLANK(E189)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M189" t="str">
@@ -9167,13 +9182,13 @@
       </c>
       <c r="N189" s="30"/>
       <c r="O189" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="190" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B190" s="30"/>
       <c r="C190" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D190" t="s">
         <v>236</v>
@@ -9186,7 +9201,7 @@
       <c r="J190"/>
       <c r="K190"/>
       <c r="L190" s="38" t="b">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="L190:L231" si="23">IF(COUNTBLANK(E190)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M190" t="str">
@@ -9195,13 +9210,13 @@
       </c>
       <c r="N190" s="30"/>
       <c r="O190" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="191" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B191" s="30"/>
       <c r="C191" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D191" t="s">
         <v>236</v>
@@ -9223,13 +9238,13 @@
       </c>
       <c r="N191" s="30"/>
       <c r="O191" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="192" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B192" s="30"/>
       <c r="C192" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D192" t="s">
         <v>236</v>
@@ -9251,13 +9266,13 @@
       </c>
       <c r="N192" s="30"/>
       <c r="O192" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="193" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B193" s="30"/>
       <c r="C193" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D193" t="s">
         <v>236</v>
@@ -9279,13 +9294,13 @@
       </c>
       <c r="N193" s="30"/>
       <c r="O193" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="194" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B194" s="30"/>
       <c r="C194" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D194" t="s">
         <v>236</v>
@@ -9307,13 +9322,13 @@
       </c>
       <c r="N194" s="30"/>
       <c r="O194" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="195" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B195" s="30"/>
       <c r="C195" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D195" t="s">
         <v>236</v>
@@ -9335,13 +9350,13 @@
       </c>
       <c r="N195" s="30"/>
       <c r="O195" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="196" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B196" s="30"/>
       <c r="C196" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D196" t="s">
         <v>236</v>
@@ -9363,13 +9378,13 @@
       </c>
       <c r="N196" s="30"/>
       <c r="O196" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="197" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B197" s="30"/>
       <c r="C197" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D197" t="s">
         <v>236</v>
@@ -9391,13 +9406,13 @@
       </c>
       <c r="N197" s="30"/>
       <c r="O197" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="198" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B198" s="30"/>
       <c r="C198" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D198" t="s">
         <v>236</v>
@@ -9410,25 +9425,25 @@
       <c r="J198"/>
       <c r="K198"/>
       <c r="L198" s="38" t="b">
-        <f t="shared" ref="L198:L222" si="24">IF(COUNTBLANK(E198)=1,FALSE,TRUE)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="M198" t="str">
-        <f t="shared" ref="M198:M222" si="25">IF(L198=TRUE," ","Please set value")</f>
+        <f t="shared" si="22"/>
         <v>Please set value</v>
       </c>
       <c r="N198" s="30"/>
       <c r="O198" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="199" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B199" s="30"/>
       <c r="C199" t="s">
-        <v>235</v>
+        <v>164</v>
       </c>
       <c r="D199" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E199" s="53"/>
       <c r="F199"/>
@@ -9438,22 +9453,22 @@
       <c r="J199"/>
       <c r="K199"/>
       <c r="L199" s="38" t="b">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="L199:L223" si="24">IF(COUNTBLANK(E199)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M199" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="M199:M223" si="25">IF(L199=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N199" s="30"/>
       <c r="O199" t="s">
-        <v>235</v>
+        <v>164</v>
       </c>
     </row>
     <row r="200" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B200" s="30"/>
       <c r="C200" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D200" t="s">
         <v>237</v>
@@ -9475,13 +9490,13 @@
       </c>
       <c r="N200" s="30"/>
       <c r="O200" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="201" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B201" s="30"/>
       <c r="C201" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D201" t="s">
         <v>237</v>
@@ -9503,13 +9518,13 @@
       </c>
       <c r="N201" s="30"/>
       <c r="O201" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="202" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B202" s="30"/>
       <c r="C202" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D202" t="s">
         <v>237</v>
@@ -9531,13 +9546,13 @@
       </c>
       <c r="N202" s="30"/>
       <c r="O202" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="203" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B203" s="30"/>
       <c r="C203" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D203" t="s">
         <v>237</v>
@@ -9559,13 +9574,13 @@
       </c>
       <c r="N203" s="30"/>
       <c r="O203" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="204" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B204" s="30"/>
       <c r="C204" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D204" t="s">
         <v>237</v>
@@ -9587,13 +9602,13 @@
       </c>
       <c r="N204" s="30"/>
       <c r="O204" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="205" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B205" s="30"/>
       <c r="C205" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D205" t="s">
         <v>237</v>
@@ -9615,13 +9630,13 @@
       </c>
       <c r="N205" s="30"/>
       <c r="O205" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="206" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B206" s="30"/>
       <c r="C206" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D206" t="s">
         <v>237</v>
@@ -9643,13 +9658,13 @@
       </c>
       <c r="N206" s="30"/>
       <c r="O206" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="207" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B207" s="30"/>
       <c r="C207" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D207" t="s">
         <v>237</v>
@@ -9671,16 +9686,16 @@
       </c>
       <c r="N207" s="30"/>
       <c r="O207" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="208" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B208" s="30"/>
       <c r="C208" t="s">
-        <v>165</v>
+        <v>227</v>
       </c>
       <c r="D208" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E208" s="53"/>
       <c r="F208"/>
@@ -9699,16 +9714,16 @@
       </c>
       <c r="N208" s="30"/>
       <c r="O208" t="s">
-        <v>165</v>
+        <v>227</v>
       </c>
     </row>
     <row r="209" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B209" s="30"/>
       <c r="C209" t="s">
-        <v>226</v>
+        <v>165</v>
       </c>
       <c r="D209" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E209" s="53"/>
       <c r="F209"/>
@@ -9727,16 +9742,16 @@
       </c>
       <c r="N209" s="30"/>
       <c r="O209" t="s">
-        <v>226</v>
+        <v>165</v>
       </c>
     </row>
     <row r="210" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B210" s="30"/>
       <c r="C210" t="s">
-        <v>166</v>
+        <v>226</v>
       </c>
       <c r="D210" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E210" s="53"/>
       <c r="F210"/>
@@ -9755,13 +9770,13 @@
       </c>
       <c r="N210" s="30"/>
       <c r="O210" t="s">
-        <v>166</v>
+        <v>226</v>
       </c>
     </row>
     <row r="211" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B211" s="30"/>
       <c r="C211" t="s">
-        <v>225</v>
+        <v>166</v>
       </c>
       <c r="D211" t="s">
         <v>238</v>
@@ -9783,13 +9798,13 @@
       </c>
       <c r="N211" s="30"/>
       <c r="O211" t="s">
-        <v>225</v>
+        <v>166</v>
       </c>
     </row>
     <row r="212" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B212" s="30"/>
       <c r="C212" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D212" t="s">
         <v>238</v>
@@ -9811,13 +9826,13 @@
       </c>
       <c r="N212" s="30"/>
       <c r="O212" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="213" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B213" s="30"/>
       <c r="C213" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D213" t="s">
         <v>238</v>
@@ -9839,16 +9854,16 @@
       </c>
       <c r="N213" s="30"/>
       <c r="O213" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="214" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B214" s="30"/>
       <c r="C214" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D214" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E214" s="53"/>
       <c r="F214"/>
@@ -9867,13 +9882,13 @@
       </c>
       <c r="N214" s="30"/>
       <c r="O214" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="215" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B215" s="30"/>
       <c r="C215" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D215" t="s">
         <v>239</v>
@@ -9895,13 +9910,13 @@
       </c>
       <c r="N215" s="30"/>
       <c r="O215" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="216" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B216" s="30"/>
       <c r="C216" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D216" t="s">
         <v>239</v>
@@ -9923,16 +9938,16 @@
       </c>
       <c r="N216" s="30"/>
       <c r="O216" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="217" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B217" s="30"/>
       <c r="C217" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D217" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E217" s="53"/>
       <c r="F217"/>
@@ -9951,13 +9966,13 @@
       </c>
       <c r="N217" s="30"/>
       <c r="O217" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="218" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B218" s="30"/>
       <c r="C218" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D218" t="s">
         <v>238</v>
@@ -9979,13 +9994,13 @@
       </c>
       <c r="N218" s="30"/>
       <c r="O218" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="219" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B219" s="30"/>
       <c r="C219" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D219" t="s">
         <v>238</v>
@@ -10007,16 +10022,16 @@
       </c>
       <c r="N219" s="30"/>
       <c r="O219" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="220" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B220" s="30"/>
       <c r="C220" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="D220" t="s">
-        <v>170</v>
+        <v>238</v>
       </c>
       <c r="E220" s="53"/>
       <c r="F220"/>
@@ -10035,13 +10050,13 @@
       </c>
       <c r="N220" s="30"/>
       <c r="O220" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
     </row>
     <row r="221" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B221" s="30"/>
       <c r="C221" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D221" t="s">
         <v>170</v>
@@ -10063,16 +10078,16 @@
       </c>
       <c r="N221" s="30"/>
       <c r="O221" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="222" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B222" s="30"/>
       <c r="C222" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="D222" t="s">
-        <v>237</v>
+        <v>170</v>
       </c>
       <c r="E222" s="53"/>
       <c r="F222"/>
@@ -10091,13 +10106,13 @@
       </c>
       <c r="N222" s="30"/>
       <c r="O222" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="223" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B223" s="30"/>
       <c r="C223" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D223" t="s">
         <v>237</v>
@@ -10110,22 +10125,22 @@
       <c r="J223"/>
       <c r="K223"/>
       <c r="L223" s="38" t="b">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M223" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>Please set value</v>
       </c>
       <c r="N223" s="30"/>
       <c r="O223" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="224" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B224" s="30"/>
       <c r="C224" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D224" t="s">
         <v>237</v>
@@ -10147,13 +10162,13 @@
       </c>
       <c r="N224" s="30"/>
       <c r="O224" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="225" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B225" s="30"/>
       <c r="C225" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D225" t="s">
         <v>237</v>
@@ -10175,13 +10190,13 @@
       </c>
       <c r="N225" s="30"/>
       <c r="O225" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="226" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B226" s="30"/>
       <c r="C226" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D226" t="s">
         <v>237</v>
@@ -10203,13 +10218,13 @@
       </c>
       <c r="N226" s="30"/>
       <c r="O226" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="227" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B227" s="30"/>
       <c r="C227" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D227" t="s">
         <v>237</v>
@@ -10231,13 +10246,13 @@
       </c>
       <c r="N227" s="30"/>
       <c r="O227" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="228" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B228" s="30"/>
       <c r="C228" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D228" t="s">
         <v>237</v>
@@ -10259,13 +10274,13 @@
       </c>
       <c r="N228" s="30"/>
       <c r="O228" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="229" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B229" s="30"/>
       <c r="C229" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D229" t="s">
         <v>237</v>
@@ -10287,13 +10302,13 @@
       </c>
       <c r="N229" s="30"/>
       <c r="O229" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="230" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B230" s="30"/>
       <c r="C230" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D230" t="s">
         <v>237</v>
@@ -10315,63 +10330,65 @@
       </c>
       <c r="N230" s="30"/>
       <c r="O230" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="231" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B231" s="30"/>
+      <c r="C231" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="231" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B231" s="30"/>
-      <c r="E231" s="50"/>
+      <c r="D231" t="s">
+        <v>237</v>
+      </c>
+      <c r="E231" s="53"/>
+      <c r="F231"/>
+      <c r="G231" s="54"/>
+      <c r="H231"/>
+      <c r="I231" s="53"/>
+      <c r="J231"/>
+      <c r="K231"/>
+      <c r="L231" s="38" t="b">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="M231" t="str">
+        <f t="shared" si="22"/>
+        <v>Please set value</v>
+      </c>
       <c r="N231" s="30"/>
-      <c r="O231" s="14"/>
-    </row>
-    <row r="232" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B232" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="C232" s="4"/>
-      <c r="D232" s="4"/>
-      <c r="E232" s="51"/>
-      <c r="F232" s="4"/>
-      <c r="G232" s="4"/>
-      <c r="H232" s="4"/>
-      <c r="I232" s="4"/>
-      <c r="J232" s="4"/>
-      <c r="K232" s="4"/>
-      <c r="L232" s="4"/>
-      <c r="M232" s="4"/>
+      <c r="O231" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="232" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B232" s="30"/>
+      <c r="E232" s="50"/>
       <c r="N232" s="30"/>
       <c r="O232" s="14"/>
     </row>
     <row r="233" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B233" s="30"/>
-      <c r="C233" t="s">
-        <v>98</v>
-      </c>
-      <c r="D233"/>
-      <c r="E233" s="49"/>
-      <c r="F233"/>
-      <c r="G233" s="54"/>
-      <c r="H233"/>
-      <c r="I233" s="53"/>
-      <c r="J233"/>
-      <c r="K233"/>
-      <c r="L233" s="38" t="b">
-        <f>IF(COUNTBLANK(E233)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M233" t="str">
-        <f t="shared" ref="M233:M241" si="26">IF(L233=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
+      <c r="B233" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C233" s="4"/>
+      <c r="D233" s="4"/>
+      <c r="E233" s="51"/>
+      <c r="F233" s="4"/>
+      <c r="G233" s="4"/>
+      <c r="H233" s="4"/>
+      <c r="I233" s="4"/>
+      <c r="J233" s="4"/>
+      <c r="K233" s="4"/>
+      <c r="L233" s="4"/>
+      <c r="M233" s="4"/>
       <c r="N233" s="30"/>
-      <c r="O233" s="14" t="s">
-        <v>98</v>
-      </c>
+      <c r="O233" s="14"/>
     </row>
     <row r="234" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B234" s="30"/>
       <c r="C234" t="s">
-        <v>197</v>
+        <v>98</v>
       </c>
       <c r="D234"/>
       <c r="E234" s="49"/>
@@ -10386,18 +10403,18 @@
         <v>0</v>
       </c>
       <c r="M234" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="M234:M242" si="26">IF(L234=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N234" s="30"/>
       <c r="O234" s="14" t="s">
-        <v>197</v>
+        <v>98</v>
       </c>
     </row>
     <row r="235" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B235" s="30"/>
       <c r="C235" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D235"/>
       <c r="E235" s="49"/>
@@ -10417,13 +10434,13 @@
       </c>
       <c r="N235" s="30"/>
       <c r="O235" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="236" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B236" s="30"/>
       <c r="C236" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D236"/>
       <c r="E236" s="49"/>
@@ -10443,16 +10460,16 @@
       </c>
       <c r="N236" s="30"/>
       <c r="O236" s="14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="237" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B237" s="30"/>
       <c r="C237" t="s">
-        <v>105</v>
+        <v>198</v>
       </c>
       <c r="D237"/>
-      <c r="E237" s="60"/>
+      <c r="E237" s="49"/>
       <c r="F237"/>
       <c r="G237" s="54"/>
       <c r="H237"/>
@@ -10460,7 +10477,7 @@
       <c r="J237"/>
       <c r="K237"/>
       <c r="L237" s="38" t="b">
-        <f t="shared" ref="L237:L241" si="27">IF(COUNTBLANK(E237)=1,FALSE,TRUE)</f>
+        <f>IF(COUNTBLANK(E237)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M237" t="str">
@@ -10469,24 +10486,24 @@
       </c>
       <c r="N237" s="30"/>
       <c r="O237" s="14" t="s">
-        <v>105</v>
+        <v>198</v>
       </c>
     </row>
     <row r="238" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B238" s="30"/>
       <c r="C238" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D238"/>
-      <c r="E238" s="99"/>
+      <c r="E238" s="60"/>
       <c r="F238"/>
       <c r="G238" s="54"/>
       <c r="H238"/>
-      <c r="I238" s="95"/>
+      <c r="I238" s="53"/>
       <c r="J238"/>
       <c r="K238"/>
       <c r="L238" s="38" t="b">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="L238:L242" si="27">IF(COUNTBLANK(E238)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M238" t="str">
@@ -10495,13 +10512,13 @@
       </c>
       <c r="N238" s="30"/>
       <c r="O238" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="239" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B239" s="30"/>
       <c r="C239" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D239"/>
       <c r="E239" s="99"/>
@@ -10521,13 +10538,13 @@
       </c>
       <c r="N239" s="30"/>
       <c r="O239" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="240" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B240" s="30"/>
       <c r="C240" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="D240"/>
       <c r="E240" s="99"/>
@@ -10547,13 +10564,13 @@
       </c>
       <c r="N240" s="30"/>
       <c r="O240" s="14" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
     </row>
     <row r="241" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B241" s="30"/>
       <c r="C241" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D241"/>
       <c r="E241" s="99"/>
@@ -10573,59 +10590,85 @@
       </c>
       <c r="N241" s="30"/>
       <c r="O241" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="242" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B242" s="30"/>
+      <c r="C242" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="242" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B242" s="41"/>
-      <c r="C242" s="34"/>
-      <c r="D242" s="34"/>
-      <c r="E242" s="48"/>
-      <c r="F242" s="34"/>
-      <c r="G242" s="34"/>
-      <c r="H242" s="34"/>
-      <c r="I242" s="34"/>
-      <c r="J242" s="34"/>
-      <c r="K242" s="34"/>
-      <c r="L242" s="34"/>
-      <c r="M242" s="34"/>
+      <c r="D242"/>
+      <c r="E242" s="99"/>
+      <c r="F242"/>
+      <c r="G242" s="54"/>
+      <c r="H242"/>
+      <c r="I242" s="95"/>
+      <c r="J242"/>
+      <c r="K242"/>
+      <c r="L242" s="38" t="b">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="M242" t="str">
+        <f t="shared" si="26"/>
+        <v>Please set value</v>
+      </c>
       <c r="N242" s="30"/>
+      <c r="O242" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="243" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B243" s="41"/>
+      <c r="C243" s="34"/>
+      <c r="D243" s="34"/>
+      <c r="E243" s="48"/>
+      <c r="F243" s="34"/>
+      <c r="G243" s="34"/>
+      <c r="H243" s="34"/>
+      <c r="I243" s="34"/>
+      <c r="J243" s="34"/>
+      <c r="K243" s="34"/>
+      <c r="L243" s="34"/>
+      <c r="M243" s="34"/>
+      <c r="N243" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:I5"/>
   </mergeCells>
-  <conditionalFormatting sqref="L20:L39 L50:L77 L84:L153 L156:L160 L188:L230 L43:L47 L81">
-    <cfRule type="cellIs" dxfId="4" priority="23" operator="equal">
+  <conditionalFormatting sqref="L20:L47">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L163:L186">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+  <conditionalFormatting sqref="L50:L81">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L233:L241">
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+  <conditionalFormatting sqref="L84:L153 L189:L231 L156:L161">
+    <cfRule type="cellIs" dxfId="2" priority="23" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L40:L42">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="L164:L187">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L78:L80">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="L234:L242">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E20" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E83 E50:E51 E55:E59 E154:E242" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E83 E50:E51 E55:E59 E154:E243" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -11117,8 +11160,8 @@
   </sheetPr>
   <dimension ref="B1:D250"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:D241"/>
+    <sheetView topLeftCell="A196" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B247" sqref="B247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11433,7 +11476,7 @@
         <v/>
       </c>
       <c r="D29" s="86" t="str">
-        <f t="shared" ref="D29:D75" si="5">IF(COUNTBLANK(B29)=0,"- "&amp;B29&amp;" = "&amp;LOWER(C29),"")</f>
+        <f t="shared" ref="D29:D36" si="5">IF(COUNTBLANK(B29)=0,"- "&amp;B29&amp;" = "&amp;LOWER(C29),"")</f>
         <v xml:space="preserve">- has_detailed_chemical_industry = </v>
       </c>
     </row>
@@ -13239,7 +13282,7 @@
         <v/>
       </c>
       <c r="D158" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="D158:D174" si="9">IF(COUNTBLANK(B158)=0,"- "&amp;B158&amp;" = "&amp;LOWER(C158),"")</f>
         <v xml:space="preserve">- co2_emission_1990_marine_bunkers = </v>
       </c>
     </row>
@@ -13253,7 +13296,7 @@
         <v/>
       </c>
       <c r="D159" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">- co2_percentage_free = </v>
       </c>
     </row>
@@ -13267,22 +13310,22 @@
         <v/>
       </c>
       <c r="D160" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">- co2_price = </v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B161" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C161)=0,Dashboard!C161,"")</f>
-        <v/>
+        <v>captured_biogenic_co2_price</v>
       </c>
       <c r="C161" t="str">
         <f>IF(COUNTBLANK(Dashboard!E161)=0,Dashboard!E161,"")</f>
         <v/>
       </c>
       <c r="D161" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- captured_biogenic_co2_price = </v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.2">
@@ -13295,974 +13338,974 @@
         <v/>
       </c>
       <c r="D162" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B163" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C163)=0,Dashboard!C163,"")</f>
-        <v>lv_net_capacity_per_step</v>
+        <v/>
       </c>
       <c r="C163" t="str">
         <f>IF(COUNTBLANK(Dashboard!E163)=0,Dashboard!E163,"")</f>
         <v/>
       </c>
       <c r="D163" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- lv_net_capacity_per_step = </v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B164" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C164)=0,Dashboard!C164,"")</f>
-        <v>lv_net_costs_per_capacity_step</v>
+        <v>lv_net_capacity_per_step</v>
       </c>
       <c r="C164" t="str">
         <f>IF(COUNTBLANK(Dashboard!E164)=0,Dashboard!E164,"")</f>
         <v/>
       </c>
       <c r="D164" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- lv_net_costs_per_capacity_step = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- lv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B165" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C165)=0,Dashboard!C165,"")</f>
-        <v>lv_net_spare_capacity</v>
+        <v>lv_net_costs_per_capacity_step</v>
       </c>
       <c r="C165" t="str">
         <f>IF(COUNTBLANK(Dashboard!E165)=0,Dashboard!E165,"")</f>
         <v/>
       </c>
       <c r="D165" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- lv_net_spare_capacity = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- lv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B166" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C166)=0,Dashboard!C166,"")</f>
-        <v>lv_net_total_costs_present</v>
+        <v>lv_net_spare_capacity</v>
       </c>
       <c r="C166" t="str">
         <f>IF(COUNTBLANK(Dashboard!E166)=0,Dashboard!E166,"")</f>
         <v/>
       </c>
       <c r="D166" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- lv_net_total_costs_present = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- lv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B167" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C167)=0,Dashboard!C167,"")</f>
-        <v>lv_mv_trafo_capacity_per_step</v>
+        <v>lv_net_total_costs_present</v>
       </c>
       <c r="C167" t="str">
         <f>IF(COUNTBLANK(Dashboard!E167)=0,Dashboard!E167,"")</f>
         <v/>
       </c>
       <c r="D167" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- lv_mv_trafo_capacity_per_step = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- lv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B168" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C168)=0,Dashboard!C168,"")</f>
-        <v>lv_mv_trafo_costs_per_capacity_step</v>
+        <v>lv_mv_trafo_capacity_per_step</v>
       </c>
       <c r="C168" t="str">
         <f>IF(COUNTBLANK(Dashboard!E168)=0,Dashboard!E168,"")</f>
         <v/>
       </c>
       <c r="D168" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- lv_mv_trafo_costs_per_capacity_step = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- lv_mv_trafo_capacity_per_step = </v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B169" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C169)=0,Dashboard!C169,"")</f>
-        <v>lv_mv_trafo_spare_capacity</v>
+        <v>lv_mv_trafo_costs_per_capacity_step</v>
       </c>
       <c r="C169" t="str">
         <f>IF(COUNTBLANK(Dashboard!E169)=0,Dashboard!E169,"")</f>
         <v/>
       </c>
       <c r="D169" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- lv_mv_trafo_spare_capacity = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- lv_mv_trafo_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B170" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C170)=0,Dashboard!C170,"")</f>
-        <v>lv_mv_trafo_total_costs_present</v>
+        <v>lv_mv_trafo_spare_capacity</v>
       </c>
       <c r="C170" t="str">
         <f>IF(COUNTBLANK(Dashboard!E170)=0,Dashboard!E170,"")</f>
         <v/>
       </c>
       <c r="D170" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- lv_mv_trafo_total_costs_present = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- lv_mv_trafo_spare_capacity = </v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B171" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C171)=0,Dashboard!C171,"")</f>
-        <v>mv_net_capacity_per_step</v>
+        <v>lv_mv_trafo_total_costs_present</v>
       </c>
       <c r="C171" t="str">
         <f>IF(COUNTBLANK(Dashboard!E171)=0,Dashboard!E171,"")</f>
         <v/>
       </c>
       <c r="D171" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- mv_net_capacity_per_step = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- lv_mv_trafo_total_costs_present = </v>
       </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B172" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C172)=0,Dashboard!C172,"")</f>
-        <v>mv_net_costs_per_capacity_step</v>
+        <v>mv_net_capacity_per_step</v>
       </c>
       <c r="C172" t="str">
         <f>IF(COUNTBLANK(Dashboard!E172)=0,Dashboard!E172,"")</f>
         <v/>
       </c>
       <c r="D172" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- mv_net_costs_per_capacity_step = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- mv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B173" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C173)=0,Dashboard!C173,"")</f>
-        <v>mv_net_spare_capacity</v>
+        <v>mv_net_costs_per_capacity_step</v>
       </c>
       <c r="C173" t="str">
         <f>IF(COUNTBLANK(Dashboard!E173)=0,Dashboard!E173,"")</f>
         <v/>
       </c>
       <c r="D173" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- mv_net_spare_capacity = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- mv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B174" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C174)=0,Dashboard!C174,"")</f>
-        <v>mv_net_total_costs_present</v>
+        <v>mv_net_spare_capacity</v>
       </c>
       <c r="C174" t="str">
         <f>IF(COUNTBLANK(Dashboard!E174)=0,Dashboard!E174,"")</f>
         <v/>
       </c>
       <c r="D174" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- mv_net_total_costs_present = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- mv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B175" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C175)=0,Dashboard!C175,"")</f>
-        <v>mv_hv_trafo_capacity_per_step</v>
+        <v>mv_net_total_costs_present</v>
       </c>
       <c r="C175" t="str">
         <f>IF(COUNTBLANK(Dashboard!E175)=0,Dashboard!E175,"")</f>
         <v/>
       </c>
       <c r="D175" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- mv_hv_trafo_capacity_per_step = </v>
+        <f t="shared" ref="D175:D212" si="10">IF(COUNTBLANK(B175)=0,"- "&amp;B175&amp;" = "&amp;LOWER(C175),"")</f>
+        <v xml:space="preserve">- mv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B176" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C176)=0,Dashboard!C176,"")</f>
-        <v>mv_hv_trafo_costs_per_capacity_step</v>
+        <v>mv_hv_trafo_capacity_per_step</v>
       </c>
       <c r="C176" t="str">
         <f>IF(COUNTBLANK(Dashboard!E176)=0,Dashboard!E176,"")</f>
         <v/>
       </c>
       <c r="D176" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- mv_hv_trafo_costs_per_capacity_step = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- mv_hv_trafo_capacity_per_step = </v>
       </c>
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B177" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C177)=0,Dashboard!C177,"")</f>
-        <v>mv_hv_trafo_spare_capacity</v>
+        <v>mv_hv_trafo_costs_per_capacity_step</v>
       </c>
       <c r="C177" t="str">
         <f>IF(COUNTBLANK(Dashboard!E177)=0,Dashboard!E177,"")</f>
         <v/>
       </c>
       <c r="D177" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- mv_hv_trafo_spare_capacity = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- mv_hv_trafo_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B178" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C178)=0,Dashboard!C178,"")</f>
-        <v>mv_hv_trafo_total_costs_present</v>
+        <v>mv_hv_trafo_spare_capacity</v>
       </c>
       <c r="C178" t="str">
         <f>IF(COUNTBLANK(Dashboard!E178)=0,Dashboard!E178,"")</f>
         <v/>
       </c>
       <c r="D178" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- mv_hv_trafo_total_costs_present = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- mv_hv_trafo_spare_capacity = </v>
       </c>
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B179" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C179)=0,Dashboard!C179,"")</f>
-        <v>hv_net_capacity_per_step</v>
+        <v>mv_hv_trafo_total_costs_present</v>
       </c>
       <c r="C179" t="str">
         <f>IF(COUNTBLANK(Dashboard!E179)=0,Dashboard!E179,"")</f>
         <v/>
       </c>
       <c r="D179" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- hv_net_capacity_per_step = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- mv_hv_trafo_total_costs_present = </v>
       </c>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B180" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C180)=0,Dashboard!C180,"")</f>
-        <v>hv_net_costs_per_capacity_step</v>
+        <v>hv_net_capacity_per_step</v>
       </c>
       <c r="C180" t="str">
         <f>IF(COUNTBLANK(Dashboard!E180)=0,Dashboard!E180,"")</f>
         <v/>
       </c>
       <c r="D180" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- hv_net_costs_per_capacity_step = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- hv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B181" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C181)=0,Dashboard!C181,"")</f>
-        <v>hv_net_spare_capacity</v>
+        <v>hv_net_costs_per_capacity_step</v>
       </c>
       <c r="C181" t="str">
         <f>IF(COUNTBLANK(Dashboard!E181)=0,Dashboard!E181,"")</f>
         <v/>
       </c>
       <c r="D181" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- hv_net_spare_capacity = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- hv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B182" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C182)=0,Dashboard!C182,"")</f>
-        <v>hv_net_total_costs_present</v>
+        <v>hv_net_spare_capacity</v>
       </c>
       <c r="C182" t="str">
         <f>IF(COUNTBLANK(Dashboard!E182)=0,Dashboard!E182,"")</f>
         <v/>
       </c>
       <c r="D182" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- hv_net_total_costs_present = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- hv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B183" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C183)=0,Dashboard!C183,"")</f>
-        <v>interconnection_net_costs_present</v>
+        <v>hv_net_total_costs_present</v>
       </c>
       <c r="C183" t="str">
         <f>IF(COUNTBLANK(Dashboard!E183)=0,Dashboard!E183,"")</f>
         <v/>
       </c>
       <c r="D183" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- interconnection_net_costs_present = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- hv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B184" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C184)=0,Dashboard!C184,"")</f>
-        <v>interconnector_capacity</v>
+        <v>interconnection_net_costs_present</v>
       </c>
       <c r="C184" t="str">
         <f>IF(COUNTBLANK(Dashboard!E184)=0,Dashboard!E184,"")</f>
         <v/>
       </c>
       <c r="D184" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- interconnector_capacity = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- interconnection_net_costs_present = </v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B185" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C185)=0,Dashboard!C185,"")</f>
-        <v>offshore_net_costs_present</v>
+        <v>interconnector_capacity</v>
       </c>
       <c r="C185" t="str">
         <f>IF(COUNTBLANK(Dashboard!E185)=0,Dashboard!E185,"")</f>
         <v/>
       </c>
       <c r="D185" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- offshore_net_costs_present = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- interconnector_capacity = </v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B186" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C186)=0,Dashboard!C186,"")</f>
-        <v>annual_infrastructure_cost_gas</v>
+        <v>offshore_net_costs_present</v>
       </c>
       <c r="C186" t="str">
         <f>IF(COUNTBLANK(Dashboard!E186)=0,Dashboard!E186,"")</f>
         <v/>
       </c>
       <c r="D186" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- annual_infrastructure_cost_gas = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- offshore_net_costs_present = </v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B187" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C187)=0,Dashboard!C187,"")</f>
-        <v/>
+        <v>annual_infrastructure_cost_gas</v>
       </c>
       <c r="C187" t="str">
         <f>IF(COUNTBLANK(Dashboard!E187)=0,Dashboard!E187,"")</f>
         <v/>
       </c>
       <c r="D187" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- annual_infrastructure_cost_gas = </v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B188" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C188)=0,Dashboard!C188,"")</f>
-        <v>heat_share_of_apartments_with_block_heating</v>
+        <v/>
       </c>
       <c r="C188" t="str">
         <f>IF(COUNTBLANK(Dashboard!E188)=0,Dashboard!E188,"")</f>
         <v/>
       </c>
       <c r="D188" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- heat_share_of_apartments_with_block_heating = </v>
+        <f t="shared" si="10"/>
+        <v/>
       </c>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B189" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C189)=0,Dashboard!C189,"")</f>
-        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket</v>
+        <v>heat_share_of_apartments_with_block_heating</v>
       </c>
       <c r="C189" t="str">
         <f>IF(COUNTBLANK(Dashboard!E189)=0,Dashboard!E189,"")</f>
         <v/>
       </c>
       <c r="D189" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_share_of_apartments_with_block_heating = </v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B190" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C190)=0,Dashboard!C190,"")</f>
-        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket</v>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket</v>
       </c>
       <c r="C190" t="str">
         <f>IF(COUNTBLANK(Dashboard!E190)=0,Dashboard!E190,"")</f>
         <v/>
       </c>
       <c r="D190" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket = </v>
       </c>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B191" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C191)=0,Dashboard!C191,"")</f>
-        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket</v>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket</v>
       </c>
       <c r="C191" t="str">
         <f>IF(COUNTBLANK(Dashboard!E191)=0,Dashboard!E191,"")</f>
         <v/>
       </c>
       <c r="D191" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket = </v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B192" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C192)=0,Dashboard!C192,"")</f>
-        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket</v>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket</v>
       </c>
       <c r="C192" t="str">
         <f>IF(COUNTBLANK(Dashboard!E192)=0,Dashboard!E192,"")</f>
         <v/>
       </c>
       <c r="D192" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket = </v>
       </c>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B193" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C193)=0,Dashboard!C193,"")</f>
-        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket</v>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket</v>
       </c>
       <c r="C193" t="str">
         <f>IF(COUNTBLANK(Dashboard!E193)=0,Dashboard!E193,"")</f>
         <v/>
       </c>
       <c r="D193" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket = </v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B194" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C194)=0,Dashboard!C194,"")</f>
-        <v>heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket</v>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket</v>
       </c>
       <c r="C194" t="str">
         <f>IF(COUNTBLANK(Dashboard!E194)=0,Dashboard!E194,"")</f>
         <v/>
       </c>
       <c r="D194" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket = </v>
       </c>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B195" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C195)=0,Dashboard!C195,"")</f>
-        <v>heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket</v>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket</v>
       </c>
       <c r="C195" t="str">
         <f>IF(COUNTBLANK(Dashboard!E195)=0,Dashboard!E195,"")</f>
         <v/>
       </c>
       <c r="D195" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket = </v>
       </c>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B196" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C196)=0,Dashboard!C196,"")</f>
-        <v>heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket</v>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket</v>
       </c>
       <c r="C196" t="str">
         <f>IF(COUNTBLANK(Dashboard!E196)=0,Dashboard!E196,"")</f>
         <v/>
       </c>
       <c r="D196" s="86" t="str">
-        <f t="shared" ref="D196:D242" si="9">IF(COUNTBLANK(B196)=0,"- "&amp;B196&amp;" = "&amp;LOWER(C196),"")</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket = </v>
       </c>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B197" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C197)=0,Dashboard!C197,"")</f>
-        <v>heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket</v>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket</v>
       </c>
       <c r="C197" t="str">
         <f>IF(COUNTBLANK(Dashboard!E197)=0,Dashboard!E197,"")</f>
         <v/>
       </c>
       <c r="D197" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket = </v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B198" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C198)=0,Dashboard!C198,"")</f>
-        <v>heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket</v>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket</v>
       </c>
       <c r="C198" t="str">
         <f>IF(COUNTBLANK(Dashboard!E198)=0,Dashboard!E198,"")</f>
         <v/>
       </c>
       <c r="D198" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket = </v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B199" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C199)=0,Dashboard!C199,"")</f>
-        <v>heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur</v>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket</v>
       </c>
       <c r="C199" t="str">
         <f>IF(COUNTBLANK(Dashboard!E199)=0,Dashboard!E199,"")</f>
         <v/>
       </c>
       <c r="D199" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket = </v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B200" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C200)=0,Dashboard!C200,"")</f>
-        <v>heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur</v>
+        <v>heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur</v>
       </c>
       <c r="C200" t="str">
         <f>IF(COUNTBLANK(Dashboard!E200)=0,Dashboard!E200,"")</f>
         <v/>
       </c>
       <c r="D200" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B201" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C201)=0,Dashboard!C201,"")</f>
-        <v>heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur</v>
+        <v>heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur</v>
       </c>
       <c r="C201" t="str">
         <f>IF(COUNTBLANK(Dashboard!E201)=0,Dashboard!E201,"")</f>
         <v/>
       </c>
       <c r="D201" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B202" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C202)=0,Dashboard!C202,"")</f>
-        <v>heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur</v>
+        <v>heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur</v>
       </c>
       <c r="C202" t="str">
         <f>IF(COUNTBLANK(Dashboard!E202)=0,Dashboard!E202,"")</f>
         <v/>
       </c>
       <c r="D202" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B203" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C203)=0,Dashboard!C203,"")</f>
-        <v>heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur</v>
+        <v>heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur</v>
       </c>
       <c r="C203" t="str">
         <f>IF(COUNTBLANK(Dashboard!E203)=0,Dashboard!E203,"")</f>
         <v/>
       </c>
       <c r="D203" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B204" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C204)=0,Dashboard!C204,"")</f>
-        <v>heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur</v>
+        <v>heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur</v>
       </c>
       <c r="C204" t="str">
         <f>IF(COUNTBLANK(Dashboard!E204)=0,Dashboard!E204,"")</f>
         <v/>
       </c>
       <c r="D204" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B205" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C205)=0,Dashboard!C205,"")</f>
-        <v>heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur</v>
+        <v>heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur</v>
       </c>
       <c r="C205" t="str">
         <f>IF(COUNTBLANK(Dashboard!E205)=0,Dashboard!E205,"")</f>
         <v/>
       </c>
       <c r="D205" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B206" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C206)=0,Dashboard!C206,"")</f>
-        <v>heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur</v>
+        <v>heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur</v>
       </c>
       <c r="C206" t="str">
         <f>IF(COUNTBLANK(Dashboard!E206)=0,Dashboard!E206,"")</f>
         <v/>
       </c>
       <c r="D206" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B207" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C207)=0,Dashboard!C207,"")</f>
-        <v>heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur</v>
+        <v>heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur</v>
       </c>
       <c r="C207" t="str">
         <f>IF(COUNTBLANK(Dashboard!E207)=0,Dashboard!E207,"")</f>
         <v/>
       </c>
       <c r="D207" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B208" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C208)=0,Dashboard!C208,"")</f>
-        <v>heat_buildings_indoor_investment_costs_eur_per_kw</v>
+        <v>heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur</v>
       </c>
       <c r="C208" t="str">
         <f>IF(COUNTBLANK(Dashboard!E208)=0,Dashboard!E208,"")</f>
         <v/>
       </c>
       <c r="D208" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_kw = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="209" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B209" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C209)=0,Dashboard!C209,"")</f>
-        <v>heat_buildings_indoor_investment_costs_eur_per_connection</v>
+        <v>heat_buildings_indoor_investment_costs_eur_per_kw</v>
       </c>
       <c r="C209" t="str">
         <f>IF(COUNTBLANK(Dashboard!E209)=0,Dashboard!E209,"")</f>
         <v/>
       </c>
       <c r="D209" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_connection = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B210" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C210)=0,Dashboard!C210,"")</f>
-        <v>heat_exchanger_station_investment_costs_eur_per_kw</v>
+        <v>heat_buildings_indoor_investment_costs_eur_per_connection</v>
       </c>
       <c r="C210" t="str">
         <f>IF(COUNTBLANK(Dashboard!E210)=0,Dashboard!E210,"")</f>
         <v/>
       </c>
       <c r="D210" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_exchanger_station_investment_costs_eur_per_kw = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B211" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C211)=0,Dashboard!C211,"")</f>
-        <v>heat_lt_sub_station_investment_costs_eur_per_kw</v>
+        <v>heat_exchanger_station_investment_costs_eur_per_kw</v>
       </c>
       <c r="C211" t="str">
         <f>IF(COUNTBLANK(Dashboard!E211)=0,Dashboard!E211,"")</f>
         <v/>
       </c>
       <c r="D211" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_lt_sub_station_investment_costs_eur_per_kw = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_exchanger_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="212" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B212" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C212)=0,Dashboard!C212,"")</f>
-        <v>heat_mt_sub_station_investment_costs_eur_per_kw</v>
+        <v>heat_lt_sub_station_investment_costs_eur_per_kw</v>
       </c>
       <c r="C212" t="str">
         <f>IF(COUNTBLANK(Dashboard!E212)=0,Dashboard!E212,"")</f>
         <v/>
       </c>
       <c r="D212" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_mt_sub_station_investment_costs_eur_per_kw = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_lt_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="213" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B213" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C213)=0,Dashboard!C213,"")</f>
-        <v>heat_ht_sub_station_investment_costs_eur_per_kw</v>
+        <v>heat_mt_sub_station_investment_costs_eur_per_kw</v>
       </c>
       <c r="C213" t="str">
         <f>IF(COUNTBLANK(Dashboard!E213)=0,Dashboard!E213,"")</f>
         <v/>
       </c>
       <c r="D213" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_ht_sub_station_investment_costs_eur_per_kw = </v>
+        <f t="shared" ref="D213:D244" si="11">IF(COUNTBLANK(B213)=0,"- "&amp;B213&amp;" = "&amp;LOWER(C213),"")</f>
+        <v xml:space="preserve">- heat_mt_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B214" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C214)=0,Dashboard!C214,"")</f>
-        <v>heat_lt_distribution_pipelines_investment_costs_eur_per_meter</v>
+        <v>heat_ht_sub_station_investment_costs_eur_per_kw</v>
       </c>
       <c r="C214" t="str">
         <f>IF(COUNTBLANK(Dashboard!E214)=0,Dashboard!E214,"")</f>
         <v/>
       </c>
       <c r="D214" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_lt_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- heat_ht_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B215" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C215)=0,Dashboard!C215,"")</f>
-        <v>heat_mt_distribution_pipelines_investment_costs_eur_per_meter</v>
+        <v>heat_lt_distribution_pipelines_investment_costs_eur_per_meter</v>
       </c>
       <c r="C215" t="str">
         <f>IF(COUNTBLANK(Dashboard!E215)=0,Dashboard!E215,"")</f>
         <v/>
       </c>
       <c r="D215" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_mt_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- heat_lt_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="216" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B216" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C216)=0,Dashboard!C216,"")</f>
-        <v>heat_ht_distribution_pipelines_investment_costs_eur_per_meter</v>
+        <v>heat_mt_distribution_pipelines_investment_costs_eur_per_meter</v>
       </c>
       <c r="C216" t="str">
         <f>IF(COUNTBLANK(Dashboard!E216)=0,Dashboard!E216,"")</f>
         <v/>
       </c>
       <c r="D216" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_ht_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- heat_mt_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B217" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C217)=0,Dashboard!C217,"")</f>
-        <v>heat_lt_primary_pipelines_investment_costs_per_kw</v>
+        <v>heat_ht_distribution_pipelines_investment_costs_eur_per_meter</v>
       </c>
       <c r="C217" t="str">
         <f>IF(COUNTBLANK(Dashboard!E217)=0,Dashboard!E217,"")</f>
         <v/>
       </c>
       <c r="D217" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_lt_primary_pipelines_investment_costs_per_kw = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- heat_ht_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="218" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B218" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C218)=0,Dashboard!C218,"")</f>
-        <v>heat_mt_primary_pipelines_investment_costs_per_kw</v>
+        <v>heat_lt_primary_pipelines_investment_costs_per_kw</v>
       </c>
       <c r="C218" t="str">
         <f>IF(COUNTBLANK(Dashboard!E218)=0,Dashboard!E218,"")</f>
         <v/>
       </c>
       <c r="D218" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_mt_primary_pipelines_investment_costs_per_kw = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- heat_lt_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B219" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C219)=0,Dashboard!C219,"")</f>
-        <v>heat_ht_primary_pipelines_investment_costs_per_kw</v>
+        <v>heat_mt_primary_pipelines_investment_costs_per_kw</v>
       </c>
       <c r="C219" t="str">
         <f>IF(COUNTBLANK(Dashboard!E219)=0,Dashboard!E219,"")</f>
         <v/>
       </c>
       <c r="D219" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_ht_primary_pipelines_investment_costs_per_kw = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- heat_mt_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B220" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C220)=0,Dashboard!C220,"")</f>
-        <v>heat_yearly_indoor_infrastructure_maintenance_costs_factor</v>
+        <v>heat_ht_primary_pipelines_investment_costs_per_kw</v>
       </c>
       <c r="C220" t="str">
         <f>IF(COUNTBLANK(Dashboard!E220)=0,Dashboard!E220,"")</f>
         <v/>
       </c>
       <c r="D220" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_yearly_indoor_infrastructure_maintenance_costs_factor = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- heat_ht_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B221" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C221)=0,Dashboard!C221,"")</f>
-        <v>heat_yearly_outdoor_infrastructure_maintenance_costs_factor</v>
+        <v>heat_yearly_indoor_infrastructure_maintenance_costs_factor</v>
       </c>
       <c r="C221" t="str">
         <f>IF(COUNTBLANK(Dashboard!E221)=0,Dashboard!E221,"")</f>
         <v/>
       </c>
       <c r="D221" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- heat_yearly_outdoor_infrastructure_maintenance_costs_factor = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- heat_yearly_indoor_infrastructure_maintenance_costs_factor = </v>
       </c>
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B222" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C222)=0,Dashboard!C222,"")</f>
-        <v>households_lt_heat_delivery_system_costs_apartments_eur_per_connection</v>
+        <v>heat_yearly_outdoor_infrastructure_maintenance_costs_factor</v>
       </c>
       <c r="C222" t="str">
         <f>IF(COUNTBLANK(Dashboard!E222)=0,Dashboard!E222,"")</f>
         <v/>
       </c>
       <c r="D222" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- heat_yearly_outdoor_infrastructure_maintenance_costs_factor = </v>
       </c>
     </row>
     <row r="223" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B223" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C223)=0,Dashboard!C223,"")</f>
-        <v>households_mt_heat_delivery_system_costs_apartments_eur_per_connection</v>
+        <v>households_lt_heat_delivery_system_costs_apartments_eur_per_connection</v>
       </c>
       <c r="C223" t="str">
         <f>IF(COUNTBLANK(Dashboard!E223)=0,Dashboard!E223,"")</f>
         <v/>
       </c>
       <c r="D223" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B224" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C224)=0,Dashboard!C224,"")</f>
-        <v>households_ht_heat_delivery_system_costs_apartments_eur_per_connection</v>
+        <v>households_mt_heat_delivery_system_costs_apartments_eur_per_connection</v>
       </c>
       <c r="C224" t="str">
         <f>IF(COUNTBLANK(Dashboard!E224)=0,Dashboard!E224,"")</f>
         <v/>
       </c>
       <c r="D224" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B225" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C225)=0,Dashboard!C225,"")</f>
-        <v>households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
+        <v>households_ht_heat_delivery_system_costs_apartments_eur_per_connection</v>
       </c>
       <c r="C225" t="str">
         <f>IF(COUNTBLANK(Dashboard!E225)=0,Dashboard!E225,"")</f>
         <v/>
       </c>
       <c r="D225" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B226" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C226)=0,Dashboard!C226,"")</f>
-        <v>households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
+        <v>households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
       </c>
       <c r="C226" t="str">
         <f>IF(COUNTBLANK(Dashboard!E226)=0,Dashboard!E226,"")</f>
         <v/>
       </c>
       <c r="D226" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="227" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B227" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C227)=0,Dashboard!C227,"")</f>
-        <v>households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
+        <v>households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
       </c>
       <c r="C227" t="str">
         <f>IF(COUNTBLANK(Dashboard!E227)=0,Dashboard!E227,"")</f>
         <v/>
       </c>
       <c r="D227" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B228" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C228)=0,Dashboard!C228,"")</f>
-        <v>buildings_lt_heat_delivery_system_costs_eur_per_connection</v>
+        <v>households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
       </c>
       <c r="C228" t="str">
         <f>IF(COUNTBLANK(Dashboard!E228)=0,Dashboard!E228,"")</f>
         <v/>
       </c>
       <c r="D228" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- buildings_lt_heat_delivery_system_costs_eur_per_connection = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B229" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C229)=0,Dashboard!C229,"")</f>
-        <v>buildings_mt_heat_delivery_system_costs_eur_per_connection</v>
+        <v>buildings_lt_heat_delivery_system_costs_eur_per_connection</v>
       </c>
       <c r="C229" t="str">
         <f>IF(COUNTBLANK(Dashboard!E229)=0,Dashboard!E229,"")</f>
         <v/>
       </c>
       <c r="D229" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- buildings_mt_heat_delivery_system_costs_eur_per_connection = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- buildings_lt_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B230" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C230)=0,Dashboard!C230,"")</f>
-        <v>buildings_ht_heat_delivery_system_costs_eur_per_connection</v>
+        <v>buildings_mt_heat_delivery_system_costs_eur_per_connection</v>
       </c>
       <c r="C230" t="str">
         <f>IF(COUNTBLANK(Dashboard!E230)=0,Dashboard!E230,"")</f>
         <v/>
       </c>
       <c r="D230" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- buildings_ht_heat_delivery_system_costs_eur_per_connection = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- buildings_mt_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B231" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C231)=0,Dashboard!C231,"")</f>
-        <v/>
+        <v>buildings_ht_heat_delivery_system_costs_eur_per_connection</v>
       </c>
       <c r="C231" t="str">
         <f>IF(COUNTBLANK(Dashboard!E231)=0,Dashboard!E231,"")</f>
         <v/>
       </c>
       <c r="D231" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- buildings_ht_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.2">
@@ -14275,140 +14318,149 @@
         <v/>
       </c>
       <c r="D232" s="86" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B233" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C233)=0,Dashboard!C233,"")</f>
-        <v>number_of_cars</v>
+        <v/>
       </c>
       <c r="C233" t="str">
         <f>IF(COUNTBLANK(Dashboard!E233)=0,Dashboard!E233,"")</f>
         <v/>
       </c>
       <c r="D233" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- number_of_cars = </v>
+        <f t="shared" si="11"/>
+        <v/>
       </c>
     </row>
     <row r="234" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B234" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C234)=0,Dashboard!C234,"")</f>
-        <v>number_of_busses</v>
+        <v>number_of_cars</v>
       </c>
       <c r="C234" t="str">
         <f>IF(COUNTBLANK(Dashboard!E234)=0,Dashboard!E234,"")</f>
         <v/>
       </c>
       <c r="D234" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- number_of_busses = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- number_of_cars = </v>
       </c>
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B235" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C235)=0,Dashboard!C235,"")</f>
-        <v>number_of_trucks</v>
+        <v>number_of_busses</v>
       </c>
       <c r="C235" t="str">
         <f>IF(COUNTBLANK(Dashboard!E235)=0,Dashboard!E235,"")</f>
         <v/>
       </c>
       <c r="D235" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- number_of_trucks = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- number_of_busses = </v>
       </c>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B236" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C236)=0,Dashboard!C236,"")</f>
-        <v>number_of_vans</v>
+        <v>number_of_trucks</v>
       </c>
       <c r="C236" t="str">
         <f>IF(COUNTBLANK(Dashboard!E236)=0,Dashboard!E236,"")</f>
         <v/>
       </c>
       <c r="D236" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- number_of_vans = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- number_of_trucks = </v>
       </c>
     </row>
     <row r="237" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B237" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C237)=0,Dashboard!C237,"")</f>
-        <v>electric_vehicle_profile_1_share</v>
+        <v>number_of_vans</v>
       </c>
       <c r="C237" t="str">
         <f>IF(COUNTBLANK(Dashboard!E237)=0,Dashboard!E237,"")</f>
         <v/>
       </c>
       <c r="D237" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- number_of_vans = </v>
       </c>
     </row>
     <row r="238" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B238" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C238)=0,Dashboard!C238,"")</f>
-        <v>electric_vehicle_profile_2_share</v>
+        <v>electric_vehicle_profile_1_share</v>
       </c>
       <c r="C238" t="str">
         <f>IF(COUNTBLANK(Dashboard!E238)=0,Dashboard!E238,"")</f>
         <v/>
       </c>
       <c r="D238" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
       </c>
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B239" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C239)=0,Dashboard!C239,"")</f>
-        <v>electric_vehicle_profile_3_share</v>
+        <v>electric_vehicle_profile_2_share</v>
       </c>
       <c r="C239" t="str">
         <f>IF(COUNTBLANK(Dashboard!E239)=0,Dashboard!E239,"")</f>
         <v/>
       </c>
       <c r="D239" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
       </c>
     </row>
     <row r="240" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B240" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C240)=0,Dashboard!C240,"")</f>
-        <v>electric_vehicle_profile_4_share</v>
+        <v>electric_vehicle_profile_3_share</v>
       </c>
       <c r="C240" t="str">
         <f>IF(COUNTBLANK(Dashboard!E240)=0,Dashboard!E240,"")</f>
         <v/>
       </c>
       <c r="D240" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- electric_vehicle_profile_4_share = </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B241" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C241)=0,Dashboard!C241,"")</f>
-        <v>electric_vehicle_profile_5_share</v>
+        <v>electric_vehicle_profile_4_share</v>
       </c>
       <c r="C241" t="str">
         <f>IF(COUNTBLANK(Dashboard!E241)=0,Dashboard!E241,"")</f>
         <v/>
       </c>
       <c r="D241" s="86" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">- electric_vehicle_profile_4_share = </v>
+      </c>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B242" s="85" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C242)=0,Dashboard!C242,"")</f>
+        <v>electric_vehicle_profile_5_share</v>
+      </c>
+      <c r="C242" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E242)=0,Dashboard!E242,"")</f>
+        <v/>
+      </c>
+      <c r="D242" s="86" t="str">
+        <f t="shared" si="11"/>
         <v xml:space="preserve">- electric_vehicle_profile_5_share = </v>
       </c>
-    </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B242" s="85"/>
-      <c r="C242"/>
-      <c r="D242" s="86"/>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B243" s="85"/>
@@ -14442,29 +14494,29 @@
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B249" s="85" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C244)=0,Dashboard!C244,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!C245)=0,Dashboard!C245,"")</f>
         <v/>
       </c>
       <c r="C249" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E242)=0,Dashboard!E242,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E243)=0,Dashboard!E243,"")</f>
         <v/>
       </c>
       <c r="D249" s="86" t="str">
-        <f t="shared" ref="D249:D250" si="10">IF(COUNTBLANK(B249)=0,"- "&amp;B249&amp;" = "&amp;LOWER(C249),"")</f>
+        <f t="shared" ref="D249:D250" si="12">IF(COUNTBLANK(B249)=0,"- "&amp;B249&amp;" = "&amp;LOWER(C249),"")</f>
         <v/>
       </c>
     </row>
     <row r="250" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B250" s="100" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C245)=0,Dashboard!C245,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!C246)=0,Dashboard!C246,"")</f>
         <v/>
       </c>
       <c r="C250" s="101" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E245)=0,Dashboard!E245,"")</f>
+        <f>IF(COUNTBLANK(Dashboard!E246)=0,Dashboard!E246,"")</f>
         <v/>
       </c>
       <c r="D250" s="102" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -14479,10 +14531,10 @@
   <sheetPr codeName="Sheet5">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:A218"/>
+  <dimension ref="A1:A219"/>
   <sheetViews>
-    <sheetView topLeftCell="A191" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A210" sqref="A210:XFD211"/>
+    <sheetView topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A220" sqref="A220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15344,457 +15396,463 @@
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="str">
-        <f>'compile results'!D163</f>
-        <v xml:space="preserve">- lv_net_capacity_per_step = </v>
+        <f>'compile results'!D161</f>
+        <v xml:space="preserve">- captured_biogenic_co2_price = </v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="str">
         <f>'compile results'!D164</f>
-        <v xml:space="preserve">- lv_net_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- lv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="str">
         <f>'compile results'!D165</f>
-        <v xml:space="preserve">- lv_net_spare_capacity = </v>
+        <v xml:space="preserve">- lv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="str">
         <f>'compile results'!D166</f>
-        <v xml:space="preserve">- lv_net_total_costs_present = </v>
+        <v xml:space="preserve">- lv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="str">
         <f>'compile results'!D167</f>
-        <v xml:space="preserve">- lv_mv_trafo_capacity_per_step = </v>
+        <v xml:space="preserve">- lv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="str">
         <f>'compile results'!D168</f>
-        <v xml:space="preserve">- lv_mv_trafo_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- lv_mv_trafo_capacity_per_step = </v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="str">
         <f>'compile results'!D169</f>
-        <v xml:space="preserve">- lv_mv_trafo_spare_capacity = </v>
+        <v xml:space="preserve">- lv_mv_trafo_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="str">
         <f>'compile results'!D170</f>
-        <v xml:space="preserve">- lv_mv_trafo_total_costs_present = </v>
+        <v xml:space="preserve">- lv_mv_trafo_spare_capacity = </v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="str">
         <f>'compile results'!D171</f>
-        <v xml:space="preserve">- mv_net_capacity_per_step = </v>
+        <v xml:space="preserve">- lv_mv_trafo_total_costs_present = </v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="str">
         <f>'compile results'!D172</f>
-        <v xml:space="preserve">- mv_net_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- mv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="str">
         <f>'compile results'!D173</f>
-        <v xml:space="preserve">- mv_net_spare_capacity = </v>
+        <v xml:space="preserve">- mv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="str">
         <f>'compile results'!D174</f>
-        <v xml:space="preserve">- mv_net_total_costs_present = </v>
+        <v xml:space="preserve">- mv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="str">
         <f>'compile results'!D175</f>
-        <v xml:space="preserve">- mv_hv_trafo_capacity_per_step = </v>
+        <v xml:space="preserve">- mv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="str">
         <f>'compile results'!D176</f>
-        <v xml:space="preserve">- mv_hv_trafo_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- mv_hv_trafo_capacity_per_step = </v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="str">
         <f>'compile results'!D177</f>
-        <v xml:space="preserve">- mv_hv_trafo_spare_capacity = </v>
+        <v xml:space="preserve">- mv_hv_trafo_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="str">
         <f>'compile results'!D178</f>
-        <v xml:space="preserve">- mv_hv_trafo_total_costs_present = </v>
+        <v xml:space="preserve">- mv_hv_trafo_spare_capacity = </v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="str">
         <f>'compile results'!D179</f>
-        <v xml:space="preserve">- hv_net_capacity_per_step = </v>
+        <v xml:space="preserve">- mv_hv_trafo_total_costs_present = </v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="str">
         <f>'compile results'!D180</f>
-        <v xml:space="preserve">- hv_net_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- hv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="str">
         <f>'compile results'!D181</f>
-        <v xml:space="preserve">- hv_net_spare_capacity = </v>
+        <v xml:space="preserve">- hv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="str">
         <f>'compile results'!D182</f>
-        <v xml:space="preserve">- hv_net_total_costs_present = </v>
+        <v xml:space="preserve">- hv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="str">
         <f>'compile results'!D183</f>
-        <v xml:space="preserve">- interconnection_net_costs_present = </v>
+        <v xml:space="preserve">- hv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="str">
         <f>'compile results'!D184</f>
-        <v xml:space="preserve">- interconnector_capacity = </v>
+        <v xml:space="preserve">- interconnection_net_costs_present = </v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="str">
         <f>'compile results'!D185</f>
-        <v xml:space="preserve">- offshore_net_costs_present = </v>
+        <v xml:space="preserve">- interconnector_capacity = </v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="str">
         <f>'compile results'!D186</f>
-        <v xml:space="preserve">- annual_infrastructure_cost_gas = </v>
+        <v xml:space="preserve">- offshore_net_costs_present = </v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="str">
-        <f>'compile results'!D188</f>
-        <v xml:space="preserve">- heat_share_of_apartments_with_block_heating = </v>
+        <f>'compile results'!D187</f>
+        <v xml:space="preserve">- annual_infrastructure_cost_gas = </v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="str">
         <f>'compile results'!D189</f>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket = </v>
+        <v xml:space="preserve">- heat_share_of_apartments_with_block_heating = </v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="str">
         <f>'compile results'!D190</f>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket = </v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="str">
         <f>'compile results'!D191</f>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket = </v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="str">
         <f>'compile results'!D192</f>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket = </v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="str">
         <f>'compile results'!D193</f>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket = </v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="str">
         <f>'compile results'!D194</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket = </v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="str">
         <f>'compile results'!D195</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket = </v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="str">
         <f>'compile results'!D196</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket = </v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="str">
         <f>'compile results'!D197</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket = </v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="str">
         <f>'compile results'!D198</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket = </v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="str">
         <f>'compile results'!D199</f>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket = </v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="str">
         <f>'compile results'!D200</f>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="str">
         <f>'compile results'!D201</f>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="str">
         <f>'compile results'!D202</f>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="str">
         <f>'compile results'!D203</f>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="str">
         <f>'compile results'!D204</f>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="str">
         <f>'compile results'!D205</f>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="str">
         <f>'compile results'!D206</f>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="str">
         <f>'compile results'!D207</f>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="str">
         <f>'compile results'!D208</f>
-        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="str">
         <f>'compile results'!D209</f>
-        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="str">
         <f>'compile results'!D210</f>
-        <v xml:space="preserve">- heat_exchanger_station_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="str">
         <f>'compile results'!D211</f>
-        <v xml:space="preserve">- heat_lt_sub_station_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_exchanger_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="str">
         <f>'compile results'!D212</f>
-        <v xml:space="preserve">- heat_mt_sub_station_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_lt_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="str">
         <f>'compile results'!D213</f>
-        <v xml:space="preserve">- heat_ht_sub_station_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_mt_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="str">
         <f>'compile results'!D214</f>
-        <v xml:space="preserve">- heat_lt_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <v xml:space="preserve">- heat_ht_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="str">
         <f>'compile results'!D215</f>
-        <v xml:space="preserve">- heat_mt_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <v xml:space="preserve">- heat_lt_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="str">
         <f>'compile results'!D216</f>
-        <v xml:space="preserve">- heat_ht_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <v xml:space="preserve">- heat_mt_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="str">
         <f>'compile results'!D217</f>
-        <v xml:space="preserve">- heat_lt_primary_pipelines_investment_costs_per_kw = </v>
+        <v xml:space="preserve">- heat_ht_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="str">
         <f>'compile results'!D218</f>
-        <v xml:space="preserve">- heat_mt_primary_pipelines_investment_costs_per_kw = </v>
+        <v xml:space="preserve">- heat_lt_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="str">
         <f>'compile results'!D219</f>
-        <v xml:space="preserve">- heat_ht_primary_pipelines_investment_costs_per_kw = </v>
+        <v xml:space="preserve">- heat_mt_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="str">
         <f>'compile results'!D220</f>
-        <v xml:space="preserve">- heat_yearly_indoor_infrastructure_maintenance_costs_factor = </v>
+        <v xml:space="preserve">- heat_ht_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="str">
         <f>'compile results'!D221</f>
-        <v xml:space="preserve">- heat_yearly_outdoor_infrastructure_maintenance_costs_factor = </v>
+        <v xml:space="preserve">- heat_yearly_indoor_infrastructure_maintenance_costs_factor = </v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="str">
         <f>'compile results'!D222</f>
-        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <v xml:space="preserve">- heat_yearly_outdoor_infrastructure_maintenance_costs_factor = </v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="str">
         <f>'compile results'!D223</f>
-        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="str">
         <f>'compile results'!D224</f>
-        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="str">
         <f>'compile results'!D225</f>
-        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="str">
         <f>'compile results'!D226</f>
-        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="str">
         <f>'compile results'!D227</f>
-        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="str">
         <f>'compile results'!D228</f>
-        <v xml:space="preserve">- buildings_lt_heat_delivery_system_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="str">
         <f>'compile results'!D229</f>
-        <v xml:space="preserve">- buildings_mt_heat_delivery_system_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- buildings_lt_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="str">
         <f>'compile results'!D230</f>
-        <v xml:space="preserve">- buildings_ht_heat_delivery_system_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- buildings_mt_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="str">
-        <f>'compile results'!D233</f>
-        <v xml:space="preserve">- number_of_cars = </v>
+        <f>'compile results'!D231</f>
+        <v xml:space="preserve">- buildings_ht_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="str">
         <f>'compile results'!D234</f>
-        <v xml:space="preserve">- number_of_busses = </v>
+        <v xml:space="preserve">- number_of_cars = </v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="str">
         <f>'compile results'!D235</f>
-        <v xml:space="preserve">- number_of_trucks = </v>
+        <v xml:space="preserve">- number_of_busses = </v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="str">
         <f>'compile results'!D236</f>
-        <v xml:space="preserve">- number_of_vans = </v>
+        <v xml:space="preserve">- number_of_trucks = </v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="str">
         <f>'compile results'!D237</f>
-        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
+        <v xml:space="preserve">- number_of_vans = </v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="str">
         <f>'compile results'!D238</f>
-        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
+        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="str">
         <f>'compile results'!D239</f>
-        <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
+        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="str">
         <f>'compile results'!D240</f>
-        <v xml:space="preserve">- electric_vehicle_profile_4_share = </v>
+        <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="str">
         <f>'compile results'!D241</f>
+        <v xml:space="preserve">- electric_vehicle_profile_4_share = </v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" t="str">
+        <f>'compile results'!D242</f>
         <v xml:space="preserve">- electric_vehicle_profile_5_share = </v>
       </c>
     </row>

</xml_diff>

<commit_message>
Published state of ETDataset for deploy October 2025
</commit_message>
<xml_diff>
--- a/analyses/11_area_analysis.xlsx
+++ b/analyses/11_area_analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Github/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A079A0-4504-144E-9646-C818E7E8D064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B738F55A-1FE4-C54C-890F-947206C278A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10380" yWindow="-28300" windowWidth="51200" windowHeight="27160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="340">
   <si>
     <t>Unit</t>
   </si>
@@ -1069,6 +1069,15 @@
   </si>
   <si>
     <t>Add captured_biogenic_co2_price</t>
+  </si>
+  <si>
+    <t>area_per_building_residence_equivalent</t>
+  </si>
+  <si>
+    <t>July 21, 2025</t>
+  </si>
+  <si>
+    <t>Add area per building residence equivalent to analysis.</t>
   </si>
 </sst>
 </file>
@@ -3845,7 +3854,7 @@
   <dimension ref="B2:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3882,7 +3891,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D5" s="8"/>
     </row>
@@ -4073,7 +4082,7 @@
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4314,10 +4323,16 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="65"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="73"/>
+    <row r="25" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B25" s="65" t="s">
+        <v>338</v>
+      </c>
+      <c r="C25" s="72" t="s">
+        <v>339</v>
+      </c>
+      <c r="D25" s="73">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="65"/>
@@ -4345,10 +4360,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:P243"/>
+  <dimension ref="A2:P244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O162" sqref="O162"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6483,7 +6498,7 @@
         <v>0</v>
       </c>
       <c r="M84" t="str">
-        <f t="shared" ref="M84:M152" si="12">IF(L84=TRUE," ","Please set value")</f>
+        <f t="shared" ref="M84:M153" si="12">IF(L84=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N84" s="30"/>
@@ -8189,8 +8204,8 @@
     </row>
     <row r="152" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B152" s="33"/>
-      <c r="C152" t="s">
-        <v>91</v>
+      <c r="C152" s="54" t="s">
+        <v>337</v>
       </c>
       <c r="D152" t="s">
         <v>316</v>
@@ -8202,28 +8217,22 @@
       <c r="I152" s="53"/>
       <c r="J152"/>
       <c r="K152"/>
-      <c r="L152" s="38" t="b">
-        <f t="shared" ref="L152:L153" si="15">IF(COUNTBLANK(E152)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M152" t="str">
-        <f t="shared" si="12"/>
-        <v>Please set value</v>
-      </c>
+      <c r="L152" s="93"/>
+      <c r="M152"/>
       <c r="N152" s="30"/>
       <c r="O152" s="78" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="153" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="33"/>
+      <c r="C153" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="153" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="30"/>
-      <c r="C153" t="s">
-        <v>92</v>
       </c>
       <c r="D153" t="s">
         <v>316</v>
       </c>
-      <c r="E153" s="55"/>
+      <c r="E153" s="57"/>
       <c r="F153"/>
       <c r="G153"/>
       <c r="H153"/>
@@ -8231,74 +8240,74 @@
       <c r="J153"/>
       <c r="K153"/>
       <c r="L153" s="38" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="L153:L154" si="15">IF(COUNTBLANK(E153)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M153" t="str">
-        <f>IF(L153=TRUE," ","Please set value")</f>
+        <f t="shared" si="12"/>
         <v>Please set value</v>
       </c>
       <c r="N153" s="30"/>
       <c r="O153" s="78" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="154" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B154" s="30"/>
+      <c r="C154" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="154" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B154" s="30"/>
-      <c r="E154" s="50"/>
+      <c r="D154" t="s">
+        <v>316</v>
+      </c>
+      <c r="E154" s="55"/>
+      <c r="F154"/>
+      <c r="G154"/>
+      <c r="H154"/>
+      <c r="I154" s="53"/>
+      <c r="J154"/>
+      <c r="K154"/>
+      <c r="L154" s="38" t="b">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="M154" t="str">
+        <f>IF(L154=TRUE," ","Please set value")</f>
+        <v>Please set value</v>
+      </c>
       <c r="N154" s="30"/>
-      <c r="O154" s="14"/>
-    </row>
-    <row r="155" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="C155" s="4"/>
-      <c r="D155" s="4"/>
-      <c r="E155" s="51"/>
-      <c r="F155" s="4"/>
-      <c r="G155" s="4"/>
-      <c r="H155" s="4"/>
-      <c r="I155" s="4"/>
-      <c r="J155" s="4"/>
-      <c r="K155" s="4"/>
-      <c r="L155" s="4"/>
-      <c r="M155" s="4"/>
+      <c r="O154" s="78" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="155" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B155" s="30"/>
+      <c r="E155" s="50"/>
       <c r="N155" s="30"/>
       <c r="O155" s="14"/>
     </row>
     <row r="156" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="30"/>
-      <c r="C156" t="s">
-        <v>66</v>
-      </c>
-      <c r="D156" t="s">
-        <v>3</v>
-      </c>
-      <c r="E156" s="49"/>
-      <c r="F156"/>
-      <c r="G156"/>
-      <c r="H156"/>
-      <c r="I156" s="53"/>
-      <c r="J156"/>
-      <c r="K156"/>
-      <c r="L156" s="38" t="b">
-        <f t="shared" ref="L156:L161" si="16">IF(COUNTBLANK(E156)=0,TRUE,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="M156" t="str">
-        <f>IF(L156=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
+      <c r="B156" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C156" s="4"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="51"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="4"/>
+      <c r="H156" s="4"/>
+      <c r="I156" s="4"/>
+      <c r="J156" s="4"/>
+      <c r="K156" s="4"/>
+      <c r="L156" s="4"/>
+      <c r="M156" s="4"/>
       <c r="N156" s="30"/>
-      <c r="O156" s="14" t="s">
-        <v>66</v>
-      </c>
+      <c r="O156" s="14"/>
     </row>
     <row r="157" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B157" s="30"/>
       <c r="C157" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="D157" t="s">
         <v>3</v>
@@ -8311,22 +8320,22 @@
       <c r="J157"/>
       <c r="K157"/>
       <c r="L157" s="38" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="L157:L162" si="16">IF(COUNTBLANK(E157)=0,TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="M157" t="str">
-        <f t="shared" ref="M157:M158" si="17">IF(L157=TRUE," ","Please set value")</f>
+        <f>IF(L157=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N157" s="30"/>
       <c r="O157" s="14" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
     </row>
     <row r="158" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B158" s="30"/>
       <c r="C158" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D158" t="s">
         <v>3</v>
@@ -8343,23 +8352,23 @@
         <v>0</v>
       </c>
       <c r="M158" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="M158:M159" si="17">IF(L158=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N158" s="30"/>
       <c r="O158" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="159" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B159" s="30"/>
       <c r="C159" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="D159" t="s">
-        <v>281</v>
-      </c>
-      <c r="E159" s="60"/>
+        <v>3</v>
+      </c>
+      <c r="E159" s="49"/>
       <c r="F159"/>
       <c r="G159"/>
       <c r="H159"/>
@@ -8371,23 +8380,23 @@
         <v>0</v>
       </c>
       <c r="M159" t="str">
-        <f t="shared" ref="M159:M161" si="18">IF(L159=TRUE," ","Please set value")</f>
+        <f t="shared" si="17"/>
         <v>Please set value</v>
       </c>
       <c r="N159" s="30"/>
       <c r="O159" s="14" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
     </row>
     <row r="160" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B160" s="30"/>
       <c r="C160" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D160" t="s">
-        <v>317</v>
-      </c>
-      <c r="E160" s="56"/>
+        <v>281</v>
+      </c>
+      <c r="E160" s="60"/>
       <c r="F160"/>
       <c r="G160"/>
       <c r="H160"/>
@@ -8399,18 +8408,18 @@
         <v>0</v>
       </c>
       <c r="M160" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="M160:M162" si="18">IF(L160=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N160" s="30"/>
       <c r="O160" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="161" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B161" s="30"/>
       <c r="C161" t="s">
-        <v>334</v>
+        <v>68</v>
       </c>
       <c r="D161" t="s">
         <v>317</v>
@@ -8432,78 +8441,78 @@
       </c>
       <c r="N161" s="30"/>
       <c r="O161" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="162" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="30"/>
+      <c r="C162" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="162" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B162" s="40"/>
-      <c r="C162" s="11"/>
-      <c r="D162" s="11"/>
-      <c r="E162" s="52"/>
-      <c r="F162" s="11"/>
-      <c r="G162" s="11"/>
-      <c r="H162" s="11"/>
-      <c r="I162" s="11"/>
-      <c r="J162" s="11"/>
-      <c r="K162" s="11"/>
-      <c r="L162" s="11"/>
-      <c r="M162" s="11"/>
+      <c r="D162" t="s">
+        <v>317</v>
+      </c>
+      <c r="E162" s="56"/>
+      <c r="F162"/>
+      <c r="G162"/>
+      <c r="H162"/>
+      <c r="I162" s="53"/>
+      <c r="J162"/>
+      <c r="K162"/>
+      <c r="L162" s="38" t="b">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M162" t="str">
+        <f t="shared" si="18"/>
+        <v>Please set value</v>
+      </c>
       <c r="N162" s="30"/>
-      <c r="O162" s="14"/>
-    </row>
-    <row r="163" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C163" s="4"/>
-      <c r="D163" s="4"/>
-      <c r="E163" s="51"/>
-      <c r="F163" s="4"/>
-      <c r="G163" s="4"/>
-      <c r="H163" s="4"/>
-      <c r="I163" s="4"/>
-      <c r="J163" s="4"/>
-      <c r="K163" s="4"/>
-      <c r="L163" s="4"/>
-      <c r="M163" s="4"/>
+      <c r="O162" s="14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="163" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B163" s="40"/>
+      <c r="C163" s="11"/>
+      <c r="D163" s="11"/>
+      <c r="E163" s="52"/>
+      <c r="F163" s="11"/>
+      <c r="G163" s="11"/>
+      <c r="H163" s="11"/>
+      <c r="I163" s="11"/>
+      <c r="J163" s="11"/>
+      <c r="K163" s="11"/>
+      <c r="L163" s="11"/>
+      <c r="M163" s="11"/>
       <c r="N163" s="30"/>
       <c r="O163" s="14"/>
     </row>
     <row r="164" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="30"/>
-      <c r="C164" t="s">
-        <v>122</v>
-      </c>
-      <c r="D164" t="s">
-        <v>137</v>
-      </c>
-      <c r="E164" s="49"/>
-      <c r="F164"/>
-      <c r="G164" s="54"/>
-      <c r="H164"/>
-      <c r="I164" s="53"/>
-      <c r="J164"/>
-      <c r="K164"/>
-      <c r="L164" s="38" t="b">
-        <f>IF(COUNTBLANK(E164)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M164" t="str">
-        <f t="shared" ref="M164:M169" si="19">IF(L164=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
+      <c r="B164" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C164" s="4"/>
+      <c r="D164" s="4"/>
+      <c r="E164" s="51"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
+      <c r="H164" s="4"/>
+      <c r="I164" s="4"/>
+      <c r="J164" s="4"/>
+      <c r="K164" s="4"/>
+      <c r="L164" s="4"/>
+      <c r="M164" s="4"/>
       <c r="N164" s="30"/>
-      <c r="O164" s="78" t="s">
-        <v>122</v>
-      </c>
+      <c r="O164" s="14"/>
     </row>
     <row r="165" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B165" s="30"/>
       <c r="C165" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D165" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E165" s="49"/>
       <c r="F165"/>
@@ -8513,25 +8522,25 @@
       <c r="J165"/>
       <c r="K165"/>
       <c r="L165" s="38" t="b">
-        <f t="shared" ref="L165:L169" si="20">IF(COUNTBLANK(E165)=1,FALSE,TRUE)</f>
+        <f>IF(COUNTBLANK(E165)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M165" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="M165:M170" si="19">IF(L165=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N165" s="30"/>
       <c r="O165" s="78" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="166" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B166" s="30"/>
       <c r="C166" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D166" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E166" s="49"/>
       <c r="F166"/>
@@ -8541,7 +8550,7 @@
       <c r="J166"/>
       <c r="K166"/>
       <c r="L166" s="38" t="b">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="L166:L170" si="20">IF(COUNTBLANK(E166)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M166" t="str">
@@ -8550,16 +8559,16 @@
       </c>
       <c r="N166" s="30"/>
       <c r="O166" s="78" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="167" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B167" s="30"/>
       <c r="C167" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D167" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="E167" s="49"/>
       <c r="F167"/>
@@ -8578,16 +8587,16 @@
       </c>
       <c r="N167" s="30"/>
       <c r="O167" s="78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="168" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B168" s="30"/>
       <c r="C168" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D168" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E168" s="49"/>
       <c r="F168"/>
@@ -8606,16 +8615,16 @@
       </c>
       <c r="N168" s="30"/>
       <c r="O168" s="78" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="169" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B169" s="30"/>
       <c r="C169" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D169" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E169" s="49"/>
       <c r="F169"/>
@@ -8634,44 +8643,44 @@
       </c>
       <c r="N169" s="30"/>
       <c r="O169" s="78" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="170" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B170" s="30"/>
       <c r="C170" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D170" t="s">
-        <v>34</v>
-      </c>
-      <c r="E170" s="98"/>
+        <v>138</v>
+      </c>
+      <c r="E170" s="49"/>
       <c r="F170"/>
       <c r="G170" s="54"/>
       <c r="H170"/>
-      <c r="I170" s="94"/>
+      <c r="I170" s="53"/>
       <c r="J170"/>
       <c r="K170"/>
       <c r="L170" s="38" t="b">
-        <f t="shared" ref="L170:L186" si="21">IF(COUNTBLANK(E170)=1,FALSE,TRUE)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M170" t="str">
-        <f t="shared" ref="M170:M231" si="22">IF(L170=TRUE," ","Please set value")</f>
+        <f t="shared" si="19"/>
         <v>Please set value</v>
       </c>
       <c r="N170" s="30"/>
       <c r="O170" s="78" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="171" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B171" s="30"/>
       <c r="C171" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D171" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="E171" s="98"/>
       <c r="F171"/>
@@ -8681,25 +8690,25 @@
       <c r="J171"/>
       <c r="K171"/>
       <c r="L171" s="38" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="L171:L187" si="21">IF(COUNTBLANK(E171)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M171" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="M171:M232" si="22">IF(L171=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N171" s="30"/>
       <c r="O171" s="78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="172" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B172" s="30"/>
       <c r="C172" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D172" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E172" s="98"/>
       <c r="F172"/>
@@ -8718,16 +8727,16 @@
       </c>
       <c r="N172" s="30"/>
       <c r="O172" s="78" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="173" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B173" s="30"/>
       <c r="C173" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D173" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E173" s="98"/>
       <c r="F173"/>
@@ -8746,16 +8755,16 @@
       </c>
       <c r="N173" s="30"/>
       <c r="O173" s="78" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="174" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B174" s="30"/>
       <c r="C174" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D174" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E174" s="98"/>
       <c r="F174"/>
@@ -8765,7 +8774,7 @@
       <c r="J174"/>
       <c r="K174"/>
       <c r="L174" s="38" t="b">
-        <f>IF(COUNTBLANK(E174)=1,FALSE,TRUE)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M174" t="str">
@@ -8774,16 +8783,16 @@
       </c>
       <c r="N174" s="30"/>
       <c r="O174" s="78" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="175" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B175" s="30"/>
       <c r="C175" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D175" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="E175" s="98"/>
       <c r="F175"/>
@@ -8793,7 +8802,7 @@
       <c r="J175"/>
       <c r="K175"/>
       <c r="L175" s="38" t="b">
-        <f t="shared" si="21"/>
+        <f>IF(COUNTBLANK(E175)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M175" t="str">
@@ -8802,16 +8811,16 @@
       </c>
       <c r="N175" s="30"/>
       <c r="O175" s="78" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="176" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B176" s="30"/>
       <c r="C176" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D176" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E176" s="98"/>
       <c r="F176"/>
@@ -8830,16 +8839,16 @@
       </c>
       <c r="N176" s="30"/>
       <c r="O176" s="78" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="177" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B177" s="30"/>
       <c r="C177" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D177" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E177" s="98"/>
       <c r="F177"/>
@@ -8858,16 +8867,16 @@
       </c>
       <c r="N177" s="30"/>
       <c r="O177" s="78" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="178" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B178" s="30"/>
       <c r="C178" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D178" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E178" s="98"/>
       <c r="F178"/>
@@ -8886,16 +8895,16 @@
       </c>
       <c r="N178" s="30"/>
       <c r="O178" s="78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="179" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B179" s="30"/>
       <c r="C179" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D179" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="E179" s="98"/>
       <c r="F179"/>
@@ -8914,16 +8923,16 @@
       </c>
       <c r="N179" s="30"/>
       <c r="O179" s="78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="180" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B180" s="30"/>
       <c r="C180" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D180" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E180" s="98"/>
       <c r="F180"/>
@@ -8942,16 +8951,16 @@
       </c>
       <c r="N180" s="30"/>
       <c r="O180" s="78" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="181" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B181" s="30"/>
       <c r="C181" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D181" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E181" s="98"/>
       <c r="F181"/>
@@ -8970,16 +8979,16 @@
       </c>
       <c r="N181" s="30"/>
       <c r="O181" s="78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="182" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B182" s="30"/>
       <c r="C182" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D182" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E182" s="98"/>
       <c r="F182"/>
@@ -8998,16 +9007,16 @@
       </c>
       <c r="N182" s="30"/>
       <c r="O182" s="78" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="183" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B183" s="30"/>
       <c r="C183" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D183" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="E183" s="98"/>
       <c r="F183"/>
@@ -9026,13 +9035,13 @@
       </c>
       <c r="N183" s="30"/>
       <c r="O183" s="78" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="184" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B184" s="30"/>
       <c r="C184" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D184" t="s">
         <v>138</v>
@@ -9054,16 +9063,16 @@
       </c>
       <c r="N184" s="30"/>
       <c r="O184" s="78" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="185" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B185" s="30"/>
       <c r="C185" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D185" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E185" s="98"/>
       <c r="F185"/>
@@ -9082,16 +9091,16 @@
       </c>
       <c r="N185" s="30"/>
       <c r="O185" s="78" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="186" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B186" s="30"/>
       <c r="C186" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="D186" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E186" s="98"/>
       <c r="F186"/>
@@ -9110,26 +9119,26 @@
       </c>
       <c r="N186" s="30"/>
       <c r="O186" s="78" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
     </row>
     <row r="187" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B187" s="30"/>
       <c r="C187" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="D187" t="s">
         <v>138</v>
       </c>
-      <c r="E187" s="53"/>
+      <c r="E187" s="98"/>
       <c r="F187"/>
       <c r="G187" s="54"/>
       <c r="H187"/>
-      <c r="I187" s="53"/>
+      <c r="I187" s="94"/>
       <c r="J187"/>
       <c r="K187"/>
       <c r="L187" s="38" t="b">
-        <f>IF(COUNTBLANK(E187)=1,FALSE,TRUE)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M187" t="str">
@@ -9138,60 +9147,60 @@
       </c>
       <c r="N187" s="30"/>
       <c r="O187" s="78" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
     </row>
     <row r="188" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B188" s="30"/>
-      <c r="C188"/>
-      <c r="D188"/>
-      <c r="E188"/>
+      <c r="C188" t="s">
+        <v>69</v>
+      </c>
+      <c r="D188" t="s">
+        <v>138</v>
+      </c>
+      <c r="E188" s="53"/>
       <c r="F188"/>
       <c r="G188" s="54"/>
       <c r="H188"/>
-      <c r="I188"/>
+      <c r="I188" s="53"/>
       <c r="J188"/>
       <c r="K188"/>
-      <c r="L188"/>
-      <c r="M188"/>
+      <c r="L188" s="38" t="b">
+        <f>IF(COUNTBLANK(E188)=1,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="M188" t="str">
+        <f t="shared" si="22"/>
+        <v>Please set value</v>
+      </c>
       <c r="N188" s="30"/>
-      <c r="O188" s="78"/>
+      <c r="O188" s="78" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="189" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B189" s="30"/>
-      <c r="C189" t="s">
-        <v>154</v>
-      </c>
-      <c r="D189" t="s">
-        <v>169</v>
-      </c>
-      <c r="E189" s="53"/>
+      <c r="C189"/>
+      <c r="D189"/>
+      <c r="E189"/>
       <c r="F189"/>
       <c r="G189" s="54"/>
       <c r="H189"/>
-      <c r="I189" s="53"/>
+      <c r="I189"/>
       <c r="J189"/>
       <c r="K189"/>
-      <c r="L189" s="38" t="b">
-        <f>IF(COUNTBLANK(E189)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M189" t="str">
-        <f t="shared" si="22"/>
-        <v>Please set value</v>
-      </c>
+      <c r="L189"/>
+      <c r="M189"/>
       <c r="N189" s="30"/>
-      <c r="O189" t="s">
-        <v>154</v>
-      </c>
+      <c r="O189" s="78"/>
     </row>
     <row r="190" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B190" s="30"/>
       <c r="C190" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D190" t="s">
-        <v>236</v>
+        <v>169</v>
       </c>
       <c r="E190" s="53"/>
       <c r="F190"/>
@@ -9201,7 +9210,7 @@
       <c r="J190"/>
       <c r="K190"/>
       <c r="L190" s="38" t="b">
-        <f t="shared" ref="L190:L231" si="23">IF(COUNTBLANK(E190)=1,FALSE,TRUE)</f>
+        <f>IF(COUNTBLANK(E190)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M190" t="str">
@@ -9210,13 +9219,13 @@
       </c>
       <c r="N190" s="30"/>
       <c r="O190" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="191" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B191" s="30"/>
       <c r="C191" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D191" t="s">
         <v>236</v>
@@ -9229,7 +9238,7 @@
       <c r="J191"/>
       <c r="K191"/>
       <c r="L191" s="38" t="b">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="L191:L232" si="23">IF(COUNTBLANK(E191)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M191" t="str">
@@ -9238,13 +9247,13 @@
       </c>
       <c r="N191" s="30"/>
       <c r="O191" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="192" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B192" s="30"/>
       <c r="C192" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D192" t="s">
         <v>236</v>
@@ -9266,13 +9275,13 @@
       </c>
       <c r="N192" s="30"/>
       <c r="O192" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="193" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B193" s="30"/>
       <c r="C193" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D193" t="s">
         <v>236</v>
@@ -9294,13 +9303,13 @@
       </c>
       <c r="N193" s="30"/>
       <c r="O193" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="194" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B194" s="30"/>
       <c r="C194" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D194" t="s">
         <v>236</v>
@@ -9322,13 +9331,13 @@
       </c>
       <c r="N194" s="30"/>
       <c r="O194" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="195" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B195" s="30"/>
       <c r="C195" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D195" t="s">
         <v>236</v>
@@ -9350,13 +9359,13 @@
       </c>
       <c r="N195" s="30"/>
       <c r="O195" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="196" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B196" s="30"/>
       <c r="C196" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D196" t="s">
         <v>236</v>
@@ -9378,13 +9387,13 @@
       </c>
       <c r="N196" s="30"/>
       <c r="O196" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="197" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B197" s="30"/>
       <c r="C197" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D197" t="s">
         <v>236</v>
@@ -9406,13 +9415,13 @@
       </c>
       <c r="N197" s="30"/>
       <c r="O197" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="198" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B198" s="30"/>
       <c r="C198" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D198" t="s">
         <v>236</v>
@@ -9434,13 +9443,13 @@
       </c>
       <c r="N198" s="30"/>
       <c r="O198" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="199" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B199" s="30"/>
       <c r="C199" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D199" t="s">
         <v>236</v>
@@ -9453,25 +9462,25 @@
       <c r="J199"/>
       <c r="K199"/>
       <c r="L199" s="38" t="b">
-        <f t="shared" ref="L199:L223" si="24">IF(COUNTBLANK(E199)=1,FALSE,TRUE)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="M199" t="str">
-        <f t="shared" ref="M199:M223" si="25">IF(L199=TRUE," ","Please set value")</f>
+        <f t="shared" si="22"/>
         <v>Please set value</v>
       </c>
       <c r="N199" s="30"/>
       <c r="O199" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="200" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B200" s="30"/>
       <c r="C200" t="s">
-        <v>235</v>
+        <v>164</v>
       </c>
       <c r="D200" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E200" s="53"/>
       <c r="F200"/>
@@ -9481,22 +9490,22 @@
       <c r="J200"/>
       <c r="K200"/>
       <c r="L200" s="38" t="b">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="L200:L224" si="24">IF(COUNTBLANK(E200)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M200" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="M200:M224" si="25">IF(L200=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N200" s="30"/>
       <c r="O200" t="s">
-        <v>235</v>
+        <v>164</v>
       </c>
     </row>
     <row r="201" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B201" s="30"/>
       <c r="C201" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D201" t="s">
         <v>237</v>
@@ -9518,13 +9527,13 @@
       </c>
       <c r="N201" s="30"/>
       <c r="O201" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="202" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B202" s="30"/>
       <c r="C202" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D202" t="s">
         <v>237</v>
@@ -9546,13 +9555,13 @@
       </c>
       <c r="N202" s="30"/>
       <c r="O202" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="203" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B203" s="30"/>
       <c r="C203" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D203" t="s">
         <v>237</v>
@@ -9574,13 +9583,13 @@
       </c>
       <c r="N203" s="30"/>
       <c r="O203" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="204" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B204" s="30"/>
       <c r="C204" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D204" t="s">
         <v>237</v>
@@ -9602,13 +9611,13 @@
       </c>
       <c r="N204" s="30"/>
       <c r="O204" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="205" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B205" s="30"/>
       <c r="C205" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D205" t="s">
         <v>237</v>
@@ -9630,13 +9639,13 @@
       </c>
       <c r="N205" s="30"/>
       <c r="O205" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="206" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B206" s="30"/>
       <c r="C206" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D206" t="s">
         <v>237</v>
@@ -9658,13 +9667,13 @@
       </c>
       <c r="N206" s="30"/>
       <c r="O206" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="207" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B207" s="30"/>
       <c r="C207" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D207" t="s">
         <v>237</v>
@@ -9686,13 +9695,13 @@
       </c>
       <c r="N207" s="30"/>
       <c r="O207" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="208" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B208" s="30"/>
       <c r="C208" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D208" t="s">
         <v>237</v>
@@ -9714,16 +9723,16 @@
       </c>
       <c r="N208" s="30"/>
       <c r="O208" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="209" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B209" s="30"/>
       <c r="C209" t="s">
-        <v>165</v>
+        <v>227</v>
       </c>
       <c r="D209" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E209" s="53"/>
       <c r="F209"/>
@@ -9742,16 +9751,16 @@
       </c>
       <c r="N209" s="30"/>
       <c r="O209" t="s">
-        <v>165</v>
+        <v>227</v>
       </c>
     </row>
     <row r="210" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B210" s="30"/>
       <c r="C210" t="s">
-        <v>226</v>
+        <v>165</v>
       </c>
       <c r="D210" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E210" s="53"/>
       <c r="F210"/>
@@ -9770,16 +9779,16 @@
       </c>
       <c r="N210" s="30"/>
       <c r="O210" t="s">
-        <v>226</v>
+        <v>165</v>
       </c>
     </row>
     <row r="211" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B211" s="30"/>
       <c r="C211" t="s">
-        <v>166</v>
+        <v>226</v>
       </c>
       <c r="D211" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E211" s="53"/>
       <c r="F211"/>
@@ -9798,13 +9807,13 @@
       </c>
       <c r="N211" s="30"/>
       <c r="O211" t="s">
-        <v>166</v>
+        <v>226</v>
       </c>
     </row>
     <row r="212" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B212" s="30"/>
       <c r="C212" t="s">
-        <v>225</v>
+        <v>166</v>
       </c>
       <c r="D212" t="s">
         <v>238</v>
@@ -9826,13 +9835,13 @@
       </c>
       <c r="N212" s="30"/>
       <c r="O212" t="s">
-        <v>225</v>
+        <v>166</v>
       </c>
     </row>
     <row r="213" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B213" s="30"/>
       <c r="C213" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D213" t="s">
         <v>238</v>
@@ -9854,13 +9863,13 @@
       </c>
       <c r="N213" s="30"/>
       <c r="O213" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="214" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B214" s="30"/>
       <c r="C214" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D214" t="s">
         <v>238</v>
@@ -9882,16 +9891,16 @@
       </c>
       <c r="N214" s="30"/>
       <c r="O214" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="215" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B215" s="30"/>
       <c r="C215" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D215" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E215" s="53"/>
       <c r="F215"/>
@@ -9910,13 +9919,13 @@
       </c>
       <c r="N215" s="30"/>
       <c r="O215" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="216" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B216" s="30"/>
       <c r="C216" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D216" t="s">
         <v>239</v>
@@ -9938,13 +9947,13 @@
       </c>
       <c r="N216" s="30"/>
       <c r="O216" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="217" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B217" s="30"/>
       <c r="C217" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D217" t="s">
         <v>239</v>
@@ -9966,16 +9975,16 @@
       </c>
       <c r="N217" s="30"/>
       <c r="O217" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="218" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B218" s="30"/>
       <c r="C218" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D218" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E218" s="53"/>
       <c r="F218"/>
@@ -9994,13 +10003,13 @@
       </c>
       <c r="N218" s="30"/>
       <c r="O218" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="219" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B219" s="30"/>
       <c r="C219" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D219" t="s">
         <v>238</v>
@@ -10022,13 +10031,13 @@
       </c>
       <c r="N219" s="30"/>
       <c r="O219" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="220" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B220" s="30"/>
       <c r="C220" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D220" t="s">
         <v>238</v>
@@ -10050,16 +10059,16 @@
       </c>
       <c r="N220" s="30"/>
       <c r="O220" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="221" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B221" s="30"/>
       <c r="C221" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="D221" t="s">
-        <v>170</v>
+        <v>238</v>
       </c>
       <c r="E221" s="53"/>
       <c r="F221"/>
@@ -10078,13 +10087,13 @@
       </c>
       <c r="N221" s="30"/>
       <c r="O221" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
     </row>
     <row r="222" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B222" s="30"/>
       <c r="C222" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D222" t="s">
         <v>170</v>
@@ -10106,16 +10115,16 @@
       </c>
       <c r="N222" s="30"/>
       <c r="O222" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="223" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B223" s="30"/>
       <c r="C223" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="D223" t="s">
-        <v>237</v>
+        <v>170</v>
       </c>
       <c r="E223" s="53"/>
       <c r="F223"/>
@@ -10134,13 +10143,13 @@
       </c>
       <c r="N223" s="30"/>
       <c r="O223" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="224" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B224" s="30"/>
       <c r="C224" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D224" t="s">
         <v>237</v>
@@ -10153,22 +10162,22 @@
       <c r="J224"/>
       <c r="K224"/>
       <c r="L224" s="38" t="b">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M224" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>Please set value</v>
       </c>
       <c r="N224" s="30"/>
       <c r="O224" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="225" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B225" s="30"/>
       <c r="C225" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D225" t="s">
         <v>237</v>
@@ -10190,13 +10199,13 @@
       </c>
       <c r="N225" s="30"/>
       <c r="O225" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="226" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B226" s="30"/>
       <c r="C226" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D226" t="s">
         <v>237</v>
@@ -10218,13 +10227,13 @@
       </c>
       <c r="N226" s="30"/>
       <c r="O226" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="227" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B227" s="30"/>
       <c r="C227" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D227" t="s">
         <v>237</v>
@@ -10246,13 +10255,13 @@
       </c>
       <c r="N227" s="30"/>
       <c r="O227" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="228" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B228" s="30"/>
       <c r="C228" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D228" t="s">
         <v>237</v>
@@ -10274,13 +10283,13 @@
       </c>
       <c r="N228" s="30"/>
       <c r="O228" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="229" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B229" s="30"/>
       <c r="C229" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D229" t="s">
         <v>237</v>
@@ -10302,13 +10311,13 @@
       </c>
       <c r="N229" s="30"/>
       <c r="O229" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="230" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B230" s="30"/>
       <c r="C230" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D230" t="s">
         <v>237</v>
@@ -10330,13 +10339,13 @@
       </c>
       <c r="N230" s="30"/>
       <c r="O230" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="231" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B231" s="30"/>
       <c r="C231" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D231" t="s">
         <v>237</v>
@@ -10358,63 +10367,65 @@
       </c>
       <c r="N231" s="30"/>
       <c r="O231" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="232" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B232" s="30"/>
+      <c r="C232" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="232" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B232" s="30"/>
-      <c r="E232" s="50"/>
+      <c r="D232" t="s">
+        <v>237</v>
+      </c>
+      <c r="E232" s="53"/>
+      <c r="F232"/>
+      <c r="G232" s="54"/>
+      <c r="H232"/>
+      <c r="I232" s="53"/>
+      <c r="J232"/>
+      <c r="K232"/>
+      <c r="L232" s="38" t="b">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="M232" t="str">
+        <f t="shared" si="22"/>
+        <v>Please set value</v>
+      </c>
       <c r="N232" s="30"/>
-      <c r="O232" s="14"/>
-    </row>
-    <row r="233" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B233" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="C233" s="4"/>
-      <c r="D233" s="4"/>
-      <c r="E233" s="51"/>
-      <c r="F233" s="4"/>
-      <c r="G233" s="4"/>
-      <c r="H233" s="4"/>
-      <c r="I233" s="4"/>
-      <c r="J233" s="4"/>
-      <c r="K233" s="4"/>
-      <c r="L233" s="4"/>
-      <c r="M233" s="4"/>
+      <c r="O232" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="233" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B233" s="30"/>
+      <c r="E233" s="50"/>
       <c r="N233" s="30"/>
       <c r="O233" s="14"/>
     </row>
     <row r="234" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B234" s="30"/>
-      <c r="C234" t="s">
-        <v>98</v>
-      </c>
-      <c r="D234"/>
-      <c r="E234" s="49"/>
-      <c r="F234"/>
-      <c r="G234" s="54"/>
-      <c r="H234"/>
-      <c r="I234" s="53"/>
-      <c r="J234"/>
-      <c r="K234"/>
-      <c r="L234" s="38" t="b">
-        <f>IF(COUNTBLANK(E234)=1,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M234" t="str">
-        <f t="shared" ref="M234:M242" si="26">IF(L234=TRUE," ","Please set value")</f>
-        <v>Please set value</v>
-      </c>
+      <c r="B234" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C234" s="4"/>
+      <c r="D234" s="4"/>
+      <c r="E234" s="51"/>
+      <c r="F234" s="4"/>
+      <c r="G234" s="4"/>
+      <c r="H234" s="4"/>
+      <c r="I234" s="4"/>
+      <c r="J234" s="4"/>
+      <c r="K234" s="4"/>
+      <c r="L234" s="4"/>
+      <c r="M234" s="4"/>
       <c r="N234" s="30"/>
-      <c r="O234" s="14" t="s">
-        <v>98</v>
-      </c>
+      <c r="O234" s="14"/>
     </row>
     <row r="235" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B235" s="30"/>
       <c r="C235" t="s">
-        <v>197</v>
+        <v>98</v>
       </c>
       <c r="D235"/>
       <c r="E235" s="49"/>
@@ -10429,18 +10440,18 @@
         <v>0</v>
       </c>
       <c r="M235" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="M235:M243" si="26">IF(L235=TRUE," ","Please set value")</f>
         <v>Please set value</v>
       </c>
       <c r="N235" s="30"/>
       <c r="O235" s="14" t="s">
-        <v>197</v>
+        <v>98</v>
       </c>
     </row>
     <row r="236" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B236" s="30"/>
       <c r="C236" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D236"/>
       <c r="E236" s="49"/>
@@ -10460,13 +10471,13 @@
       </c>
       <c r="N236" s="30"/>
       <c r="O236" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="237" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B237" s="30"/>
       <c r="C237" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D237"/>
       <c r="E237" s="49"/>
@@ -10486,16 +10497,16 @@
       </c>
       <c r="N237" s="30"/>
       <c r="O237" s="14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="238" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B238" s="30"/>
       <c r="C238" t="s">
-        <v>105</v>
+        <v>198</v>
       </c>
       <c r="D238"/>
-      <c r="E238" s="60"/>
+      <c r="E238" s="49"/>
       <c r="F238"/>
       <c r="G238" s="54"/>
       <c r="H238"/>
@@ -10503,7 +10514,7 @@
       <c r="J238"/>
       <c r="K238"/>
       <c r="L238" s="38" t="b">
-        <f t="shared" ref="L238:L242" si="27">IF(COUNTBLANK(E238)=1,FALSE,TRUE)</f>
+        <f>IF(COUNTBLANK(E238)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M238" t="str">
@@ -10512,24 +10523,24 @@
       </c>
       <c r="N238" s="30"/>
       <c r="O238" s="14" t="s">
-        <v>105</v>
+        <v>198</v>
       </c>
     </row>
     <row r="239" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B239" s="30"/>
       <c r="C239" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D239"/>
-      <c r="E239" s="99"/>
+      <c r="E239" s="60"/>
       <c r="F239"/>
       <c r="G239" s="54"/>
       <c r="H239"/>
-      <c r="I239" s="95"/>
+      <c r="I239" s="53"/>
       <c r="J239"/>
       <c r="K239"/>
       <c r="L239" s="38" t="b">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="L239:L243" si="27">IF(COUNTBLANK(E239)=1,FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="M239" t="str">
@@ -10538,13 +10549,13 @@
       </c>
       <c r="N239" s="30"/>
       <c r="O239" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="240" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B240" s="30"/>
       <c r="C240" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D240"/>
       <c r="E240" s="99"/>
@@ -10564,13 +10575,13 @@
       </c>
       <c r="N240" s="30"/>
       <c r="O240" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="241" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B241" s="30"/>
       <c r="C241" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="D241"/>
       <c r="E241" s="99"/>
@@ -10590,13 +10601,13 @@
       </c>
       <c r="N241" s="30"/>
       <c r="O241" s="14" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
     </row>
     <row r="242" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B242" s="30"/>
       <c r="C242" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D242"/>
       <c r="E242" s="99"/>
@@ -10616,23 +10627,49 @@
       </c>
       <c r="N242" s="30"/>
       <c r="O242" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="243" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B243" s="30"/>
+      <c r="C243" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="243" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B243" s="41"/>
-      <c r="C243" s="34"/>
-      <c r="D243" s="34"/>
-      <c r="E243" s="48"/>
-      <c r="F243" s="34"/>
-      <c r="G243" s="34"/>
-      <c r="H243" s="34"/>
-      <c r="I243" s="34"/>
-      <c r="J243" s="34"/>
-      <c r="K243" s="34"/>
-      <c r="L243" s="34"/>
-      <c r="M243" s="34"/>
+      <c r="D243"/>
+      <c r="E243" s="99"/>
+      <c r="F243"/>
+      <c r="G243" s="54"/>
+      <c r="H243"/>
+      <c r="I243" s="95"/>
+      <c r="J243"/>
+      <c r="K243"/>
+      <c r="L243" s="38" t="b">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="M243" t="str">
+        <f t="shared" si="26"/>
+        <v>Please set value</v>
+      </c>
       <c r="N243" s="30"/>
+      <c r="O243" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="244" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B244" s="41"/>
+      <c r="C244" s="34"/>
+      <c r="D244" s="34"/>
+      <c r="E244" s="48"/>
+      <c r="F244" s="34"/>
+      <c r="G244" s="34"/>
+      <c r="H244" s="34"/>
+      <c r="I244" s="34"/>
+      <c r="J244" s="34"/>
+      <c r="K244" s="34"/>
+      <c r="L244" s="34"/>
+      <c r="M244" s="34"/>
+      <c r="N244" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10648,17 +10685,17 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L84:L153 L189:L231 L156:L161">
+  <conditionalFormatting sqref="L84:L154 L157:L162 L190:L232">
     <cfRule type="cellIs" dxfId="2" priority="23" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L164:L187">
+  <conditionalFormatting sqref="L165:L188">
     <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L234:L242">
+  <conditionalFormatting sqref="L235:L243">
     <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -10668,7 +10705,7 @@
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E83 E50:E51 E55:E59 E154:E243" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E83 E50:E51 E55:E59 E155:E244" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -11158,10 +11195,10 @@
   <sheetPr codeName="Sheet4">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:D250"/>
+  <dimension ref="B1:D251"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B247" sqref="B247"/>
+    <sheetView topLeftCell="A102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12918,7 +12955,7 @@
         <v/>
       </c>
       <c r="D132" s="86" t="str">
-        <f t="shared" ref="D132:D195" si="8">IF(COUNTBLANK(B132)=0,"- "&amp;B132&amp;" = "&amp;LOWER(C132),"")</f>
+        <f t="shared" ref="D132:D158" si="8">IF(COUNTBLANK(B132)=0,"- "&amp;B132&amp;" = "&amp;LOWER(C132),"")</f>
         <v xml:space="preserve">- typical_useful_demand_for_space_heating_detached_houses_before_1945 = </v>
       </c>
     </row>
@@ -13189,9 +13226,8 @@
       </c>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B152" s="85" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C152)=0,Dashboard!C152,"")</f>
-        <v>residences_roof_surface_available_for_pv</v>
+      <c r="B152" s="85" t="s">
+        <v>337</v>
       </c>
       <c r="C152" t="str">
         <f>IF(COUNTBLANK(Dashboard!E152)=0,Dashboard!E152,"")</f>
@@ -13199,13 +13235,13 @@
       </c>
       <c r="D152" s="86" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">- residences_roof_surface_available_for_pv = </v>
+        <v xml:space="preserve">- area_per_building_residence_equivalent = </v>
       </c>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B153" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C153)=0,Dashboard!C153,"")</f>
-        <v>buildings_roof_surface_available_for_pv</v>
+        <v>residences_roof_surface_available_for_pv</v>
       </c>
       <c r="C153" t="str">
         <f>IF(COUNTBLANK(Dashboard!E153)=0,Dashboard!E153,"")</f>
@@ -13213,13 +13249,13 @@
       </c>
       <c r="D153" s="86" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">- buildings_roof_surface_available_for_pv = </v>
+        <v xml:space="preserve">- residences_roof_surface_available_for_pv = </v>
       </c>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B154" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C154)=0,Dashboard!C154,"")</f>
-        <v/>
+        <v>buildings_roof_surface_available_for_pv</v>
       </c>
       <c r="C154" t="str">
         <f>IF(COUNTBLANK(Dashboard!E154)=0,Dashboard!E154,"")</f>
@@ -13227,7 +13263,7 @@
       </c>
       <c r="D154" s="86" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v xml:space="preserve">- buildings_roof_surface_available_for_pv = </v>
       </c>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.2">
@@ -13247,7 +13283,7 @@
     <row r="156" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B156" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C156)=0,Dashboard!C156,"")</f>
-        <v>co2_emission_1990</v>
+        <v/>
       </c>
       <c r="C156" t="str">
         <f>IF(COUNTBLANK(Dashboard!E156)=0,Dashboard!E156,"")</f>
@@ -13255,13 +13291,13 @@
       </c>
       <c r="D156" s="86" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">- co2_emission_1990 = </v>
+        <v/>
       </c>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B157" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C157)=0,Dashboard!C157,"")</f>
-        <v>co2_emission_1990_aviation_bunkers</v>
+        <v>co2_emission_1990</v>
       </c>
       <c r="C157" t="str">
         <f>IF(COUNTBLANK(Dashboard!E157)=0,Dashboard!E157,"")</f>
@@ -13269,41 +13305,41 @@
       </c>
       <c r="D157" s="86" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">- co2_emission_1990_aviation_bunkers = </v>
+        <v xml:space="preserve">- co2_emission_1990 = </v>
       </c>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B158" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C158)=0,Dashboard!C158,"")</f>
-        <v>co2_emission_1990_marine_bunkers</v>
+        <v>co2_emission_1990_aviation_bunkers</v>
       </c>
       <c r="C158" t="str">
         <f>IF(COUNTBLANK(Dashboard!E158)=0,Dashboard!E158,"")</f>
         <v/>
       </c>
       <c r="D158" s="86" t="str">
-        <f t="shared" ref="D158:D174" si="9">IF(COUNTBLANK(B158)=0,"- "&amp;B158&amp;" = "&amp;LOWER(C158),"")</f>
-        <v xml:space="preserve">- co2_emission_1990_marine_bunkers = </v>
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">- co2_emission_1990_aviation_bunkers = </v>
       </c>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B159" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C159)=0,Dashboard!C159,"")</f>
-        <v>co2_percentage_free</v>
+        <v>co2_emission_1990_marine_bunkers</v>
       </c>
       <c r="C159" t="str">
         <f>IF(COUNTBLANK(Dashboard!E159)=0,Dashboard!E159,"")</f>
         <v/>
       </c>
       <c r="D159" s="86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">- co2_percentage_free = </v>
+        <f t="shared" ref="D159:D175" si="9">IF(COUNTBLANK(B159)=0,"- "&amp;B159&amp;" = "&amp;LOWER(C159),"")</f>
+        <v xml:space="preserve">- co2_emission_1990_marine_bunkers = </v>
       </c>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B160" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C160)=0,Dashboard!C160,"")</f>
-        <v>co2_price</v>
+        <v>co2_percentage_free</v>
       </c>
       <c r="C160" t="str">
         <f>IF(COUNTBLANK(Dashboard!E160)=0,Dashboard!E160,"")</f>
@@ -13311,13 +13347,13 @@
       </c>
       <c r="D160" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- co2_price = </v>
+        <v xml:space="preserve">- co2_percentage_free = </v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B161" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C161)=0,Dashboard!C161,"")</f>
-        <v>captured_biogenic_co2_price</v>
+        <v>co2_price</v>
       </c>
       <c r="C161" t="str">
         <f>IF(COUNTBLANK(Dashboard!E161)=0,Dashboard!E161,"")</f>
@@ -13325,13 +13361,13 @@
       </c>
       <c r="D161" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- captured_biogenic_co2_price = </v>
+        <v xml:space="preserve">- co2_price = </v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B162" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C162)=0,Dashboard!C162,"")</f>
-        <v/>
+        <v>captured_biogenic_co2_price</v>
       </c>
       <c r="C162" t="str">
         <f>IF(COUNTBLANK(Dashboard!E162)=0,Dashboard!E162,"")</f>
@@ -13339,7 +13375,7 @@
       </c>
       <c r="D162" s="86" t="str">
         <f t="shared" si="9"/>
-        <v/>
+        <v xml:space="preserve">- captured_biogenic_co2_price = </v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.2">
@@ -13359,7 +13395,7 @@
     <row r="164" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B164" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C164)=0,Dashboard!C164,"")</f>
-        <v>lv_net_capacity_per_step</v>
+        <v/>
       </c>
       <c r="C164" t="str">
         <f>IF(COUNTBLANK(Dashboard!E164)=0,Dashboard!E164,"")</f>
@@ -13367,13 +13403,13 @@
       </c>
       <c r="D164" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- lv_net_capacity_per_step = </v>
+        <v/>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B165" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C165)=0,Dashboard!C165,"")</f>
-        <v>lv_net_costs_per_capacity_step</v>
+        <v>lv_net_capacity_per_step</v>
       </c>
       <c r="C165" t="str">
         <f>IF(COUNTBLANK(Dashboard!E165)=0,Dashboard!E165,"")</f>
@@ -13381,13 +13417,13 @@
       </c>
       <c r="D165" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- lv_net_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- lv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B166" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C166)=0,Dashboard!C166,"")</f>
-        <v>lv_net_spare_capacity</v>
+        <v>lv_net_costs_per_capacity_step</v>
       </c>
       <c r="C166" t="str">
         <f>IF(COUNTBLANK(Dashboard!E166)=0,Dashboard!E166,"")</f>
@@ -13395,13 +13431,13 @@
       </c>
       <c r="D166" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- lv_net_spare_capacity = </v>
+        <v xml:space="preserve">- lv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B167" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C167)=0,Dashboard!C167,"")</f>
-        <v>lv_net_total_costs_present</v>
+        <v>lv_net_spare_capacity</v>
       </c>
       <c r="C167" t="str">
         <f>IF(COUNTBLANK(Dashboard!E167)=0,Dashboard!E167,"")</f>
@@ -13409,13 +13445,13 @@
       </c>
       <c r="D167" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- lv_net_total_costs_present = </v>
+        <v xml:space="preserve">- lv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B168" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C168)=0,Dashboard!C168,"")</f>
-        <v>lv_mv_trafo_capacity_per_step</v>
+        <v>lv_net_total_costs_present</v>
       </c>
       <c r="C168" t="str">
         <f>IF(COUNTBLANK(Dashboard!E168)=0,Dashboard!E168,"")</f>
@@ -13423,13 +13459,13 @@
       </c>
       <c r="D168" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- lv_mv_trafo_capacity_per_step = </v>
+        <v xml:space="preserve">- lv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B169" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C169)=0,Dashboard!C169,"")</f>
-        <v>lv_mv_trafo_costs_per_capacity_step</v>
+        <v>lv_mv_trafo_capacity_per_step</v>
       </c>
       <c r="C169" t="str">
         <f>IF(COUNTBLANK(Dashboard!E169)=0,Dashboard!E169,"")</f>
@@ -13437,13 +13473,13 @@
       </c>
       <c r="D169" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- lv_mv_trafo_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- lv_mv_trafo_capacity_per_step = </v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B170" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C170)=0,Dashboard!C170,"")</f>
-        <v>lv_mv_trafo_spare_capacity</v>
+        <v>lv_mv_trafo_costs_per_capacity_step</v>
       </c>
       <c r="C170" t="str">
         <f>IF(COUNTBLANK(Dashboard!E170)=0,Dashboard!E170,"")</f>
@@ -13451,13 +13487,13 @@
       </c>
       <c r="D170" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- lv_mv_trafo_spare_capacity = </v>
+        <v xml:space="preserve">- lv_mv_trafo_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B171" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C171)=0,Dashboard!C171,"")</f>
-        <v>lv_mv_trafo_total_costs_present</v>
+        <v>lv_mv_trafo_spare_capacity</v>
       </c>
       <c r="C171" t="str">
         <f>IF(COUNTBLANK(Dashboard!E171)=0,Dashboard!E171,"")</f>
@@ -13465,13 +13501,13 @@
       </c>
       <c r="D171" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- lv_mv_trafo_total_costs_present = </v>
+        <v xml:space="preserve">- lv_mv_trafo_spare_capacity = </v>
       </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B172" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C172)=0,Dashboard!C172,"")</f>
-        <v>mv_net_capacity_per_step</v>
+        <v>lv_mv_trafo_total_costs_present</v>
       </c>
       <c r="C172" t="str">
         <f>IF(COUNTBLANK(Dashboard!E172)=0,Dashboard!E172,"")</f>
@@ -13479,13 +13515,13 @@
       </c>
       <c r="D172" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- mv_net_capacity_per_step = </v>
+        <v xml:space="preserve">- lv_mv_trafo_total_costs_present = </v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B173" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C173)=0,Dashboard!C173,"")</f>
-        <v>mv_net_costs_per_capacity_step</v>
+        <v>mv_net_capacity_per_step</v>
       </c>
       <c r="C173" t="str">
         <f>IF(COUNTBLANK(Dashboard!E173)=0,Dashboard!E173,"")</f>
@@ -13493,13 +13529,13 @@
       </c>
       <c r="D173" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- mv_net_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- mv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B174" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C174)=0,Dashboard!C174,"")</f>
-        <v>mv_net_spare_capacity</v>
+        <v>mv_net_costs_per_capacity_step</v>
       </c>
       <c r="C174" t="str">
         <f>IF(COUNTBLANK(Dashboard!E174)=0,Dashboard!E174,"")</f>
@@ -13507,41 +13543,41 @@
       </c>
       <c r="D174" s="86" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">- mv_net_spare_capacity = </v>
+        <v xml:space="preserve">- mv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B175" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C175)=0,Dashboard!C175,"")</f>
-        <v>mv_net_total_costs_present</v>
+        <v>mv_net_spare_capacity</v>
       </c>
       <c r="C175" t="str">
         <f>IF(COUNTBLANK(Dashboard!E175)=0,Dashboard!E175,"")</f>
         <v/>
       </c>
       <c r="D175" s="86" t="str">
-        <f t="shared" ref="D175:D212" si="10">IF(COUNTBLANK(B175)=0,"- "&amp;B175&amp;" = "&amp;LOWER(C175),"")</f>
-        <v xml:space="preserve">- mv_net_total_costs_present = </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">- mv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B176" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C176)=0,Dashboard!C176,"")</f>
-        <v>mv_hv_trafo_capacity_per_step</v>
+        <v>mv_net_total_costs_present</v>
       </c>
       <c r="C176" t="str">
         <f>IF(COUNTBLANK(Dashboard!E176)=0,Dashboard!E176,"")</f>
         <v/>
       </c>
       <c r="D176" s="86" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">- mv_hv_trafo_capacity_per_step = </v>
+        <f t="shared" ref="D176:D213" si="10">IF(COUNTBLANK(B176)=0,"- "&amp;B176&amp;" = "&amp;LOWER(C176),"")</f>
+        <v xml:space="preserve">- mv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B177" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C177)=0,Dashboard!C177,"")</f>
-        <v>mv_hv_trafo_costs_per_capacity_step</v>
+        <v>mv_hv_trafo_capacity_per_step</v>
       </c>
       <c r="C177" t="str">
         <f>IF(COUNTBLANK(Dashboard!E177)=0,Dashboard!E177,"")</f>
@@ -13549,13 +13585,13 @@
       </c>
       <c r="D177" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- mv_hv_trafo_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- mv_hv_trafo_capacity_per_step = </v>
       </c>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B178" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C178)=0,Dashboard!C178,"")</f>
-        <v>mv_hv_trafo_spare_capacity</v>
+        <v>mv_hv_trafo_costs_per_capacity_step</v>
       </c>
       <c r="C178" t="str">
         <f>IF(COUNTBLANK(Dashboard!E178)=0,Dashboard!E178,"")</f>
@@ -13563,13 +13599,13 @@
       </c>
       <c r="D178" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- mv_hv_trafo_spare_capacity = </v>
+        <v xml:space="preserve">- mv_hv_trafo_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B179" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C179)=0,Dashboard!C179,"")</f>
-        <v>mv_hv_trafo_total_costs_present</v>
+        <v>mv_hv_trafo_spare_capacity</v>
       </c>
       <c r="C179" t="str">
         <f>IF(COUNTBLANK(Dashboard!E179)=0,Dashboard!E179,"")</f>
@@ -13577,13 +13613,13 @@
       </c>
       <c r="D179" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- mv_hv_trafo_total_costs_present = </v>
+        <v xml:space="preserve">- mv_hv_trafo_spare_capacity = </v>
       </c>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B180" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C180)=0,Dashboard!C180,"")</f>
-        <v>hv_net_capacity_per_step</v>
+        <v>mv_hv_trafo_total_costs_present</v>
       </c>
       <c r="C180" t="str">
         <f>IF(COUNTBLANK(Dashboard!E180)=0,Dashboard!E180,"")</f>
@@ -13591,13 +13627,13 @@
       </c>
       <c r="D180" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- hv_net_capacity_per_step = </v>
+        <v xml:space="preserve">- mv_hv_trafo_total_costs_present = </v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B181" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C181)=0,Dashboard!C181,"")</f>
-        <v>hv_net_costs_per_capacity_step</v>
+        <v>hv_net_capacity_per_step</v>
       </c>
       <c r="C181" t="str">
         <f>IF(COUNTBLANK(Dashboard!E181)=0,Dashboard!E181,"")</f>
@@ -13605,13 +13641,13 @@
       </c>
       <c r="D181" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- hv_net_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- hv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B182" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C182)=0,Dashboard!C182,"")</f>
-        <v>hv_net_spare_capacity</v>
+        <v>hv_net_costs_per_capacity_step</v>
       </c>
       <c r="C182" t="str">
         <f>IF(COUNTBLANK(Dashboard!E182)=0,Dashboard!E182,"")</f>
@@ -13619,13 +13655,13 @@
       </c>
       <c r="D182" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- hv_net_spare_capacity = </v>
+        <v xml:space="preserve">- hv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B183" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C183)=0,Dashboard!C183,"")</f>
-        <v>hv_net_total_costs_present</v>
+        <v>hv_net_spare_capacity</v>
       </c>
       <c r="C183" t="str">
         <f>IF(COUNTBLANK(Dashboard!E183)=0,Dashboard!E183,"")</f>
@@ -13633,13 +13669,13 @@
       </c>
       <c r="D183" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- hv_net_total_costs_present = </v>
+        <v xml:space="preserve">- hv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B184" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C184)=0,Dashboard!C184,"")</f>
-        <v>interconnection_net_costs_present</v>
+        <v>hv_net_total_costs_present</v>
       </c>
       <c r="C184" t="str">
         <f>IF(COUNTBLANK(Dashboard!E184)=0,Dashboard!E184,"")</f>
@@ -13647,13 +13683,13 @@
       </c>
       <c r="D184" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- interconnection_net_costs_present = </v>
+        <v xml:space="preserve">- hv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B185" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C185)=0,Dashboard!C185,"")</f>
-        <v>interconnector_capacity</v>
+        <v>interconnection_net_costs_present</v>
       </c>
       <c r="C185" t="str">
         <f>IF(COUNTBLANK(Dashboard!E185)=0,Dashboard!E185,"")</f>
@@ -13661,13 +13697,13 @@
       </c>
       <c r="D185" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- interconnector_capacity = </v>
+        <v xml:space="preserve">- interconnection_net_costs_present = </v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B186" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C186)=0,Dashboard!C186,"")</f>
-        <v>offshore_net_costs_present</v>
+        <v>interconnector_capacity</v>
       </c>
       <c r="C186" t="str">
         <f>IF(COUNTBLANK(Dashboard!E186)=0,Dashboard!E186,"")</f>
@@ -13675,13 +13711,13 @@
       </c>
       <c r="D186" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- offshore_net_costs_present = </v>
+        <v xml:space="preserve">- interconnector_capacity = </v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B187" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C187)=0,Dashboard!C187,"")</f>
-        <v>annual_infrastructure_cost_gas</v>
+        <v>offshore_net_costs_present</v>
       </c>
       <c r="C187" t="str">
         <f>IF(COUNTBLANK(Dashboard!E187)=0,Dashboard!E187,"")</f>
@@ -13689,13 +13725,13 @@
       </c>
       <c r="D187" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- annual_infrastructure_cost_gas = </v>
+        <v xml:space="preserve">- offshore_net_costs_present = </v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B188" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C188)=0,Dashboard!C188,"")</f>
-        <v/>
+        <v>annual_infrastructure_cost_gas</v>
       </c>
       <c r="C188" t="str">
         <f>IF(COUNTBLANK(Dashboard!E188)=0,Dashboard!E188,"")</f>
@@ -13703,13 +13739,13 @@
       </c>
       <c r="D188" s="86" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v xml:space="preserve">- annual_infrastructure_cost_gas = </v>
       </c>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B189" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C189)=0,Dashboard!C189,"")</f>
-        <v>heat_share_of_apartments_with_block_heating</v>
+        <v/>
       </c>
       <c r="C189" t="str">
         <f>IF(COUNTBLANK(Dashboard!E189)=0,Dashboard!E189,"")</f>
@@ -13717,13 +13753,13 @@
       </c>
       <c r="D189" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_share_of_apartments_with_block_heating = </v>
+        <v/>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B190" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C190)=0,Dashboard!C190,"")</f>
-        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket</v>
+        <v>heat_share_of_apartments_with_block_heating</v>
       </c>
       <c r="C190" t="str">
         <f>IF(COUNTBLANK(Dashboard!E190)=0,Dashboard!E190,"")</f>
@@ -13731,13 +13767,13 @@
       </c>
       <c r="D190" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket = </v>
+        <v xml:space="preserve">- heat_share_of_apartments_with_block_heating = </v>
       </c>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B191" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C191)=0,Dashboard!C191,"")</f>
-        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket</v>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket</v>
       </c>
       <c r="C191" t="str">
         <f>IF(COUNTBLANK(Dashboard!E191)=0,Dashboard!E191,"")</f>
@@ -13745,13 +13781,13 @@
       </c>
       <c r="D191" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket = </v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B192" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C192)=0,Dashboard!C192,"")</f>
-        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket</v>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket</v>
       </c>
       <c r="C192" t="str">
         <f>IF(COUNTBLANK(Dashboard!E192)=0,Dashboard!E192,"")</f>
@@ -13759,13 +13795,13 @@
       </c>
       <c r="D192" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket = </v>
       </c>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B193" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C193)=0,Dashboard!C193,"")</f>
-        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket</v>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket</v>
       </c>
       <c r="C193" t="str">
         <f>IF(COUNTBLANK(Dashboard!E193)=0,Dashboard!E193,"")</f>
@@ -13773,13 +13809,13 @@
       </c>
       <c r="D193" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket = </v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B194" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C194)=0,Dashboard!C194,"")</f>
-        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket</v>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket</v>
       </c>
       <c r="C194" t="str">
         <f>IF(COUNTBLANK(Dashboard!E194)=0,Dashboard!E194,"")</f>
@@ -13787,13 +13823,13 @@
       </c>
       <c r="D194" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket = </v>
       </c>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B195" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C195)=0,Dashboard!C195,"")</f>
-        <v>heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket</v>
+        <v>heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket</v>
       </c>
       <c r="C195" t="str">
         <f>IF(COUNTBLANK(Dashboard!E195)=0,Dashboard!E195,"")</f>
@@ -13801,13 +13837,13 @@
       </c>
       <c r="D195" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket = </v>
       </c>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B196" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C196)=0,Dashboard!C196,"")</f>
-        <v>heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket</v>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket</v>
       </c>
       <c r="C196" t="str">
         <f>IF(COUNTBLANK(Dashboard!E196)=0,Dashboard!E196,"")</f>
@@ -13815,13 +13851,13 @@
       </c>
       <c r="D196" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket = </v>
       </c>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B197" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C197)=0,Dashboard!C197,"")</f>
-        <v>heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket</v>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket</v>
       </c>
       <c r="C197" t="str">
         <f>IF(COUNTBLANK(Dashboard!E197)=0,Dashboard!E197,"")</f>
@@ -13829,13 +13865,13 @@
       </c>
       <c r="D197" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket = </v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B198" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C198)=0,Dashboard!C198,"")</f>
-        <v>heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket</v>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket</v>
       </c>
       <c r="C198" t="str">
         <f>IF(COUNTBLANK(Dashboard!E198)=0,Dashboard!E198,"")</f>
@@ -13843,13 +13879,13 @@
       </c>
       <c r="D198" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket = </v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B199" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C199)=0,Dashboard!C199,"")</f>
-        <v>heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket</v>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket</v>
       </c>
       <c r="C199" t="str">
         <f>IF(COUNTBLANK(Dashboard!E199)=0,Dashboard!E199,"")</f>
@@ -13857,13 +13893,13 @@
       </c>
       <c r="D199" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket = </v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B200" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C200)=0,Dashboard!C200,"")</f>
-        <v>heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur</v>
+        <v>heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket</v>
       </c>
       <c r="C200" t="str">
         <f>IF(COUNTBLANK(Dashboard!E200)=0,Dashboard!E200,"")</f>
@@ -13871,13 +13907,13 @@
       </c>
       <c r="D200" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket = </v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B201" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C201)=0,Dashboard!C201,"")</f>
-        <v>heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur</v>
+        <v>heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur</v>
       </c>
       <c r="C201" t="str">
         <f>IF(COUNTBLANK(Dashboard!E201)=0,Dashboard!E201,"")</f>
@@ -13885,13 +13921,13 @@
       </c>
       <c r="D201" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B202" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C202)=0,Dashboard!C202,"")</f>
-        <v>heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur</v>
+        <v>heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur</v>
       </c>
       <c r="C202" t="str">
         <f>IF(COUNTBLANK(Dashboard!E202)=0,Dashboard!E202,"")</f>
@@ -13899,13 +13935,13 @@
       </c>
       <c r="D202" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B203" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C203)=0,Dashboard!C203,"")</f>
-        <v>heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur</v>
+        <v>heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur</v>
       </c>
       <c r="C203" t="str">
         <f>IF(COUNTBLANK(Dashboard!E203)=0,Dashboard!E203,"")</f>
@@ -13913,13 +13949,13 @@
       </c>
       <c r="D203" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B204" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C204)=0,Dashboard!C204,"")</f>
-        <v>heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur</v>
+        <v>heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur</v>
       </c>
       <c r="C204" t="str">
         <f>IF(COUNTBLANK(Dashboard!E204)=0,Dashboard!E204,"")</f>
@@ -13927,13 +13963,13 @@
       </c>
       <c r="D204" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B205" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C205)=0,Dashboard!C205,"")</f>
-        <v>heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur</v>
+        <v>heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur</v>
       </c>
       <c r="C205" t="str">
         <f>IF(COUNTBLANK(Dashboard!E205)=0,Dashboard!E205,"")</f>
@@ -13941,13 +13977,13 @@
       </c>
       <c r="D205" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B206" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C206)=0,Dashboard!C206,"")</f>
-        <v>heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur</v>
+        <v>heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur</v>
       </c>
       <c r="C206" t="str">
         <f>IF(COUNTBLANK(Dashboard!E206)=0,Dashboard!E206,"")</f>
@@ -13955,13 +13991,13 @@
       </c>
       <c r="D206" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B207" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C207)=0,Dashboard!C207,"")</f>
-        <v>heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur</v>
+        <v>heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur</v>
       </c>
       <c r="C207" t="str">
         <f>IF(COUNTBLANK(Dashboard!E207)=0,Dashboard!E207,"")</f>
@@ -13969,13 +14005,13 @@
       </c>
       <c r="D207" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B208" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C208)=0,Dashboard!C208,"")</f>
-        <v>heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur</v>
+        <v>heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur</v>
       </c>
       <c r="C208" t="str">
         <f>IF(COUNTBLANK(Dashboard!E208)=0,Dashboard!E208,"")</f>
@@ -13983,13 +14019,13 @@
       </c>
       <c r="D208" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="209" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B209" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C209)=0,Dashboard!C209,"")</f>
-        <v>heat_buildings_indoor_investment_costs_eur_per_kw</v>
+        <v>heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur</v>
       </c>
       <c r="C209" t="str">
         <f>IF(COUNTBLANK(Dashboard!E209)=0,Dashboard!E209,"")</f>
@@ -13997,13 +14033,13 @@
       </c>
       <c r="D209" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B210" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C210)=0,Dashboard!C210,"")</f>
-        <v>heat_buildings_indoor_investment_costs_eur_per_connection</v>
+        <v>heat_buildings_indoor_investment_costs_eur_per_kw</v>
       </c>
       <c r="C210" t="str">
         <f>IF(COUNTBLANK(Dashboard!E210)=0,Dashboard!E210,"")</f>
@@ -14011,13 +14047,13 @@
       </c>
       <c r="D210" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B211" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C211)=0,Dashboard!C211,"")</f>
-        <v>heat_exchanger_station_investment_costs_eur_per_kw</v>
+        <v>heat_buildings_indoor_investment_costs_eur_per_connection</v>
       </c>
       <c r="C211" t="str">
         <f>IF(COUNTBLANK(Dashboard!E211)=0,Dashboard!E211,"")</f>
@@ -14025,13 +14061,13 @@
       </c>
       <c r="D211" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_exchanger_station_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="212" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B212" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C212)=0,Dashboard!C212,"")</f>
-        <v>heat_lt_sub_station_investment_costs_eur_per_kw</v>
+        <v>heat_exchanger_station_investment_costs_eur_per_kw</v>
       </c>
       <c r="C212" t="str">
         <f>IF(COUNTBLANK(Dashboard!E212)=0,Dashboard!E212,"")</f>
@@ -14039,41 +14075,41 @@
       </c>
       <c r="D212" s="86" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">- heat_lt_sub_station_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_exchanger_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="213" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B213" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C213)=0,Dashboard!C213,"")</f>
-        <v>heat_mt_sub_station_investment_costs_eur_per_kw</v>
+        <v>heat_lt_sub_station_investment_costs_eur_per_kw</v>
       </c>
       <c r="C213" t="str">
         <f>IF(COUNTBLANK(Dashboard!E213)=0,Dashboard!E213,"")</f>
         <v/>
       </c>
       <c r="D213" s="86" t="str">
-        <f t="shared" ref="D213:D244" si="11">IF(COUNTBLANK(B213)=0,"- "&amp;B213&amp;" = "&amp;LOWER(C213),"")</f>
-        <v xml:space="preserve">- heat_mt_sub_station_investment_costs_eur_per_kw = </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">- heat_lt_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B214" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C214)=0,Dashboard!C214,"")</f>
-        <v>heat_ht_sub_station_investment_costs_eur_per_kw</v>
+        <v>heat_mt_sub_station_investment_costs_eur_per_kw</v>
       </c>
       <c r="C214" t="str">
         <f>IF(COUNTBLANK(Dashboard!E214)=0,Dashboard!E214,"")</f>
         <v/>
       </c>
       <c r="D214" s="86" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">- heat_ht_sub_station_investment_costs_eur_per_kw = </v>
+        <f t="shared" ref="D214:D243" si="11">IF(COUNTBLANK(B214)=0,"- "&amp;B214&amp;" = "&amp;LOWER(C214),"")</f>
+        <v xml:space="preserve">- heat_mt_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B215" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C215)=0,Dashboard!C215,"")</f>
-        <v>heat_lt_distribution_pipelines_investment_costs_eur_per_meter</v>
+        <v>heat_ht_sub_station_investment_costs_eur_per_kw</v>
       </c>
       <c r="C215" t="str">
         <f>IF(COUNTBLANK(Dashboard!E215)=0,Dashboard!E215,"")</f>
@@ -14081,13 +14117,13 @@
       </c>
       <c r="D215" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- heat_lt_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <v xml:space="preserve">- heat_ht_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="216" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B216" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C216)=0,Dashboard!C216,"")</f>
-        <v>heat_mt_distribution_pipelines_investment_costs_eur_per_meter</v>
+        <v>heat_lt_distribution_pipelines_investment_costs_eur_per_meter</v>
       </c>
       <c r="C216" t="str">
         <f>IF(COUNTBLANK(Dashboard!E216)=0,Dashboard!E216,"")</f>
@@ -14095,13 +14131,13 @@
       </c>
       <c r="D216" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- heat_mt_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <v xml:space="preserve">- heat_lt_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B217" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C217)=0,Dashboard!C217,"")</f>
-        <v>heat_ht_distribution_pipelines_investment_costs_eur_per_meter</v>
+        <v>heat_mt_distribution_pipelines_investment_costs_eur_per_meter</v>
       </c>
       <c r="C217" t="str">
         <f>IF(COUNTBLANK(Dashboard!E217)=0,Dashboard!E217,"")</f>
@@ -14109,13 +14145,13 @@
       </c>
       <c r="D217" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- heat_ht_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <v xml:space="preserve">- heat_mt_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="218" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B218" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C218)=0,Dashboard!C218,"")</f>
-        <v>heat_lt_primary_pipelines_investment_costs_per_kw</v>
+        <v>heat_ht_distribution_pipelines_investment_costs_eur_per_meter</v>
       </c>
       <c r="C218" t="str">
         <f>IF(COUNTBLANK(Dashboard!E218)=0,Dashboard!E218,"")</f>
@@ -14123,13 +14159,13 @@
       </c>
       <c r="D218" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- heat_lt_primary_pipelines_investment_costs_per_kw = </v>
+        <v xml:space="preserve">- heat_ht_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B219" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C219)=0,Dashboard!C219,"")</f>
-        <v>heat_mt_primary_pipelines_investment_costs_per_kw</v>
+        <v>heat_lt_primary_pipelines_investment_costs_per_kw</v>
       </c>
       <c r="C219" t="str">
         <f>IF(COUNTBLANK(Dashboard!E219)=0,Dashboard!E219,"")</f>
@@ -14137,13 +14173,13 @@
       </c>
       <c r="D219" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- heat_mt_primary_pipelines_investment_costs_per_kw = </v>
+        <v xml:space="preserve">- heat_lt_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B220" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C220)=0,Dashboard!C220,"")</f>
-        <v>heat_ht_primary_pipelines_investment_costs_per_kw</v>
+        <v>heat_mt_primary_pipelines_investment_costs_per_kw</v>
       </c>
       <c r="C220" t="str">
         <f>IF(COUNTBLANK(Dashboard!E220)=0,Dashboard!E220,"")</f>
@@ -14151,13 +14187,13 @@
       </c>
       <c r="D220" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- heat_ht_primary_pipelines_investment_costs_per_kw = </v>
+        <v xml:space="preserve">- heat_mt_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B221" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C221)=0,Dashboard!C221,"")</f>
-        <v>heat_yearly_indoor_infrastructure_maintenance_costs_factor</v>
+        <v>heat_ht_primary_pipelines_investment_costs_per_kw</v>
       </c>
       <c r="C221" t="str">
         <f>IF(COUNTBLANK(Dashboard!E221)=0,Dashboard!E221,"")</f>
@@ -14165,13 +14201,13 @@
       </c>
       <c r="D221" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- heat_yearly_indoor_infrastructure_maintenance_costs_factor = </v>
+        <v xml:space="preserve">- heat_ht_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B222" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C222)=0,Dashboard!C222,"")</f>
-        <v>heat_yearly_outdoor_infrastructure_maintenance_costs_factor</v>
+        <v>heat_yearly_indoor_infrastructure_maintenance_costs_factor</v>
       </c>
       <c r="C222" t="str">
         <f>IF(COUNTBLANK(Dashboard!E222)=0,Dashboard!E222,"")</f>
@@ -14179,13 +14215,13 @@
       </c>
       <c r="D222" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- heat_yearly_outdoor_infrastructure_maintenance_costs_factor = </v>
+        <v xml:space="preserve">- heat_yearly_indoor_infrastructure_maintenance_costs_factor = </v>
       </c>
     </row>
     <row r="223" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B223" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C223)=0,Dashboard!C223,"")</f>
-        <v>households_lt_heat_delivery_system_costs_apartments_eur_per_connection</v>
+        <v>heat_yearly_outdoor_infrastructure_maintenance_costs_factor</v>
       </c>
       <c r="C223" t="str">
         <f>IF(COUNTBLANK(Dashboard!E223)=0,Dashboard!E223,"")</f>
@@ -14193,13 +14229,13 @@
       </c>
       <c r="D223" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <v xml:space="preserve">- heat_yearly_outdoor_infrastructure_maintenance_costs_factor = </v>
       </c>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B224" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C224)=0,Dashboard!C224,"")</f>
-        <v>households_mt_heat_delivery_system_costs_apartments_eur_per_connection</v>
+        <v>households_lt_heat_delivery_system_costs_apartments_eur_per_connection</v>
       </c>
       <c r="C224" t="str">
         <f>IF(COUNTBLANK(Dashboard!E224)=0,Dashboard!E224,"")</f>
@@ -14207,13 +14243,13 @@
       </c>
       <c r="D224" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B225" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C225)=0,Dashboard!C225,"")</f>
-        <v>households_ht_heat_delivery_system_costs_apartments_eur_per_connection</v>
+        <v>households_mt_heat_delivery_system_costs_apartments_eur_per_connection</v>
       </c>
       <c r="C225" t="str">
         <f>IF(COUNTBLANK(Dashboard!E225)=0,Dashboard!E225,"")</f>
@@ -14221,13 +14257,13 @@
       </c>
       <c r="D225" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B226" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C226)=0,Dashboard!C226,"")</f>
-        <v>households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
+        <v>households_ht_heat_delivery_system_costs_apartments_eur_per_connection</v>
       </c>
       <c r="C226" t="str">
         <f>IF(COUNTBLANK(Dashboard!E226)=0,Dashboard!E226,"")</f>
@@ -14235,13 +14271,13 @@
       </c>
       <c r="D226" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="227" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B227" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C227)=0,Dashboard!C227,"")</f>
-        <v>households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
+        <v>households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
       </c>
       <c r="C227" t="str">
         <f>IF(COUNTBLANK(Dashboard!E227)=0,Dashboard!E227,"")</f>
@@ -14249,13 +14285,13 @@
       </c>
       <c r="D227" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B228" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C228)=0,Dashboard!C228,"")</f>
-        <v>households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
+        <v>households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
       </c>
       <c r="C228" t="str">
         <f>IF(COUNTBLANK(Dashboard!E228)=0,Dashboard!E228,"")</f>
@@ -14263,13 +14299,13 @@
       </c>
       <c r="D228" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B229" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C229)=0,Dashboard!C229,"")</f>
-        <v>buildings_lt_heat_delivery_system_costs_eur_per_connection</v>
+        <v>households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection</v>
       </c>
       <c r="C229" t="str">
         <f>IF(COUNTBLANK(Dashboard!E229)=0,Dashboard!E229,"")</f>
@@ -14277,13 +14313,13 @@
       </c>
       <c r="D229" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- buildings_lt_heat_delivery_system_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B230" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C230)=0,Dashboard!C230,"")</f>
-        <v>buildings_mt_heat_delivery_system_costs_eur_per_connection</v>
+        <v>buildings_lt_heat_delivery_system_costs_eur_per_connection</v>
       </c>
       <c r="C230" t="str">
         <f>IF(COUNTBLANK(Dashboard!E230)=0,Dashboard!E230,"")</f>
@@ -14291,13 +14327,13 @@
       </c>
       <c r="D230" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- buildings_mt_heat_delivery_system_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- buildings_lt_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B231" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C231)=0,Dashboard!C231,"")</f>
-        <v>buildings_ht_heat_delivery_system_costs_eur_per_connection</v>
+        <v>buildings_mt_heat_delivery_system_costs_eur_per_connection</v>
       </c>
       <c r="C231" t="str">
         <f>IF(COUNTBLANK(Dashboard!E231)=0,Dashboard!E231,"")</f>
@@ -14305,13 +14341,13 @@
       </c>
       <c r="D231" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- buildings_ht_heat_delivery_system_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- buildings_mt_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B232" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C232)=0,Dashboard!C232,"")</f>
-        <v/>
+        <v>buildings_ht_heat_delivery_system_costs_eur_per_connection</v>
       </c>
       <c r="C232" t="str">
         <f>IF(COUNTBLANK(Dashboard!E232)=0,Dashboard!E232,"")</f>
@@ -14319,7 +14355,7 @@
       </c>
       <c r="D232" s="86" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v xml:space="preserve">- buildings_ht_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.2">
@@ -14339,7 +14375,7 @@
     <row r="234" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B234" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C234)=0,Dashboard!C234,"")</f>
-        <v>number_of_cars</v>
+        <v/>
       </c>
       <c r="C234" t="str">
         <f>IF(COUNTBLANK(Dashboard!E234)=0,Dashboard!E234,"")</f>
@@ -14347,13 +14383,13 @@
       </c>
       <c r="D234" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- number_of_cars = </v>
+        <v/>
       </c>
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B235" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C235)=0,Dashboard!C235,"")</f>
-        <v>number_of_busses</v>
+        <v>number_of_cars</v>
       </c>
       <c r="C235" t="str">
         <f>IF(COUNTBLANK(Dashboard!E235)=0,Dashboard!E235,"")</f>
@@ -14361,13 +14397,13 @@
       </c>
       <c r="D235" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- number_of_busses = </v>
+        <v xml:space="preserve">- number_of_cars = </v>
       </c>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B236" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C236)=0,Dashboard!C236,"")</f>
-        <v>number_of_trucks</v>
+        <v>number_of_busses</v>
       </c>
       <c r="C236" t="str">
         <f>IF(COUNTBLANK(Dashboard!E236)=0,Dashboard!E236,"")</f>
@@ -14375,13 +14411,13 @@
       </c>
       <c r="D236" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- number_of_trucks = </v>
+        <v xml:space="preserve">- number_of_busses = </v>
       </c>
     </row>
     <row r="237" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B237" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C237)=0,Dashboard!C237,"")</f>
-        <v>number_of_vans</v>
+        <v>number_of_trucks</v>
       </c>
       <c r="C237" t="str">
         <f>IF(COUNTBLANK(Dashboard!E237)=0,Dashboard!E237,"")</f>
@@ -14389,13 +14425,13 @@
       </c>
       <c r="D237" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- number_of_vans = </v>
+        <v xml:space="preserve">- number_of_trucks = </v>
       </c>
     </row>
     <row r="238" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B238" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C238)=0,Dashboard!C238,"")</f>
-        <v>electric_vehicle_profile_1_share</v>
+        <v>number_of_vans</v>
       </c>
       <c r="C238" t="str">
         <f>IF(COUNTBLANK(Dashboard!E238)=0,Dashboard!E238,"")</f>
@@ -14403,13 +14439,13 @@
       </c>
       <c r="D238" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
+        <v xml:space="preserve">- number_of_vans = </v>
       </c>
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B239" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C239)=0,Dashboard!C239,"")</f>
-        <v>electric_vehicle_profile_2_share</v>
+        <v>electric_vehicle_profile_1_share</v>
       </c>
       <c r="C239" t="str">
         <f>IF(COUNTBLANK(Dashboard!E239)=0,Dashboard!E239,"")</f>
@@ -14417,13 +14453,13 @@
       </c>
       <c r="D239" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
+        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
       </c>
     </row>
     <row r="240" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B240" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C240)=0,Dashboard!C240,"")</f>
-        <v>electric_vehicle_profile_3_share</v>
+        <v>electric_vehicle_profile_2_share</v>
       </c>
       <c r="C240" t="str">
         <f>IF(COUNTBLANK(Dashboard!E240)=0,Dashboard!E240,"")</f>
@@ -14431,13 +14467,13 @@
       </c>
       <c r="D240" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
+        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B241" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C241)=0,Dashboard!C241,"")</f>
-        <v>electric_vehicle_profile_4_share</v>
+        <v>electric_vehicle_profile_3_share</v>
       </c>
       <c r="C241" t="str">
         <f>IF(COUNTBLANK(Dashboard!E241)=0,Dashboard!E241,"")</f>
@@ -14445,13 +14481,13 @@
       </c>
       <c r="D241" s="86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">- electric_vehicle_profile_4_share = </v>
+        <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B242" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C242)=0,Dashboard!C242,"")</f>
-        <v>electric_vehicle_profile_5_share</v>
+        <v>electric_vehicle_profile_4_share</v>
       </c>
       <c r="C242" t="str">
         <f>IF(COUNTBLANK(Dashboard!E242)=0,Dashboard!E242,"")</f>
@@ -14459,13 +14495,22 @@
       </c>
       <c r="D242" s="86" t="str">
         <f t="shared" si="11"/>
+        <v xml:space="preserve">- electric_vehicle_profile_4_share = </v>
+      </c>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B243" s="85" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C243)=0,Dashboard!C243,"")</f>
+        <v>electric_vehicle_profile_5_share</v>
+      </c>
+      <c r="C243" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E243)=0,Dashboard!E243,"")</f>
+        <v/>
+      </c>
+      <c r="D243" s="86" t="str">
+        <f t="shared" si="11"/>
         <v xml:space="preserve">- electric_vehicle_profile_5_share = </v>
       </c>
-    </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B243" s="85"/>
-      <c r="C243"/>
-      <c r="D243" s="86"/>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B244" s="85"/>
@@ -14493,29 +14538,34 @@
       <c r="D248" s="86"/>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B249" s="85" t="str">
-        <f>IF(COUNTBLANK(Dashboard!C245)=0,Dashboard!C245,"")</f>
-        <v/>
-      </c>
-      <c r="C249" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E243)=0,Dashboard!E243,"")</f>
-        <v/>
-      </c>
-      <c r="D249" s="86" t="str">
-        <f t="shared" ref="D249:D250" si="12">IF(COUNTBLANK(B249)=0,"- "&amp;B249&amp;" = "&amp;LOWER(C249),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="250" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B250" s="100" t="str">
+      <c r="B249" s="85"/>
+      <c r="C249"/>
+      <c r="D249" s="86"/>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B250" s="85" t="str">
         <f>IF(COUNTBLANK(Dashboard!C246)=0,Dashboard!C246,"")</f>
         <v/>
       </c>
-      <c r="C250" s="101" t="str">
-        <f>IF(COUNTBLANK(Dashboard!E246)=0,Dashboard!E246,"")</f>
-        <v/>
-      </c>
-      <c r="D250" s="102" t="str">
+      <c r="C250" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E244)=0,Dashboard!E244,"")</f>
+        <v/>
+      </c>
+      <c r="D250" s="86" t="str">
+        <f t="shared" ref="D250:D251" si="12">IF(COUNTBLANK(B250)=0,"- "&amp;B250&amp;" = "&amp;LOWER(C250),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="251" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B251" s="100" t="str">
+        <f>IF(COUNTBLANK(Dashboard!C247)=0,Dashboard!C247,"")</f>
+        <v/>
+      </c>
+      <c r="C251" s="101" t="str">
+        <f>IF(COUNTBLANK(Dashboard!E247)=0,Dashboard!E247,"")</f>
+        <v/>
+      </c>
+      <c r="D251" s="102" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
@@ -14531,10 +14581,10 @@
   <sheetPr codeName="Sheet5">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:A219"/>
+  <dimension ref="A1:A220"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A220" sqref="A220"/>
+    <sheetView topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15355,504 +15405,510 @@
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="str">
         <f>'compile results'!D152</f>
-        <v xml:space="preserve">- residences_roof_surface_available_for_pv = </v>
+        <v xml:space="preserve">- area_per_building_residence_equivalent = </v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="str">
         <f>'compile results'!D153</f>
-        <v xml:space="preserve">- buildings_roof_surface_available_for_pv = </v>
+        <v xml:space="preserve">- residences_roof_surface_available_for_pv = </v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="str">
-        <f>'compile results'!D156</f>
-        <v xml:space="preserve">- co2_emission_1990 = </v>
+        <f>'compile results'!D154</f>
+        <v xml:space="preserve">- buildings_roof_surface_available_for_pv = </v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="str">
         <f>'compile results'!D157</f>
-        <v xml:space="preserve">- co2_emission_1990_aviation_bunkers = </v>
+        <v xml:space="preserve">- co2_emission_1990 = </v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="str">
         <f>'compile results'!D158</f>
-        <v xml:space="preserve">- co2_emission_1990_marine_bunkers = </v>
+        <v xml:space="preserve">- co2_emission_1990_aviation_bunkers = </v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="str">
         <f>'compile results'!D159</f>
-        <v xml:space="preserve">- co2_percentage_free = </v>
+        <v xml:space="preserve">- co2_emission_1990_marine_bunkers = </v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="str">
         <f>'compile results'!D160</f>
-        <v xml:space="preserve">- co2_price = </v>
+        <v xml:space="preserve">- co2_percentage_free = </v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="str">
         <f>'compile results'!D161</f>
-        <v xml:space="preserve">- captured_biogenic_co2_price = </v>
+        <v xml:space="preserve">- co2_price = </v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="str">
-        <f>'compile results'!D164</f>
-        <v xml:space="preserve">- lv_net_capacity_per_step = </v>
+        <f>'compile results'!D162</f>
+        <v xml:space="preserve">- captured_biogenic_co2_price = </v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="str">
         <f>'compile results'!D165</f>
-        <v xml:space="preserve">- lv_net_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- lv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="str">
         <f>'compile results'!D166</f>
-        <v xml:space="preserve">- lv_net_spare_capacity = </v>
+        <v xml:space="preserve">- lv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="str">
         <f>'compile results'!D167</f>
-        <v xml:space="preserve">- lv_net_total_costs_present = </v>
+        <v xml:space="preserve">- lv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="str">
         <f>'compile results'!D168</f>
-        <v xml:space="preserve">- lv_mv_trafo_capacity_per_step = </v>
+        <v xml:space="preserve">- lv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="str">
         <f>'compile results'!D169</f>
-        <v xml:space="preserve">- lv_mv_trafo_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- lv_mv_trafo_capacity_per_step = </v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="str">
         <f>'compile results'!D170</f>
-        <v xml:space="preserve">- lv_mv_trafo_spare_capacity = </v>
+        <v xml:space="preserve">- lv_mv_trafo_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="str">
         <f>'compile results'!D171</f>
-        <v xml:space="preserve">- lv_mv_trafo_total_costs_present = </v>
+        <v xml:space="preserve">- lv_mv_trafo_spare_capacity = </v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="str">
         <f>'compile results'!D172</f>
-        <v xml:space="preserve">- mv_net_capacity_per_step = </v>
+        <v xml:space="preserve">- lv_mv_trafo_total_costs_present = </v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="str">
         <f>'compile results'!D173</f>
-        <v xml:space="preserve">- mv_net_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- mv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="str">
         <f>'compile results'!D174</f>
-        <v xml:space="preserve">- mv_net_spare_capacity = </v>
+        <v xml:space="preserve">- mv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="str">
         <f>'compile results'!D175</f>
-        <v xml:space="preserve">- mv_net_total_costs_present = </v>
+        <v xml:space="preserve">- mv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="str">
         <f>'compile results'!D176</f>
-        <v xml:space="preserve">- mv_hv_trafo_capacity_per_step = </v>
+        <v xml:space="preserve">- mv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="str">
         <f>'compile results'!D177</f>
-        <v xml:space="preserve">- mv_hv_trafo_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- mv_hv_trafo_capacity_per_step = </v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="str">
         <f>'compile results'!D178</f>
-        <v xml:space="preserve">- mv_hv_trafo_spare_capacity = </v>
+        <v xml:space="preserve">- mv_hv_trafo_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="str">
         <f>'compile results'!D179</f>
-        <v xml:space="preserve">- mv_hv_trafo_total_costs_present = </v>
+        <v xml:space="preserve">- mv_hv_trafo_spare_capacity = </v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="str">
         <f>'compile results'!D180</f>
-        <v xml:space="preserve">- hv_net_capacity_per_step = </v>
+        <v xml:space="preserve">- mv_hv_trafo_total_costs_present = </v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="str">
         <f>'compile results'!D181</f>
-        <v xml:space="preserve">- hv_net_costs_per_capacity_step = </v>
+        <v xml:space="preserve">- hv_net_capacity_per_step = </v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="str">
         <f>'compile results'!D182</f>
-        <v xml:space="preserve">- hv_net_spare_capacity = </v>
+        <v xml:space="preserve">- hv_net_costs_per_capacity_step = </v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="str">
         <f>'compile results'!D183</f>
-        <v xml:space="preserve">- hv_net_total_costs_present = </v>
+        <v xml:space="preserve">- hv_net_spare_capacity = </v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="str">
         <f>'compile results'!D184</f>
-        <v xml:space="preserve">- interconnection_net_costs_present = </v>
+        <v xml:space="preserve">- hv_net_total_costs_present = </v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="str">
         <f>'compile results'!D185</f>
-        <v xml:space="preserve">- interconnector_capacity = </v>
+        <v xml:space="preserve">- interconnection_net_costs_present = </v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="str">
         <f>'compile results'!D186</f>
-        <v xml:space="preserve">- offshore_net_costs_present = </v>
+        <v xml:space="preserve">- interconnector_capacity = </v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="str">
         <f>'compile results'!D187</f>
-        <v xml:space="preserve">- annual_infrastructure_cost_gas = </v>
+        <v xml:space="preserve">- offshore_net_costs_present = </v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="str">
-        <f>'compile results'!D189</f>
-        <v xml:space="preserve">- heat_share_of_apartments_with_block_heating = </v>
+        <f>'compile results'!D188</f>
+        <v xml:space="preserve">- annual_infrastructure_cost_gas = </v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="str">
         <f>'compile results'!D190</f>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket = </v>
+        <v xml:space="preserve">- heat_share_of_apartments_with_block_heating = </v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="str">
         <f>'compile results'!D191</f>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_first_bracket = </v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="str">
         <f>'compile results'!D192</f>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_second_bracket = </v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="str">
         <f>'compile results'!D193</f>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_third_bracket = </v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="str">
         <f>'compile results'!D194</f>
-        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fourth_bracket = </v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="str">
         <f>'compile results'!D195</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_distribution_pipelines_in_meter_per_residence_object_fifth_bracket = </v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="str">
         <f>'compile results'!D196</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_first_bracket = </v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="str">
         <f>'compile results'!D197</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_second_bracket = </v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="str">
         <f>'compile results'!D198</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_third_bracket = </v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="str">
         <f>'compile results'!D199</f>
-        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fourth_bracket = </v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="str">
         <f>'compile results'!D200</f>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_length_of_connection_pipelines_in_meter_per_residence_fifth_bracket = </v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="str">
         <f>'compile results'!D201</f>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="str">
         <f>'compile results'!D202</f>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="str">
         <f>'compile results'!D203</f>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_without_block_heating_eur = </v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="str">
         <f>'compile results'!D204</f>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="str">
         <f>'compile results'!D205</f>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="str">
         <f>'compile results'!D206</f>
-        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_apartments_with_block_heating_eur = </v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="str">
         <f>'compile results'!D207</f>
-        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_lt_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="str">
         <f>'compile results'!D208</f>
-        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_mt_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="str">
         <f>'compile results'!D209</f>
-        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_infrastructure_households_ht_indoor_investment_costs_ground_level_houses_eur = </v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="str">
         <f>'compile results'!D210</f>
-        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="str">
         <f>'compile results'!D211</f>
-        <v xml:space="preserve">- heat_exchanger_station_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_buildings_indoor_investment_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="str">
         <f>'compile results'!D212</f>
-        <v xml:space="preserve">- heat_lt_sub_station_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_exchanger_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="str">
         <f>'compile results'!D213</f>
-        <v xml:space="preserve">- heat_mt_sub_station_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_lt_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="str">
         <f>'compile results'!D214</f>
-        <v xml:space="preserve">- heat_ht_sub_station_investment_costs_eur_per_kw = </v>
+        <v xml:space="preserve">- heat_mt_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="str">
         <f>'compile results'!D215</f>
-        <v xml:space="preserve">- heat_lt_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <v xml:space="preserve">- heat_ht_sub_station_investment_costs_eur_per_kw = </v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="str">
         <f>'compile results'!D216</f>
-        <v xml:space="preserve">- heat_mt_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <v xml:space="preserve">- heat_lt_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="str">
         <f>'compile results'!D217</f>
-        <v xml:space="preserve">- heat_ht_distribution_pipelines_investment_costs_eur_per_meter = </v>
+        <v xml:space="preserve">- heat_mt_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="str">
         <f>'compile results'!D218</f>
-        <v xml:space="preserve">- heat_lt_primary_pipelines_investment_costs_per_kw = </v>
+        <v xml:space="preserve">- heat_ht_distribution_pipelines_investment_costs_eur_per_meter = </v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="str">
         <f>'compile results'!D219</f>
-        <v xml:space="preserve">- heat_mt_primary_pipelines_investment_costs_per_kw = </v>
+        <v xml:space="preserve">- heat_lt_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="str">
         <f>'compile results'!D220</f>
-        <v xml:space="preserve">- heat_ht_primary_pipelines_investment_costs_per_kw = </v>
+        <v xml:space="preserve">- heat_mt_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="str">
         <f>'compile results'!D221</f>
-        <v xml:space="preserve">- heat_yearly_indoor_infrastructure_maintenance_costs_factor = </v>
+        <v xml:space="preserve">- heat_ht_primary_pipelines_investment_costs_per_kw = </v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="str">
         <f>'compile results'!D222</f>
-        <v xml:space="preserve">- heat_yearly_outdoor_infrastructure_maintenance_costs_factor = </v>
+        <v xml:space="preserve">- heat_yearly_indoor_infrastructure_maintenance_costs_factor = </v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="str">
         <f>'compile results'!D223</f>
-        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <v xml:space="preserve">- heat_yearly_outdoor_infrastructure_maintenance_costs_factor = </v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="str">
         <f>'compile results'!D224</f>
-        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="str">
         <f>'compile results'!D225</f>
-        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_apartments_eur_per_connection = </v>
+        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="str">
         <f>'compile results'!D226</f>
-        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_apartments_eur_per_connection = </v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="str">
         <f>'compile results'!D227</f>
-        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <v xml:space="preserve">- households_lt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="str">
         <f>'compile results'!D228</f>
-        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
+        <v xml:space="preserve">- households_mt_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="str">
         <f>'compile results'!D229</f>
-        <v xml:space="preserve">- buildings_lt_heat_delivery_system_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- households_ht_heat_delivery_system_costs_ground_level_houses_eur_per_connection = </v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="str">
         <f>'compile results'!D230</f>
-        <v xml:space="preserve">- buildings_mt_heat_delivery_system_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- buildings_lt_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="str">
         <f>'compile results'!D231</f>
-        <v xml:space="preserve">- buildings_ht_heat_delivery_system_costs_eur_per_connection = </v>
+        <v xml:space="preserve">- buildings_mt_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="str">
-        <f>'compile results'!D234</f>
-        <v xml:space="preserve">- number_of_cars = </v>
+        <f>'compile results'!D232</f>
+        <v xml:space="preserve">- buildings_ht_heat_delivery_system_costs_eur_per_connection = </v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="str">
         <f>'compile results'!D235</f>
-        <v xml:space="preserve">- number_of_busses = </v>
+        <v xml:space="preserve">- number_of_cars = </v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="str">
         <f>'compile results'!D236</f>
-        <v xml:space="preserve">- number_of_trucks = </v>
+        <v xml:space="preserve">- number_of_busses = </v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="str">
         <f>'compile results'!D237</f>
-        <v xml:space="preserve">- number_of_vans = </v>
+        <v xml:space="preserve">- number_of_trucks = </v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="str">
         <f>'compile results'!D238</f>
-        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
+        <v xml:space="preserve">- number_of_vans = </v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="str">
         <f>'compile results'!D239</f>
-        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
+        <v xml:space="preserve">- electric_vehicle_profile_1_share = </v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="str">
         <f>'compile results'!D240</f>
-        <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
+        <v xml:space="preserve">- electric_vehicle_profile_2_share = </v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="str">
         <f>'compile results'!D241</f>
-        <v xml:space="preserve">- electric_vehicle_profile_4_share = </v>
+        <v xml:space="preserve">- electric_vehicle_profile_3_share = </v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="str">
         <f>'compile results'!D242</f>
+        <v xml:space="preserve">- electric_vehicle_profile_4_share = </v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" t="str">
+        <f>'compile results'!D243</f>
         <v xml:space="preserve">- electric_vehicle_profile_5_share = </v>
       </c>
     </row>

</xml_diff>